<commit_message>
update infilled stock-recruit data time series
</commit_message>
<xml_diff>
--- a/3. outputs/Stock-recruit data/Barkley_Sockeye_stock-recruit_infilled.xlsx
+++ b/3. outputs/Stock-recruit data/Barkley_Sockeye_stock-recruit_infilled.xlsx
@@ -469,12 +469,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>H</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Annual terminal catch</t>
+          <t>Annual terminal harvest (i.e. catch)</t>
         </is>
       </c>
     </row>
@@ -505,24 +505,24 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>hr_pred</t>
+          <t>H_cv</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Retrospective prediction of harvest rate for Hucuktlis Sockeye based on a linear model with Somass Sockeye harvest rate as a predictor. Used to estimate Hucuktlis catch in years with missing data</t>
+          <t>Coefficient of variation on harvest data. Historical (prior to 2011) Hucuktlis Sockeye harvest rate predictions were derived from a linear model. CV for these data is calculated as RMSE of the model residuals divided by the mean of the observed Hucuktlis Sockeye harvest rates that informed the model fit (i.e. the dependent variable). Harvest data for Somass and Hucuktlis post-2011 are assumed to be precise.</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>hr_pred_cv</t>
+          <t>S_cv</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Coefficient of variation of Hucuktlis Sockeye harvest rate predictions derived from the linear model. Calculated as RMSE of the model residuals divided by the mean of the observed Hucuktlis Sockeye harvest rates that informed the model fit (i.e. the dependent variable)</t>
+          <t>Coefficient of variation on spawner data. Currently based on ____</t>
         </is>
       </c>
     </row>
@@ -582,7 +582,7 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>H</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
@@ -597,12 +597,12 @@
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>hr_pred</t>
+          <t>H_cv</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>hr_pred_cv</t>
+          <t>S_cv</t>
         </is>
       </c>
     </row>
@@ -642,6 +642,12 @@
       <c r="K2">
         <v>633742.5637903768</v>
       </c>
+      <c r="L2">
+        <v>0.05</v>
+      </c>
+      <c r="M2">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3">
@@ -679,6 +685,12 @@
       <c r="K3">
         <v>495061.8834075385</v>
       </c>
+      <c r="L3">
+        <v>0.05</v>
+      </c>
+      <c r="M3">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4">
@@ -716,6 +728,12 @@
       <c r="K4">
         <v>526832.3053483891</v>
       </c>
+      <c r="L4">
+        <v>0.05</v>
+      </c>
+      <c r="M4">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5">
@@ -753,6 +771,12 @@
       <c r="K5">
         <v>552803.0040534479</v>
       </c>
+      <c r="L5">
+        <v>0.05</v>
+      </c>
+      <c r="M5">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -790,6 +814,12 @@
       <c r="K6">
         <v>913809.5845034227</v>
       </c>
+      <c r="L6">
+        <v>0.05</v>
+      </c>
+      <c r="M6">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7">
@@ -827,6 +857,12 @@
       <c r="K7">
         <v>570766.8540090187</v>
       </c>
+      <c r="L7">
+        <v>0.05</v>
+      </c>
+      <c r="M7">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8">
@@ -864,6 +900,12 @@
       <c r="K8">
         <v>480598.2568144404</v>
       </c>
+      <c r="L8">
+        <v>0.05</v>
+      </c>
+      <c r="M8">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9">
@@ -901,6 +943,12 @@
       <c r="K9">
         <v>391376.4267260354</v>
       </c>
+      <c r="L9">
+        <v>0.05</v>
+      </c>
+      <c r="M9">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10">
@@ -938,6 +986,12 @@
       <c r="K10">
         <v>224122.9386567897</v>
       </c>
+      <c r="L10">
+        <v>0.05</v>
+      </c>
+      <c r="M10">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11">
@@ -975,6 +1029,12 @@
       <c r="K11">
         <v>288014.3071424381</v>
       </c>
+      <c r="L11">
+        <v>0.05</v>
+      </c>
+      <c r="M11">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12">
@@ -1012,6 +1072,12 @@
       <c r="K12">
         <v>137076.4333190075</v>
       </c>
+      <c r="L12">
+        <v>0.05</v>
+      </c>
+      <c r="M12">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13">
@@ -1049,6 +1115,12 @@
       <c r="K13">
         <v>203184.164250254</v>
       </c>
+      <c r="L13">
+        <v>0.05</v>
+      </c>
+      <c r="M13">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14">
@@ -1086,6 +1158,12 @@
       <c r="K14">
         <v>503092.30271186</v>
       </c>
+      <c r="L14">
+        <v>0.05</v>
+      </c>
+      <c r="M14">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15">
@@ -1123,6 +1201,12 @@
       <c r="K15">
         <v>371601.962535504</v>
       </c>
+      <c r="L15">
+        <v>0.05</v>
+      </c>
+      <c r="M15">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16">
@@ -1160,6 +1244,12 @@
       <c r="K16">
         <v>206726.5366225715</v>
       </c>
+      <c r="L16">
+        <v>0.05</v>
+      </c>
+      <c r="M16">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17">
@@ -1197,6 +1287,12 @@
       <c r="K17">
         <v>340157.6785086803</v>
       </c>
+      <c r="L17">
+        <v>0.05</v>
+      </c>
+      <c r="M17">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18">
@@ -1234,6 +1330,12 @@
       <c r="K18">
         <v>292061.9392067303</v>
       </c>
+      <c r="L18">
+        <v>0.05</v>
+      </c>
+      <c r="M18">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19">
@@ -1271,6 +1373,12 @@
       <c r="K19">
         <v>172160.3662147925</v>
       </c>
+      <c r="L19">
+        <v>0.05</v>
+      </c>
+      <c r="M19">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20">
@@ -1308,6 +1416,12 @@
       <c r="K20">
         <v>274311.7730009329</v>
       </c>
+      <c r="L20">
+        <v>0.05</v>
+      </c>
+      <c r="M20">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21">
@@ -1345,6 +1459,12 @@
       <c r="K21">
         <v>265697.028795797</v>
       </c>
+      <c r="L21">
+        <v>0.05</v>
+      </c>
+      <c r="M21">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22">
@@ -1382,6 +1502,12 @@
       <c r="K22">
         <v>1258256.636990258</v>
       </c>
+      <c r="L22">
+        <v>0.05</v>
+      </c>
+      <c r="M22">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23">
@@ -1419,6 +1545,12 @@
       <c r="K23">
         <v>652446.9029476116</v>
       </c>
+      <c r="L23">
+        <v>0.05</v>
+      </c>
+      <c r="M23">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24">
@@ -1456,6 +1588,12 @@
       <c r="K24">
         <v>599789.3466079192</v>
       </c>
+      <c r="L24">
+        <v>0.05</v>
+      </c>
+      <c r="M24">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25">
@@ -1493,6 +1631,12 @@
       <c r="K25">
         <v>625355.4802804298</v>
       </c>
+      <c r="L25">
+        <v>0.05</v>
+      </c>
+      <c r="M25">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26">
@@ -1530,6 +1674,12 @@
       <c r="K26">
         <v>400875.0350328542</v>
       </c>
+      <c r="L26">
+        <v>0.05</v>
+      </c>
+      <c r="M26">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27">
@@ -1567,6 +1717,12 @@
       <c r="K27">
         <v>407468.2247957478</v>
       </c>
+      <c r="L27">
+        <v>0.05</v>
+      </c>
+      <c r="M27">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28">
@@ -1604,6 +1760,12 @@
       <c r="K28">
         <v>138601.997986058</v>
       </c>
+      <c r="L28">
+        <v>0.05</v>
+      </c>
+      <c r="M28">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29">
@@ -1641,6 +1803,12 @@
       <c r="K29">
         <v>181984.1898199186</v>
       </c>
+      <c r="L29">
+        <v>0.05</v>
+      </c>
+      <c r="M29">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30">
@@ -1678,6 +1846,12 @@
       <c r="K30">
         <v>74102.68990164486</v>
       </c>
+      <c r="L30">
+        <v>0.05</v>
+      </c>
+      <c r="M30">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31">
@@ -1715,6 +1889,12 @@
       <c r="K31">
         <v>59697.7030353223</v>
       </c>
+      <c r="L31">
+        <v>0.05</v>
+      </c>
+      <c r="M31">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32">
@@ -1752,6 +1932,12 @@
       <c r="K32">
         <v>290004.5944304451</v>
       </c>
+      <c r="L32">
+        <v>0.05</v>
+      </c>
+      <c r="M32">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33">
@@ -1789,6 +1975,12 @@
       <c r="K33">
         <v>320116.8393461921</v>
       </c>
+      <c r="L33">
+        <v>0.05</v>
+      </c>
+      <c r="M33">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34">
@@ -1826,6 +2018,12 @@
       <c r="K34">
         <v>421979.6878094974</v>
       </c>
+      <c r="L34">
+        <v>0.05</v>
+      </c>
+      <c r="M34">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35">
@@ -1863,6 +2061,12 @@
       <c r="K35">
         <v>263927.9811106482</v>
       </c>
+      <c r="L35">
+        <v>0.05</v>
+      </c>
+      <c r="M35">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36">
@@ -1900,6 +2104,12 @@
       <c r="K36">
         <v>240203.9760283087</v>
       </c>
+      <c r="L36">
+        <v>0.05</v>
+      </c>
+      <c r="M36">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37">
@@ -1937,6 +2147,12 @@
       <c r="K37">
         <v>189096.9567127897</v>
       </c>
+      <c r="L37">
+        <v>0.05</v>
+      </c>
+      <c r="M37">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38">
@@ -1974,6 +2190,12 @@
       <c r="K38">
         <v>241682.5691475399</v>
       </c>
+      <c r="L38">
+        <v>0.05</v>
+      </c>
+      <c r="M38">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39">
@@ -2011,6 +2233,12 @@
       <c r="K39">
         <v>386548.9231194458</v>
       </c>
+      <c r="L39">
+        <v>0.05</v>
+      </c>
+      <c r="M39">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40">
@@ -2048,6 +2276,12 @@
       <c r="K40">
         <v>261943.5622247388</v>
       </c>
+      <c r="L40">
+        <v>0.05</v>
+      </c>
+      <c r="M40">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41">
@@ -2085,6 +2319,12 @@
       <c r="K41">
         <v>145416.8103652774</v>
       </c>
+      <c r="L41">
+        <v>0.05</v>
+      </c>
+      <c r="M41">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42">
@@ -2122,6 +2362,12 @@
       <c r="K42">
         <v>717175.1613370343</v>
       </c>
+      <c r="L42">
+        <v>0.05</v>
+      </c>
+      <c r="M42">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43">
@@ -2159,6 +2405,12 @@
       <c r="K43">
         <v>326804.0013846449</v>
       </c>
+      <c r="L43">
+        <v>0.05</v>
+      </c>
+      <c r="M43">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44">
@@ -2196,6 +2448,12 @@
       <c r="K44">
         <v>518419.7394188421</v>
       </c>
+      <c r="L44">
+        <v>0.05</v>
+      </c>
+      <c r="M44">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45">
@@ -2233,6 +2491,12 @@
       <c r="K45">
         <v>732603.6241928141</v>
       </c>
+      <c r="L45">
+        <v>0.05</v>
+      </c>
+      <c r="M45">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46">
@@ -2270,6 +2534,12 @@
       <c r="K46">
         <v>569643.4153128543</v>
       </c>
+      <c r="L46">
+        <v>0.05</v>
+      </c>
+      <c r="M46">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47">
@@ -2307,6 +2577,12 @@
       <c r="K47">
         <v>353959.4130974241</v>
       </c>
+      <c r="L47">
+        <v>0.05</v>
+      </c>
+      <c r="M47">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48">
@@ -2344,6 +2620,12 @@
       <c r="K48">
         <v>213509.8577738418</v>
       </c>
+      <c r="L48">
+        <v>0.05</v>
+      </c>
+      <c r="M48">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49">
@@ -2381,6 +2663,12 @@
       <c r="K49">
         <v>219482.3284506314</v>
       </c>
+      <c r="L49">
+        <v>0.05</v>
+      </c>
+      <c r="M49">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50">
@@ -2418,6 +2706,12 @@
       <c r="K50">
         <v>329840.2664919504</v>
       </c>
+      <c r="L50">
+        <v>0.05</v>
+      </c>
+      <c r="M50">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51">
@@ -2455,6 +2749,12 @@
       <c r="K51">
         <v>150478.2895093822</v>
       </c>
+      <c r="L51">
+        <v>0.05</v>
+      </c>
+      <c r="M51">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52">
@@ -2492,6 +2792,12 @@
       <c r="K52">
         <v>97065.40537030963</v>
       </c>
+      <c r="L52">
+        <v>0.05</v>
+      </c>
+      <c r="M52">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53">
@@ -2529,6 +2835,12 @@
       <c r="K53">
         <v>131772.1820819404</v>
       </c>
+      <c r="L53">
+        <v>0.05</v>
+      </c>
+      <c r="M53">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54">
@@ -2566,6 +2878,12 @@
       <c r="K54">
         <v>17687.78978304791</v>
       </c>
+      <c r="L54">
+        <v>0.05</v>
+      </c>
+      <c r="M54">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55">
@@ -2603,6 +2921,12 @@
       <c r="K55">
         <v>21882.51302978364</v>
       </c>
+      <c r="L55">
+        <v>0.05</v>
+      </c>
+      <c r="M55">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56">
@@ -2640,6 +2964,12 @@
       <c r="K56">
         <v>189217.8905235089</v>
       </c>
+      <c r="L56">
+        <v>0.05</v>
+      </c>
+      <c r="M56">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57">
@@ -2677,6 +3007,12 @@
       <c r="K57">
         <v>114009.339885825</v>
       </c>
+      <c r="L57">
+        <v>0.05</v>
+      </c>
+      <c r="M57">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58">
@@ -2714,6 +3050,12 @@
       <c r="K58">
         <v>454549.7827114371</v>
       </c>
+      <c r="L58">
+        <v>0.05</v>
+      </c>
+      <c r="M58">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59">
@@ -2751,6 +3093,12 @@
       <c r="K59">
         <v>333891.8889857767</v>
       </c>
+      <c r="L59">
+        <v>0.05</v>
+      </c>
+      <c r="M59">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60">
@@ -2788,6 +3136,12 @@
       <c r="K60">
         <v>966912.7522210542</v>
       </c>
+      <c r="L60">
+        <v>0.05</v>
+      </c>
+      <c r="M60">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61">
@@ -2825,6 +3179,12 @@
       <c r="K61">
         <v>885638.3882038471</v>
       </c>
+      <c r="L61">
+        <v>0.05</v>
+      </c>
+      <c r="M61">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62">
@@ -2862,6 +3222,12 @@
       <c r="K62">
         <v>645290.4618712433</v>
       </c>
+      <c r="L62">
+        <v>0.05</v>
+      </c>
+      <c r="M62">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63">
@@ -2899,6 +3265,12 @@
       <c r="K63">
         <v>811357.3188160737</v>
       </c>
+      <c r="L63">
+        <v>0.05</v>
+      </c>
+      <c r="M63">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64">
@@ -2936,6 +3308,12 @@
       <c r="K64">
         <v>100032.3097210799</v>
       </c>
+      <c r="L64">
+        <v>0.05</v>
+      </c>
+      <c r="M64">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65">
@@ -2973,6 +3351,12 @@
       <c r="K65">
         <v>271240.703074521</v>
       </c>
+      <c r="L65">
+        <v>0.05</v>
+      </c>
+      <c r="M65">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66">
@@ -3010,6 +3394,12 @@
       <c r="K66">
         <v>147482.6115069279</v>
       </c>
+      <c r="L66">
+        <v>0.05</v>
+      </c>
+      <c r="M66">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67">
@@ -3047,6 +3437,12 @@
       <c r="K67">
         <v>304274.706182281</v>
       </c>
+      <c r="L67">
+        <v>0.05</v>
+      </c>
+      <c r="M67">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68">
@@ -3084,6 +3480,12 @@
       <c r="K68">
         <v>530209.3761206279</v>
       </c>
+      <c r="L68">
+        <v>0.05</v>
+      </c>
+      <c r="M68">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69">
@@ -3121,6 +3523,12 @@
       <c r="K69">
         <v>1046784.042950014</v>
       </c>
+      <c r="L69">
+        <v>0.05</v>
+      </c>
+      <c r="M69">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70">
@@ -3158,6 +3566,12 @@
       <c r="K70">
         <v>1383229.190991441</v>
       </c>
+      <c r="L70">
+        <v>0.05</v>
+      </c>
+      <c r="M70">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71">
@@ -3195,6 +3609,12 @@
       <c r="K71">
         <v>1456288.889933172</v>
       </c>
+      <c r="L71">
+        <v>0.05</v>
+      </c>
+      <c r="M71">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72">
@@ -3232,6 +3652,12 @@
       <c r="K72">
         <v>189975.3795417092</v>
       </c>
+      <c r="L72">
+        <v>0.05</v>
+      </c>
+      <c r="M72">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73">
@@ -3269,6 +3695,12 @@
       <c r="K73">
         <v>265560.8989697707</v>
       </c>
+      <c r="L73">
+        <v>0.05</v>
+      </c>
+      <c r="M73">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74">
@@ -3306,6 +3738,12 @@
       <c r="K74">
         <v>31701.9128248074</v>
       </c>
+      <c r="L74">
+        <v>0.05</v>
+      </c>
+      <c r="M74">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75">
@@ -3343,6 +3781,12 @@
       <c r="K75">
         <v>74647.11735710694</v>
       </c>
+      <c r="L75">
+        <v>0.05</v>
+      </c>
+      <c r="M75">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76">
@@ -3380,6 +3824,12 @@
       <c r="K76">
         <v>99890.87941789668</v>
       </c>
+      <c r="L76">
+        <v>0.05</v>
+      </c>
+      <c r="M76">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77">
@@ -3417,6 +3867,12 @@
       <c r="K77">
         <v>421399.4024497316</v>
       </c>
+      <c r="L77">
+        <v>0.05</v>
+      </c>
+      <c r="M77">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78">
@@ -3454,6 +3910,12 @@
       <c r="K78">
         <v>140758.2659394757</v>
       </c>
+      <c r="L78">
+        <v>0.05</v>
+      </c>
+      <c r="M78">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79">
@@ -3491,6 +3953,12 @@
       <c r="K79">
         <v>103582.4907797132</v>
       </c>
+      <c r="L79">
+        <v>0.05</v>
+      </c>
+      <c r="M79">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80">
@@ -3528,6 +3996,12 @@
       <c r="K80">
         <v>291403.081691474</v>
       </c>
+      <c r="L80">
+        <v>0.05</v>
+      </c>
+      <c r="M80">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81">
@@ -3565,6 +4039,12 @@
       <c r="K81">
         <v>293354.5109088812</v>
       </c>
+      <c r="L81">
+        <v>0.05</v>
+      </c>
+      <c r="M81">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82">
@@ -3602,6 +4082,12 @@
       <c r="K82">
         <v>340480.2751862371</v>
       </c>
+      <c r="L82">
+        <v>0.05</v>
+      </c>
+      <c r="M82">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83">
@@ -3639,6 +4125,12 @@
       <c r="K83">
         <v>132750.731163154</v>
       </c>
+      <c r="L83">
+        <v>0.05</v>
+      </c>
+      <c r="M83">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84">
@@ -3676,6 +4168,12 @@
       <c r="K84">
         <v>134672.3830344016</v>
       </c>
+      <c r="L84">
+        <v>0.05</v>
+      </c>
+      <c r="M84">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85">
@@ -3713,6 +4211,12 @@
       <c r="K85">
         <v>749912.0346085769</v>
       </c>
+      <c r="L85">
+        <v>0.05</v>
+      </c>
+      <c r="M85">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86">
@@ -3750,6 +4254,12 @@
       <c r="K86">
         <v>225085.0063342566</v>
       </c>
+      <c r="L86">
+        <v>0.05</v>
+      </c>
+      <c r="M86">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87">
@@ -3787,6 +4297,12 @@
       <c r="K87">
         <v>226137.5012402972</v>
       </c>
+      <c r="L87">
+        <v>0.05</v>
+      </c>
+      <c r="M87">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88">
@@ -3824,6 +4340,12 @@
       <c r="K88">
         <v>90778.66436880779</v>
       </c>
+      <c r="L88">
+        <v>0.05</v>
+      </c>
+      <c r="M88">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89">
@@ -3861,6 +4383,12 @@
       <c r="K89">
         <v>34453.35591884049</v>
       </c>
+      <c r="L89">
+        <v>0.05</v>
+      </c>
+      <c r="M89">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90">
@@ -3895,6 +4423,12 @@
       <c r="J90">
         <v>1000</v>
       </c>
+      <c r="L90">
+        <v>0.05</v>
+      </c>
+      <c r="M90">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91">
@@ -3929,6 +4463,12 @@
       <c r="J91">
         <v>1000</v>
       </c>
+      <c r="L91">
+        <v>0.05</v>
+      </c>
+      <c r="M91">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92">
@@ -3963,6 +4503,12 @@
       <c r="J92">
         <v>1000</v>
       </c>
+      <c r="L92">
+        <v>0.05</v>
+      </c>
+      <c r="M92">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93">
@@ -3997,6 +4543,12 @@
       <c r="J93">
         <v>1000</v>
       </c>
+      <c r="L93">
+        <v>0.05</v>
+      </c>
+      <c r="M93">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94">
@@ -4031,6 +4583,12 @@
       <c r="J94">
         <v>1000</v>
       </c>
+      <c r="L94">
+        <v>0.05</v>
+      </c>
+      <c r="M94">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95">
@@ -4065,6 +4623,12 @@
       <c r="J95">
         <v>1000</v>
       </c>
+      <c r="L95">
+        <v>0.05</v>
+      </c>
+      <c r="M95">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96">
@@ -4091,10 +4655,10 @@
         <v>221</v>
       </c>
       <c r="L96">
-        <v>0.7414725101597354</v>
+        <v>0.3899491183848233</v>
       </c>
       <c r="M96">
-        <v>0.3899491183848233</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="97">
@@ -4122,10 +4686,10 @@
         <v>214</v>
       </c>
       <c r="L97">
-        <v>0.485512768769336</v>
+        <v>0.3899491183848233</v>
       </c>
       <c r="M97">
-        <v>0.3899491183848233</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="98">
@@ -4153,10 +4717,10 @@
         <v>83</v>
       </c>
       <c r="L98">
-        <v>0.610714806835185</v>
+        <v>0.3899491183848233</v>
       </c>
       <c r="M98">
-        <v>0.3899491183848233</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="99">
@@ -4193,10 +4757,10 @@
         <v>187</v>
       </c>
       <c r="L99">
-        <v>0.5547049582226626</v>
+        <v>0.3899491183848233</v>
       </c>
       <c r="M99">
-        <v>0.3899491183848233</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="100">
@@ -4233,10 +4797,10 @@
         <v>288</v>
       </c>
       <c r="L100">
-        <v>0.6676769174853291</v>
+        <v>0.3899491183848233</v>
       </c>
       <c r="M100">
-        <v>0.3899491183848233</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="101">
@@ -4273,10 +4837,10 @@
         <v>294</v>
       </c>
       <c r="L101">
-        <v>0.4273394033349465</v>
+        <v>0.3899491183848233</v>
       </c>
       <c r="M101">
-        <v>0.3899491183848233</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="102">
@@ -4313,10 +4877,10 @@
         <v>293</v>
       </c>
       <c r="L102">
-        <v>0.5229290731442615</v>
+        <v>0.3899491183848233</v>
       </c>
       <c r="M102">
-        <v>0.3899491183848233</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="103">
@@ -4353,10 +4917,10 @@
         <v>159</v>
       </c>
       <c r="L103">
-        <v>0.7631938199023311</v>
+        <v>0.3899491183848233</v>
       </c>
       <c r="M103">
-        <v>0.3899491183848233</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="104">
@@ -4393,10 +4957,10 @@
         <v>82</v>
       </c>
       <c r="L104">
-        <v>0.5652470201792948</v>
+        <v>0.3899491183848233</v>
       </c>
       <c r="M104">
-        <v>0.3899491183848233</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="105">
@@ -4433,10 +4997,10 @@
         <v>122</v>
       </c>
       <c r="L105">
-        <v>0.02440289664453979</v>
+        <v>0.3899491183848233</v>
       </c>
       <c r="M105">
-        <v>0.3899491183848233</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="106">
@@ -4473,10 +5037,10 @@
         <v>446</v>
       </c>
       <c r="L106">
-        <v>0.2679638588650132</v>
+        <v>0.3899491183848233</v>
       </c>
       <c r="M106">
-        <v>0.3899491183848233</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="107">
@@ -4513,10 +5077,10 @@
         <v>151</v>
       </c>
       <c r="L107">
-        <v>0.3335498306913548</v>
+        <v>0.3899491183848233</v>
       </c>
       <c r="M107">
-        <v>0.3899491183848233</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="108">
@@ -4553,10 +5117,10 @@
         <v>309</v>
       </c>
       <c r="L108">
-        <v>0</v>
+        <v>0.3899491183848233</v>
       </c>
       <c r="M108">
-        <v>0.3899491183848233</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="109">
@@ -4593,10 +5157,10 @@
         <v>312</v>
       </c>
       <c r="L109">
-        <v>0</v>
+        <v>0.3899491183848233</v>
       </c>
       <c r="M109">
-        <v>0.3899491183848233</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="110">
@@ -4633,10 +5197,10 @@
         <v>325</v>
       </c>
       <c r="L110">
-        <v>0.5809874085884461</v>
+        <v>0.3899491183848233</v>
       </c>
       <c r="M110">
-        <v>0.3899491183848233</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="111">
@@ -4673,10 +5237,10 @@
         <v>312</v>
       </c>
       <c r="L111">
-        <v>0.5101595069430539</v>
+        <v>0.3899491183848233</v>
       </c>
       <c r="M111">
-        <v>0.3899491183848233</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="112">
@@ -4713,10 +5277,10 @@
         <v>234</v>
       </c>
       <c r="L112">
-        <v>0.570325061128269</v>
+        <v>0.3899491183848233</v>
       </c>
       <c r="M112">
-        <v>0.3899491183848233</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="113">
@@ -4753,10 +5317,10 @@
         <v>254</v>
       </c>
       <c r="L113">
-        <v>0.3190950571486335</v>
+        <v>0.3899491183848233</v>
       </c>
       <c r="M113">
-        <v>0.3899491183848233</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="114">
@@ -4793,10 +5357,10 @@
         <v>70</v>
       </c>
       <c r="L114">
-        <v>0.03315770876945662</v>
+        <v>0.3899491183848233</v>
       </c>
       <c r="M114">
-        <v>0.3899491183848233</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="115">
@@ -4833,10 +5397,10 @@
         <v>253</v>
       </c>
       <c r="L115">
-        <v>0</v>
+        <v>0.3899491183848233</v>
       </c>
       <c r="M115">
-        <v>0.3899491183848233</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="116">
@@ -4873,10 +5437,10 @@
         <v>97</v>
       </c>
       <c r="L116">
-        <v>0.2128433186821031</v>
+        <v>0.3899491183848233</v>
       </c>
       <c r="M116">
-        <v>0.3899491183848233</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="117">
@@ -4913,10 +5477,10 @@
         <v>364</v>
       </c>
       <c r="L117">
-        <v>0.1675522394757942</v>
+        <v>0.3899491183848233</v>
       </c>
       <c r="M117">
-        <v>0.3899491183848233</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="118">
@@ -4953,10 +5517,10 @@
         <v>33</v>
       </c>
       <c r="L118">
-        <v>0.1186747358609</v>
+        <v>0.3899491183848233</v>
       </c>
       <c r="M118">
-        <v>0.3899491183848233</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="119">
@@ -4993,10 +5557,10 @@
         <v>247</v>
       </c>
       <c r="L119">
-        <v>0.2471314403711639</v>
+        <v>0.3899491183848233</v>
       </c>
       <c r="M119">
-        <v>0.3899491183848233</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="120">
@@ -5033,10 +5597,10 @@
         <v>230</v>
       </c>
       <c r="L120">
-        <v>0.1161069924638074</v>
+        <v>0.3899491183848233</v>
       </c>
       <c r="M120">
-        <v>0.3899491183848233</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="121">
@@ -5073,10 +5637,10 @@
         <v>137</v>
       </c>
       <c r="L121">
-        <v>0.4650251294531451</v>
+        <v>0.3899491183848233</v>
       </c>
       <c r="M121">
-        <v>0.3899491183848233</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="122">
@@ -5101,10 +5665,10 @@
         <v>0</v>
       </c>
       <c r="L122">
-        <v>0.4711059479127299</v>
+        <v>0.3899491183848233</v>
       </c>
       <c r="M122">
-        <v>0.3899491183848233</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="123">
@@ -5129,10 +5693,10 @@
         <v>0</v>
       </c>
       <c r="L123">
-        <v>0.3866800884207761</v>
+        <v>0.3899491183848233</v>
       </c>
       <c r="M123">
-        <v>0.3899491183848233</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="124">
@@ -5157,10 +5721,10 @@
         <v>0</v>
       </c>
       <c r="L124">
-        <v>0.1205894356355219</v>
+        <v>0.3899491183848233</v>
       </c>
       <c r="M124">
-        <v>0.3899491183848233</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="125">
@@ -5185,10 +5749,10 @@
         <v>0</v>
       </c>
       <c r="L125">
-        <v>0.2074441584542309</v>
+        <v>0.3899491183848233</v>
       </c>
       <c r="M125">
-        <v>0.3899491183848233</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="126">
@@ -5225,10 +5789,10 @@
         <v>94</v>
       </c>
       <c r="L126">
-        <v>0</v>
+        <v>0.3899491183848233</v>
       </c>
       <c r="M126">
-        <v>0.3899491183848233</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="127">
@@ -5265,10 +5829,10 @@
         <v>52</v>
       </c>
       <c r="L127">
-        <v>0</v>
+        <v>0.3899491183848233</v>
       </c>
       <c r="M127">
-        <v>0.3899491183848233</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="128">
@@ -5305,10 +5869,10 @@
         <v>303</v>
       </c>
       <c r="L128">
-        <v>0.16420697329429</v>
+        <v>0.3899491183848233</v>
       </c>
       <c r="M128">
-        <v>0.3899491183848233</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="129">
@@ -5345,10 +5909,10 @@
         <v>67</v>
       </c>
       <c r="L129">
-        <v>0.4628687243855083</v>
+        <v>0.3899491183848233</v>
       </c>
       <c r="M129">
-        <v>0.3899491183848233</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="130">
@@ -5384,6 +5948,12 @@
       <c r="J130">
         <v>62</v>
       </c>
+      <c r="L130">
+        <v>0.05</v>
+      </c>
+      <c r="M130">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131">
@@ -5418,6 +5988,12 @@
       <c r="J131">
         <v>47</v>
       </c>
+      <c r="L131">
+        <v>0.05</v>
+      </c>
+      <c r="M131">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132">
@@ -5452,6 +6028,12 @@
       <c r="J132">
         <v>36</v>
       </c>
+      <c r="L132">
+        <v>0.05</v>
+      </c>
+      <c r="M132">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133">
@@ -5486,6 +6068,12 @@
       <c r="J133">
         <v>76</v>
       </c>
+      <c r="L133">
+        <v>0.05</v>
+      </c>
+      <c r="M133">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134">
@@ -5520,6 +6108,12 @@
       <c r="J134">
         <v>2</v>
       </c>
+      <c r="L134">
+        <v>0.05</v>
+      </c>
+      <c r="M134">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135">
@@ -5554,6 +6148,12 @@
       <c r="J135">
         <v>119</v>
       </c>
+      <c r="L135">
+        <v>0.05</v>
+      </c>
+      <c r="M135">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136">
@@ -5588,6 +6188,12 @@
       <c r="J136">
         <v>44</v>
       </c>
+      <c r="L136">
+        <v>0.05</v>
+      </c>
+      <c r="M136">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137">
@@ -5622,6 +6228,12 @@
       <c r="J137">
         <v>28</v>
       </c>
+      <c r="L137">
+        <v>0.05</v>
+      </c>
+      <c r="M137">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138">
@@ -5644,6 +6256,12 @@
       <c r="J138">
         <v>0</v>
       </c>
+      <c r="L138">
+        <v>0.05</v>
+      </c>
+      <c r="M138">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139">
@@ -5666,6 +6284,12 @@
       <c r="J139">
         <v>0</v>
       </c>
+      <c r="L139">
+        <v>0.05</v>
+      </c>
+      <c r="M139">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140">
@@ -5700,6 +6324,12 @@
       <c r="J140">
         <v>7</v>
       </c>
+      <c r="L140">
+        <v>0.05</v>
+      </c>
+      <c r="M140">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141">
@@ -5734,6 +6364,12 @@
       <c r="J141">
         <v>67</v>
       </c>
+      <c r="L141">
+        <v>0.05</v>
+      </c>
+      <c r="M141">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142">
@@ -5768,6 +6404,12 @@
       <c r="J142">
         <v>151</v>
       </c>
+      <c r="L142">
+        <v>0.05</v>
+      </c>
+      <c r="M142">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143">
@@ -5793,8 +6435,11 @@
       <c r="J143">
         <v>43</v>
       </c>
+      <c r="L143">
+        <v>0.3899491183848233</v>
+      </c>
       <c r="M143">
-        <v>0.3899491183848233</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="144">
@@ -5821,8 +6466,11 @@
       <c r="J144">
         <v>99</v>
       </c>
+      <c r="L144">
+        <v>0.3899491183848233</v>
+      </c>
       <c r="M144">
-        <v>0.3899491183848233</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="145">
@@ -5849,8 +6497,11 @@
       <c r="J145">
         <v>113</v>
       </c>
+      <c r="L145">
+        <v>0.3899491183848233</v>
+      </c>
       <c r="M145">
-        <v>0.3899491183848233</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="146">
@@ -5877,8 +6528,11 @@
       <c r="J146">
         <v>195</v>
       </c>
+      <c r="L146">
+        <v>0.3899491183848233</v>
+      </c>
       <c r="M146">
-        <v>0.3899491183848233</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="147">
@@ -5905,8 +6559,11 @@
       <c r="J147">
         <v>191</v>
       </c>
+      <c r="L147">
+        <v>0.3899491183848233</v>
+      </c>
       <c r="M147">
-        <v>0.3899491183848233</v>
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update collated S-R data with new Hucuktlis age samples
</commit_message>
<xml_diff>
--- a/3. outputs/Stock-recruit data/Barkley_Sockeye_stock-recruit_infilled.xlsx
+++ b/3. outputs/Stock-recruit data/Barkley_Sockeye_stock-recruit_infilled.xlsx
@@ -6247,6 +6247,18 @@
       <c r="C138">
         <v>13549</v>
       </c>
+      <c r="D138">
+        <v>0</v>
+      </c>
+      <c r="E138">
+        <v>0</v>
+      </c>
+      <c r="F138">
+        <v>1</v>
+      </c>
+      <c r="G138">
+        <v>0</v>
+      </c>
       <c r="H138">
         <v>13703</v>
       </c>
@@ -6254,7 +6266,7 @@
         <v>154</v>
       </c>
       <c r="J138">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="L138">
         <v>0.05</v>
@@ -6347,13 +6359,13 @@
         <v>0</v>
       </c>
       <c r="E141">
-        <v>0.3582089552238806</v>
+        <v>0.3536585365853658</v>
       </c>
       <c r="F141">
-        <v>0.6268656716417911</v>
+        <v>0.6341463414634146</v>
       </c>
       <c r="G141">
-        <v>0.01492537313432836</v>
+        <v>0.01219512195121951</v>
       </c>
       <c r="H141">
         <v>26377</v>
@@ -6362,7 +6374,7 @@
         <v>7731</v>
       </c>
       <c r="J141">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="L141">
         <v>0.05</v>
@@ -6387,13 +6399,13 @@
         <v>0</v>
       </c>
       <c r="E142">
-        <v>0.1986754966887417</v>
+        <v>0.1962025316455696</v>
       </c>
       <c r="F142">
-        <v>0.7880794701986755</v>
+        <v>0.7911392405063291</v>
       </c>
       <c r="G142">
-        <v>0.01324503311258278</v>
+        <v>0.01265822784810127</v>
       </c>
       <c r="H142">
         <v>21309</v>
@@ -6402,7 +6414,7 @@
         <v>8196</v>
       </c>
       <c r="J142">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="L142">
         <v>0.05</v>

</xml_diff>

<commit_message>
save new output stock-recruit data file
</commit_message>
<xml_diff>
--- a/3. outputs/Stock-recruit data/Barkley_Sockeye_stock-recruit_infilled.xlsx
+++ b/3. outputs/Stock-recruit data/Barkley_Sockeye_stock-recruit_infilled.xlsx
@@ -533,7 +533,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M147"/>
+  <dimension ref="A1:M201"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4639,6 +4639,9 @@
           <t>HED</t>
         </is>
       </c>
+      <c r="C96">
+        <v>4800</v>
+      </c>
       <c r="D96">
         <v>0</v>
       </c>
@@ -4651,11 +4654,17 @@
       <c r="G96">
         <v>0</v>
       </c>
+      <c r="H96">
+        <v>30860</v>
+      </c>
+      <c r="I96">
+        <v>26060</v>
+      </c>
       <c r="J96">
         <v>221</v>
       </c>
       <c r="L96">
-        <v>0.3899491183848233</v>
+        <v>0.05</v>
       </c>
       <c r="M96">
         <v>0.2</v>
@@ -4670,6 +4679,9 @@
           <t>HED</t>
         </is>
       </c>
+      <c r="C97">
+        <v>7000</v>
+      </c>
       <c r="D97">
         <v>0</v>
       </c>
@@ -4682,11 +4694,17 @@
       <c r="G97">
         <v>0</v>
       </c>
+      <c r="H97">
+        <v>10832</v>
+      </c>
+      <c r="I97">
+        <v>3832</v>
+      </c>
       <c r="J97">
         <v>214</v>
       </c>
       <c r="L97">
-        <v>0.3899491183848233</v>
+        <v>0.05</v>
       </c>
       <c r="M97">
         <v>0.2</v>
@@ -4701,6 +4719,9 @@
           <t>HED</t>
         </is>
       </c>
+      <c r="C98">
+        <v>20000</v>
+      </c>
       <c r="D98">
         <v>0</v>
       </c>
@@ -4713,11 +4734,17 @@
       <c r="G98">
         <v>0</v>
       </c>
+      <c r="H98">
+        <v>143488</v>
+      </c>
+      <c r="I98">
+        <v>123488</v>
+      </c>
       <c r="J98">
         <v>83</v>
       </c>
       <c r="L98">
-        <v>0.3899491183848233</v>
+        <v>0.05</v>
       </c>
       <c r="M98">
         <v>0.2</v>
@@ -4733,7 +4760,7 @@
         </is>
       </c>
       <c r="C99">
-        <v>21000</v>
+        <v>20706</v>
       </c>
       <c r="D99">
         <v>0</v>
@@ -4748,16 +4775,16 @@
         <v>0</v>
       </c>
       <c r="H99">
-        <v>47159.7436077016</v>
+        <v>67869</v>
       </c>
       <c r="I99">
-        <v>26159.7436077016</v>
+        <v>47163</v>
       </c>
       <c r="J99">
         <v>187</v>
       </c>
       <c r="L99">
-        <v>0.3899491183848233</v>
+        <v>0.05</v>
       </c>
       <c r="M99">
         <v>0.2</v>
@@ -4773,7 +4800,7 @@
         </is>
       </c>
       <c r="C100">
-        <v>40000</v>
+        <v>58000</v>
       </c>
       <c r="D100">
         <v>0</v>
@@ -4788,16 +4815,16 @@
         <v>0</v>
       </c>
       <c r="H100">
-        <v>120364.7959007907</v>
+        <v>175758</v>
       </c>
       <c r="I100">
-        <v>80364.79590079072</v>
+        <v>117758</v>
       </c>
       <c r="J100">
         <v>288</v>
       </c>
       <c r="L100">
-        <v>0.3899491183848233</v>
+        <v>0.05</v>
       </c>
       <c r="M100">
         <v>0.2</v>
@@ -4813,7 +4840,7 @@
         </is>
       </c>
       <c r="C101">
-        <v>56000</v>
+        <v>36700</v>
       </c>
       <c r="D101">
         <v>0</v>
@@ -4828,16 +4855,16 @@
         <v>0</v>
       </c>
       <c r="H101">
-        <v>97789.16224744922</v>
+        <v>47662</v>
       </c>
       <c r="I101">
-        <v>41789.16224744923</v>
+        <v>10962</v>
       </c>
       <c r="J101">
         <v>294</v>
       </c>
       <c r="L101">
-        <v>0.3899491183848233</v>
+        <v>0.05</v>
       </c>
       <c r="M101">
         <v>0.2</v>
@@ -4853,7 +4880,7 @@
         </is>
       </c>
       <c r="C102">
-        <v>45000</v>
+        <v>31000</v>
       </c>
       <c r="D102">
         <v>0.0101010101010101</v>
@@ -4868,16 +4895,16 @@
         <v>0</v>
       </c>
       <c r="H102">
-        <v>94325.59702722685</v>
+        <v>35227</v>
       </c>
       <c r="I102">
-        <v>49325.59702722684</v>
+        <v>4227</v>
       </c>
       <c r="J102">
         <v>293</v>
       </c>
       <c r="L102">
-        <v>0.3899491183848233</v>
+        <v>0.05</v>
       </c>
       <c r="M102">
         <v>0.2</v>
@@ -4893,7 +4920,7 @@
         </is>
       </c>
       <c r="C103">
-        <v>61000</v>
+        <v>73400</v>
       </c>
       <c r="D103">
         <v>0</v>
@@ -4908,16 +4935,16 @@
         <v>0.1111111111111111</v>
       </c>
       <c r="H103">
-        <v>257594.6285474519</v>
+        <v>79532</v>
       </c>
       <c r="I103">
-        <v>196594.6285474519</v>
+        <v>6132</v>
       </c>
       <c r="J103">
         <v>159</v>
       </c>
       <c r="L103">
-        <v>0.3899491183848233</v>
+        <v>0.05</v>
       </c>
       <c r="M103">
         <v>0.2</v>
@@ -4933,7 +4960,7 @@
         </is>
       </c>
       <c r="C104">
-        <v>16000</v>
+        <v>18500</v>
       </c>
       <c r="D104">
         <v>0</v>
@@ -4948,16 +4975,16 @@
         <v>0</v>
       </c>
       <c r="H104">
-        <v>36802.50795888391</v>
+        <v>18949</v>
       </c>
       <c r="I104">
-        <v>20802.50795888392</v>
+        <v>449</v>
       </c>
       <c r="J104">
         <v>82</v>
       </c>
       <c r="L104">
-        <v>0.3899491183848233</v>
+        <v>0.05</v>
       </c>
       <c r="M104">
         <v>0.2</v>
@@ -4973,7 +5000,7 @@
         </is>
       </c>
       <c r="C105">
-        <v>3000</v>
+        <v>3900</v>
       </c>
       <c r="D105">
         <v>0</v>
@@ -4988,16 +5015,16 @@
         <v>0.03</v>
       </c>
       <c r="H105">
-        <v>3075.03988037872</v>
+        <v>3930</v>
       </c>
       <c r="I105">
-        <v>75.0398803787199</v>
+        <v>30</v>
       </c>
       <c r="J105">
         <v>122</v>
       </c>
       <c r="L105">
-        <v>0.3899491183848233</v>
+        <v>0.05</v>
       </c>
       <c r="M105">
         <v>0.2</v>
@@ -5013,7 +5040,7 @@
         </is>
       </c>
       <c r="C106">
-        <v>26000</v>
+        <v>30800</v>
       </c>
       <c r="D106">
         <v>0</v>
@@ -5028,16 +5055,16 @@
         <v>0.01</v>
       </c>
       <c r="H106">
-        <v>35517.37207904551</v>
+        <v>39677</v>
       </c>
       <c r="I106">
-        <v>9517.37207904551</v>
+        <v>8877</v>
       </c>
       <c r="J106">
         <v>446</v>
       </c>
       <c r="L106">
-        <v>0.3899491183848233</v>
+        <v>0.05</v>
       </c>
       <c r="M106">
         <v>0.2</v>
@@ -5053,7 +5080,7 @@
         </is>
       </c>
       <c r="C107">
-        <v>35000</v>
+        <v>40300</v>
       </c>
       <c r="D107">
         <v>0</v>
@@ -5068,16 +5095,16 @@
         <v>0.01</v>
       </c>
       <c r="H107">
-        <v>52517.05470539218</v>
+        <v>42094</v>
       </c>
       <c r="I107">
-        <v>17517.05470539218</v>
+        <v>1794</v>
       </c>
       <c r="J107">
         <v>151</v>
       </c>
       <c r="L107">
-        <v>0.3899491183848233</v>
+        <v>0.05</v>
       </c>
       <c r="M107">
         <v>0.2</v>
@@ -5093,7 +5120,7 @@
         </is>
       </c>
       <c r="C108">
-        <v>36000</v>
+        <v>40600</v>
       </c>
       <c r="D108">
         <v>0</v>
@@ -5108,16 +5135,16 @@
         <v>0.01</v>
       </c>
       <c r="H108">
-        <v>36000</v>
+        <v>40656</v>
       </c>
       <c r="I108">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="J108">
         <v>309</v>
       </c>
       <c r="L108">
-        <v>0.3899491183848233</v>
+        <v>0.05</v>
       </c>
       <c r="M108">
         <v>0.2</v>
@@ -5133,7 +5160,7 @@
         </is>
       </c>
       <c r="C109">
-        <v>32000</v>
+        <v>31400</v>
       </c>
       <c r="D109">
         <v>0</v>
@@ -5148,16 +5175,16 @@
         <v>0</v>
       </c>
       <c r="H109">
-        <v>32000</v>
+        <v>32201</v>
       </c>
       <c r="I109">
-        <v>0</v>
+        <v>801</v>
       </c>
       <c r="J109">
         <v>312</v>
       </c>
       <c r="L109">
-        <v>0.3899491183848233</v>
+        <v>0.05</v>
       </c>
       <c r="M109">
         <v>0.2</v>
@@ -5173,7 +5200,7 @@
         </is>
       </c>
       <c r="C110">
-        <v>37000</v>
+        <v>38100</v>
       </c>
       <c r="D110">
         <v>0</v>
@@ -5188,16 +5215,16 @@
         <v>0</v>
       </c>
       <c r="H110">
-        <v>88302.83566266061</v>
+        <v>49295</v>
       </c>
       <c r="I110">
-        <v>51302.83566266061</v>
+        <v>11195</v>
       </c>
       <c r="J110">
         <v>325</v>
       </c>
       <c r="L110">
-        <v>0.3899491183848233</v>
+        <v>0.05</v>
       </c>
       <c r="M110">
         <v>0.2</v>
@@ -5213,7 +5240,7 @@
         </is>
       </c>
       <c r="C111">
-        <v>35000</v>
+        <v>27700</v>
       </c>
       <c r="D111">
         <v>0</v>
@@ -5228,16 +5255,16 @@
         <v>0</v>
       </c>
       <c r="H111">
-        <v>71451.83074101451</v>
+        <v>36772</v>
       </c>
       <c r="I111">
-        <v>36451.8307410145</v>
+        <v>9072</v>
       </c>
       <c r="J111">
         <v>312</v>
       </c>
       <c r="L111">
-        <v>0.3899491183848233</v>
+        <v>0.05</v>
       </c>
       <c r="M111">
         <v>0.2</v>
@@ -5253,7 +5280,7 @@
         </is>
       </c>
       <c r="C112">
-        <v>150000</v>
+        <v>180500</v>
       </c>
       <c r="D112">
         <v>0</v>
@@ -5268,16 +5295,16 @@
         <v>0</v>
       </c>
       <c r="H112">
-        <v>349101.1144235686</v>
+        <v>217239</v>
       </c>
       <c r="I112">
-        <v>199101.1144235686</v>
+        <v>36739</v>
       </c>
       <c r="J112">
         <v>234</v>
       </c>
       <c r="L112">
-        <v>0.3899491183848233</v>
+        <v>0.05</v>
       </c>
       <c r="M112">
         <v>0.2</v>
@@ -5293,7 +5320,7 @@
         </is>
       </c>
       <c r="C113">
-        <v>18000</v>
+        <v>17400</v>
       </c>
       <c r="D113">
         <v>0.09</v>
@@ -5308,16 +5335,16 @@
         <v>0.03</v>
       </c>
       <c r="H113">
-        <v>26435.40803892973</v>
+        <v>52598</v>
       </c>
       <c r="I113">
-        <v>8435.408038929727</v>
+        <v>35198</v>
       </c>
       <c r="J113">
         <v>254</v>
       </c>
       <c r="L113">
-        <v>0.3899491183848233</v>
+        <v>0.05</v>
       </c>
       <c r="M113">
         <v>0.2</v>
@@ -5333,7 +5360,7 @@
         </is>
       </c>
       <c r="C114">
-        <v>4000</v>
+        <v>4400</v>
       </c>
       <c r="D114">
         <v>0</v>
@@ -5348,16 +5375,16 @@
         <v>0.02</v>
       </c>
       <c r="H114">
-        <v>4137.179389318005</v>
+        <v>4489</v>
       </c>
       <c r="I114">
-        <v>137.1793893180048</v>
+        <v>89</v>
       </c>
       <c r="J114">
         <v>70</v>
       </c>
       <c r="L114">
-        <v>0.3899491183848233</v>
+        <v>0.05</v>
       </c>
       <c r="M114">
         <v>0.2</v>
@@ -5373,7 +5400,7 @@
         </is>
       </c>
       <c r="C115">
-        <v>56000</v>
+        <v>59900</v>
       </c>
       <c r="D115">
         <v>0</v>
@@ -5388,16 +5415,16 @@
         <v>0</v>
       </c>
       <c r="H115">
-        <v>56000</v>
+        <v>61811</v>
       </c>
       <c r="I115">
-        <v>0</v>
+        <v>1911</v>
       </c>
       <c r="J115">
         <v>253</v>
       </c>
       <c r="L115">
-        <v>0.3899491183848233</v>
+        <v>0.05</v>
       </c>
       <c r="M115">
         <v>0.2</v>
@@ -5413,7 +5440,7 @@
         </is>
       </c>
       <c r="C116">
-        <v>49000</v>
+        <v>46200</v>
       </c>
       <c r="D116">
         <v>0</v>
@@ -5428,16 +5455,16 @@
         <v>0.0202020202020202</v>
       </c>
       <c r="H116">
-        <v>62249.36046780644</v>
+        <v>59613</v>
       </c>
       <c r="I116">
-        <v>13249.36046780644</v>
+        <v>13413</v>
       </c>
       <c r="J116">
         <v>97</v>
       </c>
       <c r="L116">
-        <v>0.3899491183848233</v>
+        <v>0.05</v>
       </c>
       <c r="M116">
         <v>0.2</v>
@@ -5453,7 +5480,7 @@
         </is>
       </c>
       <c r="C117">
-        <v>82000</v>
+        <v>92100</v>
       </c>
       <c r="D117">
         <v>0.00304945054945055</v>
@@ -5468,16 +5495,16 @@
         <v>0.02531746031746032</v>
       </c>
       <c r="H117">
-        <v>98504.67967907473</v>
+        <v>119301</v>
       </c>
       <c r="I117">
-        <v>16504.67967907473</v>
+        <v>27201</v>
       </c>
       <c r="J117">
         <v>364</v>
       </c>
       <c r="L117">
-        <v>0.3899491183848233</v>
+        <v>0.05</v>
       </c>
       <c r="M117">
         <v>0.2</v>
@@ -5493,7 +5520,7 @@
         </is>
       </c>
       <c r="C118">
-        <v>12000</v>
+        <v>13400</v>
       </c>
       <c r="D118">
         <v>0</v>
@@ -5508,16 +5535,16 @@
         <v>0.0891089108910891</v>
       </c>
       <c r="H118">
-        <v>13615.85839902353</v>
+        <v>14709</v>
       </c>
       <c r="I118">
-        <v>1615.858399023534</v>
+        <v>1309</v>
       </c>
       <c r="J118">
         <v>33</v>
       </c>
       <c r="L118">
-        <v>0.3899491183848233</v>
+        <v>0.05</v>
       </c>
       <c r="M118">
         <v>0.2</v>
@@ -5533,7 +5560,7 @@
         </is>
       </c>
       <c r="C119">
-        <v>23000</v>
+        <v>25100</v>
       </c>
       <c r="D119">
         <v>0</v>
@@ -5548,16 +5575,16 @@
         <v>0</v>
       </c>
       <c r="H119">
-        <v>30549.82135439285</v>
+        <v>25354</v>
       </c>
       <c r="I119">
-        <v>7549.821354392847</v>
+        <v>254</v>
       </c>
       <c r="J119">
         <v>247</v>
       </c>
       <c r="L119">
-        <v>0.3899491183848233</v>
+        <v>0.05</v>
       </c>
       <c r="M119">
         <v>0.2</v>
@@ -5573,7 +5600,7 @@
         </is>
       </c>
       <c r="C120">
-        <v>11000</v>
+        <v>19900</v>
       </c>
       <c r="D120">
         <v>0</v>
@@ -5588,16 +5615,16 @@
         <v>0.03640551011622901</v>
       </c>
       <c r="H120">
-        <v>12444.94515310393</v>
+        <v>21940</v>
       </c>
       <c r="I120">
-        <v>1444.945153103935</v>
+        <v>2040</v>
       </c>
       <c r="J120">
         <v>230</v>
       </c>
       <c r="L120">
-        <v>0.3899491183848233</v>
+        <v>0.05</v>
       </c>
       <c r="M120">
         <v>0.2</v>
@@ -5613,7 +5640,7 @@
         </is>
       </c>
       <c r="C121">
-        <v>18000</v>
+        <v>17700</v>
       </c>
       <c r="D121">
         <v>0</v>
@@ -5628,16 +5655,16 @@
         <v>0.0891089108910891</v>
       </c>
       <c r="H121">
-        <v>33646.44021802422</v>
+        <v>21612</v>
       </c>
       <c r="I121">
-        <v>15646.44021802422</v>
+        <v>3912</v>
       </c>
       <c r="J121">
         <v>137</v>
       </c>
       <c r="L121">
-        <v>0.3899491183848233</v>
+        <v>0.05</v>
       </c>
       <c r="M121">
         <v>0.2</v>
@@ -5653,19 +5680,19 @@
         </is>
       </c>
       <c r="C122">
-        <v>3000</v>
+        <v>3300</v>
       </c>
       <c r="H122">
-        <v>5672.213533429915</v>
+        <v>3537</v>
       </c>
       <c r="I122">
-        <v>2672.213533429915</v>
+        <v>237</v>
       </c>
       <c r="J122">
         <v>0</v>
       </c>
       <c r="L122">
-        <v>0.3899491183848233</v>
+        <v>0.05</v>
       </c>
       <c r="M122">
         <v>0.2</v>
@@ -5681,19 +5708,19 @@
         </is>
       </c>
       <c r="C123">
-        <v>3000</v>
+        <v>2600</v>
       </c>
       <c r="H123">
-        <v>4891.411388023203</v>
+        <v>2610</v>
       </c>
       <c r="I123">
-        <v>1891.411388023203</v>
+        <v>10</v>
       </c>
       <c r="J123">
         <v>0</v>
       </c>
       <c r="L123">
-        <v>0.3899491183848233</v>
+        <v>0.05</v>
       </c>
       <c r="M123">
         <v>0.2</v>
@@ -5709,19 +5736,19 @@
         </is>
       </c>
       <c r="C124">
-        <v>2000</v>
+        <v>1300</v>
       </c>
       <c r="H124">
-        <v>2274.250595846931</v>
+        <v>1601</v>
       </c>
       <c r="I124">
-        <v>274.2505958469307</v>
+        <v>301</v>
       </c>
       <c r="J124">
         <v>0</v>
       </c>
       <c r="L124">
-        <v>0.3899491183848233</v>
+        <v>0.05</v>
       </c>
       <c r="M124">
         <v>0.2</v>
@@ -5737,19 +5764,19 @@
         </is>
       </c>
       <c r="C125">
-        <v>3000</v>
+        <v>3600</v>
       </c>
       <c r="H125">
-        <v>3785.222242698912</v>
+        <v>3897</v>
       </c>
       <c r="I125">
-        <v>785.2222426989124</v>
+        <v>297</v>
       </c>
       <c r="J125">
         <v>0</v>
       </c>
       <c r="L125">
-        <v>0.3899491183848233</v>
+        <v>0.05</v>
       </c>
       <c r="M125">
         <v>0.2</v>
@@ -5765,7 +5792,7 @@
         </is>
       </c>
       <c r="C126">
-        <v>12000</v>
+        <v>12500</v>
       </c>
       <c r="D126">
         <v>0</v>
@@ -5780,16 +5807,16 @@
         <v>0.01116494628186223</v>
       </c>
       <c r="H126">
-        <v>12000</v>
+        <v>12781</v>
       </c>
       <c r="I126">
-        <v>0</v>
+        <v>281</v>
       </c>
       <c r="J126">
         <v>94</v>
       </c>
       <c r="L126">
-        <v>0.3899491183848233</v>
+        <v>0.05</v>
       </c>
       <c r="M126">
         <v>0.2</v>
@@ -5805,7 +5832,7 @@
         </is>
       </c>
       <c r="C127">
-        <v>11000</v>
+        <v>13100</v>
       </c>
       <c r="D127">
         <v>0.06</v>
@@ -5820,7 +5847,7 @@
         <v>0</v>
       </c>
       <c r="H127">
-        <v>11000</v>
+        <v>13100</v>
       </c>
       <c r="I127">
         <v>0</v>
@@ -5829,7 +5856,7 @@
         <v>52</v>
       </c>
       <c r="L127">
-        <v>0.3899491183848233</v>
+        <v>0.399812753899036</v>
       </c>
       <c r="M127">
         <v>0.2</v>
@@ -5860,16 +5887,16 @@
         <v>0.00693069306930693</v>
       </c>
       <c r="H128">
-        <v>35894.05396004011</v>
+        <v>36055.16288364011</v>
       </c>
       <c r="I128">
-        <v>5894.05396004011</v>
+        <v>6055.162883640109</v>
       </c>
       <c r="J128">
         <v>303</v>
       </c>
       <c r="L128">
-        <v>0.3899491183848233</v>
+        <v>0.399812753899036</v>
       </c>
       <c r="M128">
         <v>0.2</v>
@@ -5900,16 +5927,16 @@
         <v>0</v>
       </c>
       <c r="H129">
-        <v>55852.2680804227</v>
+        <v>56370.16995668155</v>
       </c>
       <c r="I129">
-        <v>25852.26808042269</v>
+        <v>26370.16995668155</v>
       </c>
       <c r="J129">
         <v>67</v>
       </c>
       <c r="L129">
-        <v>0.3899491183848233</v>
+        <v>0.399812753899036</v>
       </c>
       <c r="M129">
         <v>0.2</v>
@@ -6425,30 +6452,21 @@
     </row>
     <row r="143">
       <c r="A143">
-        <v>1972</v>
+        <v>1918</v>
       </c>
       <c r="B143" t="inlineStr">
         <is>
           <t>HED</t>
         </is>
       </c>
-      <c r="D143">
-        <v>0</v>
-      </c>
-      <c r="E143">
-        <v>0.91</v>
-      </c>
-      <c r="F143">
-        <v>0.06999999999999999</v>
-      </c>
-      <c r="G143">
-        <v>0.02</v>
+      <c r="C143">
+        <v>7000</v>
       </c>
       <c r="J143">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="L143">
-        <v>0.3899491183848233</v>
+        <v>0.399812753899036</v>
       </c>
       <c r="M143">
         <v>0.2</v>
@@ -6456,30 +6474,21 @@
     </row>
     <row r="144">
       <c r="A144">
-        <v>1973</v>
+        <v>1919</v>
       </c>
       <c r="B144" t="inlineStr">
         <is>
           <t>HED</t>
         </is>
       </c>
-      <c r="D144">
-        <v>0</v>
-      </c>
-      <c r="E144">
-        <v>0.66</v>
-      </c>
-      <c r="F144">
-        <v>0.34</v>
-      </c>
-      <c r="G144">
-        <v>0</v>
+      <c r="C144">
+        <v>8000</v>
       </c>
       <c r="J144">
-        <v>99</v>
+        <v>0</v>
       </c>
       <c r="L144">
-        <v>0.3899491183848233</v>
+        <v>0.399812753899036</v>
       </c>
       <c r="M144">
         <v>0.2</v>
@@ -6487,30 +6496,21 @@
     </row>
     <row r="145">
       <c r="A145">
-        <v>1974</v>
+        <v>1920</v>
       </c>
       <c r="B145" t="inlineStr">
         <is>
           <t>HED</t>
         </is>
       </c>
-      <c r="D145">
-        <v>0</v>
-      </c>
-      <c r="E145">
-        <v>0.57</v>
-      </c>
-      <c r="F145">
-        <v>0.43</v>
-      </c>
-      <c r="G145">
-        <v>0</v>
+      <c r="C145">
+        <v>38000</v>
       </c>
       <c r="J145">
-        <v>113</v>
+        <v>0</v>
       </c>
       <c r="L145">
-        <v>0.3899491183848233</v>
+        <v>0.399812753899036</v>
       </c>
       <c r="M145">
         <v>0.2</v>
@@ -6518,30 +6518,21 @@
     </row>
     <row r="146">
       <c r="A146">
-        <v>1975</v>
+        <v>1921</v>
       </c>
       <c r="B146" t="inlineStr">
         <is>
           <t>HED</t>
         </is>
       </c>
-      <c r="D146">
-        <v>0</v>
-      </c>
-      <c r="E146">
-        <v>0.5742574257425742</v>
-      </c>
-      <c r="F146">
-        <v>0.4158415841584159</v>
-      </c>
-      <c r="G146">
-        <v>0.009900990099009901</v>
+      <c r="C146">
+        <v>1000</v>
       </c>
       <c r="J146">
-        <v>195</v>
+        <v>0</v>
       </c>
       <c r="L146">
-        <v>0.3899491183848233</v>
+        <v>0.399812753899036</v>
       </c>
       <c r="M146">
         <v>0.2</v>
@@ -6549,32 +6540,1313 @@
     </row>
     <row r="147">
       <c r="A147">
+        <v>1922</v>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C147">
+        <v>70000</v>
+      </c>
+      <c r="J147">
+        <v>0</v>
+      </c>
+      <c r="L147">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="M147">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148">
+        <v>1923</v>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C148">
+        <v>90000</v>
+      </c>
+      <c r="J148">
+        <v>0</v>
+      </c>
+      <c r="L148">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="M148">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149">
+        <v>1924</v>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C149">
+        <v>120000</v>
+      </c>
+      <c r="J149">
+        <v>0</v>
+      </c>
+      <c r="L149">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="M149">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150">
+        <v>1925</v>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C150">
+        <v>80000</v>
+      </c>
+      <c r="J150">
+        <v>0</v>
+      </c>
+      <c r="L150">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="M150">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151">
+        <v>1926</v>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C151">
+        <v>65000</v>
+      </c>
+      <c r="J151">
+        <v>0</v>
+      </c>
+      <c r="L151">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="M151">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152">
+        <v>1927</v>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C152">
+        <v>70000</v>
+      </c>
+      <c r="J152">
+        <v>0</v>
+      </c>
+      <c r="L152">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="M152">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153">
+        <v>1928</v>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C153">
+        <v>70000</v>
+      </c>
+      <c r="J153">
+        <v>0</v>
+      </c>
+      <c r="L153">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="M153">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154">
+        <v>1929</v>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C154">
+        <v>135000</v>
+      </c>
+      <c r="J154">
+        <v>0</v>
+      </c>
+      <c r="L154">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="M154">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155">
+        <v>1930</v>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C155">
+        <v>40000</v>
+      </c>
+      <c r="J155">
+        <v>0</v>
+      </c>
+      <c r="L155">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="M155">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156">
+        <v>1931</v>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C156">
+        <v>50000</v>
+      </c>
+      <c r="J156">
+        <v>0</v>
+      </c>
+      <c r="L156">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="M156">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157">
+        <v>1932</v>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C157">
+        <v>35000</v>
+      </c>
+      <c r="J157">
+        <v>0</v>
+      </c>
+      <c r="L157">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="M157">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158">
+        <v>1933</v>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C158">
+        <v>7500</v>
+      </c>
+      <c r="J158">
+        <v>0</v>
+      </c>
+      <c r="L158">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="M158">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159">
+        <v>1934</v>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C159">
+        <v>15000</v>
+      </c>
+      <c r="J159">
+        <v>0</v>
+      </c>
+      <c r="L159">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="M159">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160">
+        <v>1935</v>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C160">
+        <v>45000</v>
+      </c>
+      <c r="J160">
+        <v>0</v>
+      </c>
+      <c r="L160">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="M160">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161">
+        <v>1936</v>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C161">
+        <v>2000</v>
+      </c>
+      <c r="J161">
+        <v>0</v>
+      </c>
+      <c r="L161">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="M161">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162">
+        <v>1937</v>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C162">
+        <v>38000</v>
+      </c>
+      <c r="J162">
+        <v>0</v>
+      </c>
+      <c r="L162">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="M162">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163">
+        <v>1938</v>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C163">
+        <v>10000</v>
+      </c>
+      <c r="J163">
+        <v>0</v>
+      </c>
+      <c r="L163">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="M163">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164">
+        <v>1939</v>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C164">
+        <v>14000</v>
+      </c>
+      <c r="J164">
+        <v>0</v>
+      </c>
+      <c r="L164">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="M164">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165">
+        <v>1940</v>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C165">
+        <v>60000</v>
+      </c>
+      <c r="J165">
+        <v>0</v>
+      </c>
+      <c r="L165">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="M165">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166">
+        <v>1941</v>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C166">
+        <v>2000</v>
+      </c>
+      <c r="J166">
+        <v>0</v>
+      </c>
+      <c r="L166">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="M166">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167">
+        <v>1942</v>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C167">
+        <v>7000</v>
+      </c>
+      <c r="J167">
+        <v>0</v>
+      </c>
+      <c r="L167">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="M167">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168">
+        <v>1943</v>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C168">
+        <v>5000</v>
+      </c>
+      <c r="J168">
+        <v>0</v>
+      </c>
+      <c r="L168">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="M168">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169">
+        <v>1944</v>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C169">
+        <v>5000</v>
+      </c>
+      <c r="J169">
+        <v>0</v>
+      </c>
+      <c r="L169">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="M169">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170">
+        <v>1945</v>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C170">
+        <v>14000</v>
+      </c>
+      <c r="J170">
+        <v>0</v>
+      </c>
+      <c r="L170">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="M170">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171">
+        <v>1946</v>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C171">
+        <v>14000</v>
+      </c>
+      <c r="J171">
+        <v>0</v>
+      </c>
+      <c r="L171">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="M171">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172">
+        <v>1947</v>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C172">
+        <v>7000</v>
+      </c>
+      <c r="J172">
+        <v>0</v>
+      </c>
+      <c r="L172">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="M172">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173">
+        <v>1948</v>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C173">
+        <v>7000</v>
+      </c>
+      <c r="J173">
+        <v>0</v>
+      </c>
+      <c r="L173">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="M173">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174">
+        <v>1949</v>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C174">
+        <v>30000</v>
+      </c>
+      <c r="J174">
+        <v>0</v>
+      </c>
+      <c r="L174">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="M174">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175">
+        <v>1950</v>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C175">
+        <v>14000</v>
+      </c>
+      <c r="J175">
+        <v>0</v>
+      </c>
+      <c r="L175">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="M175">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176">
+        <v>1951</v>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C176">
+        <v>14000</v>
+      </c>
+      <c r="J176">
+        <v>0</v>
+      </c>
+      <c r="L176">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="M176">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177">
+        <v>1952</v>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C177">
+        <v>14000</v>
+      </c>
+      <c r="J177">
+        <v>0</v>
+      </c>
+      <c r="L177">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="M177">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178">
+        <v>1953</v>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C178">
+        <v>14000</v>
+      </c>
+      <c r="J178">
+        <v>0</v>
+      </c>
+      <c r="L178">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="M178">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179">
+        <v>1954</v>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C179">
+        <v>30000</v>
+      </c>
+      <c r="J179">
+        <v>0</v>
+      </c>
+      <c r="L179">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="M179">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180">
+        <v>1955</v>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C180">
+        <v>14000</v>
+      </c>
+      <c r="J180">
+        <v>0</v>
+      </c>
+      <c r="L180">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="M180">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181">
+        <v>1956</v>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C181">
+        <v>7000</v>
+      </c>
+      <c r="J181">
+        <v>0</v>
+      </c>
+      <c r="L181">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="M181">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182">
+        <v>1957</v>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C182">
+        <v>7000</v>
+      </c>
+      <c r="J182">
+        <v>0</v>
+      </c>
+      <c r="L182">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="M182">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183">
+        <v>1958</v>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C183">
+        <v>14000</v>
+      </c>
+      <c r="J183">
+        <v>0</v>
+      </c>
+      <c r="L183">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="M183">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184">
+        <v>1959</v>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C184">
+        <v>14000</v>
+      </c>
+      <c r="J184">
+        <v>0</v>
+      </c>
+      <c r="L184">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="M184">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185">
+        <v>1960</v>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C185">
+        <v>10000</v>
+      </c>
+      <c r="J185">
+        <v>0</v>
+      </c>
+      <c r="L185">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="M185">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186">
+        <v>1961</v>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C186">
+        <v>14000</v>
+      </c>
+      <c r="J186">
+        <v>0</v>
+      </c>
+      <c r="L186">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="M186">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187">
+        <v>1962</v>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C187">
+        <v>30000</v>
+      </c>
+      <c r="J187">
+        <v>0</v>
+      </c>
+      <c r="L187">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="M187">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188">
+        <v>1963</v>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C188">
+        <v>18000</v>
+      </c>
+      <c r="J188">
+        <v>0</v>
+      </c>
+      <c r="L188">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="M188">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189">
+        <v>1964</v>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C189">
+        <v>30000</v>
+      </c>
+      <c r="J189">
+        <v>0</v>
+      </c>
+      <c r="L189">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="M189">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190">
+        <v>1965</v>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C190">
+        <v>18000</v>
+      </c>
+      <c r="J190">
+        <v>0</v>
+      </c>
+      <c r="L190">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="M190">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191">
+        <v>1966</v>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C191">
+        <v>80000</v>
+      </c>
+      <c r="J191">
+        <v>0</v>
+      </c>
+      <c r="L191">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="M191">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192">
+        <v>1967</v>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C192">
+        <v>80000</v>
+      </c>
+      <c r="J192">
+        <v>0</v>
+      </c>
+      <c r="L192">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="M192">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193">
+        <v>1968</v>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C193">
+        <v>30000</v>
+      </c>
+      <c r="J193">
+        <v>0</v>
+      </c>
+      <c r="L193">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="M193">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194">
+        <v>1969</v>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C194">
+        <v>18000</v>
+      </c>
+      <c r="J194">
+        <v>0</v>
+      </c>
+      <c r="L194">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="M194">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195">
+        <v>1970</v>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C195">
+        <v>9000</v>
+      </c>
+      <c r="H195">
+        <v>14317</v>
+      </c>
+      <c r="I195">
+        <v>5317</v>
+      </c>
+      <c r="J195">
+        <v>0</v>
+      </c>
+      <c r="L195">
+        <v>0.05</v>
+      </c>
+      <c r="M195">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196">
+        <v>1971</v>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C196">
+        <v>7500</v>
+      </c>
+      <c r="H196">
+        <v>8522</v>
+      </c>
+      <c r="I196">
+        <v>1022</v>
+      </c>
+      <c r="J196">
+        <v>0</v>
+      </c>
+      <c r="L196">
+        <v>0.05</v>
+      </c>
+      <c r="M196">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197">
+        <v>1972</v>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C197">
+        <v>3500</v>
+      </c>
+      <c r="D197">
+        <v>0</v>
+      </c>
+      <c r="E197">
+        <v>0.91</v>
+      </c>
+      <c r="F197">
+        <v>0.06999999999999999</v>
+      </c>
+      <c r="G197">
+        <v>0.02</v>
+      </c>
+      <c r="H197">
+        <v>4407</v>
+      </c>
+      <c r="I197">
+        <v>907</v>
+      </c>
+      <c r="J197">
+        <v>43</v>
+      </c>
+      <c r="L197">
+        <v>0.05</v>
+      </c>
+      <c r="M197">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198">
+        <v>1973</v>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C198">
+        <v>40000</v>
+      </c>
+      <c r="D198">
+        <v>0</v>
+      </c>
+      <c r="E198">
+        <v>0.66</v>
+      </c>
+      <c r="F198">
+        <v>0.34</v>
+      </c>
+      <c r="G198">
+        <v>0</v>
+      </c>
+      <c r="H198">
+        <v>58495</v>
+      </c>
+      <c r="I198">
+        <v>18495</v>
+      </c>
+      <c r="J198">
+        <v>99</v>
+      </c>
+      <c r="L198">
+        <v>0.05</v>
+      </c>
+      <c r="M198">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199">
+        <v>1974</v>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C199">
+        <v>6000</v>
+      </c>
+      <c r="D199">
+        <v>0</v>
+      </c>
+      <c r="E199">
+        <v>0.57</v>
+      </c>
+      <c r="F199">
+        <v>0.43</v>
+      </c>
+      <c r="G199">
+        <v>0</v>
+      </c>
+      <c r="H199">
+        <v>8936</v>
+      </c>
+      <c r="I199">
+        <v>2936</v>
+      </c>
+      <c r="J199">
+        <v>113</v>
+      </c>
+      <c r="L199">
+        <v>0.05</v>
+      </c>
+      <c r="M199">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200">
+        <v>1975</v>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C200">
+        <v>10000</v>
+      </c>
+      <c r="D200">
+        <v>0</v>
+      </c>
+      <c r="E200">
+        <v>0.5742574257425742</v>
+      </c>
+      <c r="F200">
+        <v>0.4158415841584159</v>
+      </c>
+      <c r="G200">
+        <v>0.009900990099009901</v>
+      </c>
+      <c r="H200">
+        <v>17635</v>
+      </c>
+      <c r="I200">
+        <v>7635</v>
+      </c>
+      <c r="J200">
+        <v>195</v>
+      </c>
+      <c r="L200">
+        <v>0.05</v>
+      </c>
+      <c r="M200">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201">
         <v>1976</v>
       </c>
-      <c r="B147" t="inlineStr">
-        <is>
-          <t>HED</t>
-        </is>
-      </c>
-      <c r="D147">
-        <v>0</v>
-      </c>
-      <c r="E147">
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>HED</t>
+        </is>
+      </c>
+      <c r="C201">
+        <v>3500</v>
+      </c>
+      <c r="D201">
+        <v>0</v>
+      </c>
+      <c r="E201">
         <v>0.7319587628865979</v>
       </c>
-      <c r="F147">
+      <c r="F201">
         <v>0.2680412371134021</v>
       </c>
-      <c r="G147">
-        <v>0</v>
-      </c>
-      <c r="J147">
+      <c r="G201">
+        <v>0</v>
+      </c>
+      <c r="H201">
+        <v>8825</v>
+      </c>
+      <c r="I201">
+        <v>5325</v>
+      </c>
+      <c r="J201">
         <v>191</v>
       </c>
-      <c r="L147">
-        <v>0.3899491183848233</v>
-      </c>
-      <c r="M147">
+      <c r="L201">
+        <v>0.05</v>
+      </c>
+      <c r="M201">
         <v>0.2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update stock-recruit output data
</commit_message>
<xml_diff>
--- a/3. outputs/Stock-recruit data/Barkley_Sockeye_stock-recruit_infilled.xlsx
+++ b/3. outputs/Stock-recruit data/Barkley_Sockeye_stock-recruit_infilled.xlsx
@@ -352,7 +352,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -505,22 +505,34 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>H_cv</t>
+          <t>comments</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Coefficient of variation on harvest data. Historical (prior to 2011) Hucuktlis Sockeye harvest rate predictions were derived from a linear model. CV for these data is calculated as RMSE of the model residuals divided by the mean of the observed Hucuktlis Sockeye harvest rates that informed the model fit (i.e. the dependent variable). Harvest data for Somass and Hucuktlis post-2011 are assumed to be precise.</t>
+          <t>!definition required!</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>H_cv</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Coefficient of variation on harvest data. Historical (prior to 2011) Hucuktlis Sockeye harvest rate predictions were derived from a linear model. CV for these data is calculated as RMSE of the model residuals divided by the mean of the observed Hucuktlis Sockeye harvest rates that informed the model fit (i.e. the dependent variable). Harvest data for Somass and Hucuktlis post-2011 are assumed to be precise.</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
           <t>S_cv</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="B15" t="inlineStr">
         <is>
           <t>Coefficient of variation on spawner data. Currently based on ____</t>
         </is>
@@ -533,7 +545,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M201"/>
+  <dimension ref="A1:N201"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -597,10 +609,15 @@
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
+          <t>comments</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
           <t>H_cv</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>S_cv</t>
         </is>
@@ -642,10 +659,10 @@
       <c r="K2">
         <v>633742.5637903768</v>
       </c>
-      <c r="L2">
-        <v>0.05</v>
-      </c>
       <c r="M2">
+        <v>0.05</v>
+      </c>
+      <c r="N2">
         <v>0.05</v>
       </c>
     </row>
@@ -685,10 +702,10 @@
       <c r="K3">
         <v>495061.8834075385</v>
       </c>
-      <c r="L3">
-        <v>0.05</v>
-      </c>
       <c r="M3">
+        <v>0.05</v>
+      </c>
+      <c r="N3">
         <v>0.05</v>
       </c>
     </row>
@@ -728,10 +745,10 @@
       <c r="K4">
         <v>526832.3053483891</v>
       </c>
-      <c r="L4">
-        <v>0.05</v>
-      </c>
       <c r="M4">
+        <v>0.05</v>
+      </c>
+      <c r="N4">
         <v>0.05</v>
       </c>
     </row>
@@ -771,10 +788,10 @@
       <c r="K5">
         <v>552803.0040534479</v>
       </c>
-      <c r="L5">
-        <v>0.05</v>
-      </c>
       <c r="M5">
+        <v>0.05</v>
+      </c>
+      <c r="N5">
         <v>0.05</v>
       </c>
     </row>
@@ -814,10 +831,10 @@
       <c r="K6">
         <v>913809.5845034227</v>
       </c>
-      <c r="L6">
-        <v>0.05</v>
-      </c>
       <c r="M6">
+        <v>0.05</v>
+      </c>
+      <c r="N6">
         <v>0.05</v>
       </c>
     </row>
@@ -857,10 +874,10 @@
       <c r="K7">
         <v>570766.8540090187</v>
       </c>
-      <c r="L7">
-        <v>0.05</v>
-      </c>
       <c r="M7">
+        <v>0.05</v>
+      </c>
+      <c r="N7">
         <v>0.05</v>
       </c>
     </row>
@@ -900,10 +917,10 @@
       <c r="K8">
         <v>480598.2568144404</v>
       </c>
-      <c r="L8">
-        <v>0.05</v>
-      </c>
       <c r="M8">
+        <v>0.05</v>
+      </c>
+      <c r="N8">
         <v>0.05</v>
       </c>
     </row>
@@ -943,10 +960,10 @@
       <c r="K9">
         <v>391376.4267260354</v>
       </c>
-      <c r="L9">
-        <v>0.05</v>
-      </c>
       <c r="M9">
+        <v>0.05</v>
+      </c>
+      <c r="N9">
         <v>0.05</v>
       </c>
     </row>
@@ -986,10 +1003,10 @@
       <c r="K10">
         <v>224122.9386567897</v>
       </c>
-      <c r="L10">
-        <v>0.05</v>
-      </c>
       <c r="M10">
+        <v>0.05</v>
+      </c>
+      <c r="N10">
         <v>0.05</v>
       </c>
     </row>
@@ -1029,10 +1046,10 @@
       <c r="K11">
         <v>288014.3071424381</v>
       </c>
-      <c r="L11">
-        <v>0.05</v>
-      </c>
       <c r="M11">
+        <v>0.05</v>
+      </c>
+      <c r="N11">
         <v>0.05</v>
       </c>
     </row>
@@ -1072,10 +1089,10 @@
       <c r="K12">
         <v>137076.4333190075</v>
       </c>
-      <c r="L12">
-        <v>0.05</v>
-      </c>
       <c r="M12">
+        <v>0.05</v>
+      </c>
+      <c r="N12">
         <v>0.05</v>
       </c>
     </row>
@@ -1115,10 +1132,10 @@
       <c r="K13">
         <v>203184.164250254</v>
       </c>
-      <c r="L13">
-        <v>0.05</v>
-      </c>
       <c r="M13">
+        <v>0.05</v>
+      </c>
+      <c r="N13">
         <v>0.05</v>
       </c>
     </row>
@@ -1158,10 +1175,10 @@
       <c r="K14">
         <v>503092.30271186</v>
       </c>
-      <c r="L14">
-        <v>0.05</v>
-      </c>
       <c r="M14">
+        <v>0.05</v>
+      </c>
+      <c r="N14">
         <v>0.05</v>
       </c>
     </row>
@@ -1201,10 +1218,10 @@
       <c r="K15">
         <v>371601.962535504</v>
       </c>
-      <c r="L15">
-        <v>0.05</v>
-      </c>
       <c r="M15">
+        <v>0.05</v>
+      </c>
+      <c r="N15">
         <v>0.05</v>
       </c>
     </row>
@@ -1244,10 +1261,10 @@
       <c r="K16">
         <v>206726.5366225715</v>
       </c>
-      <c r="L16">
-        <v>0.05</v>
-      </c>
       <c r="M16">
+        <v>0.05</v>
+      </c>
+      <c r="N16">
         <v>0.05</v>
       </c>
     </row>
@@ -1287,10 +1304,10 @@
       <c r="K17">
         <v>340157.6785086803</v>
       </c>
-      <c r="L17">
-        <v>0.05</v>
-      </c>
       <c r="M17">
+        <v>0.05</v>
+      </c>
+      <c r="N17">
         <v>0.05</v>
       </c>
     </row>
@@ -1330,10 +1347,10 @@
       <c r="K18">
         <v>292061.9392067303</v>
       </c>
-      <c r="L18">
-        <v>0.05</v>
-      </c>
       <c r="M18">
+        <v>0.05</v>
+      </c>
+      <c r="N18">
         <v>0.05</v>
       </c>
     </row>
@@ -1373,10 +1390,10 @@
       <c r="K19">
         <v>172160.3662147925</v>
       </c>
-      <c r="L19">
-        <v>0.05</v>
-      </c>
       <c r="M19">
+        <v>0.05</v>
+      </c>
+      <c r="N19">
         <v>0.05</v>
       </c>
     </row>
@@ -1416,10 +1433,10 @@
       <c r="K20">
         <v>274311.7730009329</v>
       </c>
-      <c r="L20">
-        <v>0.05</v>
-      </c>
       <c r="M20">
+        <v>0.05</v>
+      </c>
+      <c r="N20">
         <v>0.05</v>
       </c>
     </row>
@@ -1459,10 +1476,10 @@
       <c r="K21">
         <v>265697.028795797</v>
       </c>
-      <c r="L21">
-        <v>0.05</v>
-      </c>
       <c r="M21">
+        <v>0.05</v>
+      </c>
+      <c r="N21">
         <v>0.05</v>
       </c>
     </row>
@@ -1502,10 +1519,10 @@
       <c r="K22">
         <v>1258256.636990258</v>
       </c>
-      <c r="L22">
-        <v>0.05</v>
-      </c>
       <c r="M22">
+        <v>0.05</v>
+      </c>
+      <c r="N22">
         <v>0.05</v>
       </c>
     </row>
@@ -1545,10 +1562,10 @@
       <c r="K23">
         <v>652446.9029476116</v>
       </c>
-      <c r="L23">
-        <v>0.05</v>
-      </c>
       <c r="M23">
+        <v>0.05</v>
+      </c>
+      <c r="N23">
         <v>0.05</v>
       </c>
     </row>
@@ -1588,10 +1605,10 @@
       <c r="K24">
         <v>599789.3466079192</v>
       </c>
-      <c r="L24">
-        <v>0.05</v>
-      </c>
       <c r="M24">
+        <v>0.05</v>
+      </c>
+      <c r="N24">
         <v>0.05</v>
       </c>
     </row>
@@ -1631,10 +1648,10 @@
       <c r="K25">
         <v>625355.4802804298</v>
       </c>
-      <c r="L25">
-        <v>0.05</v>
-      </c>
       <c r="M25">
+        <v>0.05</v>
+      </c>
+      <c r="N25">
         <v>0.05</v>
       </c>
     </row>
@@ -1674,10 +1691,10 @@
       <c r="K26">
         <v>400875.0350328542</v>
       </c>
-      <c r="L26">
-        <v>0.05</v>
-      </c>
       <c r="M26">
+        <v>0.05</v>
+      </c>
+      <c r="N26">
         <v>0.05</v>
       </c>
     </row>
@@ -1717,10 +1734,10 @@
       <c r="K27">
         <v>407468.2247957478</v>
       </c>
-      <c r="L27">
-        <v>0.05</v>
-      </c>
       <c r="M27">
+        <v>0.05</v>
+      </c>
+      <c r="N27">
         <v>0.05</v>
       </c>
     </row>
@@ -1760,10 +1777,10 @@
       <c r="K28">
         <v>138601.997986058</v>
       </c>
-      <c r="L28">
-        <v>0.05</v>
-      </c>
       <c r="M28">
+        <v>0.05</v>
+      </c>
+      <c r="N28">
         <v>0.05</v>
       </c>
     </row>
@@ -1803,10 +1820,10 @@
       <c r="K29">
         <v>181984.1898199186</v>
       </c>
-      <c r="L29">
-        <v>0.05</v>
-      </c>
       <c r="M29">
+        <v>0.05</v>
+      </c>
+      <c r="N29">
         <v>0.05</v>
       </c>
     </row>
@@ -1846,10 +1863,10 @@
       <c r="K30">
         <v>74102.68990164486</v>
       </c>
-      <c r="L30">
-        <v>0.05</v>
-      </c>
       <c r="M30">
+        <v>0.05</v>
+      </c>
+      <c r="N30">
         <v>0.05</v>
       </c>
     </row>
@@ -1889,10 +1906,10 @@
       <c r="K31">
         <v>59697.7030353223</v>
       </c>
-      <c r="L31">
-        <v>0.05</v>
-      </c>
       <c r="M31">
+        <v>0.05</v>
+      </c>
+      <c r="N31">
         <v>0.05</v>
       </c>
     </row>
@@ -1932,10 +1949,10 @@
       <c r="K32">
         <v>290004.5944304451</v>
       </c>
-      <c r="L32">
-        <v>0.05</v>
-      </c>
       <c r="M32">
+        <v>0.05</v>
+      </c>
+      <c r="N32">
         <v>0.05</v>
       </c>
     </row>
@@ -1975,10 +1992,10 @@
       <c r="K33">
         <v>320116.8393461921</v>
       </c>
-      <c r="L33">
-        <v>0.05</v>
-      </c>
       <c r="M33">
+        <v>0.05</v>
+      </c>
+      <c r="N33">
         <v>0.05</v>
       </c>
     </row>
@@ -2018,10 +2035,10 @@
       <c r="K34">
         <v>421979.6878094974</v>
       </c>
-      <c r="L34">
-        <v>0.05</v>
-      </c>
       <c r="M34">
+        <v>0.05</v>
+      </c>
+      <c r="N34">
         <v>0.05</v>
       </c>
     </row>
@@ -2061,10 +2078,10 @@
       <c r="K35">
         <v>263927.9811106482</v>
       </c>
-      <c r="L35">
-        <v>0.05</v>
-      </c>
       <c r="M35">
+        <v>0.05</v>
+      </c>
+      <c r="N35">
         <v>0.05</v>
       </c>
     </row>
@@ -2104,10 +2121,10 @@
       <c r="K36">
         <v>240203.9760283087</v>
       </c>
-      <c r="L36">
-        <v>0.05</v>
-      </c>
       <c r="M36">
+        <v>0.05</v>
+      </c>
+      <c r="N36">
         <v>0.05</v>
       </c>
     </row>
@@ -2147,10 +2164,10 @@
       <c r="K37">
         <v>189096.9567127897</v>
       </c>
-      <c r="L37">
-        <v>0.05</v>
-      </c>
       <c r="M37">
+        <v>0.05</v>
+      </c>
+      <c r="N37">
         <v>0.05</v>
       </c>
     </row>
@@ -2190,10 +2207,10 @@
       <c r="K38">
         <v>241682.5691475399</v>
       </c>
-      <c r="L38">
-        <v>0.05</v>
-      </c>
       <c r="M38">
+        <v>0.05</v>
+      </c>
+      <c r="N38">
         <v>0.05</v>
       </c>
     </row>
@@ -2233,10 +2250,10 @@
       <c r="K39">
         <v>386548.9231194458</v>
       </c>
-      <c r="L39">
-        <v>0.05</v>
-      </c>
       <c r="M39">
+        <v>0.05</v>
+      </c>
+      <c r="N39">
         <v>0.05</v>
       </c>
     </row>
@@ -2276,10 +2293,10 @@
       <c r="K40">
         <v>261943.5622247388</v>
       </c>
-      <c r="L40">
-        <v>0.05</v>
-      </c>
       <c r="M40">
+        <v>0.05</v>
+      </c>
+      <c r="N40">
         <v>0.05</v>
       </c>
     </row>
@@ -2319,10 +2336,10 @@
       <c r="K41">
         <v>145416.8103652774</v>
       </c>
-      <c r="L41">
-        <v>0.05</v>
-      </c>
       <c r="M41">
+        <v>0.05</v>
+      </c>
+      <c r="N41">
         <v>0.05</v>
       </c>
     </row>
@@ -2362,10 +2379,10 @@
       <c r="K42">
         <v>717175.1613370343</v>
       </c>
-      <c r="L42">
-        <v>0.05</v>
-      </c>
       <c r="M42">
+        <v>0.05</v>
+      </c>
+      <c r="N42">
         <v>0.05</v>
       </c>
     </row>
@@ -2405,10 +2422,10 @@
       <c r="K43">
         <v>326804.0013846449</v>
       </c>
-      <c r="L43">
-        <v>0.05</v>
-      </c>
       <c r="M43">
+        <v>0.05</v>
+      </c>
+      <c r="N43">
         <v>0.05</v>
       </c>
     </row>
@@ -2448,10 +2465,10 @@
       <c r="K44">
         <v>518419.7394188421</v>
       </c>
-      <c r="L44">
-        <v>0.05</v>
-      </c>
       <c r="M44">
+        <v>0.05</v>
+      </c>
+      <c r="N44">
         <v>0.05</v>
       </c>
     </row>
@@ -2491,10 +2508,10 @@
       <c r="K45">
         <v>732603.6241928141</v>
       </c>
-      <c r="L45">
-        <v>0.05</v>
-      </c>
       <c r="M45">
+        <v>0.05</v>
+      </c>
+      <c r="N45">
         <v>0.05</v>
       </c>
     </row>
@@ -2534,10 +2551,10 @@
       <c r="K46">
         <v>569643.4153128543</v>
       </c>
-      <c r="L46">
-        <v>0.05</v>
-      </c>
       <c r="M46">
+        <v>0.05</v>
+      </c>
+      <c r="N46">
         <v>0.05</v>
       </c>
     </row>
@@ -2577,10 +2594,10 @@
       <c r="K47">
         <v>353959.4130974241</v>
       </c>
-      <c r="L47">
-        <v>0.05</v>
-      </c>
       <c r="M47">
+        <v>0.05</v>
+      </c>
+      <c r="N47">
         <v>0.05</v>
       </c>
     </row>
@@ -2620,10 +2637,10 @@
       <c r="K48">
         <v>213509.8577738418</v>
       </c>
-      <c r="L48">
-        <v>0.05</v>
-      </c>
       <c r="M48">
+        <v>0.05</v>
+      </c>
+      <c r="N48">
         <v>0.05</v>
       </c>
     </row>
@@ -2663,10 +2680,10 @@
       <c r="K49">
         <v>219482.3284506314</v>
       </c>
-      <c r="L49">
-        <v>0.05</v>
-      </c>
       <c r="M49">
+        <v>0.05</v>
+      </c>
+      <c r="N49">
         <v>0.05</v>
       </c>
     </row>
@@ -2706,10 +2723,10 @@
       <c r="K50">
         <v>329840.2664919504</v>
       </c>
-      <c r="L50">
-        <v>0.05</v>
-      </c>
       <c r="M50">
+        <v>0.05</v>
+      </c>
+      <c r="N50">
         <v>0.05</v>
       </c>
     </row>
@@ -2749,10 +2766,10 @@
       <c r="K51">
         <v>150478.2895093822</v>
       </c>
-      <c r="L51">
-        <v>0.05</v>
-      </c>
       <c r="M51">
+        <v>0.05</v>
+      </c>
+      <c r="N51">
         <v>0.05</v>
       </c>
     </row>
@@ -2792,10 +2809,10 @@
       <c r="K52">
         <v>97065.40537030963</v>
       </c>
-      <c r="L52">
-        <v>0.05</v>
-      </c>
       <c r="M52">
+        <v>0.05</v>
+      </c>
+      <c r="N52">
         <v>0.05</v>
       </c>
     </row>
@@ -2835,10 +2852,10 @@
       <c r="K53">
         <v>131772.1820819404</v>
       </c>
-      <c r="L53">
-        <v>0.05</v>
-      </c>
       <c r="M53">
+        <v>0.05</v>
+      </c>
+      <c r="N53">
         <v>0.05</v>
       </c>
     </row>
@@ -2878,10 +2895,10 @@
       <c r="K54">
         <v>17687.78978304791</v>
       </c>
-      <c r="L54">
-        <v>0.05</v>
-      </c>
       <c r="M54">
+        <v>0.05</v>
+      </c>
+      <c r="N54">
         <v>0.05</v>
       </c>
     </row>
@@ -2921,10 +2938,10 @@
       <c r="K55">
         <v>21882.51302978364</v>
       </c>
-      <c r="L55">
-        <v>0.05</v>
-      </c>
       <c r="M55">
+        <v>0.05</v>
+      </c>
+      <c r="N55">
         <v>0.05</v>
       </c>
     </row>
@@ -2964,10 +2981,10 @@
       <c r="K56">
         <v>189217.8905235089</v>
       </c>
-      <c r="L56">
-        <v>0.05</v>
-      </c>
       <c r="M56">
+        <v>0.05</v>
+      </c>
+      <c r="N56">
         <v>0.05</v>
       </c>
     </row>
@@ -3007,10 +3024,10 @@
       <c r="K57">
         <v>114009.339885825</v>
       </c>
-      <c r="L57">
-        <v>0.05</v>
-      </c>
       <c r="M57">
+        <v>0.05</v>
+      </c>
+      <c r="N57">
         <v>0.05</v>
       </c>
     </row>
@@ -3050,10 +3067,10 @@
       <c r="K58">
         <v>454549.7827114371</v>
       </c>
-      <c r="L58">
-        <v>0.05</v>
-      </c>
       <c r="M58">
+        <v>0.05</v>
+      </c>
+      <c r="N58">
         <v>0.05</v>
       </c>
     </row>
@@ -3093,10 +3110,10 @@
       <c r="K59">
         <v>333891.8889857767</v>
       </c>
-      <c r="L59">
-        <v>0.05</v>
-      </c>
       <c r="M59">
+        <v>0.05</v>
+      </c>
+      <c r="N59">
         <v>0.05</v>
       </c>
     </row>
@@ -3136,10 +3153,10 @@
       <c r="K60">
         <v>966912.7522210542</v>
       </c>
-      <c r="L60">
-        <v>0.05</v>
-      </c>
       <c r="M60">
+        <v>0.05</v>
+      </c>
+      <c r="N60">
         <v>0.05</v>
       </c>
     </row>
@@ -3179,10 +3196,10 @@
       <c r="K61">
         <v>885638.3882038471</v>
       </c>
-      <c r="L61">
-        <v>0.05</v>
-      </c>
       <c r="M61">
+        <v>0.05</v>
+      </c>
+      <c r="N61">
         <v>0.05</v>
       </c>
     </row>
@@ -3222,10 +3239,10 @@
       <c r="K62">
         <v>645290.4618712433</v>
       </c>
-      <c r="L62">
-        <v>0.05</v>
-      </c>
       <c r="M62">
+        <v>0.05</v>
+      </c>
+      <c r="N62">
         <v>0.05</v>
       </c>
     </row>
@@ -3265,10 +3282,10 @@
       <c r="K63">
         <v>811357.3188160737</v>
       </c>
-      <c r="L63">
-        <v>0.05</v>
-      </c>
       <c r="M63">
+        <v>0.05</v>
+      </c>
+      <c r="N63">
         <v>0.05</v>
       </c>
     </row>
@@ -3308,10 +3325,10 @@
       <c r="K64">
         <v>100032.3097210799</v>
       </c>
-      <c r="L64">
-        <v>0.05</v>
-      </c>
       <c r="M64">
+        <v>0.05</v>
+      </c>
+      <c r="N64">
         <v>0.05</v>
       </c>
     </row>
@@ -3351,10 +3368,10 @@
       <c r="K65">
         <v>271240.703074521</v>
       </c>
-      <c r="L65">
-        <v>0.05</v>
-      </c>
       <c r="M65">
+        <v>0.05</v>
+      </c>
+      <c r="N65">
         <v>0.05</v>
       </c>
     </row>
@@ -3394,10 +3411,10 @@
       <c r="K66">
         <v>147482.6115069279</v>
       </c>
-      <c r="L66">
-        <v>0.05</v>
-      </c>
       <c r="M66">
+        <v>0.05</v>
+      </c>
+      <c r="N66">
         <v>0.05</v>
       </c>
     </row>
@@ -3437,10 +3454,10 @@
       <c r="K67">
         <v>304274.706182281</v>
       </c>
-      <c r="L67">
-        <v>0.05</v>
-      </c>
       <c r="M67">
+        <v>0.05</v>
+      </c>
+      <c r="N67">
         <v>0.05</v>
       </c>
     </row>
@@ -3480,10 +3497,10 @@
       <c r="K68">
         <v>530209.3761206279</v>
       </c>
-      <c r="L68">
-        <v>0.05</v>
-      </c>
       <c r="M68">
+        <v>0.05</v>
+      </c>
+      <c r="N68">
         <v>0.05</v>
       </c>
     </row>
@@ -3523,10 +3540,10 @@
       <c r="K69">
         <v>1046784.042950014</v>
       </c>
-      <c r="L69">
-        <v>0.05</v>
-      </c>
       <c r="M69">
+        <v>0.05</v>
+      </c>
+      <c r="N69">
         <v>0.05</v>
       </c>
     </row>
@@ -3566,10 +3583,10 @@
       <c r="K70">
         <v>1383229.190991441</v>
       </c>
-      <c r="L70">
-        <v>0.05</v>
-      </c>
       <c r="M70">
+        <v>0.05</v>
+      </c>
+      <c r="N70">
         <v>0.05</v>
       </c>
     </row>
@@ -3609,10 +3626,10 @@
       <c r="K71">
         <v>1456288.889933172</v>
       </c>
-      <c r="L71">
-        <v>0.05</v>
-      </c>
       <c r="M71">
+        <v>0.05</v>
+      </c>
+      <c r="N71">
         <v>0.05</v>
       </c>
     </row>
@@ -3652,10 +3669,10 @@
       <c r="K72">
         <v>189975.3795417092</v>
       </c>
-      <c r="L72">
-        <v>0.05</v>
-      </c>
       <c r="M72">
+        <v>0.05</v>
+      </c>
+      <c r="N72">
         <v>0.05</v>
       </c>
     </row>
@@ -3695,10 +3712,10 @@
       <c r="K73">
         <v>265560.8989697707</v>
       </c>
-      <c r="L73">
-        <v>0.05</v>
-      </c>
       <c r="M73">
+        <v>0.05</v>
+      </c>
+      <c r="N73">
         <v>0.05</v>
       </c>
     </row>
@@ -3738,10 +3755,10 @@
       <c r="K74">
         <v>31701.9128248074</v>
       </c>
-      <c r="L74">
-        <v>0.05</v>
-      </c>
       <c r="M74">
+        <v>0.05</v>
+      </c>
+      <c r="N74">
         <v>0.05</v>
       </c>
     </row>
@@ -3781,10 +3798,10 @@
       <c r="K75">
         <v>74647.11735710694</v>
       </c>
-      <c r="L75">
-        <v>0.05</v>
-      </c>
       <c r="M75">
+        <v>0.05</v>
+      </c>
+      <c r="N75">
         <v>0.05</v>
       </c>
     </row>
@@ -3824,10 +3841,10 @@
       <c r="K76">
         <v>99890.87941789668</v>
       </c>
-      <c r="L76">
-        <v>0.05</v>
-      </c>
       <c r="M76">
+        <v>0.05</v>
+      </c>
+      <c r="N76">
         <v>0.05</v>
       </c>
     </row>
@@ -3867,10 +3884,10 @@
       <c r="K77">
         <v>421399.4024497316</v>
       </c>
-      <c r="L77">
-        <v>0.05</v>
-      </c>
       <c r="M77">
+        <v>0.05</v>
+      </c>
+      <c r="N77">
         <v>0.05</v>
       </c>
     </row>
@@ -3910,10 +3927,10 @@
       <c r="K78">
         <v>140758.2659394757</v>
       </c>
-      <c r="L78">
-        <v>0.05</v>
-      </c>
       <c r="M78">
+        <v>0.05</v>
+      </c>
+      <c r="N78">
         <v>0.05</v>
       </c>
     </row>
@@ -3953,10 +3970,10 @@
       <c r="K79">
         <v>103582.4907797132</v>
       </c>
-      <c r="L79">
-        <v>0.05</v>
-      </c>
       <c r="M79">
+        <v>0.05</v>
+      </c>
+      <c r="N79">
         <v>0.05</v>
       </c>
     </row>
@@ -3996,10 +4013,10 @@
       <c r="K80">
         <v>291403.081691474</v>
       </c>
-      <c r="L80">
-        <v>0.05</v>
-      </c>
       <c r="M80">
+        <v>0.05</v>
+      </c>
+      <c r="N80">
         <v>0.05</v>
       </c>
     </row>
@@ -4039,10 +4056,10 @@
       <c r="K81">
         <v>293354.5109088812</v>
       </c>
-      <c r="L81">
-        <v>0.05</v>
-      </c>
       <c r="M81">
+        <v>0.05</v>
+      </c>
+      <c r="N81">
         <v>0.05</v>
       </c>
     </row>
@@ -4082,10 +4099,10 @@
       <c r="K82">
         <v>340480.2751862371</v>
       </c>
-      <c r="L82">
-        <v>0.05</v>
-      </c>
       <c r="M82">
+        <v>0.05</v>
+      </c>
+      <c r="N82">
         <v>0.05</v>
       </c>
     </row>
@@ -4125,10 +4142,10 @@
       <c r="K83">
         <v>132750.731163154</v>
       </c>
-      <c r="L83">
-        <v>0.05</v>
-      </c>
       <c r="M83">
+        <v>0.05</v>
+      </c>
+      <c r="N83">
         <v>0.05</v>
       </c>
     </row>
@@ -4168,10 +4185,10 @@
       <c r="K84">
         <v>134672.3830344016</v>
       </c>
-      <c r="L84">
-        <v>0.05</v>
-      </c>
       <c r="M84">
+        <v>0.05</v>
+      </c>
+      <c r="N84">
         <v>0.05</v>
       </c>
     </row>
@@ -4211,10 +4228,10 @@
       <c r="K85">
         <v>749912.0346085769</v>
       </c>
-      <c r="L85">
-        <v>0.05</v>
-      </c>
       <c r="M85">
+        <v>0.05</v>
+      </c>
+      <c r="N85">
         <v>0.05</v>
       </c>
     </row>
@@ -4254,10 +4271,10 @@
       <c r="K86">
         <v>225085.0063342566</v>
       </c>
-      <c r="L86">
-        <v>0.05</v>
-      </c>
       <c r="M86">
+        <v>0.05</v>
+      </c>
+      <c r="N86">
         <v>0.05</v>
       </c>
     </row>
@@ -4297,10 +4314,10 @@
       <c r="K87">
         <v>226137.5012402972</v>
       </c>
-      <c r="L87">
-        <v>0.05</v>
-      </c>
       <c r="M87">
+        <v>0.05</v>
+      </c>
+      <c r="N87">
         <v>0.05</v>
       </c>
     </row>
@@ -4340,10 +4357,10 @@
       <c r="K88">
         <v>90778.66436880779</v>
       </c>
-      <c r="L88">
-        <v>0.05</v>
-      </c>
       <c r="M88">
+        <v>0.05</v>
+      </c>
+      <c r="N88">
         <v>0.05</v>
       </c>
     </row>
@@ -4383,10 +4400,10 @@
       <c r="K89">
         <v>34453.35591884049</v>
       </c>
-      <c r="L89">
-        <v>0.05</v>
-      </c>
       <c r="M89">
+        <v>0.05</v>
+      </c>
+      <c r="N89">
         <v>0.05</v>
       </c>
     </row>
@@ -4423,10 +4440,10 @@
       <c r="J90">
         <v>1000</v>
       </c>
-      <c r="L90">
-        <v>0.05</v>
-      </c>
       <c r="M90">
+        <v>0.05</v>
+      </c>
+      <c r="N90">
         <v>0.05</v>
       </c>
     </row>
@@ -4463,10 +4480,10 @@
       <c r="J91">
         <v>1000</v>
       </c>
-      <c r="L91">
-        <v>0.05</v>
-      </c>
       <c r="M91">
+        <v>0.05</v>
+      </c>
+      <c r="N91">
         <v>0.05</v>
       </c>
     </row>
@@ -4503,10 +4520,10 @@
       <c r="J92">
         <v>1000</v>
       </c>
-      <c r="L92">
-        <v>0.05</v>
-      </c>
       <c r="M92">
+        <v>0.05</v>
+      </c>
+      <c r="N92">
         <v>0.05</v>
       </c>
     </row>
@@ -4543,10 +4560,10 @@
       <c r="J93">
         <v>1000</v>
       </c>
-      <c r="L93">
-        <v>0.05</v>
-      </c>
       <c r="M93">
+        <v>0.05</v>
+      </c>
+      <c r="N93">
         <v>0.05</v>
       </c>
     </row>
@@ -4583,10 +4600,10 @@
       <c r="J94">
         <v>1000</v>
       </c>
-      <c r="L94">
-        <v>0.05</v>
-      </c>
       <c r="M94">
+        <v>0.05</v>
+      </c>
+      <c r="N94">
         <v>0.05</v>
       </c>
     </row>
@@ -4623,10 +4640,10 @@
       <c r="J95">
         <v>1000</v>
       </c>
-      <c r="L95">
-        <v>0.05</v>
-      </c>
       <c r="M95">
+        <v>0.05</v>
+      </c>
+      <c r="N95">
         <v>0.05</v>
       </c>
     </row>
@@ -4663,10 +4680,15 @@
       <c r="J96">
         <v>221</v>
       </c>
-      <c r="L96">
-        <v>0.05</v>
+      <c r="L96" t="inlineStr">
+        <is>
+          <t>data from Starr, P. J., A. T. Charles and M. A. Henderson 1984. Reconstruction of British Columbia sockeye salmon (Oncorhynchus nerka) stocks: 1970-1982. Can. MS. Rep. Fish. Aquat. Sci</t>
+        </is>
       </c>
       <c r="M96">
+        <v>0.05</v>
+      </c>
+      <c r="N96">
         <v>0.2</v>
       </c>
     </row>
@@ -4703,10 +4725,15 @@
       <c r="J97">
         <v>214</v>
       </c>
-      <c r="L97">
-        <v>0.05</v>
+      <c r="L97" t="inlineStr">
+        <is>
+          <t>data from Starr, P. J., A. T. Charles and M. A. Henderson 1984. Reconstruction of British Columbia sockeye salmon (Oncorhynchus nerka) stocks: 1970-1982. Can. MS. Rep. Fish. Aquat. Sci</t>
+        </is>
       </c>
       <c r="M97">
+        <v>0.05</v>
+      </c>
+      <c r="N97">
         <v>0.2</v>
       </c>
     </row>
@@ -4743,10 +4770,15 @@
       <c r="J98">
         <v>83</v>
       </c>
-      <c r="L98">
-        <v>0.05</v>
+      <c r="L98" t="inlineStr">
+        <is>
+          <t>data from Starr, P. J., A. T. Charles and M. A. Henderson 1984. Reconstruction of British Columbia sockeye salmon (Oncorhynchus nerka) stocks: 1970-1982. Can. MS. Rep. Fish. Aquat. Sci</t>
+        </is>
       </c>
       <c r="M98">
+        <v>0.05</v>
+      </c>
+      <c r="N98">
         <v>0.2</v>
       </c>
     </row>
@@ -4783,10 +4815,15 @@
       <c r="J99">
         <v>187</v>
       </c>
-      <c r="L99">
-        <v>0.05</v>
+      <c r="L99" t="inlineStr">
+        <is>
+          <t>data from Starr, P. J., A. T. Charles and M. A. Henderson 1984. Reconstruction of British Columbia sockeye salmon (Oncorhynchus nerka) stocks: 1970-1982. Can. MS. Rep. Fish. Aquat. Sci</t>
+        </is>
       </c>
       <c r="M99">
+        <v>0.05</v>
+      </c>
+      <c r="N99">
         <v>0.2</v>
       </c>
     </row>
@@ -4823,10 +4860,15 @@
       <c r="J100">
         <v>288</v>
       </c>
-      <c r="L100">
-        <v>0.05</v>
+      <c r="L100" t="inlineStr">
+        <is>
+          <t>data from draft Henderson paper</t>
+        </is>
       </c>
       <c r="M100">
+        <v>0.05</v>
+      </c>
+      <c r="N100">
         <v>0.2</v>
       </c>
     </row>
@@ -4863,10 +4905,15 @@
       <c r="J101">
         <v>294</v>
       </c>
-      <c r="L101">
-        <v>0.05</v>
+      <c r="L101" t="inlineStr">
+        <is>
+          <t>data from draft Henderson paper</t>
+        </is>
       </c>
       <c r="M101">
+        <v>0.05</v>
+      </c>
+      <c r="N101">
         <v>0.2</v>
       </c>
     </row>
@@ -4903,10 +4950,15 @@
       <c r="J102">
         <v>293</v>
       </c>
-      <c r="L102">
-        <v>0.05</v>
+      <c r="L102" t="inlineStr">
+        <is>
+          <t>data from draft Henderson paper</t>
+        </is>
       </c>
       <c r="M102">
+        <v>0.05</v>
+      </c>
+      <c r="N102">
         <v>0.2</v>
       </c>
     </row>
@@ -4943,10 +4995,15 @@
       <c r="J103">
         <v>159</v>
       </c>
-      <c r="L103">
-        <v>0.05</v>
+      <c r="L103" t="inlineStr">
+        <is>
+          <t>data from draft Henderson paper</t>
+        </is>
       </c>
       <c r="M103">
+        <v>0.05</v>
+      </c>
+      <c r="N103">
         <v>0.2</v>
       </c>
     </row>
@@ -4983,10 +5040,15 @@
       <c r="J104">
         <v>82</v>
       </c>
-      <c r="L104">
-        <v>0.05</v>
+      <c r="L104" t="inlineStr">
+        <is>
+          <t>data from draft Henderson paper</t>
+        </is>
       </c>
       <c r="M104">
+        <v>0.05</v>
+      </c>
+      <c r="N104">
         <v>0.2</v>
       </c>
     </row>
@@ -5023,10 +5085,15 @@
       <c r="J105">
         <v>122</v>
       </c>
-      <c r="L105">
-        <v>0.05</v>
+      <c r="L105" t="inlineStr">
+        <is>
+          <t>data from draft Henderson paper</t>
+        </is>
       </c>
       <c r="M105">
+        <v>0.05</v>
+      </c>
+      <c r="N105">
         <v>0.2</v>
       </c>
     </row>
@@ -5063,10 +5130,15 @@
       <c r="J106">
         <v>446</v>
       </c>
-      <c r="L106">
-        <v>0.05</v>
+      <c r="L106" t="inlineStr">
+        <is>
+          <t>data from draft Henderson paper</t>
+        </is>
       </c>
       <c r="M106">
+        <v>0.05</v>
+      </c>
+      <c r="N106">
         <v>0.2</v>
       </c>
     </row>
@@ -5103,10 +5175,15 @@
       <c r="J107">
         <v>151</v>
       </c>
-      <c r="L107">
-        <v>0.05</v>
+      <c r="L107" t="inlineStr">
+        <is>
+          <t>data from draft Henderson paper</t>
+        </is>
       </c>
       <c r="M107">
+        <v>0.05</v>
+      </c>
+      <c r="N107">
         <v>0.2</v>
       </c>
     </row>
@@ -5143,10 +5220,15 @@
       <c r="J108">
         <v>309</v>
       </c>
-      <c r="L108">
-        <v>0.05</v>
+      <c r="L108" t="inlineStr">
+        <is>
+          <t>data from draft Henderson paper</t>
+        </is>
       </c>
       <c r="M108">
+        <v>0.05</v>
+      </c>
+      <c r="N108">
         <v>0.2</v>
       </c>
     </row>
@@ -5183,10 +5265,15 @@
       <c r="J109">
         <v>312</v>
       </c>
-      <c r="L109">
-        <v>0.05</v>
+      <c r="L109" t="inlineStr">
+        <is>
+          <t>data from draft Henderson paper</t>
+        </is>
       </c>
       <c r="M109">
+        <v>0.05</v>
+      </c>
+      <c r="N109">
         <v>0.2</v>
       </c>
     </row>
@@ -5223,10 +5310,15 @@
       <c r="J110">
         <v>325</v>
       </c>
-      <c r="L110">
-        <v>0.05</v>
+      <c r="L110" t="inlineStr">
+        <is>
+          <t>data from draft Henderson paper</t>
+        </is>
       </c>
       <c r="M110">
+        <v>0.05</v>
+      </c>
+      <c r="N110">
         <v>0.2</v>
       </c>
     </row>
@@ -5263,10 +5355,15 @@
       <c r="J111">
         <v>312</v>
       </c>
-      <c r="L111">
-        <v>0.05</v>
+      <c r="L111" t="inlineStr">
+        <is>
+          <t>data from draft Henderson paper</t>
+        </is>
       </c>
       <c r="M111">
+        <v>0.05</v>
+      </c>
+      <c r="N111">
         <v>0.2</v>
       </c>
     </row>
@@ -5303,10 +5400,15 @@
       <c r="J112">
         <v>234</v>
       </c>
-      <c r="L112">
-        <v>0.05</v>
+      <c r="L112" t="inlineStr">
+        <is>
+          <t>data from draft Henderson paper</t>
+        </is>
       </c>
       <c r="M112">
+        <v>0.05</v>
+      </c>
+      <c r="N112">
         <v>0.2</v>
       </c>
     </row>
@@ -5343,10 +5445,15 @@
       <c r="J113">
         <v>254</v>
       </c>
-      <c r="L113">
-        <v>0.05</v>
+      <c r="L113" t="inlineStr">
+        <is>
+          <t>data from draft Henderson paper</t>
+        </is>
       </c>
       <c r="M113">
+        <v>0.05</v>
+      </c>
+      <c r="N113">
         <v>0.2</v>
       </c>
     </row>
@@ -5383,10 +5490,15 @@
       <c r="J114">
         <v>70</v>
       </c>
-      <c r="L114">
-        <v>0.05</v>
+      <c r="L114" t="inlineStr">
+        <is>
+          <t>data from draft Henderson paper</t>
+        </is>
       </c>
       <c r="M114">
+        <v>0.05</v>
+      </c>
+      <c r="N114">
         <v>0.2</v>
       </c>
     </row>
@@ -5423,10 +5535,15 @@
       <c r="J115">
         <v>253</v>
       </c>
-      <c r="L115">
-        <v>0.05</v>
+      <c r="L115" t="inlineStr">
+        <is>
+          <t>data from draft Henderson paper</t>
+        </is>
       </c>
       <c r="M115">
+        <v>0.05</v>
+      </c>
+      <c r="N115">
         <v>0.2</v>
       </c>
     </row>
@@ -5463,10 +5580,15 @@
       <c r="J116">
         <v>97</v>
       </c>
-      <c r="L116">
-        <v>0.05</v>
+      <c r="L116" t="inlineStr">
+        <is>
+          <t>data from draft Henderson paper</t>
+        </is>
       </c>
       <c r="M116">
+        <v>0.05</v>
+      </c>
+      <c r="N116">
         <v>0.2</v>
       </c>
     </row>
@@ -5503,10 +5625,15 @@
       <c r="J117">
         <v>364</v>
       </c>
-      <c r="L117">
-        <v>0.05</v>
+      <c r="L117" t="inlineStr">
+        <is>
+          <t>data from draft Henderson paper</t>
+        </is>
       </c>
       <c r="M117">
+        <v>0.05</v>
+      </c>
+      <c r="N117">
         <v>0.2</v>
       </c>
     </row>
@@ -5543,10 +5670,15 @@
       <c r="J118">
         <v>33</v>
       </c>
-      <c r="L118">
-        <v>0.05</v>
+      <c r="L118" t="inlineStr">
+        <is>
+          <t>data from draft Henderson paper</t>
+        </is>
       </c>
       <c r="M118">
+        <v>0.05</v>
+      </c>
+      <c r="N118">
         <v>0.2</v>
       </c>
     </row>
@@ -5583,10 +5715,15 @@
       <c r="J119">
         <v>247</v>
       </c>
-      <c r="L119">
-        <v>0.05</v>
+      <c r="L119" t="inlineStr">
+        <is>
+          <t>data from draft Henderson paper</t>
+        </is>
       </c>
       <c r="M119">
+        <v>0.05</v>
+      </c>
+      <c r="N119">
         <v>0.2</v>
       </c>
     </row>
@@ -5623,10 +5760,15 @@
       <c r="J120">
         <v>230</v>
       </c>
-      <c r="L120">
-        <v>0.05</v>
+      <c r="L120" t="inlineStr">
+        <is>
+          <t>data from draft Henderson paper</t>
+        </is>
       </c>
       <c r="M120">
+        <v>0.05</v>
+      </c>
+      <c r="N120">
         <v>0.2</v>
       </c>
     </row>
@@ -5663,10 +5805,15 @@
       <c r="J121">
         <v>137</v>
       </c>
-      <c r="L121">
-        <v>0.05</v>
+      <c r="L121" t="inlineStr">
+        <is>
+          <t>data from draft Henderson paper</t>
+        </is>
       </c>
       <c r="M121">
+        <v>0.05</v>
+      </c>
+      <c r="N121">
         <v>0.2</v>
       </c>
     </row>
@@ -5691,10 +5838,15 @@
       <c r="J122">
         <v>0</v>
       </c>
-      <c r="L122">
-        <v>0.05</v>
+      <c r="L122" t="inlineStr">
+        <is>
+          <t>data from draft Henderson paper</t>
+        </is>
       </c>
       <c r="M122">
+        <v>0.05</v>
+      </c>
+      <c r="N122">
         <v>0.2</v>
       </c>
     </row>
@@ -5719,10 +5871,15 @@
       <c r="J123">
         <v>0</v>
       </c>
-      <c r="L123">
-        <v>0.05</v>
+      <c r="L123" t="inlineStr">
+        <is>
+          <t>data from draft Henderson paper</t>
+        </is>
       </c>
       <c r="M123">
+        <v>0.05</v>
+      </c>
+      <c r="N123">
         <v>0.2</v>
       </c>
     </row>
@@ -5747,10 +5904,15 @@
       <c r="J124">
         <v>0</v>
       </c>
-      <c r="L124">
-        <v>0.05</v>
+      <c r="L124" t="inlineStr">
+        <is>
+          <t>data from draft Henderson paper</t>
+        </is>
       </c>
       <c r="M124">
+        <v>0.05</v>
+      </c>
+      <c r="N124">
         <v>0.2</v>
       </c>
     </row>
@@ -5775,10 +5937,15 @@
       <c r="J125">
         <v>0</v>
       </c>
-      <c r="L125">
-        <v>0.05</v>
+      <c r="L125" t="inlineStr">
+        <is>
+          <t>data from draft Henderson paper</t>
+        </is>
       </c>
       <c r="M125">
+        <v>0.05</v>
+      </c>
+      <c r="N125">
         <v>0.2</v>
       </c>
     </row>
@@ -5815,10 +5982,15 @@
       <c r="J126">
         <v>94</v>
       </c>
-      <c r="L126">
-        <v>0.05</v>
+      <c r="L126" t="inlineStr">
+        <is>
+          <t>data from draft Henderson paper</t>
+        </is>
       </c>
       <c r="M126">
+        <v>0.05</v>
+      </c>
+      <c r="N126">
         <v>0.2</v>
       </c>
     </row>
@@ -5855,10 +6027,15 @@
       <c r="J127">
         <v>52</v>
       </c>
-      <c r="L127">
+      <c r="L127" t="inlineStr">
+        <is>
+          <t>data from draft Henderson paper</t>
+        </is>
+      </c>
+      <c r="M127">
         <v>0.399812753899036</v>
       </c>
-      <c r="M127">
+      <c r="N127">
         <v>0.2</v>
       </c>
     </row>
@@ -5895,10 +6072,10 @@
       <c r="J128">
         <v>303</v>
       </c>
-      <c r="L128">
+      <c r="M128">
         <v>0.399812753899036</v>
       </c>
-      <c r="M128">
+      <c r="N128">
         <v>0.2</v>
       </c>
     </row>
@@ -5935,10 +6112,10 @@
       <c r="J129">
         <v>67</v>
       </c>
-      <c r="L129">
+      <c r="M129">
         <v>0.399812753899036</v>
       </c>
-      <c r="M129">
+      <c r="N129">
         <v>0.2</v>
       </c>
     </row>
@@ -5975,10 +6152,10 @@
       <c r="J130">
         <v>62</v>
       </c>
-      <c r="L130">
-        <v>0.05</v>
-      </c>
       <c r="M130">
+        <v>0.05</v>
+      </c>
+      <c r="N130">
         <v>0.2</v>
       </c>
     </row>
@@ -6015,10 +6192,10 @@
       <c r="J131">
         <v>47</v>
       </c>
-      <c r="L131">
-        <v>0.05</v>
-      </c>
       <c r="M131">
+        <v>0.05</v>
+      </c>
+      <c r="N131">
         <v>0.1</v>
       </c>
     </row>
@@ -6055,10 +6232,10 @@
       <c r="J132">
         <v>36</v>
       </c>
-      <c r="L132">
-        <v>0.05</v>
-      </c>
       <c r="M132">
+        <v>0.05</v>
+      </c>
+      <c r="N132">
         <v>0.1</v>
       </c>
     </row>
@@ -6095,10 +6272,10 @@
       <c r="J133">
         <v>76</v>
       </c>
-      <c r="L133">
-        <v>0.05</v>
-      </c>
       <c r="M133">
+        <v>0.05</v>
+      </c>
+      <c r="N133">
         <v>0.1</v>
       </c>
     </row>
@@ -6135,10 +6312,10 @@
       <c r="J134">
         <v>2</v>
       </c>
-      <c r="L134">
-        <v>0.05</v>
-      </c>
       <c r="M134">
+        <v>0.05</v>
+      </c>
+      <c r="N134">
         <v>0.1</v>
       </c>
     </row>
@@ -6175,10 +6352,10 @@
       <c r="J135">
         <v>119</v>
       </c>
-      <c r="L135">
-        <v>0.05</v>
-      </c>
       <c r="M135">
+        <v>0.05</v>
+      </c>
+      <c r="N135">
         <v>0.1</v>
       </c>
     </row>
@@ -6215,10 +6392,10 @@
       <c r="J136">
         <v>44</v>
       </c>
-      <c r="L136">
-        <v>0.05</v>
-      </c>
       <c r="M136">
+        <v>0.05</v>
+      </c>
+      <c r="N136">
         <v>0.1</v>
       </c>
     </row>
@@ -6255,10 +6432,10 @@
       <c r="J137">
         <v>28</v>
       </c>
-      <c r="L137">
-        <v>0.05</v>
-      </c>
       <c r="M137">
+        <v>0.05</v>
+      </c>
+      <c r="N137">
         <v>0.1</v>
       </c>
     </row>
@@ -6295,10 +6472,10 @@
       <c r="J138">
         <v>16</v>
       </c>
-      <c r="L138">
-        <v>0.05</v>
-      </c>
       <c r="M138">
+        <v>0.05</v>
+      </c>
+      <c r="N138">
         <v>0.1</v>
       </c>
     </row>
@@ -6323,10 +6500,10 @@
       <c r="J139">
         <v>0</v>
       </c>
-      <c r="L139">
-        <v>0.05</v>
-      </c>
       <c r="M139">
+        <v>0.05</v>
+      </c>
+      <c r="N139">
         <v>0.1</v>
       </c>
     </row>
@@ -6363,10 +6540,10 @@
       <c r="J140">
         <v>7</v>
       </c>
-      <c r="L140">
-        <v>0.05</v>
-      </c>
       <c r="M140">
+        <v>0.05</v>
+      </c>
+      <c r="N140">
         <v>0.1</v>
       </c>
     </row>
@@ -6403,10 +6580,10 @@
       <c r="J141">
         <v>82</v>
       </c>
-      <c r="L141">
-        <v>0.05</v>
-      </c>
       <c r="M141">
+        <v>0.05</v>
+      </c>
+      <c r="N141">
         <v>0.1</v>
       </c>
     </row>
@@ -6443,10 +6620,10 @@
       <c r="J142">
         <v>158</v>
       </c>
-      <c r="L142">
-        <v>0.05</v>
-      </c>
       <c r="M142">
+        <v>0.05</v>
+      </c>
+      <c r="N142">
         <v>0.1</v>
       </c>
     </row>
@@ -6465,10 +6642,15 @@
       <c r="J143">
         <v>0</v>
       </c>
-      <c r="L143">
+      <c r="L143" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
+      </c>
+      <c r="M143">
         <v>0.399812753899036</v>
       </c>
-      <c r="M143">
+      <c r="N143">
         <v>0.2</v>
       </c>
     </row>
@@ -6487,10 +6669,15 @@
       <c r="J144">
         <v>0</v>
       </c>
-      <c r="L144">
+      <c r="L144" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
+      </c>
+      <c r="M144">
         <v>0.399812753899036</v>
       </c>
-      <c r="M144">
+      <c r="N144">
         <v>0.2</v>
       </c>
     </row>
@@ -6509,10 +6696,15 @@
       <c r="J145">
         <v>0</v>
       </c>
-      <c r="L145">
+      <c r="L145" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
+      </c>
+      <c r="M145">
         <v>0.399812753899036</v>
       </c>
-      <c r="M145">
+      <c r="N145">
         <v>0.2</v>
       </c>
     </row>
@@ -6531,10 +6723,15 @@
       <c r="J146">
         <v>0</v>
       </c>
-      <c r="L146">
+      <c r="L146" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
+      </c>
+      <c r="M146">
         <v>0.399812753899036</v>
       </c>
-      <c r="M146">
+      <c r="N146">
         <v>0.2</v>
       </c>
     </row>
@@ -6553,10 +6750,15 @@
       <c r="J147">
         <v>0</v>
       </c>
-      <c r="L147">
+      <c r="L147" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
+      </c>
+      <c r="M147">
         <v>0.399812753899036</v>
       </c>
-      <c r="M147">
+      <c r="N147">
         <v>0.2</v>
       </c>
     </row>
@@ -6575,10 +6777,15 @@
       <c r="J148">
         <v>0</v>
       </c>
-      <c r="L148">
+      <c r="L148" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
+      </c>
+      <c r="M148">
         <v>0.399812753899036</v>
       </c>
-      <c r="M148">
+      <c r="N148">
         <v>0.2</v>
       </c>
     </row>
@@ -6597,10 +6804,15 @@
       <c r="J149">
         <v>0</v>
       </c>
-      <c r="L149">
+      <c r="L149" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
+      </c>
+      <c r="M149">
         <v>0.399812753899036</v>
       </c>
-      <c r="M149">
+      <c r="N149">
         <v>0.2</v>
       </c>
     </row>
@@ -6619,10 +6831,15 @@
       <c r="J150">
         <v>0</v>
       </c>
-      <c r="L150">
+      <c r="L150" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
+      </c>
+      <c r="M150">
         <v>0.399812753899036</v>
       </c>
-      <c r="M150">
+      <c r="N150">
         <v>0.2</v>
       </c>
     </row>
@@ -6638,13 +6855,24 @@
       <c r="C151">
         <v>65000</v>
       </c>
+      <c r="H151">
+        <v>100412</v>
+      </c>
+      <c r="I151">
+        <v>35412</v>
+      </c>
       <c r="J151">
         <v>0</v>
       </c>
-      <c r="L151">
-        <v>0.399812753899036</v>
+      <c r="L151" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
       </c>
       <c r="M151">
+        <v>0.05</v>
+      </c>
+      <c r="N151">
         <v>0.2</v>
       </c>
     </row>
@@ -6660,13 +6888,24 @@
       <c r="C152">
         <v>70000</v>
       </c>
+      <c r="H152">
+        <v>95669</v>
+      </c>
+      <c r="I152">
+        <v>25669</v>
+      </c>
       <c r="J152">
         <v>0</v>
       </c>
-      <c r="L152">
-        <v>0.399812753899036</v>
+      <c r="L152" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
       </c>
       <c r="M152">
+        <v>0.05</v>
+      </c>
+      <c r="N152">
         <v>0.2</v>
       </c>
     </row>
@@ -6682,13 +6921,24 @@
       <c r="C153">
         <v>70000</v>
       </c>
+      <c r="H153">
+        <v>85000</v>
+      </c>
+      <c r="I153">
+        <v>15000</v>
+      </c>
       <c r="J153">
         <v>0</v>
       </c>
-      <c r="L153">
-        <v>0.399812753899036</v>
+      <c r="L153" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
       </c>
       <c r="M153">
+        <v>0.05</v>
+      </c>
+      <c r="N153">
         <v>0.2</v>
       </c>
     </row>
@@ -6707,10 +6957,15 @@
       <c r="J154">
         <v>0</v>
       </c>
-      <c r="L154">
+      <c r="L154" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
+      </c>
+      <c r="M154">
         <v>0.399812753899036</v>
       </c>
-      <c r="M154">
+      <c r="N154">
         <v>0.2</v>
       </c>
     </row>
@@ -6726,13 +6981,24 @@
       <c r="C155">
         <v>40000</v>
       </c>
+      <c r="H155">
+        <v>50600</v>
+      </c>
+      <c r="I155">
+        <v>10600</v>
+      </c>
       <c r="J155">
         <v>0</v>
       </c>
-      <c r="L155">
-        <v>0.399812753899036</v>
+      <c r="L155" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
       </c>
       <c r="M155">
+        <v>0.05</v>
+      </c>
+      <c r="N155">
         <v>0.2</v>
       </c>
     </row>
@@ -6748,13 +7014,24 @@
       <c r="C156">
         <v>50000</v>
       </c>
+      <c r="H156">
+        <v>70260</v>
+      </c>
+      <c r="I156">
+        <v>20260</v>
+      </c>
       <c r="J156">
         <v>0</v>
       </c>
-      <c r="L156">
-        <v>0.399812753899036</v>
+      <c r="L156" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
       </c>
       <c r="M156">
+        <v>0.05</v>
+      </c>
+      <c r="N156">
         <v>0.2</v>
       </c>
     </row>
@@ -6770,13 +7047,24 @@
       <c r="C157">
         <v>35000</v>
       </c>
+      <c r="H157">
+        <v>63000</v>
+      </c>
+      <c r="I157">
+        <v>28000</v>
+      </c>
       <c r="J157">
         <v>0</v>
       </c>
-      <c r="L157">
-        <v>0.399812753899036</v>
+      <c r="L157" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
       </c>
       <c r="M157">
+        <v>0.05</v>
+      </c>
+      <c r="N157">
         <v>0.2</v>
       </c>
     </row>
@@ -6792,13 +7080,24 @@
       <c r="C158">
         <v>7500</v>
       </c>
+      <c r="H158">
+        <v>28000</v>
+      </c>
+      <c r="I158">
+        <v>20500</v>
+      </c>
       <c r="J158">
         <v>0</v>
       </c>
-      <c r="L158">
-        <v>0.399812753899036</v>
+      <c r="L158" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
       </c>
       <c r="M158">
+        <v>0.05</v>
+      </c>
+      <c r="N158">
         <v>0.2</v>
       </c>
     </row>
@@ -6814,13 +7113,24 @@
       <c r="C159">
         <v>15000</v>
       </c>
+      <c r="H159">
+        <v>21500</v>
+      </c>
+      <c r="I159">
+        <v>6500</v>
+      </c>
       <c r="J159">
         <v>0</v>
       </c>
-      <c r="L159">
-        <v>0.399812753899036</v>
+      <c r="L159" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
       </c>
       <c r="M159">
+        <v>0.05</v>
+      </c>
+      <c r="N159">
         <v>0.2</v>
       </c>
     </row>
@@ -6839,10 +7149,15 @@
       <c r="J160">
         <v>0</v>
       </c>
-      <c r="L160">
+      <c r="L160" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
+      </c>
+      <c r="M160">
         <v>0.399812753899036</v>
       </c>
-      <c r="M160">
+      <c r="N160">
         <v>0.2</v>
       </c>
     </row>
@@ -6861,10 +7176,15 @@
       <c r="J161">
         <v>0</v>
       </c>
-      <c r="L161">
+      <c r="L161" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
+      </c>
+      <c r="M161">
         <v>0.399812753899036</v>
       </c>
-      <c r="M161">
+      <c r="N161">
         <v>0.2</v>
       </c>
     </row>
@@ -6883,10 +7203,15 @@
       <c r="J162">
         <v>0</v>
       </c>
-      <c r="L162">
+      <c r="L162" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
+      </c>
+      <c r="M162">
         <v>0.399812753899036</v>
       </c>
-      <c r="M162">
+      <c r="N162">
         <v>0.2</v>
       </c>
     </row>
@@ -6905,10 +7230,15 @@
       <c r="J163">
         <v>0</v>
       </c>
-      <c r="L163">
+      <c r="L163" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
+      </c>
+      <c r="M163">
         <v>0.399812753899036</v>
       </c>
-      <c r="M163">
+      <c r="N163">
         <v>0.2</v>
       </c>
     </row>
@@ -6927,10 +7257,15 @@
       <c r="J164">
         <v>0</v>
       </c>
-      <c r="L164">
+      <c r="L164" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
+      </c>
+      <c r="M164">
         <v>0.399812753899036</v>
       </c>
-      <c r="M164">
+      <c r="N164">
         <v>0.2</v>
       </c>
     </row>
@@ -6949,10 +7284,15 @@
       <c r="J165">
         <v>0</v>
       </c>
-      <c r="L165">
+      <c r="L165" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
+      </c>
+      <c r="M165">
         <v>0.399812753899036</v>
       </c>
-      <c r="M165">
+      <c r="N165">
         <v>0.2</v>
       </c>
     </row>
@@ -6971,10 +7311,15 @@
       <c r="J166">
         <v>0</v>
       </c>
-      <c r="L166">
+      <c r="L166" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
+      </c>
+      <c r="M166">
         <v>0.399812753899036</v>
       </c>
-      <c r="M166">
+      <c r="N166">
         <v>0.2</v>
       </c>
     </row>
@@ -6993,10 +7338,15 @@
       <c r="J167">
         <v>0</v>
       </c>
-      <c r="L167">
+      <c r="L167" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
+      </c>
+      <c r="M167">
         <v>0.399812753899036</v>
       </c>
-      <c r="M167">
+      <c r="N167">
         <v>0.2</v>
       </c>
     </row>
@@ -7015,10 +7365,15 @@
       <c r="J168">
         <v>0</v>
       </c>
-      <c r="L168">
+      <c r="L168" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
+      </c>
+      <c r="M168">
         <v>0.399812753899036</v>
       </c>
-      <c r="M168">
+      <c r="N168">
         <v>0.2</v>
       </c>
     </row>
@@ -7037,10 +7392,15 @@
       <c r="J169">
         <v>0</v>
       </c>
-      <c r="L169">
+      <c r="L169" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
+      </c>
+      <c r="M169">
         <v>0.399812753899036</v>
       </c>
-      <c r="M169">
+      <c r="N169">
         <v>0.2</v>
       </c>
     </row>
@@ -7059,10 +7419,15 @@
       <c r="J170">
         <v>0</v>
       </c>
-      <c r="L170">
+      <c r="L170" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
+      </c>
+      <c r="M170">
         <v>0.399812753899036</v>
       </c>
-      <c r="M170">
+      <c r="N170">
         <v>0.2</v>
       </c>
     </row>
@@ -7081,10 +7446,15 @@
       <c r="J171">
         <v>0</v>
       </c>
-      <c r="L171">
+      <c r="L171" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
+      </c>
+      <c r="M171">
         <v>0.399812753899036</v>
       </c>
-      <c r="M171">
+      <c r="N171">
         <v>0.2</v>
       </c>
     </row>
@@ -7103,10 +7473,15 @@
       <c r="J172">
         <v>0</v>
       </c>
-      <c r="L172">
+      <c r="L172" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
+      </c>
+      <c r="M172">
         <v>0.399812753899036</v>
       </c>
-      <c r="M172">
+      <c r="N172">
         <v>0.2</v>
       </c>
     </row>
@@ -7125,10 +7500,15 @@
       <c r="J173">
         <v>0</v>
       </c>
-      <c r="L173">
+      <c r="L173" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
+      </c>
+      <c r="M173">
         <v>0.399812753899036</v>
       </c>
-      <c r="M173">
+      <c r="N173">
         <v>0.2</v>
       </c>
     </row>
@@ -7147,10 +7527,15 @@
       <c r="J174">
         <v>0</v>
       </c>
-      <c r="L174">
+      <c r="L174" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
+      </c>
+      <c r="M174">
         <v>0.399812753899036</v>
       </c>
-      <c r="M174">
+      <c r="N174">
         <v>0.2</v>
       </c>
     </row>
@@ -7169,10 +7554,15 @@
       <c r="J175">
         <v>0</v>
       </c>
-      <c r="L175">
+      <c r="L175" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
+      </c>
+      <c r="M175">
         <v>0.399812753899036</v>
       </c>
-      <c r="M175">
+      <c r="N175">
         <v>0.2</v>
       </c>
     </row>
@@ -7191,10 +7581,15 @@
       <c r="J176">
         <v>0</v>
       </c>
-      <c r="L176">
+      <c r="L176" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
+      </c>
+      <c r="M176">
         <v>0.399812753899036</v>
       </c>
-      <c r="M176">
+      <c r="N176">
         <v>0.2</v>
       </c>
     </row>
@@ -7213,10 +7608,15 @@
       <c r="J177">
         <v>0</v>
       </c>
-      <c r="L177">
+      <c r="L177" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
+      </c>
+      <c r="M177">
         <v>0.399812753899036</v>
       </c>
-      <c r="M177">
+      <c r="N177">
         <v>0.2</v>
       </c>
     </row>
@@ -7235,10 +7635,15 @@
       <c r="J178">
         <v>0</v>
       </c>
-      <c r="L178">
+      <c r="L178" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
+      </c>
+      <c r="M178">
         <v>0.399812753899036</v>
       </c>
-      <c r="M178">
+      <c r="N178">
         <v>0.2</v>
       </c>
     </row>
@@ -7257,10 +7662,15 @@
       <c r="J179">
         <v>0</v>
       </c>
-      <c r="L179">
+      <c r="L179" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
+      </c>
+      <c r="M179">
         <v>0.399812753899036</v>
       </c>
-      <c r="M179">
+      <c r="N179">
         <v>0.2</v>
       </c>
     </row>
@@ -7279,10 +7689,15 @@
       <c r="J180">
         <v>0</v>
       </c>
-      <c r="L180">
+      <c r="L180" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
+      </c>
+      <c r="M180">
         <v>0.399812753899036</v>
       </c>
-      <c r="M180">
+      <c r="N180">
         <v>0.2</v>
       </c>
     </row>
@@ -7301,10 +7716,15 @@
       <c r="J181">
         <v>0</v>
       </c>
-      <c r="L181">
+      <c r="L181" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
+      </c>
+      <c r="M181">
         <v>0.399812753899036</v>
       </c>
-      <c r="M181">
+      <c r="N181">
         <v>0.2</v>
       </c>
     </row>
@@ -7323,10 +7743,15 @@
       <c r="J182">
         <v>0</v>
       </c>
-      <c r="L182">
+      <c r="L182" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
+      </c>
+      <c r="M182">
         <v>0.399812753899036</v>
       </c>
-      <c r="M182">
+      <c r="N182">
         <v>0.2</v>
       </c>
     </row>
@@ -7345,10 +7770,15 @@
       <c r="J183">
         <v>0</v>
       </c>
-      <c r="L183">
+      <c r="L183" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
+      </c>
+      <c r="M183">
         <v>0.399812753899036</v>
       </c>
-      <c r="M183">
+      <c r="N183">
         <v>0.2</v>
       </c>
     </row>
@@ -7367,10 +7797,15 @@
       <c r="J184">
         <v>0</v>
       </c>
-      <c r="L184">
+      <c r="L184" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
+      </c>
+      <c r="M184">
         <v>0.399812753899036</v>
       </c>
-      <c r="M184">
+      <c r="N184">
         <v>0.2</v>
       </c>
     </row>
@@ -7389,10 +7824,15 @@
       <c r="J185">
         <v>0</v>
       </c>
-      <c r="L185">
+      <c r="L185" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
+      </c>
+      <c r="M185">
         <v>0.399812753899036</v>
       </c>
-      <c r="M185">
+      <c r="N185">
         <v>0.2</v>
       </c>
     </row>
@@ -7411,10 +7851,15 @@
       <c r="J186">
         <v>0</v>
       </c>
-      <c r="L186">
+      <c r="L186" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
+      </c>
+      <c r="M186">
         <v>0.399812753899036</v>
       </c>
-      <c r="M186">
+      <c r="N186">
         <v>0.2</v>
       </c>
     </row>
@@ -7433,10 +7878,15 @@
       <c r="J187">
         <v>0</v>
       </c>
-      <c r="L187">
+      <c r="L187" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
+      </c>
+      <c r="M187">
         <v>0.399812753899036</v>
       </c>
-      <c r="M187">
+      <c r="N187">
         <v>0.2</v>
       </c>
     </row>
@@ -7455,10 +7905,15 @@
       <c r="J188">
         <v>0</v>
       </c>
-      <c r="L188">
+      <c r="L188" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
+      </c>
+      <c r="M188">
         <v>0.399812753899036</v>
       </c>
-      <c r="M188">
+      <c r="N188">
         <v>0.2</v>
       </c>
     </row>
@@ -7477,10 +7932,15 @@
       <c r="J189">
         <v>0</v>
       </c>
-      <c r="L189">
+      <c r="L189" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
+      </c>
+      <c r="M189">
         <v>0.399812753899036</v>
       </c>
-      <c r="M189">
+      <c r="N189">
         <v>0.2</v>
       </c>
     </row>
@@ -7499,10 +7959,15 @@
       <c r="J190">
         <v>0</v>
       </c>
-      <c r="L190">
+      <c r="L190" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
+      </c>
+      <c r="M190">
         <v>0.399812753899036</v>
       </c>
-      <c r="M190">
+      <c r="N190">
         <v>0.2</v>
       </c>
     </row>
@@ -7521,10 +7986,15 @@
       <c r="J191">
         <v>0</v>
       </c>
-      <c r="L191">
+      <c r="L191" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
+      </c>
+      <c r="M191">
         <v>0.399812753899036</v>
       </c>
-      <c r="M191">
+      <c r="N191">
         <v>0.2</v>
       </c>
     </row>
@@ -7543,10 +8013,15 @@
       <c r="J192">
         <v>0</v>
       </c>
-      <c r="L192">
+      <c r="L192" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
+      </c>
+      <c r="M192">
         <v>0.399812753899036</v>
       </c>
-      <c r="M192">
+      <c r="N192">
         <v>0.2</v>
       </c>
     </row>
@@ -7565,10 +8040,15 @@
       <c r="J193">
         <v>0</v>
       </c>
-      <c r="L193">
+      <c r="L193" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
+      </c>
+      <c r="M193">
         <v>0.399812753899036</v>
       </c>
-      <c r="M193">
+      <c r="N193">
         <v>0.2</v>
       </c>
     </row>
@@ -7587,10 +8067,15 @@
       <c r="J194">
         <v>0</v>
       </c>
-      <c r="L194">
+      <c r="L194" t="inlineStr">
+        <is>
+          <t>data from Hyatt and Steer 1987</t>
+        </is>
+      </c>
+      <c r="M194">
         <v>0.399812753899036</v>
       </c>
-      <c r="M194">
+      <c r="N194">
         <v>0.2</v>
       </c>
     </row>
@@ -7615,10 +8100,15 @@
       <c r="J195">
         <v>0</v>
       </c>
-      <c r="L195">
-        <v>0.05</v>
+      <c r="L195" t="inlineStr">
+        <is>
+          <t>data from Starr, P. J., A. T. Charles and M. A. Henderson 1984. Reconstruction of British Columbia sockeye salmon (Oncorhynchus nerka) stocks: 1970-1982. Can. MS. Rep. Fish. Aquat. Sci</t>
+        </is>
       </c>
       <c r="M195">
+        <v>0.05</v>
+      </c>
+      <c r="N195">
         <v>0.2</v>
       </c>
     </row>
@@ -7643,10 +8133,15 @@
       <c r="J196">
         <v>0</v>
       </c>
-      <c r="L196">
-        <v>0.05</v>
+      <c r="L196" t="inlineStr">
+        <is>
+          <t>data from Starr, P. J., A. T. Charles and M. A. Henderson 1984. Reconstruction of British Columbia sockeye salmon (Oncorhynchus nerka) stocks: 1970-1982. Can. MS. Rep. Fish. Aquat. Sci</t>
+        </is>
       </c>
       <c r="M196">
+        <v>0.05</v>
+      </c>
+      <c r="N196">
         <v>0.2</v>
       </c>
     </row>
@@ -7683,10 +8178,15 @@
       <c r="J197">
         <v>43</v>
       </c>
-      <c r="L197">
-        <v>0.05</v>
+      <c r="L197" t="inlineStr">
+        <is>
+          <t>data from Starr, P. J., A. T. Charles and M. A. Henderson 1984. Reconstruction of British Columbia sockeye salmon (Oncorhynchus nerka) stocks: 1970-1982. Can. MS. Rep. Fish. Aquat. Sci</t>
+        </is>
       </c>
       <c r="M197">
+        <v>0.05</v>
+      </c>
+      <c r="N197">
         <v>0.2</v>
       </c>
     </row>
@@ -7723,10 +8223,15 @@
       <c r="J198">
         <v>99</v>
       </c>
-      <c r="L198">
-        <v>0.05</v>
+      <c r="L198" t="inlineStr">
+        <is>
+          <t>data from Starr, P. J., A. T. Charles and M. A. Henderson 1984. Reconstruction of British Columbia sockeye salmon (Oncorhynchus nerka) stocks: 1970-1982. Can. MS. Rep. Fish. Aquat. Sci</t>
+        </is>
       </c>
       <c r="M198">
+        <v>0.05</v>
+      </c>
+      <c r="N198">
         <v>0.2</v>
       </c>
     </row>
@@ -7763,10 +8268,15 @@
       <c r="J199">
         <v>113</v>
       </c>
-      <c r="L199">
-        <v>0.05</v>
+      <c r="L199" t="inlineStr">
+        <is>
+          <t>data from Starr, P. J., A. T. Charles and M. A. Henderson 1984. Reconstruction of British Columbia sockeye salmon (Oncorhynchus nerka) stocks: 1970-1982. Can. MS. Rep. Fish. Aquat. Sci</t>
+        </is>
       </c>
       <c r="M199">
+        <v>0.05</v>
+      </c>
+      <c r="N199">
         <v>0.2</v>
       </c>
     </row>
@@ -7803,10 +8313,15 @@
       <c r="J200">
         <v>195</v>
       </c>
-      <c r="L200">
-        <v>0.05</v>
+      <c r="L200" t="inlineStr">
+        <is>
+          <t>data from Starr, P. J., A. T. Charles and M. A. Henderson 1984. Reconstruction of British Columbia sockeye salmon (Oncorhynchus nerka) stocks: 1970-1982. Can. MS. Rep. Fish. Aquat. Sci</t>
+        </is>
       </c>
       <c r="M200">
+        <v>0.05</v>
+      </c>
+      <c r="N200">
         <v>0.2</v>
       </c>
     </row>
@@ -7843,10 +8358,15 @@
       <c r="J201">
         <v>191</v>
       </c>
-      <c r="L201">
-        <v>0.05</v>
+      <c r="L201" t="inlineStr">
+        <is>
+          <t>data from Starr, P. J., A. T. Charles and M. A. Henderson 1984. Reconstruction of British Columbia sockeye salmon (Oncorhynchus nerka) stocks: 1970-1982. Can. MS. Rep. Fish. Aquat. Sci</t>
+        </is>
       </c>
       <c r="M201">
+        <v>0.05</v>
+      </c>
+      <c r="N201">
         <v>0.2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update output files with fertilization and hatchery releases history
</commit_message>
<xml_diff>
--- a/3. outputs/Stock-recruit data/Barkley_Sockeye_stock-recruit_infilled.xlsx
+++ b/3. outputs/Stock-recruit data/Barkley_Sockeye_stock-recruit_infilled.xlsx
@@ -352,7 +352,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -493,46 +493,70 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>fertilized</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Recruitment that arose from S in subsequent years. Calculated based on annual age compositions</t>
+          <t>Binary variable describing whether (1) or not (0) the CU nursary lake was fertilized in each year. Note that fertilization affects abundances of pre-smolts in year + 1 (e.g. fertilizing a lake in 2010 is expected to bolster the abundances of pre-smolts counted during the winter 2011 ATS.</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>hr_pred</t>
+          <t>hatchery_fry_release</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Retrospective prediction of harvest rate for Hucuktlis Sockeye based on a linear model with Somass Sockeye harvest rate as a predictor. Used to estimate Hucuktlis catch in years with missing data</t>
+          <t>Numbers of Sockeye fry released by the Hucuktlis/Henderson hatchery in each year. Pertains only to the Hucuktlis CU because outplants were discontinued in the 1930s. The hatchery ceased operations in 2007.</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>H_cv</t>
+          <t>R</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Coefficient of variation on harvest data. Historical (prior to 2011) Hucuktlis Sockeye harvest rate predictions were derived from a linear model. CV for these data is calculated as RMSE of the model residuals divided by the mean of the observed Hucuktlis Sockeye harvest rates that informed the model fit (i.e. the dependent variable). Harvest data for Somass and Hucuktlis post-2011 are assumed to be precise.</t>
+          <t>Recruitment that arose from S in subsequent years. Calculated based on annual age compositions</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t>hr_pred</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Retrospective prediction of harvest rate for Hucuktlis Sockeye based on a linear model with Somass Sockeye harvest rate as a predictor. Used to estimate Hucuktlis catch in years with missing data</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>H_cv</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Coefficient of variation on harvest data. Historical (prior to 2011) Hucuktlis Sockeye harvest rate predictions were derived from a linear model. CV for these data is calculated as RMSE of the model residuals divided by the mean of the observed Hucuktlis Sockeye harvest rates that informed the model fit (i.e. the dependent variable). Harvest data for Somass and Hucuktlis post-2011 are assumed to be precise.</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
           <t>S_cv</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="B17" t="inlineStr">
         <is>
           <t>Coefficient of variation on spawner data. Currently based on ____</t>
         </is>
@@ -545,7 +569,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N144"/>
+  <dimension ref="A1:P144"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -604,20 +628,30 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
+          <t>fertilized</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>hatchery_fry_release</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
           <t>R</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>hr_pred</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>H_cv</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>S_cv</t>
         </is>
@@ -657,12 +691,15 @@
         <v>958</v>
       </c>
       <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="M2">
         <v>633742.5637903768</v>
       </c>
-      <c r="M2">
-        <v>0.05</v>
-      </c>
-      <c r="N2">
+      <c r="O2">
+        <v>0.05</v>
+      </c>
+      <c r="P2">
         <v>0.05</v>
       </c>
     </row>
@@ -700,12 +737,15 @@
         <v>785</v>
       </c>
       <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="M3">
         <v>495061.8834075385</v>
       </c>
-      <c r="M3">
-        <v>0.05</v>
-      </c>
-      <c r="N3">
+      <c r="O3">
+        <v>0.05</v>
+      </c>
+      <c r="P3">
         <v>0.05</v>
       </c>
     </row>
@@ -743,12 +783,15 @@
         <v>958</v>
       </c>
       <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="M4">
         <v>526832.3053483891</v>
       </c>
-      <c r="M4">
-        <v>0.05</v>
-      </c>
-      <c r="N4">
+      <c r="O4">
+        <v>0.05</v>
+      </c>
+      <c r="P4">
         <v>0.05</v>
       </c>
     </row>
@@ -786,12 +829,15 @@
         <v>785</v>
       </c>
       <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="M5">
         <v>552803.0040534479</v>
       </c>
-      <c r="M5">
-        <v>0.05</v>
-      </c>
-      <c r="N5">
+      <c r="O5">
+        <v>0.05</v>
+      </c>
+      <c r="P5">
         <v>0.05</v>
       </c>
     </row>
@@ -829,12 +875,15 @@
         <v>958</v>
       </c>
       <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="M6">
         <v>913809.5845034227</v>
       </c>
-      <c r="M6">
-        <v>0.05</v>
-      </c>
-      <c r="N6">
+      <c r="O6">
+        <v>0.05</v>
+      </c>
+      <c r="P6">
         <v>0.05</v>
       </c>
     </row>
@@ -872,12 +921,15 @@
         <v>785</v>
       </c>
       <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="M7">
         <v>570766.8540090187</v>
       </c>
-      <c r="M7">
-        <v>0.05</v>
-      </c>
-      <c r="N7">
+      <c r="O7">
+        <v>0.05</v>
+      </c>
+      <c r="P7">
         <v>0.05</v>
       </c>
     </row>
@@ -915,12 +967,15 @@
         <v>1608</v>
       </c>
       <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="M8">
         <v>480598.2568144404</v>
       </c>
-      <c r="M8">
-        <v>0.05</v>
-      </c>
-      <c r="N8">
+      <c r="O8">
+        <v>0.05</v>
+      </c>
+      <c r="P8">
         <v>0.05</v>
       </c>
     </row>
@@ -958,12 +1013,15 @@
         <v>865</v>
       </c>
       <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="M9">
         <v>391376.4267260354</v>
       </c>
-      <c r="M9">
-        <v>0.05</v>
-      </c>
-      <c r="N9">
+      <c r="O9">
+        <v>0.05</v>
+      </c>
+      <c r="P9">
         <v>0.05</v>
       </c>
     </row>
@@ -1001,12 +1059,15 @@
         <v>1505</v>
       </c>
       <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="M10">
         <v>224122.9386567897</v>
       </c>
-      <c r="M10">
-        <v>0.05</v>
-      </c>
-      <c r="N10">
+      <c r="O10">
+        <v>0.05</v>
+      </c>
+      <c r="P10">
         <v>0.05</v>
       </c>
     </row>
@@ -1044,12 +1105,15 @@
         <v>982</v>
       </c>
       <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="M11">
         <v>288014.3071424381</v>
       </c>
-      <c r="M11">
-        <v>0.05</v>
-      </c>
-      <c r="N11">
+      <c r="O11">
+        <v>0.05</v>
+      </c>
+      <c r="P11">
         <v>0.05</v>
       </c>
     </row>
@@ -1087,12 +1151,15 @@
         <v>743</v>
       </c>
       <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="M12">
         <v>137076.4333190075</v>
       </c>
-      <c r="M12">
-        <v>0.05</v>
-      </c>
-      <c r="N12">
+      <c r="O12">
+        <v>0.05</v>
+      </c>
+      <c r="P12">
         <v>0.05</v>
       </c>
     </row>
@@ -1130,12 +1197,15 @@
         <v>1031</v>
       </c>
       <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="M13">
         <v>203184.164250254</v>
       </c>
-      <c r="M13">
-        <v>0.05</v>
-      </c>
-      <c r="N13">
+      <c r="O13">
+        <v>0.05</v>
+      </c>
+      <c r="P13">
         <v>0.05</v>
       </c>
     </row>
@@ -1173,12 +1243,15 @@
         <v>1191</v>
       </c>
       <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="M14">
         <v>503092.30271186</v>
       </c>
-      <c r="M14">
-        <v>0.05</v>
-      </c>
-      <c r="N14">
+      <c r="O14">
+        <v>0.05</v>
+      </c>
+      <c r="P14">
         <v>0.05</v>
       </c>
     </row>
@@ -1216,12 +1289,15 @@
         <v>881</v>
       </c>
       <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="M15">
         <v>371601.962535504</v>
       </c>
-      <c r="M15">
-        <v>0.05</v>
-      </c>
-      <c r="N15">
+      <c r="O15">
+        <v>0.05</v>
+      </c>
+      <c r="P15">
         <v>0.05</v>
       </c>
     </row>
@@ -1259,12 +1335,15 @@
         <v>846</v>
       </c>
       <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="M16">
         <v>206726.5366225715</v>
       </c>
-      <c r="M16">
-        <v>0.05</v>
-      </c>
-      <c r="N16">
+      <c r="O16">
+        <v>0.05</v>
+      </c>
+      <c r="P16">
         <v>0.05</v>
       </c>
     </row>
@@ -1302,12 +1381,15 @@
         <v>661</v>
       </c>
       <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="M17">
         <v>340157.6785086803</v>
       </c>
-      <c r="M17">
-        <v>0.05</v>
-      </c>
-      <c r="N17">
+      <c r="O17">
+        <v>0.05</v>
+      </c>
+      <c r="P17">
         <v>0.05</v>
       </c>
     </row>
@@ -1345,12 +1427,15 @@
         <v>361</v>
       </c>
       <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="M18">
         <v>292061.9392067303</v>
       </c>
-      <c r="M18">
-        <v>0.05</v>
-      </c>
-      <c r="N18">
+      <c r="O18">
+        <v>0.05</v>
+      </c>
+      <c r="P18">
         <v>0.05</v>
       </c>
     </row>
@@ -1373,7 +1458,7 @@
         <v>140205.9808822382</v>
       </c>
       <c r="F19">
-        <v>39662.13671849496</v>
+        <v>39662.13671849497</v>
       </c>
       <c r="G19">
         <v>145886.7713032815</v>
@@ -1388,12 +1473,15 @@
         <v>237</v>
       </c>
       <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="M19">
         <v>172160.3662147925</v>
       </c>
-      <c r="M19">
-        <v>0.05</v>
-      </c>
-      <c r="N19">
+      <c r="O19">
+        <v>0.05</v>
+      </c>
+      <c r="P19">
         <v>0.05</v>
       </c>
     </row>
@@ -1431,12 +1519,15 @@
         <v>219</v>
       </c>
       <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="M20">
         <v>274311.7730009329</v>
       </c>
-      <c r="M20">
-        <v>0.05</v>
-      </c>
-      <c r="N20">
+      <c r="O20">
+        <v>0.05</v>
+      </c>
+      <c r="P20">
         <v>0.05</v>
       </c>
     </row>
@@ -1474,12 +1565,15 @@
         <v>353</v>
       </c>
       <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="M21">
         <v>265697.028795797</v>
       </c>
-      <c r="M21">
-        <v>0.05</v>
-      </c>
-      <c r="N21">
+      <c r="O21">
+        <v>0.05</v>
+      </c>
+      <c r="P21">
         <v>0.05</v>
       </c>
     </row>
@@ -1517,12 +1611,15 @@
         <v>958</v>
       </c>
       <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="M22">
         <v>1258256.636990258</v>
       </c>
-      <c r="M22">
-        <v>0.05</v>
-      </c>
-      <c r="N22">
+      <c r="O22">
+        <v>0.05</v>
+      </c>
+      <c r="P22">
         <v>0.05</v>
       </c>
     </row>
@@ -1560,12 +1657,15 @@
         <v>785</v>
       </c>
       <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="M23">
         <v>652446.9029476116</v>
       </c>
-      <c r="M23">
-        <v>0.05</v>
-      </c>
-      <c r="N23">
+      <c r="O23">
+        <v>0.05</v>
+      </c>
+      <c r="P23">
         <v>0.05</v>
       </c>
     </row>
@@ -1603,12 +1703,15 @@
         <v>1160</v>
       </c>
       <c r="K24">
+        <v>1</v>
+      </c>
+      <c r="M24">
         <v>599789.3466079192</v>
       </c>
-      <c r="M24">
-        <v>0.05</v>
-      </c>
-      <c r="N24">
+      <c r="O24">
+        <v>0.05</v>
+      </c>
+      <c r="P24">
         <v>0.05</v>
       </c>
     </row>
@@ -1646,12 +1749,15 @@
         <v>1357</v>
       </c>
       <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="M25">
         <v>625355.4802804298</v>
       </c>
-      <c r="M25">
-        <v>0.05</v>
-      </c>
-      <c r="N25">
+      <c r="O25">
+        <v>0.05</v>
+      </c>
+      <c r="P25">
         <v>0.05</v>
       </c>
     </row>
@@ -1689,12 +1795,15 @@
         <v>987</v>
       </c>
       <c r="K26">
+        <v>1</v>
+      </c>
+      <c r="M26">
         <v>400875.0350328542</v>
       </c>
-      <c r="M26">
-        <v>0.05</v>
-      </c>
-      <c r="N26">
+      <c r="O26">
+        <v>0.05</v>
+      </c>
+      <c r="P26">
         <v>0.05</v>
       </c>
     </row>
@@ -1732,12 +1841,15 @@
         <v>699</v>
       </c>
       <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="M27">
         <v>407468.2247957478</v>
       </c>
-      <c r="M27">
-        <v>0.05</v>
-      </c>
-      <c r="N27">
+      <c r="O27">
+        <v>0.05</v>
+      </c>
+      <c r="P27">
         <v>0.05</v>
       </c>
     </row>
@@ -1775,12 +1887,15 @@
         <v>900</v>
       </c>
       <c r="K28">
+        <v>1</v>
+      </c>
+      <c r="M28">
         <v>138601.997986058</v>
       </c>
-      <c r="M28">
-        <v>0.05</v>
-      </c>
-      <c r="N28">
+      <c r="O28">
+        <v>0.05</v>
+      </c>
+      <c r="P28">
         <v>0.05</v>
       </c>
     </row>
@@ -1818,12 +1933,15 @@
         <v>590</v>
       </c>
       <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="M29">
         <v>181984.1898199186</v>
       </c>
-      <c r="M29">
-        <v>0.05</v>
-      </c>
-      <c r="N29">
+      <c r="O29">
+        <v>0.05</v>
+      </c>
+      <c r="P29">
         <v>0.05</v>
       </c>
     </row>
@@ -1861,12 +1979,15 @@
         <v>1728</v>
       </c>
       <c r="K30">
+        <v>1</v>
+      </c>
+      <c r="M30">
         <v>74102.68990164486</v>
       </c>
-      <c r="M30">
-        <v>0.05</v>
-      </c>
-      <c r="N30">
+      <c r="O30">
+        <v>0.05</v>
+      </c>
+      <c r="P30">
         <v>0.05</v>
       </c>
     </row>
@@ -1904,12 +2025,15 @@
         <v>797</v>
       </c>
       <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="M31">
         <v>59697.7030353223</v>
       </c>
-      <c r="M31">
-        <v>0.05</v>
-      </c>
-      <c r="N31">
+      <c r="O31">
+        <v>0.05</v>
+      </c>
+      <c r="P31">
         <v>0.05</v>
       </c>
     </row>
@@ -1947,12 +2071,15 @@
         <v>1098</v>
       </c>
       <c r="K32">
+        <v>1</v>
+      </c>
+      <c r="M32">
         <v>290004.5944304451</v>
       </c>
-      <c r="M32">
-        <v>0.05</v>
-      </c>
-      <c r="N32">
+      <c r="O32">
+        <v>0.05</v>
+      </c>
+      <c r="P32">
         <v>0.05</v>
       </c>
     </row>
@@ -1990,12 +2117,15 @@
         <v>1839</v>
       </c>
       <c r="K33">
+        <v>0</v>
+      </c>
+      <c r="M33">
         <v>320116.8393461921</v>
       </c>
-      <c r="M33">
-        <v>0.05</v>
-      </c>
-      <c r="N33">
+      <c r="O33">
+        <v>0.05</v>
+      </c>
+      <c r="P33">
         <v>0.05</v>
       </c>
     </row>
@@ -2033,12 +2163,15 @@
         <v>1364</v>
       </c>
       <c r="K34">
+        <v>1</v>
+      </c>
+      <c r="M34">
         <v>421979.6878094974</v>
       </c>
-      <c r="M34">
-        <v>0.05</v>
-      </c>
-      <c r="N34">
+      <c r="O34">
+        <v>0.05</v>
+      </c>
+      <c r="P34">
         <v>0.05</v>
       </c>
     </row>
@@ -2076,12 +2209,15 @@
         <v>1120</v>
       </c>
       <c r="K35">
+        <v>0</v>
+      </c>
+      <c r="M35">
         <v>263927.9811106482</v>
       </c>
-      <c r="M35">
-        <v>0.05</v>
-      </c>
-      <c r="N35">
+      <c r="O35">
+        <v>0.05</v>
+      </c>
+      <c r="P35">
         <v>0.05</v>
       </c>
     </row>
@@ -2119,12 +2255,15 @@
         <v>891</v>
       </c>
       <c r="K36">
+        <v>1</v>
+      </c>
+      <c r="M36">
         <v>240203.9760283087</v>
       </c>
-      <c r="M36">
-        <v>0.05</v>
-      </c>
-      <c r="N36">
+      <c r="O36">
+        <v>0.05</v>
+      </c>
+      <c r="P36">
         <v>0.05</v>
       </c>
     </row>
@@ -2162,12 +2301,15 @@
         <v>955</v>
       </c>
       <c r="K37">
+        <v>0</v>
+      </c>
+      <c r="M37">
         <v>189096.9567127897</v>
       </c>
-      <c r="M37">
-        <v>0.05</v>
-      </c>
-      <c r="N37">
+      <c r="O37">
+        <v>0.05</v>
+      </c>
+      <c r="P37">
         <v>0.05</v>
       </c>
     </row>
@@ -2205,12 +2347,15 @@
         <v>500</v>
       </c>
       <c r="K38">
+        <v>1</v>
+      </c>
+      <c r="M38">
         <v>241682.5691475399</v>
       </c>
-      <c r="M38">
-        <v>0.05</v>
-      </c>
-      <c r="N38">
+      <c r="O38">
+        <v>0.05</v>
+      </c>
+      <c r="P38">
         <v>0.05</v>
       </c>
     </row>
@@ -2248,12 +2393,15 @@
         <v>702</v>
       </c>
       <c r="K39">
+        <v>0</v>
+      </c>
+      <c r="M39">
         <v>386548.9231194458</v>
       </c>
-      <c r="M39">
-        <v>0.05</v>
-      </c>
-      <c r="N39">
+      <c r="O39">
+        <v>0.05</v>
+      </c>
+      <c r="P39">
         <v>0.05</v>
       </c>
     </row>
@@ -2291,12 +2439,15 @@
         <v>1000</v>
       </c>
       <c r="K40">
+        <v>1</v>
+      </c>
+      <c r="M40">
         <v>261943.5622247388</v>
       </c>
-      <c r="M40">
-        <v>0.05</v>
-      </c>
-      <c r="N40">
+      <c r="O40">
+        <v>0.05</v>
+      </c>
+      <c r="P40">
         <v>0.05</v>
       </c>
     </row>
@@ -2334,12 +2485,15 @@
         <v>1357</v>
       </c>
       <c r="K41">
+        <v>0</v>
+      </c>
+      <c r="M41">
         <v>145416.8103652774</v>
       </c>
-      <c r="M41">
-        <v>0.05</v>
-      </c>
-      <c r="N41">
+      <c r="O41">
+        <v>0.05</v>
+      </c>
+      <c r="P41">
         <v>0.05</v>
       </c>
     </row>
@@ -2377,12 +2531,15 @@
         <v>1751</v>
       </c>
       <c r="K42">
+        <v>1</v>
+      </c>
+      <c r="M42">
         <v>717175.1613370343</v>
       </c>
-      <c r="M42">
-        <v>0.05</v>
-      </c>
-      <c r="N42">
+      <c r="O42">
+        <v>0.05</v>
+      </c>
+      <c r="P42">
         <v>0.05</v>
       </c>
     </row>
@@ -2420,12 +2577,15 @@
         <v>1129</v>
       </c>
       <c r="K43">
+        <v>0</v>
+      </c>
+      <c r="M43">
         <v>326804.0013846449</v>
       </c>
-      <c r="M43">
-        <v>0.05</v>
-      </c>
-      <c r="N43">
+      <c r="O43">
+        <v>0.05</v>
+      </c>
+      <c r="P43">
         <v>0.05</v>
       </c>
     </row>
@@ -2463,12 +2623,15 @@
         <v>1116</v>
       </c>
       <c r="K44">
+        <v>1</v>
+      </c>
+      <c r="M44">
         <v>518419.7394188421</v>
       </c>
-      <c r="M44">
-        <v>0.05</v>
-      </c>
-      <c r="N44">
+      <c r="O44">
+        <v>0.05</v>
+      </c>
+      <c r="P44">
         <v>0.05</v>
       </c>
     </row>
@@ -2506,12 +2669,15 @@
         <v>958</v>
       </c>
       <c r="K45">
+        <v>0</v>
+      </c>
+      <c r="M45">
         <v>732603.6241928141</v>
       </c>
-      <c r="M45">
-        <v>0.05</v>
-      </c>
-      <c r="N45">
+      <c r="O45">
+        <v>0.05</v>
+      </c>
+      <c r="P45">
         <v>0.05</v>
       </c>
     </row>
@@ -2549,12 +2715,15 @@
         <v>3221</v>
       </c>
       <c r="K46">
+        <v>1</v>
+      </c>
+      <c r="M46">
         <v>569643.4153128543</v>
       </c>
-      <c r="M46">
-        <v>0.05</v>
-      </c>
-      <c r="N46">
+      <c r="O46">
+        <v>0.05</v>
+      </c>
+      <c r="P46">
         <v>0.05</v>
       </c>
     </row>
@@ -2592,12 +2761,15 @@
         <v>2694</v>
       </c>
       <c r="K47">
+        <v>0</v>
+      </c>
+      <c r="M47">
         <v>353959.4130974241</v>
       </c>
-      <c r="M47">
-        <v>0.05</v>
-      </c>
-      <c r="N47">
+      <c r="O47">
+        <v>0.05</v>
+      </c>
+      <c r="P47">
         <v>0.05</v>
       </c>
     </row>
@@ -2635,12 +2807,15 @@
         <v>591</v>
       </c>
       <c r="K48">
+        <v>1</v>
+      </c>
+      <c r="M48">
         <v>213509.8577738418</v>
       </c>
-      <c r="M48">
-        <v>0.05</v>
-      </c>
-      <c r="N48">
+      <c r="O48">
+        <v>0.05</v>
+      </c>
+      <c r="P48">
         <v>0.05</v>
       </c>
     </row>
@@ -2678,12 +2853,15 @@
         <v>1056</v>
       </c>
       <c r="K49">
+        <v>0</v>
+      </c>
+      <c r="M49">
         <v>219482.3284506314</v>
       </c>
-      <c r="M49">
-        <v>0.05</v>
-      </c>
-      <c r="N49">
+      <c r="O49">
+        <v>0.05</v>
+      </c>
+      <c r="P49">
         <v>0.05</v>
       </c>
     </row>
@@ -2721,12 +2899,15 @@
         <v>1987</v>
       </c>
       <c r="K50">
+        <v>1</v>
+      </c>
+      <c r="M50">
         <v>329840.2664919504</v>
       </c>
-      <c r="M50">
-        <v>0.05</v>
-      </c>
-      <c r="N50">
+      <c r="O50">
+        <v>0.05</v>
+      </c>
+      <c r="P50">
         <v>0.05</v>
       </c>
     </row>
@@ -2764,12 +2945,15 @@
         <v>1860</v>
       </c>
       <c r="K51">
+        <v>0</v>
+      </c>
+      <c r="M51">
         <v>150478.2895093822</v>
       </c>
-      <c r="M51">
-        <v>0.05</v>
-      </c>
-      <c r="N51">
+      <c r="O51">
+        <v>0.05</v>
+      </c>
+      <c r="P51">
         <v>0.05</v>
       </c>
     </row>
@@ -2807,12 +2991,15 @@
         <v>3067</v>
       </c>
       <c r="K52">
+        <v>1</v>
+      </c>
+      <c r="M52">
         <v>97065.40537030963</v>
       </c>
-      <c r="M52">
-        <v>0.05</v>
-      </c>
-      <c r="N52">
+      <c r="O52">
+        <v>0.05</v>
+      </c>
+      <c r="P52">
         <v>0.05</v>
       </c>
     </row>
@@ -2850,12 +3037,15 @@
         <v>1979</v>
       </c>
       <c r="K53">
+        <v>0</v>
+      </c>
+      <c r="M53">
         <v>131772.1820819404</v>
       </c>
-      <c r="M53">
-        <v>0.05</v>
-      </c>
-      <c r="N53">
+      <c r="O53">
+        <v>0.05</v>
+      </c>
+      <c r="P53">
         <v>0.05</v>
       </c>
     </row>
@@ -2893,12 +3083,15 @@
         <v>2266</v>
       </c>
       <c r="K54">
+        <v>1</v>
+      </c>
+      <c r="M54">
         <v>17687.78978304791</v>
       </c>
-      <c r="M54">
-        <v>0.05</v>
-      </c>
-      <c r="N54">
+      <c r="O54">
+        <v>0.05</v>
+      </c>
+      <c r="P54">
         <v>0.05</v>
       </c>
     </row>
@@ -2936,12 +3129,15 @@
         <v>1904</v>
       </c>
       <c r="K55">
+        <v>0</v>
+      </c>
+      <c r="M55">
         <v>21882.51302978364</v>
       </c>
-      <c r="M55">
-        <v>0.05</v>
-      </c>
-      <c r="N55">
+      <c r="O55">
+        <v>0.05</v>
+      </c>
+      <c r="P55">
         <v>0.05</v>
       </c>
     </row>
@@ -2979,12 +3175,15 @@
         <v>1754</v>
       </c>
       <c r="K56">
+        <v>1</v>
+      </c>
+      <c r="M56">
         <v>189217.8905235089</v>
       </c>
-      <c r="M56">
-        <v>0.05</v>
-      </c>
-      <c r="N56">
+      <c r="O56">
+        <v>0.05</v>
+      </c>
+      <c r="P56">
         <v>0.05</v>
       </c>
     </row>
@@ -3022,12 +3221,15 @@
         <v>1160</v>
       </c>
       <c r="K57">
+        <v>0</v>
+      </c>
+      <c r="M57">
         <v>114009.339885825</v>
       </c>
-      <c r="M57">
-        <v>0.05</v>
-      </c>
-      <c r="N57">
+      <c r="O57">
+        <v>0.05</v>
+      </c>
+      <c r="P57">
         <v>0.05</v>
       </c>
     </row>
@@ -3065,12 +3267,15 @@
         <v>1689</v>
       </c>
       <c r="K58">
+        <v>1</v>
+      </c>
+      <c r="M58">
         <v>454549.7827114371</v>
       </c>
-      <c r="M58">
-        <v>0.05</v>
-      </c>
-      <c r="N58">
+      <c r="O58">
+        <v>0.05</v>
+      </c>
+      <c r="P58">
         <v>0.05</v>
       </c>
     </row>
@@ -3108,12 +3313,15 @@
         <v>1263</v>
       </c>
       <c r="K59">
+        <v>0</v>
+      </c>
+      <c r="M59">
         <v>333891.8889857767</v>
       </c>
-      <c r="M59">
-        <v>0.05</v>
-      </c>
-      <c r="N59">
+      <c r="O59">
+        <v>0.05</v>
+      </c>
+      <c r="P59">
         <v>0.05</v>
       </c>
     </row>
@@ -3151,12 +3359,15 @@
         <v>1279</v>
       </c>
       <c r="K60">
+        <v>1</v>
+      </c>
+      <c r="M60">
         <v>966912.7522210542</v>
       </c>
-      <c r="M60">
-        <v>0.05</v>
-      </c>
-      <c r="N60">
+      <c r="O60">
+        <v>0.05</v>
+      </c>
+      <c r="P60">
         <v>0.05</v>
       </c>
     </row>
@@ -3194,12 +3405,15 @@
         <v>600</v>
       </c>
       <c r="K61">
+        <v>0</v>
+      </c>
+      <c r="M61">
         <v>885638.3882038471</v>
       </c>
-      <c r="M61">
-        <v>0.05</v>
-      </c>
-      <c r="N61">
+      <c r="O61">
+        <v>0.05</v>
+      </c>
+      <c r="P61">
         <v>0.05</v>
       </c>
     </row>
@@ -3237,12 +3451,15 @@
         <v>686</v>
       </c>
       <c r="K62">
+        <v>1</v>
+      </c>
+      <c r="M62">
         <v>645290.4618712433</v>
       </c>
-      <c r="M62">
-        <v>0.05</v>
-      </c>
-      <c r="N62">
+      <c r="O62">
+        <v>0.05</v>
+      </c>
+      <c r="P62">
         <v>0.05</v>
       </c>
     </row>
@@ -3280,12 +3497,15 @@
         <v>643</v>
       </c>
       <c r="K63">
+        <v>0</v>
+      </c>
+      <c r="M63">
         <v>811357.3188160737</v>
       </c>
-      <c r="M63">
-        <v>0.05</v>
-      </c>
-      <c r="N63">
+      <c r="O63">
+        <v>0.05</v>
+      </c>
+      <c r="P63">
         <v>0.05</v>
       </c>
     </row>
@@ -3323,12 +3543,15 @@
         <v>393</v>
       </c>
       <c r="K64">
+        <v>1</v>
+      </c>
+      <c r="M64">
         <v>100032.3097210799</v>
       </c>
-      <c r="M64">
-        <v>0.05</v>
-      </c>
-      <c r="N64">
+      <c r="O64">
+        <v>0.05</v>
+      </c>
+      <c r="P64">
         <v>0.05</v>
       </c>
     </row>
@@ -3366,12 +3589,15 @@
         <v>621</v>
       </c>
       <c r="K65">
+        <v>0</v>
+      </c>
+      <c r="M65">
         <v>271240.703074521</v>
       </c>
-      <c r="M65">
-        <v>0.05</v>
-      </c>
-      <c r="N65">
+      <c r="O65">
+        <v>0.05</v>
+      </c>
+      <c r="P65">
         <v>0.05</v>
       </c>
     </row>
@@ -3409,12 +3635,15 @@
         <v>1283</v>
       </c>
       <c r="K66">
+        <v>1</v>
+      </c>
+      <c r="M66">
         <v>147482.6115069279</v>
       </c>
-      <c r="M66">
-        <v>0.05</v>
-      </c>
-      <c r="N66">
+      <c r="O66">
+        <v>0.05</v>
+      </c>
+      <c r="P66">
         <v>0.05</v>
       </c>
     </row>
@@ -3452,12 +3681,15 @@
         <v>999</v>
       </c>
       <c r="K67">
+        <v>0</v>
+      </c>
+      <c r="M67">
         <v>304274.706182281</v>
       </c>
-      <c r="M67">
-        <v>0.05</v>
-      </c>
-      <c r="N67">
+      <c r="O67">
+        <v>0.05</v>
+      </c>
+      <c r="P67">
         <v>0.05</v>
       </c>
     </row>
@@ -3495,12 +3727,15 @@
         <v>2211</v>
       </c>
       <c r="K68">
+        <v>1</v>
+      </c>
+      <c r="M68">
         <v>530209.3761206279</v>
       </c>
-      <c r="M68">
-        <v>0.05</v>
-      </c>
-      <c r="N68">
+      <c r="O68">
+        <v>0.05</v>
+      </c>
+      <c r="P68">
         <v>0.05</v>
       </c>
     </row>
@@ -3538,12 +3773,15 @@
         <v>2362</v>
       </c>
       <c r="K69">
+        <v>0</v>
+      </c>
+      <c r="M69">
         <v>1046784.042950014</v>
       </c>
-      <c r="M69">
-        <v>0.05</v>
-      </c>
-      <c r="N69">
+      <c r="O69">
+        <v>0.05</v>
+      </c>
+      <c r="P69">
         <v>0.05</v>
       </c>
     </row>
@@ -3581,12 +3819,15 @@
         <v>1732</v>
       </c>
       <c r="K70">
+        <v>1</v>
+      </c>
+      <c r="M70">
         <v>1383229.190991441</v>
       </c>
-      <c r="M70">
-        <v>0.05</v>
-      </c>
-      <c r="N70">
+      <c r="O70">
+        <v>0.05</v>
+      </c>
+      <c r="P70">
         <v>0.05</v>
       </c>
     </row>
@@ -3624,12 +3865,15 @@
         <v>1585</v>
       </c>
       <c r="K71">
+        <v>0</v>
+      </c>
+      <c r="M71">
         <v>1456288.889933172</v>
       </c>
-      <c r="M71">
-        <v>0.05</v>
-      </c>
-      <c r="N71">
+      <c r="O71">
+        <v>0.05</v>
+      </c>
+      <c r="P71">
         <v>0.05</v>
       </c>
     </row>
@@ -3667,12 +3911,15 @@
         <v>1373</v>
       </c>
       <c r="K72">
+        <v>1</v>
+      </c>
+      <c r="M72">
         <v>189975.3795417092</v>
       </c>
-      <c r="M72">
-        <v>0.05</v>
-      </c>
-      <c r="N72">
+      <c r="O72">
+        <v>0.05</v>
+      </c>
+      <c r="P72">
         <v>0.05</v>
       </c>
     </row>
@@ -3710,12 +3957,15 @@
         <v>1773</v>
       </c>
       <c r="K73">
+        <v>0</v>
+      </c>
+      <c r="M73">
         <v>265560.8989697707</v>
       </c>
-      <c r="M73">
-        <v>0.05</v>
-      </c>
-      <c r="N73">
+      <c r="O73">
+        <v>0.05</v>
+      </c>
+      <c r="P73">
         <v>0.05</v>
       </c>
     </row>
@@ -3753,12 +4003,15 @@
         <v>728</v>
       </c>
       <c r="K74">
+        <v>1</v>
+      </c>
+      <c r="M74">
         <v>31701.9128248074</v>
       </c>
-      <c r="M74">
-        <v>0.05</v>
-      </c>
-      <c r="N74">
+      <c r="O74">
+        <v>0.05</v>
+      </c>
+      <c r="P74">
         <v>0.05</v>
       </c>
     </row>
@@ -3796,12 +4049,15 @@
         <v>1823</v>
       </c>
       <c r="K75">
+        <v>0</v>
+      </c>
+      <c r="M75">
         <v>74647.11735710694</v>
       </c>
-      <c r="M75">
-        <v>0.05</v>
-      </c>
-      <c r="N75">
+      <c r="O75">
+        <v>0.05</v>
+      </c>
+      <c r="P75">
         <v>0.05</v>
       </c>
     </row>
@@ -3839,12 +4095,15 @@
         <v>1387</v>
       </c>
       <c r="K76">
+        <v>1</v>
+      </c>
+      <c r="M76">
         <v>99890.87941789668</v>
       </c>
-      <c r="M76">
-        <v>0.05</v>
-      </c>
-      <c r="N76">
+      <c r="O76">
+        <v>0.05</v>
+      </c>
+      <c r="P76">
         <v>0.05</v>
       </c>
     </row>
@@ -3882,12 +4141,15 @@
         <v>3241</v>
       </c>
       <c r="K77">
+        <v>0</v>
+      </c>
+      <c r="M77">
         <v>421399.4024497316</v>
       </c>
-      <c r="M77">
-        <v>0.05</v>
-      </c>
-      <c r="N77">
+      <c r="O77">
+        <v>0.05</v>
+      </c>
+      <c r="P77">
         <v>0.05</v>
       </c>
     </row>
@@ -3925,12 +4187,15 @@
         <v>2940</v>
       </c>
       <c r="K78">
+        <v>1</v>
+      </c>
+      <c r="M78">
         <v>140758.2659394757</v>
       </c>
-      <c r="M78">
-        <v>0.05</v>
-      </c>
-      <c r="N78">
+      <c r="O78">
+        <v>0.05</v>
+      </c>
+      <c r="P78">
         <v>0.05</v>
       </c>
     </row>
@@ -3968,12 +4233,15 @@
         <v>3100</v>
       </c>
       <c r="K79">
+        <v>0</v>
+      </c>
+      <c r="M79">
         <v>103582.4907797132</v>
       </c>
-      <c r="M79">
-        <v>0.05</v>
-      </c>
-      <c r="N79">
+      <c r="O79">
+        <v>0.05</v>
+      </c>
+      <c r="P79">
         <v>0.05</v>
       </c>
     </row>
@@ -4011,12 +4279,15 @@
         <v>2190</v>
       </c>
       <c r="K80">
+        <v>1</v>
+      </c>
+      <c r="M80">
         <v>291403.081691474</v>
       </c>
-      <c r="M80">
-        <v>0.05</v>
-      </c>
-      <c r="N80">
+      <c r="O80">
+        <v>0.05</v>
+      </c>
+      <c r="P80">
         <v>0.05</v>
       </c>
     </row>
@@ -4054,12 +4325,15 @@
         <v>2016</v>
       </c>
       <c r="K81">
+        <v>0</v>
+      </c>
+      <c r="M81">
         <v>293354.5109088812</v>
       </c>
-      <c r="M81">
-        <v>0.05</v>
-      </c>
-      <c r="N81">
+      <c r="O81">
+        <v>0.05</v>
+      </c>
+      <c r="P81">
         <v>0.05</v>
       </c>
     </row>
@@ -4097,12 +4371,15 @@
         <v>1109</v>
       </c>
       <c r="K82">
+        <v>1</v>
+      </c>
+      <c r="M82">
         <v>340480.2751862371</v>
       </c>
-      <c r="M82">
-        <v>0.05</v>
-      </c>
-      <c r="N82">
+      <c r="O82">
+        <v>0.05</v>
+      </c>
+      <c r="P82">
         <v>0.05</v>
       </c>
     </row>
@@ -4140,12 +4417,15 @@
         <v>2250</v>
       </c>
       <c r="K83">
+        <v>0</v>
+      </c>
+      <c r="M83">
         <v>132750.731163154</v>
       </c>
-      <c r="M83">
-        <v>0.05</v>
-      </c>
-      <c r="N83">
+      <c r="O83">
+        <v>0.05</v>
+      </c>
+      <c r="P83">
         <v>0.05</v>
       </c>
     </row>
@@ -4182,10 +4462,13 @@
       <c r="J84">
         <v>455</v>
       </c>
-      <c r="M84">
-        <v>0.05</v>
-      </c>
-      <c r="N84">
+      <c r="K84">
+        <v>1</v>
+      </c>
+      <c r="O84">
+        <v>0.05</v>
+      </c>
+      <c r="P84">
         <v>0.05</v>
       </c>
     </row>
@@ -4222,10 +4505,13 @@
       <c r="J85">
         <v>1893</v>
       </c>
-      <c r="M85">
-        <v>0.05</v>
-      </c>
-      <c r="N85">
+      <c r="K85">
+        <v>0</v>
+      </c>
+      <c r="O85">
+        <v>0.05</v>
+      </c>
+      <c r="P85">
         <v>0.05</v>
       </c>
     </row>
@@ -4262,10 +4548,13 @@
       <c r="J86">
         <v>699</v>
       </c>
-      <c r="M86">
-        <v>0.05</v>
-      </c>
-      <c r="N86">
+      <c r="K86">
+        <v>1</v>
+      </c>
+      <c r="O86">
+        <v>0.05</v>
+      </c>
+      <c r="P86">
         <v>0.05</v>
       </c>
     </row>
@@ -4302,10 +4591,13 @@
       <c r="J87">
         <v>1857</v>
       </c>
-      <c r="M87">
-        <v>0.05</v>
-      </c>
-      <c r="N87">
+      <c r="K87">
+        <v>0</v>
+      </c>
+      <c r="O87">
+        <v>0.05</v>
+      </c>
+      <c r="P87">
         <v>0.05</v>
       </c>
     </row>
@@ -4342,10 +4634,13 @@
       <c r="J88">
         <v>860</v>
       </c>
-      <c r="M88">
-        <v>0.05</v>
-      </c>
-      <c r="N88">
+      <c r="K88">
+        <v>1</v>
+      </c>
+      <c r="O88">
+        <v>0.05</v>
+      </c>
+      <c r="P88">
         <v>0.05</v>
       </c>
     </row>
@@ -4382,10 +4677,13 @@
       <c r="J89">
         <v>1032</v>
       </c>
-      <c r="M89">
-        <v>0.05</v>
-      </c>
-      <c r="N89">
+      <c r="K89">
+        <v>0</v>
+      </c>
+      <c r="O89">
+        <v>0.05</v>
+      </c>
+      <c r="P89">
         <v>0.05</v>
       </c>
     </row>
@@ -4422,10 +4720,13 @@
       <c r="J90">
         <v>2240</v>
       </c>
-      <c r="M90">
-        <v>0.05</v>
-      </c>
-      <c r="N90">
+      <c r="K90">
+        <v>1</v>
+      </c>
+      <c r="O90">
+        <v>0.05</v>
+      </c>
+      <c r="P90">
         <v>0.05</v>
       </c>
     </row>
@@ -4462,10 +4763,13 @@
       <c r="J91">
         <v>1662</v>
       </c>
-      <c r="M91">
-        <v>0.05</v>
-      </c>
-      <c r="N91">
+      <c r="K91">
+        <v>0</v>
+      </c>
+      <c r="O91">
+        <v>0.05</v>
+      </c>
+      <c r="P91">
         <v>0.05</v>
       </c>
     </row>
@@ -4502,10 +4806,13 @@
       <c r="J92">
         <v>753</v>
       </c>
-      <c r="M92">
-        <v>0.05</v>
-      </c>
-      <c r="N92">
+      <c r="K92">
+        <v>1</v>
+      </c>
+      <c r="O92">
+        <v>0.05</v>
+      </c>
+      <c r="P92">
         <v>0.05</v>
       </c>
     </row>
@@ -4542,10 +4849,13 @@
       <c r="J93">
         <v>1688</v>
       </c>
-      <c r="M93">
-        <v>0.05</v>
-      </c>
-      <c r="N93">
+      <c r="K93">
+        <v>0</v>
+      </c>
+      <c r="O93">
+        <v>0.05</v>
+      </c>
+      <c r="P93">
         <v>0.05</v>
       </c>
     </row>
@@ -4582,10 +4892,13 @@
       <c r="J94">
         <v>1908</v>
       </c>
-      <c r="M94">
-        <v>0.05</v>
-      </c>
-      <c r="N94">
+      <c r="K94">
+        <v>1</v>
+      </c>
+      <c r="O94">
+        <v>0.05</v>
+      </c>
+      <c r="P94">
         <v>0.05</v>
       </c>
     </row>
@@ -4622,10 +4935,13 @@
       <c r="J95">
         <v>2569</v>
       </c>
-      <c r="M95">
-        <v>0.05</v>
-      </c>
-      <c r="N95">
+      <c r="K95">
+        <v>0</v>
+      </c>
+      <c r="O95">
+        <v>0.05</v>
+      </c>
+      <c r="P95">
         <v>0.05</v>
       </c>
     </row>
@@ -4663,12 +4979,18 @@
         <v>43</v>
       </c>
       <c r="K96">
+        <v>0</v>
+      </c>
+      <c r="L96">
+        <v>0</v>
+      </c>
+      <c r="M96">
         <v>15100.33608247423</v>
       </c>
-      <c r="M96">
-        <v>0.05</v>
-      </c>
-      <c r="N96">
+      <c r="O96">
+        <v>0.05</v>
+      </c>
+      <c r="P96">
         <v>0.05</v>
       </c>
     </row>
@@ -4706,12 +5028,18 @@
         <v>99</v>
       </c>
       <c r="K97">
+        <v>0</v>
+      </c>
+      <c r="L97">
+        <v>0</v>
+      </c>
+      <c r="M97">
         <v>30906.24950495049</v>
       </c>
-      <c r="M97">
-        <v>0.05</v>
-      </c>
-      <c r="N97">
+      <c r="O97">
+        <v>0.05</v>
+      </c>
+      <c r="P97">
         <v>0.05</v>
       </c>
     </row>
@@ -4749,12 +5077,18 @@
         <v>113</v>
       </c>
       <c r="K98">
+        <v>0</v>
+      </c>
+      <c r="L98">
+        <v>0</v>
+      </c>
+      <c r="M98">
         <v>23668.15049504951</v>
       </c>
-      <c r="M98">
-        <v>0.05</v>
-      </c>
-      <c r="N98">
+      <c r="O98">
+        <v>0.05</v>
+      </c>
+      <c r="P98">
         <v>0.05</v>
       </c>
     </row>
@@ -4792,12 +5126,18 @@
         <v>195</v>
       </c>
       <c r="K99">
+        <v>0</v>
+      </c>
+      <c r="L99">
+        <v>0</v>
+      </c>
+      <c r="M99">
         <v>153237.7705882353</v>
       </c>
-      <c r="M99">
-        <v>0.05</v>
-      </c>
-      <c r="N99">
+      <c r="O99">
+        <v>0.05</v>
+      </c>
+      <c r="P99">
         <v>0.05</v>
       </c>
     </row>
@@ -4835,12 +5175,18 @@
         <v>191</v>
       </c>
       <c r="K100">
+        <v>1</v>
+      </c>
+      <c r="L100">
+        <v>0</v>
+      </c>
+      <c r="M100">
         <v>127138.0294117647</v>
       </c>
-      <c r="M100">
-        <v>0.05</v>
-      </c>
-      <c r="N100">
+      <c r="O100">
+        <v>0.05</v>
+      </c>
+      <c r="P100">
         <v>0.05</v>
       </c>
     </row>
@@ -4878,12 +5224,18 @@
         <v>221</v>
       </c>
       <c r="K101">
+        <v>1</v>
+      </c>
+      <c r="L101">
+        <v>0</v>
+      </c>
+      <c r="M101">
         <v>120962.5</v>
       </c>
-      <c r="M101">
-        <v>0.05</v>
-      </c>
-      <c r="N101">
+      <c r="O101">
+        <v>0.05</v>
+      </c>
+      <c r="P101">
         <v>0.05</v>
       </c>
     </row>
@@ -4921,12 +5273,18 @@
         <v>214</v>
       </c>
       <c r="K102">
+        <v>1</v>
+      </c>
+      <c r="L102">
+        <v>0</v>
+      </c>
+      <c r="M102">
         <v>44237.05555555555</v>
       </c>
-      <c r="M102">
-        <v>0.05</v>
-      </c>
-      <c r="N102">
+      <c r="O102">
+        <v>0.05</v>
+      </c>
+      <c r="P102">
         <v>0.05</v>
       </c>
     </row>
@@ -4964,12 +5322,18 @@
         <v>83</v>
       </c>
       <c r="K103">
+        <v>1</v>
+      </c>
+      <c r="L103">
+        <v>0</v>
+      </c>
+      <c r="M103">
         <v>55570.94949494949</v>
       </c>
-      <c r="M103">
-        <v>0.05</v>
-      </c>
-      <c r="N103">
+      <c r="O103">
+        <v>0.05</v>
+      </c>
+      <c r="P103">
         <v>0.05</v>
       </c>
     </row>
@@ -5007,12 +5371,18 @@
         <v>187</v>
       </c>
       <c r="K104">
+        <v>1</v>
+      </c>
+      <c r="L104">
+        <v>0</v>
+      </c>
+      <c r="M104">
         <v>43470.02494949495</v>
       </c>
-      <c r="M104">
-        <v>0.05</v>
-      </c>
-      <c r="N104">
+      <c r="O104">
+        <v>0.05</v>
+      </c>
+      <c r="P104">
         <v>0.05</v>
       </c>
     </row>
@@ -5050,12 +5420,18 @@
         <v>288</v>
       </c>
       <c r="K105">
+        <v>1</v>
+      </c>
+      <c r="L105">
+        <v>0</v>
+      </c>
+      <c r="M105">
         <v>6318.54</v>
       </c>
-      <c r="M105">
-        <v>0.05</v>
-      </c>
-      <c r="N105">
+      <c r="O105">
+        <v>0.05</v>
+      </c>
+      <c r="P105">
         <v>0.05</v>
       </c>
     </row>
@@ -5093,12 +5469,18 @@
         <v>294</v>
       </c>
       <c r="K106">
+        <v>1</v>
+      </c>
+      <c r="L106">
+        <v>0</v>
+      </c>
+      <c r="M106">
         <v>9106.809999999999</v>
       </c>
-      <c r="M106">
-        <v>0.05</v>
-      </c>
-      <c r="N106">
+      <c r="O106">
+        <v>0.05</v>
+      </c>
+      <c r="P106">
         <v>0.05</v>
       </c>
     </row>
@@ -5136,12 +5518,18 @@
         <v>293</v>
       </c>
       <c r="K107">
+        <v>1</v>
+      </c>
+      <c r="L107">
+        <v>0</v>
+      </c>
+      <c r="M107">
         <v>60399.48</v>
       </c>
-      <c r="M107">
-        <v>0.05</v>
-      </c>
-      <c r="N107">
+      <c r="O107">
+        <v>0.05</v>
+      </c>
+      <c r="P107">
         <v>0.05</v>
       </c>
     </row>
@@ -5179,12 +5567,18 @@
         <v>159</v>
       </c>
       <c r="K108">
+        <v>1</v>
+      </c>
+      <c r="L108">
+        <v>0</v>
+      </c>
+      <c r="M108">
         <v>28890.6</v>
       </c>
-      <c r="M108">
-        <v>0.05</v>
-      </c>
-      <c r="N108">
+      <c r="O108">
+        <v>0.05</v>
+      </c>
+      <c r="P108">
         <v>0.05</v>
       </c>
     </row>
@@ -5222,12 +5616,18 @@
         <v>82</v>
       </c>
       <c r="K109">
+        <v>1</v>
+      </c>
+      <c r="L109">
+        <v>0</v>
+      </c>
+      <c r="M109">
         <v>49682.78747474747</v>
       </c>
-      <c r="M109">
-        <v>0.05</v>
-      </c>
-      <c r="N109">
+      <c r="O109">
+        <v>0.05</v>
+      </c>
+      <c r="P109">
         <v>0.05</v>
       </c>
     </row>
@@ -5265,12 +5665,18 @@
         <v>122</v>
       </c>
       <c r="K110">
+        <v>1</v>
+      </c>
+      <c r="L110">
+        <v>0</v>
+      </c>
+      <c r="M110">
         <v>20800.80252525253</v>
       </c>
-      <c r="M110">
-        <v>0.05</v>
-      </c>
-      <c r="N110">
+      <c r="O110">
+        <v>0.05</v>
+      </c>
+      <c r="P110">
         <v>0.05</v>
       </c>
     </row>
@@ -5308,12 +5714,18 @@
         <v>446</v>
       </c>
       <c r="K111">
+        <v>1</v>
+      </c>
+      <c r="L111">
+        <v>0</v>
+      </c>
+      <c r="M111">
         <v>54856.33</v>
       </c>
-      <c r="M111">
-        <v>0.05</v>
-      </c>
-      <c r="N111">
+      <c r="O111">
+        <v>0.05</v>
+      </c>
+      <c r="P111">
         <v>0.05</v>
       </c>
     </row>
@@ -5351,12 +5763,18 @@
         <v>151</v>
       </c>
       <c r="K112">
+        <v>1</v>
+      </c>
+      <c r="L112">
+        <v>0</v>
+      </c>
+      <c r="M112">
         <v>200973.82</v>
       </c>
-      <c r="M112">
-        <v>0.05</v>
-      </c>
-      <c r="N112">
+      <c r="O112">
+        <v>0.05</v>
+      </c>
+      <c r="P112">
         <v>0.05</v>
       </c>
     </row>
@@ -5394,12 +5812,18 @@
         <v>309</v>
       </c>
       <c r="K113">
+        <v>1</v>
+      </c>
+      <c r="L113">
+        <v>0</v>
+      </c>
+      <c r="M113">
         <v>45367.62</v>
       </c>
-      <c r="M113">
-        <v>0.05</v>
-      </c>
-      <c r="N113">
+      <c r="O113">
+        <v>0.05</v>
+      </c>
+      <c r="P113">
         <v>0.05</v>
       </c>
     </row>
@@ -5437,12 +5861,18 @@
         <v>312</v>
       </c>
       <c r="K114">
+        <v>1</v>
+      </c>
+      <c r="L114">
+        <v>0</v>
+      </c>
+      <c r="M114">
         <v>39447.62</v>
       </c>
-      <c r="M114">
-        <v>0.05</v>
-      </c>
-      <c r="N114">
+      <c r="O114">
+        <v>0.05</v>
+      </c>
+      <c r="P114">
         <v>0.05</v>
       </c>
     </row>
@@ -5480,12 +5910,18 @@
         <v>325</v>
       </c>
       <c r="K115">
+        <v>1</v>
+      </c>
+      <c r="L115">
+        <v>0</v>
+      </c>
+      <c r="M115">
         <v>14078.56927536232</v>
       </c>
-      <c r="M115">
-        <v>0.05</v>
-      </c>
-      <c r="N115">
+      <c r="O115">
+        <v>0.05</v>
+      </c>
+      <c r="P115">
         <v>0.05</v>
       </c>
     </row>
@@ -5523,12 +5959,18 @@
         <v>312</v>
       </c>
       <c r="K116">
+        <v>1</v>
+      </c>
+      <c r="L116">
+        <v>70000</v>
+      </c>
+      <c r="M116">
         <v>109194.2223913043</v>
       </c>
-      <c r="M116">
-        <v>0.05</v>
-      </c>
-      <c r="N116">
+      <c r="O116">
+        <v>0.05</v>
+      </c>
+      <c r="P116">
         <v>0.05</v>
       </c>
     </row>
@@ -5566,12 +6008,18 @@
         <v>234</v>
       </c>
       <c r="K117">
+        <v>1</v>
+      </c>
+      <c r="L117">
+        <v>659000</v>
+      </c>
+      <c r="M117">
         <v>113334.7638036304</v>
       </c>
-      <c r="M117">
-        <v>0.05</v>
-      </c>
-      <c r="N117">
+      <c r="O117">
+        <v>0.05</v>
+      </c>
+      <c r="P117">
         <v>0.05</v>
       </c>
     </row>
@@ -5609,12 +6057,18 @@
         <v>254</v>
       </c>
       <c r="K118">
+        <v>1</v>
+      </c>
+      <c r="L118">
+        <v>658000</v>
+      </c>
+      <c r="M118">
         <v>21002.02876237624</v>
       </c>
-      <c r="M118">
-        <v>0.05</v>
-      </c>
-      <c r="N118">
+      <c r="O118">
+        <v>0.05</v>
+      </c>
+      <c r="P118">
         <v>0.05</v>
       </c>
     </row>
@@ -5652,12 +6106,18 @@
         <v>70</v>
       </c>
       <c r="K119">
+        <v>1</v>
+      </c>
+      <c r="L119">
+        <v>206000</v>
+      </c>
+      <c r="M119">
         <v>6103.532659276798</v>
       </c>
-      <c r="M119">
-        <v>0.05</v>
-      </c>
-      <c r="N119">
+      <c r="O119">
+        <v>0.05</v>
+      </c>
+      <c r="P119">
         <v>0.05</v>
       </c>
     </row>
@@ -5695,12 +6155,18 @@
         <v>253</v>
       </c>
       <c r="K120">
+        <v>1</v>
+      </c>
+      <c r="L120">
+        <v>862000</v>
+      </c>
+      <c r="M120">
         <v>40080.33552053925</v>
       </c>
-      <c r="M120">
-        <v>0.05</v>
-      </c>
-      <c r="N120">
+      <c r="O120">
+        <v>0.05</v>
+      </c>
+      <c r="P120">
         <v>0.05</v>
       </c>
     </row>
@@ -5738,12 +6204,18 @@
         <v>97</v>
       </c>
       <c r="K121">
+        <v>1</v>
+      </c>
+      <c r="L121">
+        <v>1025000</v>
+      </c>
+      <c r="M121">
         <v>19458.13390432388</v>
       </c>
-      <c r="M121">
-        <v>0.05</v>
-      </c>
-      <c r="N121">
+      <c r="O121">
+        <v>0.05</v>
+      </c>
+      <c r="P121">
         <v>0.05</v>
       </c>
     </row>
@@ -5780,10 +6252,16 @@
       <c r="J122">
         <v>364</v>
       </c>
-      <c r="M122">
-        <v>0.05</v>
-      </c>
-      <c r="N122">
+      <c r="K122">
+        <v>0</v>
+      </c>
+      <c r="L122">
+        <v>860000</v>
+      </c>
+      <c r="O122">
+        <v>0.05</v>
+      </c>
+      <c r="P122">
         <v>0.05</v>
       </c>
     </row>
@@ -5820,10 +6298,16 @@
       <c r="J123">
         <v>33</v>
       </c>
-      <c r="M123">
-        <v>0.05</v>
-      </c>
-      <c r="N123">
+      <c r="K123">
+        <v>1</v>
+      </c>
+      <c r="L123">
+        <v>1200000</v>
+      </c>
+      <c r="O123">
+        <v>0.05</v>
+      </c>
+      <c r="P123">
         <v>0.05</v>
       </c>
     </row>
@@ -5860,10 +6344,16 @@
       <c r="J124">
         <v>247</v>
       </c>
-      <c r="M124">
-        <v>0.05</v>
-      </c>
-      <c r="N124">
+      <c r="K124">
+        <v>0</v>
+      </c>
+      <c r="L124">
+        <v>1900000</v>
+      </c>
+      <c r="O124">
+        <v>0.05</v>
+      </c>
+      <c r="P124">
         <v>0.05</v>
       </c>
     </row>
@@ -5900,10 +6390,16 @@
       <c r="J125">
         <v>230</v>
       </c>
-      <c r="M125">
-        <v>0.05</v>
-      </c>
-      <c r="N125">
+      <c r="K125">
+        <v>0</v>
+      </c>
+      <c r="L125">
+        <v>2100000</v>
+      </c>
+      <c r="O125">
+        <v>0.05</v>
+      </c>
+      <c r="P125">
         <v>0.05</v>
       </c>
     </row>
@@ -5940,10 +6436,16 @@
       <c r="J126">
         <v>152</v>
       </c>
-      <c r="M126">
-        <v>0.05</v>
-      </c>
-      <c r="N126">
+      <c r="K126">
+        <v>0</v>
+      </c>
+      <c r="L126">
+        <v>2300000</v>
+      </c>
+      <c r="O126">
+        <v>0.05</v>
+      </c>
+      <c r="P126">
         <v>0.05</v>
       </c>
     </row>
@@ -5981,12 +6483,18 @@
         <v>109</v>
       </c>
       <c r="K127">
+        <v>0</v>
+      </c>
+      <c r="L127">
+        <v>783000</v>
+      </c>
+      <c r="M127">
         <v>4457.478632583055</v>
       </c>
-      <c r="M127">
-        <v>0.05</v>
-      </c>
-      <c r="N127">
+      <c r="O127">
+        <v>0.05</v>
+      </c>
+      <c r="P127">
         <v>0.05</v>
       </c>
     </row>
@@ -6024,12 +6532,18 @@
         <v>94</v>
       </c>
       <c r="K128">
+        <v>1</v>
+      </c>
+      <c r="L128">
+        <v>0</v>
+      </c>
+      <c r="M128">
         <v>14304.31984967649</v>
       </c>
-      <c r="M128">
-        <v>0.05</v>
-      </c>
-      <c r="N128">
+      <c r="O128">
+        <v>0.05</v>
+      </c>
+      <c r="P128">
         <v>0.05</v>
       </c>
     </row>
@@ -6067,12 +6581,18 @@
         <v>52</v>
       </c>
       <c r="K129">
+        <v>0</v>
+      </c>
+      <c r="L129">
+        <v>0</v>
+      </c>
+      <c r="M129">
         <v>17385.5835483871</v>
       </c>
-      <c r="M129">
-        <v>0.05</v>
-      </c>
-      <c r="N129">
+      <c r="O129">
+        <v>0.05</v>
+      </c>
+      <c r="P129">
         <v>0.05</v>
       </c>
     </row>
@@ -6110,15 +6630,21 @@
         <v>303</v>
       </c>
       <c r="K130">
+        <v>0</v>
+      </c>
+      <c r="L130">
+        <v>0</v>
+      </c>
+      <c r="M130">
         <v>34386.77385321101</v>
       </c>
-      <c r="L130">
+      <c r="N130">
         <v>0.1679416316376597</v>
       </c>
-      <c r="M130">
+      <c r="O130">
         <v>0.399812753899036</v>
       </c>
-      <c r="N130">
+      <c r="P130">
         <v>0.05</v>
       </c>
     </row>
@@ -6156,15 +6682,21 @@
         <v>67</v>
       </c>
       <c r="K131">
+        <v>0</v>
+      </c>
+      <c r="L131">
+        <v>0</v>
+      </c>
+      <c r="M131">
         <v>8643.726146788991</v>
       </c>
-      <c r="L131">
+      <c r="N131">
         <v>0.4678036269350629</v>
       </c>
-      <c r="M131">
+      <c r="O131">
         <v>0.399812753899036</v>
       </c>
-      <c r="N131">
+      <c r="P131">
         <v>0.05</v>
       </c>
     </row>
@@ -6202,12 +6734,18 @@
         <v>62</v>
       </c>
       <c r="K132">
+        <v>0</v>
+      </c>
+      <c r="L132">
+        <v>0</v>
+      </c>
+      <c r="M132">
         <v>43839.87877920145</v>
       </c>
-      <c r="M132">
-        <v>0.05</v>
-      </c>
-      <c r="N132">
+      <c r="O132">
+        <v>0.05</v>
+      </c>
+      <c r="P132">
         <v>0.05</v>
       </c>
     </row>
@@ -6245,12 +6783,18 @@
         <v>47</v>
       </c>
       <c r="K133">
+        <v>0</v>
+      </c>
+      <c r="L133">
+        <v>0</v>
+      </c>
+      <c r="M133">
         <v>10937.88288746522</v>
       </c>
-      <c r="M133">
-        <v>0.05</v>
-      </c>
-      <c r="N133">
+      <c r="O133">
+        <v>0.05</v>
+      </c>
+      <c r="P133">
         <v>0.05</v>
       </c>
     </row>
@@ -6288,12 +6832,18 @@
         <v>36</v>
       </c>
       <c r="K134">
+        <v>0</v>
+      </c>
+      <c r="L134">
+        <v>0</v>
+      </c>
+      <c r="M134">
         <v>26414.05275956284</v>
       </c>
-      <c r="M134">
-        <v>0.05</v>
-      </c>
-      <c r="N134">
+      <c r="O134">
+        <v>0.05</v>
+      </c>
+      <c r="P134">
         <v>0.05</v>
       </c>
     </row>
@@ -6331,12 +6881,18 @@
         <v>109</v>
       </c>
       <c r="K135">
+        <v>0</v>
+      </c>
+      <c r="L135">
+        <v>0</v>
+      </c>
+      <c r="M135">
         <v>17167.38557377049</v>
       </c>
-      <c r="M135">
-        <v>0.05</v>
-      </c>
-      <c r="N135">
+      <c r="O135">
+        <v>0.05</v>
+      </c>
+      <c r="P135">
         <v>0.05</v>
       </c>
     </row>
@@ -6374,12 +6930,18 @@
         <v>10</v>
       </c>
       <c r="K136">
+        <v>0</v>
+      </c>
+      <c r="L136">
+        <v>0</v>
+      </c>
+      <c r="M136">
         <v>1239.474074074074</v>
       </c>
-      <c r="M136">
-        <v>0.05</v>
-      </c>
-      <c r="N136">
+      <c r="O136">
+        <v>0.05</v>
+      </c>
+      <c r="P136">
         <v>0.05</v>
       </c>
     </row>
@@ -6417,12 +6979,18 @@
         <v>119</v>
       </c>
       <c r="K137">
+        <v>0</v>
+      </c>
+      <c r="L137">
+        <v>0</v>
+      </c>
+      <c r="M137">
         <v>6640.959620596205</v>
       </c>
-      <c r="M137">
-        <v>0.05</v>
-      </c>
-      <c r="N137">
+      <c r="O137">
+        <v>0.05</v>
+      </c>
+      <c r="P137">
         <v>0.05</v>
       </c>
     </row>
@@ -6460,12 +7028,18 @@
         <v>72</v>
       </c>
       <c r="K138">
+        <v>0</v>
+      </c>
+      <c r="L138">
+        <v>0</v>
+      </c>
+      <c r="M138">
         <v>32845.64926303271</v>
       </c>
-      <c r="M138">
-        <v>0.05</v>
-      </c>
-      <c r="N138">
+      <c r="O138">
+        <v>0.05</v>
+      </c>
+      <c r="P138">
         <v>0.05</v>
       </c>
     </row>
@@ -6502,10 +7076,16 @@
       <c r="J139">
         <v>61</v>
       </c>
-      <c r="M139">
-        <v>0.05</v>
-      </c>
-      <c r="N139">
+      <c r="K139">
+        <v>0</v>
+      </c>
+      <c r="L139">
+        <v>0</v>
+      </c>
+      <c r="O139">
+        <v>0.05</v>
+      </c>
+      <c r="P139">
         <v>0.05</v>
       </c>
     </row>
@@ -6542,10 +7122,16 @@
       <c r="J140">
         <v>21</v>
       </c>
-      <c r="M140">
-        <v>0.05</v>
-      </c>
-      <c r="N140">
+      <c r="K140">
+        <v>0</v>
+      </c>
+      <c r="L140">
+        <v>0</v>
+      </c>
+      <c r="O140">
+        <v>0.05</v>
+      </c>
+      <c r="P140">
         <v>0.05</v>
       </c>
     </row>
@@ -6582,10 +7168,16 @@
       <c r="J141">
         <v>10</v>
       </c>
-      <c r="M141">
-        <v>0.05</v>
-      </c>
-      <c r="N141">
+      <c r="K141">
+        <v>0</v>
+      </c>
+      <c r="L141">
+        <v>0</v>
+      </c>
+      <c r="O141">
+        <v>0.05</v>
+      </c>
+      <c r="P141">
         <v>0.05</v>
       </c>
     </row>
@@ -6622,10 +7214,16 @@
       <c r="J142">
         <v>162</v>
       </c>
-      <c r="M142">
-        <v>0.05</v>
-      </c>
-      <c r="N142">
+      <c r="K142">
+        <v>0</v>
+      </c>
+      <c r="L142">
+        <v>0</v>
+      </c>
+      <c r="O142">
+        <v>0.05</v>
+      </c>
+      <c r="P142">
         <v>0.05</v>
       </c>
     </row>
@@ -6662,10 +7260,16 @@
       <c r="J143">
         <v>82</v>
       </c>
-      <c r="M143">
-        <v>0.05</v>
-      </c>
-      <c r="N143">
+      <c r="K143">
+        <v>0</v>
+      </c>
+      <c r="L143">
+        <v>0</v>
+      </c>
+      <c r="O143">
+        <v>0.05</v>
+      </c>
+      <c r="P143">
         <v>0.05</v>
       </c>
     </row>
@@ -6702,10 +7306,16 @@
       <c r="J144">
         <v>158</v>
       </c>
-      <c r="M144">
-        <v>0.05</v>
-      </c>
-      <c r="N144">
+      <c r="K144">
+        <v>0</v>
+      </c>
+      <c r="L144">
+        <v>0</v>
+      </c>
+      <c r="O144">
+        <v>0.05</v>
+      </c>
+      <c r="P144">
         <v>0.05</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add years without age data back into Hucuktlis time series
</commit_message>
<xml_diff>
--- a/3. outputs/Stock-recruit data/Barkley_Sockeye_stock-recruit_infilled.xlsx
+++ b/3. outputs/Stock-recruit data/Barkley_Sockeye_stock-recruit_infilled.xlsx
@@ -581,7 +581,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q144"/>
+  <dimension ref="A1:Q205"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5246,7 +5246,7 @@
     </row>
     <row r="96">
       <c r="A96">
-        <v>1972</v>
+        <v>1970</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
@@ -5254,31 +5254,16 @@
         </is>
       </c>
       <c r="C96">
-        <v>3500</v>
-      </c>
-      <c r="D96">
-        <v>3500</v>
+        <v>9000</v>
       </c>
       <c r="E96">
-        <v>4407</v>
+        <v>14317</v>
       </c>
       <c r="F96">
-        <v>907</v>
-      </c>
-      <c r="G96">
-        <v>0</v>
-      </c>
-      <c r="H96">
-        <v>0.91</v>
-      </c>
-      <c r="I96">
-        <v>0.06999999999999999</v>
-      </c>
-      <c r="J96">
-        <v>0.02</v>
+        <v>5317</v>
       </c>
       <c r="K96">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="L96">
         <v>0</v>
@@ -5287,7 +5272,7 @@
         <v>0</v>
       </c>
       <c r="N96">
-        <v>15100.33608247423</v>
+        <v>12426.88633663366</v>
       </c>
       <c r="P96">
         <v>0.05</v>
@@ -5298,7 +5283,7 @@
     </row>
     <row r="97">
       <c r="A97">
-        <v>1973</v>
+        <v>1971</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
@@ -5306,31 +5291,16 @@
         </is>
       </c>
       <c r="C97">
-        <v>40000</v>
-      </c>
-      <c r="D97">
-        <v>40000</v>
+        <v>7500</v>
       </c>
       <c r="E97">
-        <v>58495</v>
+        <v>8522</v>
       </c>
       <c r="F97">
-        <v>18495</v>
-      </c>
-      <c r="G97">
-        <v>0</v>
-      </c>
-      <c r="H97">
-        <v>0.66</v>
-      </c>
-      <c r="I97">
-        <v>0.34</v>
-      </c>
-      <c r="J97">
-        <v>0</v>
+        <v>1022</v>
       </c>
       <c r="K97">
-        <v>99</v>
+        <v>0</v>
       </c>
       <c r="L97">
         <v>0</v>
@@ -5339,7 +5309,7 @@
         <v>0</v>
       </c>
       <c r="N97">
-        <v>30906.24950495049</v>
+        <v>12492.49362049607</v>
       </c>
       <c r="P97">
         <v>0.05</v>
@@ -5350,7 +5320,7 @@
     </row>
     <row r="98">
       <c r="A98">
-        <v>1974</v>
+        <v>1972</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
@@ -5358,31 +5328,31 @@
         </is>
       </c>
       <c r="C98">
-        <v>6000</v>
+        <v>3500</v>
       </c>
       <c r="D98">
-        <v>6000</v>
+        <v>3500</v>
       </c>
       <c r="E98">
-        <v>8936</v>
+        <v>4407</v>
       </c>
       <c r="F98">
-        <v>2936</v>
+        <v>907</v>
       </c>
       <c r="G98">
         <v>0</v>
       </c>
       <c r="H98">
-        <v>0.57</v>
+        <v>0.91</v>
       </c>
       <c r="I98">
-        <v>0.43</v>
+        <v>0.06999999999999999</v>
       </c>
       <c r="J98">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="K98">
-        <v>113</v>
+        <v>43</v>
       </c>
       <c r="L98">
         <v>0</v>
@@ -5391,7 +5361,7 @@
         <v>0</v>
       </c>
       <c r="N98">
-        <v>23668.15049504951</v>
+        <v>15100.33608247423</v>
       </c>
       <c r="P98">
         <v>0.05</v>
@@ -5402,7 +5372,7 @@
     </row>
     <row r="99">
       <c r="A99">
-        <v>1975</v>
+        <v>1973</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
@@ -5410,31 +5380,31 @@
         </is>
       </c>
       <c r="C99">
-        <v>10000</v>
+        <v>40000</v>
       </c>
       <c r="D99">
-        <v>10000</v>
+        <v>40000</v>
       </c>
       <c r="E99">
-        <v>17635</v>
+        <v>58495</v>
       </c>
       <c r="F99">
-        <v>7635</v>
+        <v>18495</v>
       </c>
       <c r="G99">
         <v>0</v>
       </c>
       <c r="H99">
-        <v>0.5742574257425742</v>
+        <v>0.66</v>
       </c>
       <c r="I99">
-        <v>0.4158415841584159</v>
+        <v>0.34</v>
       </c>
       <c r="J99">
-        <v>0.009900990099009901</v>
+        <v>0</v>
       </c>
       <c r="K99">
-        <v>195</v>
+        <v>99</v>
       </c>
       <c r="L99">
         <v>0</v>
@@ -5443,7 +5413,7 @@
         <v>0</v>
       </c>
       <c r="N99">
-        <v>153237.7705882353</v>
+        <v>30906.24950495049</v>
       </c>
       <c r="P99">
         <v>0.05</v>
@@ -5454,7 +5424,7 @@
     </row>
     <row r="100">
       <c r="A100">
-        <v>1976</v>
+        <v>1974</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
@@ -5462,40 +5432,40 @@
         </is>
       </c>
       <c r="C100">
-        <v>3500</v>
+        <v>6000</v>
       </c>
       <c r="D100">
-        <v>3500</v>
+        <v>6000</v>
       </c>
       <c r="E100">
-        <v>8825</v>
+        <v>8936</v>
       </c>
       <c r="F100">
-        <v>5325</v>
+        <v>2936</v>
       </c>
       <c r="G100">
         <v>0</v>
       </c>
       <c r="H100">
-        <v>0.7319587628865979</v>
+        <v>0.57</v>
       </c>
       <c r="I100">
-        <v>0.2680412371134021</v>
+        <v>0.43</v>
       </c>
       <c r="J100">
         <v>0</v>
       </c>
       <c r="K100">
-        <v>191</v>
+        <v>113</v>
       </c>
       <c r="L100">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M100">
         <v>0</v>
       </c>
       <c r="N100">
-        <v>127138.0294117647</v>
+        <v>23668.15049504951</v>
       </c>
       <c r="P100">
         <v>0.05</v>
@@ -5506,7 +5476,7 @@
     </row>
     <row r="101">
       <c r="A101">
-        <v>1977</v>
+        <v>1975</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
@@ -5514,40 +5484,40 @@
         </is>
       </c>
       <c r="C101">
-        <v>4800</v>
+        <v>10000</v>
       </c>
       <c r="D101">
-        <v>4800</v>
+        <v>10000</v>
       </c>
       <c r="E101">
-        <v>30860</v>
+        <v>17635</v>
       </c>
       <c r="F101">
-        <v>26060</v>
+        <v>7635</v>
       </c>
       <c r="G101">
         <v>0</v>
       </c>
       <c r="H101">
-        <v>0.72</v>
+        <v>0.5742574257425742</v>
       </c>
       <c r="I101">
-        <v>0.28</v>
+        <v>0.4158415841584159</v>
       </c>
       <c r="J101">
-        <v>0</v>
+        <v>0.009900990099009901</v>
       </c>
       <c r="K101">
-        <v>221</v>
+        <v>195</v>
       </c>
       <c r="L101">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M101">
         <v>0</v>
       </c>
       <c r="N101">
-        <v>120962.5</v>
+        <v>153237.7705882353</v>
       </c>
       <c r="P101">
         <v>0.05</v>
@@ -5558,7 +5528,7 @@
     </row>
     <row r="102">
       <c r="A102">
-        <v>1978</v>
+        <v>1976</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
@@ -5566,31 +5536,31 @@
         </is>
       </c>
       <c r="C102">
-        <v>7000</v>
+        <v>3500</v>
       </c>
       <c r="D102">
-        <v>7000</v>
+        <v>3500</v>
       </c>
       <c r="E102">
-        <v>10832</v>
+        <v>8825</v>
       </c>
       <c r="F102">
-        <v>3832</v>
+        <v>5325</v>
       </c>
       <c r="G102">
         <v>0</v>
       </c>
       <c r="H102">
-        <v>0.198019801980198</v>
+        <v>0.7319587628865979</v>
       </c>
       <c r="I102">
-        <v>0.801980198019802</v>
+        <v>0.2680412371134021</v>
       </c>
       <c r="J102">
         <v>0</v>
       </c>
       <c r="K102">
-        <v>214</v>
+        <v>191</v>
       </c>
       <c r="L102">
         <v>1</v>
@@ -5599,7 +5569,7 @@
         <v>0</v>
       </c>
       <c r="N102">
-        <v>44237.05555555555</v>
+        <v>127138.0294117647</v>
       </c>
       <c r="P102">
         <v>0.05</v>
@@ -5610,7 +5580,7 @@
     </row>
     <row r="103">
       <c r="A103">
-        <v>1979</v>
+        <v>1977</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
@@ -5618,31 +5588,31 @@
         </is>
       </c>
       <c r="C103">
-        <v>20000</v>
+        <v>4800</v>
       </c>
       <c r="D103">
-        <v>20000</v>
+        <v>4800</v>
       </c>
       <c r="E103">
-        <v>143488</v>
+        <v>30860</v>
       </c>
       <c r="F103">
-        <v>123488</v>
+        <v>26060</v>
       </c>
       <c r="G103">
         <v>0</v>
       </c>
       <c r="H103">
-        <v>0.85</v>
+        <v>0.72</v>
       </c>
       <c r="I103">
-        <v>0.15</v>
+        <v>0.28</v>
       </c>
       <c r="J103">
         <v>0</v>
       </c>
       <c r="K103">
-        <v>83</v>
+        <v>221</v>
       </c>
       <c r="L103">
         <v>1</v>
@@ -5651,7 +5621,7 @@
         <v>0</v>
       </c>
       <c r="N103">
-        <v>55570.94949494949</v>
+        <v>120962.5</v>
       </c>
       <c r="P103">
         <v>0.05</v>
@@ -5662,7 +5632,7 @@
     </row>
     <row r="104">
       <c r="A104">
-        <v>1980</v>
+        <v>1978</v>
       </c>
       <c r="B104" t="inlineStr">
         <is>
@@ -5670,31 +5640,31 @@
         </is>
       </c>
       <c r="C104">
-        <v>20706</v>
+        <v>7000</v>
       </c>
       <c r="D104">
-        <v>20706</v>
+        <v>7000</v>
       </c>
       <c r="E104">
-        <v>67869</v>
+        <v>10832</v>
       </c>
       <c r="F104">
-        <v>47163</v>
+        <v>3832</v>
       </c>
       <c r="G104">
         <v>0</v>
       </c>
       <c r="H104">
-        <v>0.5392156862745099</v>
+        <v>0.198019801980198</v>
       </c>
       <c r="I104">
-        <v>0.4607843137254902</v>
+        <v>0.801980198019802</v>
       </c>
       <c r="J104">
         <v>0</v>
       </c>
       <c r="K104">
-        <v>187</v>
+        <v>214</v>
       </c>
       <c r="L104">
         <v>1</v>
@@ -5703,7 +5673,7 @@
         <v>0</v>
       </c>
       <c r="N104">
-        <v>43470.02494949495</v>
+        <v>44237.05555555555</v>
       </c>
       <c r="P104">
         <v>0.05</v>
@@ -5714,7 +5684,7 @@
     </row>
     <row r="105">
       <c r="A105">
-        <v>1981</v>
+        <v>1979</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
@@ -5722,31 +5692,31 @@
         </is>
       </c>
       <c r="C105">
-        <v>58000</v>
+        <v>20000</v>
       </c>
       <c r="D105">
-        <v>58000</v>
+        <v>20000</v>
       </c>
       <c r="E105">
-        <v>175758</v>
+        <v>143488</v>
       </c>
       <c r="F105">
-        <v>117758</v>
+        <v>123488</v>
       </c>
       <c r="G105">
         <v>0</v>
       </c>
       <c r="H105">
-        <v>0.4848484848484848</v>
+        <v>0.85</v>
       </c>
       <c r="I105">
-        <v>0.5151515151515151</v>
+        <v>0.15</v>
       </c>
       <c r="J105">
         <v>0</v>
       </c>
       <c r="K105">
-        <v>288</v>
+        <v>83</v>
       </c>
       <c r="L105">
         <v>1</v>
@@ -5755,7 +5725,7 @@
         <v>0</v>
       </c>
       <c r="N105">
-        <v>6318.54</v>
+        <v>55570.94949494949</v>
       </c>
       <c r="P105">
         <v>0.05</v>
@@ -5766,7 +5736,7 @@
     </row>
     <row r="106">
       <c r="A106">
-        <v>1982</v>
+        <v>1980</v>
       </c>
       <c r="B106" t="inlineStr">
         <is>
@@ -5774,31 +5744,31 @@
         </is>
       </c>
       <c r="C106">
-        <v>36700</v>
+        <v>20706</v>
       </c>
       <c r="D106">
-        <v>36700</v>
+        <v>20706</v>
       </c>
       <c r="E106">
-        <v>47662</v>
+        <v>67869</v>
       </c>
       <c r="F106">
-        <v>10962</v>
+        <v>47163</v>
       </c>
       <c r="G106">
         <v>0</v>
       </c>
       <c r="H106">
-        <v>0.25</v>
+        <v>0.5392156862745099</v>
       </c>
       <c r="I106">
-        <v>0.75</v>
+        <v>0.4607843137254902</v>
       </c>
       <c r="J106">
         <v>0</v>
       </c>
       <c r="K106">
-        <v>294</v>
+        <v>187</v>
       </c>
       <c r="L106">
         <v>1</v>
@@ -5807,7 +5777,7 @@
         <v>0</v>
       </c>
       <c r="N106">
-        <v>9106.809999999999</v>
+        <v>43470.02494949495</v>
       </c>
       <c r="P106">
         <v>0.05</v>
@@ -5818,7 +5788,7 @@
     </row>
     <row r="107">
       <c r="A107">
-        <v>1983</v>
+        <v>1981</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
@@ -5826,31 +5796,31 @@
         </is>
       </c>
       <c r="C107">
-        <v>31000</v>
+        <v>58000</v>
       </c>
       <c r="D107">
-        <v>30686.86868686869</v>
+        <v>58000</v>
       </c>
       <c r="E107">
-        <v>35227</v>
+        <v>175758</v>
       </c>
       <c r="F107">
-        <v>4227</v>
+        <v>117758</v>
       </c>
       <c r="G107">
-        <v>0.0101010101010101</v>
+        <v>0</v>
       </c>
       <c r="H107">
-        <v>0.3232323232323233</v>
+        <v>0.4848484848484848</v>
       </c>
       <c r="I107">
-        <v>0.6666666666666667</v>
+        <v>0.5151515151515151</v>
       </c>
       <c r="J107">
         <v>0</v>
       </c>
       <c r="K107">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="L107">
         <v>1</v>
@@ -5859,7 +5829,7 @@
         <v>0</v>
       </c>
       <c r="N107">
-        <v>60399.48</v>
+        <v>6318.54</v>
       </c>
       <c r="P107">
         <v>0.05</v>
@@ -5870,7 +5840,7 @@
     </row>
     <row r="108">
       <c r="A108">
-        <v>1984</v>
+        <v>1982</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
@@ -5878,31 +5848,31 @@
         </is>
       </c>
       <c r="C108">
-        <v>73400</v>
+        <v>36700</v>
       </c>
       <c r="D108">
-        <v>73399.99999999999</v>
+        <v>36700</v>
       </c>
       <c r="E108">
-        <v>79532</v>
+        <v>47662</v>
       </c>
       <c r="F108">
-        <v>6132</v>
+        <v>10962</v>
       </c>
       <c r="G108">
         <v>0</v>
       </c>
       <c r="H108">
-        <v>0.3333333333333333</v>
+        <v>0.25</v>
       </c>
       <c r="I108">
-        <v>0.5555555555555555</v>
+        <v>0.75</v>
       </c>
       <c r="J108">
-        <v>0.1111111111111111</v>
+        <v>0</v>
       </c>
       <c r="K108">
-        <v>159</v>
+        <v>294</v>
       </c>
       <c r="L108">
         <v>1</v>
@@ -5911,7 +5881,7 @@
         <v>0</v>
       </c>
       <c r="N108">
-        <v>28890.6</v>
+        <v>9106.809999999999</v>
       </c>
       <c r="P108">
         <v>0.05</v>
@@ -5922,7 +5892,7 @@
     </row>
     <row r="109">
       <c r="A109">
-        <v>1985</v>
+        <v>1983</v>
       </c>
       <c r="B109" t="inlineStr">
         <is>
@@ -5930,31 +5900,31 @@
         </is>
       </c>
       <c r="C109">
-        <v>18500</v>
+        <v>31000</v>
       </c>
       <c r="D109">
-        <v>18500</v>
+        <v>30686.86868686869</v>
       </c>
       <c r="E109">
-        <v>18949</v>
+        <v>35227</v>
       </c>
       <c r="F109">
-        <v>449</v>
+        <v>4227</v>
       </c>
       <c r="G109">
-        <v>0</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="H109">
-        <v>0.13</v>
+        <v>0.3232323232323233</v>
       </c>
       <c r="I109">
-        <v>0.87</v>
+        <v>0.6666666666666667</v>
       </c>
       <c r="J109">
         <v>0</v>
       </c>
       <c r="K109">
-        <v>82</v>
+        <v>293</v>
       </c>
       <c r="L109">
         <v>1</v>
@@ -5963,7 +5933,7 @@
         <v>0</v>
       </c>
       <c r="N109">
-        <v>49682.78747474747</v>
+        <v>60399.48</v>
       </c>
       <c r="P109">
         <v>0.05</v>
@@ -5974,7 +5944,7 @@
     </row>
     <row r="110">
       <c r="A110">
-        <v>1986</v>
+        <v>1984</v>
       </c>
       <c r="B110" t="inlineStr">
         <is>
@@ -5982,31 +5952,31 @@
         </is>
       </c>
       <c r="C110">
-        <v>3900</v>
+        <v>73400</v>
       </c>
       <c r="D110">
-        <v>3900</v>
+        <v>73399.99999999999</v>
       </c>
       <c r="E110">
-        <v>3930</v>
+        <v>79532</v>
       </c>
       <c r="F110">
-        <v>30</v>
+        <v>6132</v>
       </c>
       <c r="G110">
         <v>0</v>
       </c>
       <c r="H110">
-        <v>0.09</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="I110">
-        <v>0.88</v>
+        <v>0.5555555555555555</v>
       </c>
       <c r="J110">
-        <v>0.03</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="K110">
-        <v>122</v>
+        <v>159</v>
       </c>
       <c r="L110">
         <v>1</v>
@@ -6015,7 +5985,7 @@
         <v>0</v>
       </c>
       <c r="N110">
-        <v>20800.80252525253</v>
+        <v>28890.6</v>
       </c>
       <c r="P110">
         <v>0.05</v>
@@ -6026,7 +5996,7 @@
     </row>
     <row r="111">
       <c r="A111">
-        <v>1987</v>
+        <v>1985</v>
       </c>
       <c r="B111" t="inlineStr">
         <is>
@@ -6034,31 +6004,31 @@
         </is>
       </c>
       <c r="C111">
-        <v>30800</v>
+        <v>18500</v>
       </c>
       <c r="D111">
-        <v>30800</v>
+        <v>18500</v>
       </c>
       <c r="E111">
-        <v>39677</v>
+        <v>18949</v>
       </c>
       <c r="F111">
-        <v>8877</v>
+        <v>449</v>
       </c>
       <c r="G111">
         <v>0</v>
       </c>
       <c r="H111">
-        <v>0.78</v>
+        <v>0.13</v>
       </c>
       <c r="I111">
-        <v>0.21</v>
+        <v>0.87</v>
       </c>
       <c r="J111">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="K111">
-        <v>446</v>
+        <v>82</v>
       </c>
       <c r="L111">
         <v>1</v>
@@ -6067,7 +6037,7 @@
         <v>0</v>
       </c>
       <c r="N111">
-        <v>54856.33</v>
+        <v>49682.78747474747</v>
       </c>
       <c r="P111">
         <v>0.05</v>
@@ -6078,7 +6048,7 @@
     </row>
     <row r="112">
       <c r="A112">
-        <v>1988</v>
+        <v>1986</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
@@ -6086,31 +6056,31 @@
         </is>
       </c>
       <c r="C112">
-        <v>40300</v>
+        <v>3900</v>
       </c>
       <c r="D112">
-        <v>40300</v>
+        <v>3900</v>
       </c>
       <c r="E112">
-        <v>42094</v>
+        <v>3930</v>
       </c>
       <c r="F112">
-        <v>1794</v>
+        <v>30</v>
       </c>
       <c r="G112">
         <v>0</v>
       </c>
       <c r="H112">
-        <v>0.3</v>
+        <v>0.09</v>
       </c>
       <c r="I112">
-        <v>0.6899999999999999</v>
+        <v>0.88</v>
       </c>
       <c r="J112">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="K112">
-        <v>151</v>
+        <v>122</v>
       </c>
       <c r="L112">
         <v>1</v>
@@ -6119,7 +6089,7 @@
         <v>0</v>
       </c>
       <c r="N112">
-        <v>200973.82</v>
+        <v>20800.80252525253</v>
       </c>
       <c r="P112">
         <v>0.05</v>
@@ -6130,7 +6100,7 @@
     </row>
     <row r="113">
       <c r="A113">
-        <v>1989</v>
+        <v>1987</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>
@@ -6138,31 +6108,31 @@
         </is>
       </c>
       <c r="C113">
-        <v>40600</v>
+        <v>30800</v>
       </c>
       <c r="D113">
-        <v>40600</v>
+        <v>30800</v>
       </c>
       <c r="E113">
-        <v>40656</v>
+        <v>39677</v>
       </c>
       <c r="F113">
-        <v>56</v>
+        <v>8877</v>
       </c>
       <c r="G113">
         <v>0</v>
       </c>
       <c r="H113">
-        <v>0.59</v>
+        <v>0.78</v>
       </c>
       <c r="I113">
-        <v>0.4</v>
+        <v>0.21</v>
       </c>
       <c r="J113">
         <v>0.01</v>
       </c>
       <c r="K113">
-        <v>309</v>
+        <v>446</v>
       </c>
       <c r="L113">
         <v>1</v>
@@ -6171,7 +6141,7 @@
         <v>0</v>
       </c>
       <c r="N113">
-        <v>45367.62</v>
+        <v>54856.33</v>
       </c>
       <c r="P113">
         <v>0.05</v>
@@ -6182,7 +6152,7 @@
     </row>
     <row r="114">
       <c r="A114">
-        <v>1990</v>
+        <v>1988</v>
       </c>
       <c r="B114" t="inlineStr">
         <is>
@@ -6190,31 +6160,31 @@
         </is>
       </c>
       <c r="C114">
-        <v>31400</v>
+        <v>40300</v>
       </c>
       <c r="D114">
-        <v>31400</v>
+        <v>40300</v>
       </c>
       <c r="E114">
-        <v>32201</v>
+        <v>42094</v>
       </c>
       <c r="F114">
-        <v>801</v>
+        <v>1794</v>
       </c>
       <c r="G114">
         <v>0</v>
       </c>
       <c r="H114">
-        <v>0.202020202020202</v>
+        <v>0.3</v>
       </c>
       <c r="I114">
-        <v>0.797979797979798</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="J114">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="K114">
-        <v>312</v>
+        <v>151</v>
       </c>
       <c r="L114">
         <v>1</v>
@@ -6223,7 +6193,7 @@
         <v>0</v>
       </c>
       <c r="N114">
-        <v>39447.62</v>
+        <v>200973.82</v>
       </c>
       <c r="P114">
         <v>0.05</v>
@@ -6234,7 +6204,7 @@
     </row>
     <row r="115">
       <c r="A115">
-        <v>1991</v>
+        <v>1989</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
@@ -6242,31 +6212,31 @@
         </is>
       </c>
       <c r="C115">
-        <v>38100</v>
+        <v>40600</v>
       </c>
       <c r="D115">
-        <v>38100</v>
+        <v>40600</v>
       </c>
       <c r="E115">
-        <v>49295</v>
+        <v>40656</v>
       </c>
       <c r="F115">
-        <v>11195</v>
+        <v>56</v>
       </c>
       <c r="G115">
         <v>0</v>
       </c>
       <c r="H115">
-        <v>0.71</v>
+        <v>0.59</v>
       </c>
       <c r="I115">
-        <v>0.29</v>
+        <v>0.4</v>
       </c>
       <c r="J115">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="K115">
-        <v>325</v>
+        <v>309</v>
       </c>
       <c r="L115">
         <v>1</v>
@@ -6275,7 +6245,7 @@
         <v>0</v>
       </c>
       <c r="N115">
-        <v>14078.56927536232</v>
+        <v>45367.62</v>
       </c>
       <c r="P115">
         <v>0.05</v>
@@ -6286,7 +6256,7 @@
     </row>
     <row r="116">
       <c r="A116">
-        <v>1992</v>
+        <v>1990</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
@@ -6294,25 +6264,25 @@
         </is>
       </c>
       <c r="C116">
-        <v>27700</v>
+        <v>31400</v>
       </c>
       <c r="D116">
-        <v>27700</v>
+        <v>31400</v>
       </c>
       <c r="E116">
-        <v>36772</v>
+        <v>32201</v>
       </c>
       <c r="F116">
-        <v>9072</v>
+        <v>801</v>
       </c>
       <c r="G116">
         <v>0</v>
       </c>
       <c r="H116">
-        <v>0.46</v>
+        <v>0.202020202020202</v>
       </c>
       <c r="I116">
-        <v>0.54</v>
+        <v>0.797979797979798</v>
       </c>
       <c r="J116">
         <v>0</v>
@@ -6324,10 +6294,10 @@
         <v>1</v>
       </c>
       <c r="M116">
-        <v>70000</v>
+        <v>0</v>
       </c>
       <c r="N116">
-        <v>109194.2223913043</v>
+        <v>39447.62</v>
       </c>
       <c r="P116">
         <v>0.05</v>
@@ -6338,7 +6308,7 @@
     </row>
     <row r="117">
       <c r="A117">
-        <v>1993</v>
+        <v>1991</v>
       </c>
       <c r="B117" t="inlineStr">
         <is>
@@ -6346,40 +6316,40 @@
         </is>
       </c>
       <c r="C117">
-        <v>180500</v>
+        <v>38100</v>
       </c>
       <c r="D117">
-        <v>180500</v>
+        <v>38100</v>
       </c>
       <c r="E117">
-        <v>217239</v>
+        <v>49295</v>
       </c>
       <c r="F117">
-        <v>36739</v>
+        <v>11195</v>
       </c>
       <c r="G117">
         <v>0</v>
       </c>
       <c r="H117">
-        <v>0.16</v>
+        <v>0.71</v>
       </c>
       <c r="I117">
-        <v>0.84</v>
+        <v>0.29</v>
       </c>
       <c r="J117">
         <v>0</v>
       </c>
       <c r="K117">
-        <v>234</v>
+        <v>325</v>
       </c>
       <c r="L117">
         <v>1</v>
       </c>
       <c r="M117">
-        <v>659000</v>
+        <v>0</v>
       </c>
       <c r="N117">
-        <v>113334.7638036304</v>
+        <v>14078.56927536232</v>
       </c>
       <c r="P117">
         <v>0.05</v>
@@ -6390,7 +6360,7 @@
     </row>
     <row r="118">
       <c r="A118">
-        <v>1994</v>
+        <v>1992</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
@@ -6398,40 +6368,40 @@
         </is>
       </c>
       <c r="C118">
-        <v>17400</v>
+        <v>27700</v>
       </c>
       <c r="D118">
-        <v>15834</v>
+        <v>27700</v>
       </c>
       <c r="E118">
-        <v>52598</v>
+        <v>36772</v>
       </c>
       <c r="F118">
-        <v>35198</v>
+        <v>9072</v>
       </c>
       <c r="G118">
-        <v>0.09</v>
+        <v>0</v>
       </c>
       <c r="H118">
-        <v>0.68</v>
+        <v>0.46</v>
       </c>
       <c r="I118">
-        <v>0.2</v>
+        <v>0.54</v>
       </c>
       <c r="J118">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="K118">
-        <v>254</v>
+        <v>312</v>
       </c>
       <c r="L118">
         <v>1</v>
       </c>
       <c r="M118">
-        <v>658000</v>
+        <v>70000</v>
       </c>
       <c r="N118">
-        <v>21002.02876237624</v>
+        <v>109194.2223913043</v>
       </c>
       <c r="P118">
         <v>0.05</v>
@@ -6442,7 +6412,7 @@
     </row>
     <row r="119">
       <c r="A119">
-        <v>1995</v>
+        <v>1993</v>
       </c>
       <c r="B119" t="inlineStr">
         <is>
@@ -6450,16 +6420,16 @@
         </is>
       </c>
       <c r="C119">
-        <v>4400</v>
+        <v>180500</v>
       </c>
       <c r="D119">
-        <v>4400</v>
+        <v>180500</v>
       </c>
       <c r="E119">
-        <v>4489</v>
+        <v>217239</v>
       </c>
       <c r="F119">
-        <v>89</v>
+        <v>36739</v>
       </c>
       <c r="G119">
         <v>0</v>
@@ -6468,22 +6438,22 @@
         <v>0.16</v>
       </c>
       <c r="I119">
-        <v>0.82</v>
+        <v>0.84</v>
       </c>
       <c r="J119">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="K119">
-        <v>70</v>
+        <v>234</v>
       </c>
       <c r="L119">
         <v>1</v>
       </c>
       <c r="M119">
-        <v>206000</v>
+        <v>659000</v>
       </c>
       <c r="N119">
-        <v>6103.532659276798</v>
+        <v>113334.7638036304</v>
       </c>
       <c r="P119">
         <v>0.05</v>
@@ -6494,7 +6464,7 @@
     </row>
     <row r="120">
       <c r="A120">
-        <v>1996</v>
+        <v>1994</v>
       </c>
       <c r="B120" t="inlineStr">
         <is>
@@ -6502,40 +6472,40 @@
         </is>
       </c>
       <c r="C120">
-        <v>59900</v>
+        <v>17400</v>
       </c>
       <c r="D120">
-        <v>59900</v>
+        <v>15834</v>
       </c>
       <c r="E120">
-        <v>61811</v>
+        <v>52598</v>
       </c>
       <c r="F120">
-        <v>1911</v>
+        <v>35198</v>
       </c>
       <c r="G120">
-        <v>0</v>
+        <v>0.09</v>
       </c>
       <c r="H120">
-        <v>0.8799209486166009</v>
+        <v>0.68</v>
       </c>
       <c r="I120">
-        <v>0.1200790513833992</v>
+        <v>0.2</v>
       </c>
       <c r="J120">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="K120">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="L120">
         <v>1</v>
       </c>
       <c r="M120">
-        <v>862000</v>
+        <v>658000</v>
       </c>
       <c r="N120">
-        <v>40080.33552053925</v>
+        <v>21002.02876237624</v>
       </c>
       <c r="P120">
         <v>0.05</v>
@@ -6546,7 +6516,7 @@
     </row>
     <row r="121">
       <c r="A121">
-        <v>1997</v>
+        <v>1995</v>
       </c>
       <c r="B121" t="inlineStr">
         <is>
@@ -6554,40 +6524,40 @@
         </is>
       </c>
       <c r="C121">
-        <v>46200</v>
+        <v>4400</v>
       </c>
       <c r="D121">
-        <v>46200</v>
+        <v>4400</v>
       </c>
       <c r="E121">
-        <v>59613</v>
+        <v>4489</v>
       </c>
       <c r="F121">
-        <v>13413</v>
+        <v>89</v>
       </c>
       <c r="G121">
         <v>0</v>
       </c>
       <c r="H121">
-        <v>0.1111111111111111</v>
+        <v>0.16</v>
       </c>
       <c r="I121">
-        <v>0.8686868686868686</v>
+        <v>0.82</v>
       </c>
       <c r="J121">
-        <v>0.0202020202020202</v>
+        <v>0.02</v>
       </c>
       <c r="K121">
-        <v>97</v>
+        <v>70</v>
       </c>
       <c r="L121">
         <v>1</v>
       </c>
       <c r="M121">
-        <v>1025000</v>
+        <v>206000</v>
       </c>
       <c r="N121">
-        <v>19458.13390432388</v>
+        <v>7055.651212871287</v>
       </c>
       <c r="P121">
         <v>0.05</v>
@@ -6598,7 +6568,7 @@
     </row>
     <row r="122">
       <c r="A122">
-        <v>1998</v>
+        <v>1996</v>
       </c>
       <c r="B122" t="inlineStr">
         <is>
@@ -6606,37 +6576,40 @@
         </is>
       </c>
       <c r="C122">
-        <v>92100</v>
+        <v>59900</v>
       </c>
       <c r="D122">
-        <v>91819.1456043956</v>
+        <v>59900</v>
       </c>
       <c r="E122">
-        <v>119301</v>
+        <v>61811</v>
       </c>
       <c r="F122">
-        <v>27201</v>
+        <v>1911</v>
       </c>
       <c r="G122">
-        <v>0.00304945054945055</v>
+        <v>0</v>
       </c>
       <c r="H122">
-        <v>0.08815018315018315</v>
+        <v>0.8799209486166009</v>
       </c>
       <c r="I122">
-        <v>0.8834829059829059</v>
+        <v>0.1200790513833992</v>
       </c>
       <c r="J122">
-        <v>0.02531746031746032</v>
+        <v>0</v>
       </c>
       <c r="K122">
-        <v>364</v>
+        <v>253</v>
       </c>
       <c r="L122">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M122">
-        <v>860000</v>
+        <v>862000</v>
+      </c>
+      <c r="N122">
+        <v>54860.41533112901</v>
       </c>
       <c r="P122">
         <v>0.05</v>
@@ -6647,7 +6620,7 @@
     </row>
     <row r="123">
       <c r="A123">
-        <v>1999</v>
+        <v>1997</v>
       </c>
       <c r="B123" t="inlineStr">
         <is>
@@ -6655,37 +6628,40 @@
         </is>
       </c>
       <c r="C123">
-        <v>13400</v>
+        <v>46200</v>
       </c>
       <c r="D123">
-        <v>13400</v>
+        <v>46200</v>
       </c>
       <c r="E123">
-        <v>14709</v>
+        <v>59613</v>
       </c>
       <c r="F123">
-        <v>1309</v>
+        <v>13413</v>
       </c>
       <c r="G123">
         <v>0</v>
       </c>
       <c r="H123">
-        <v>0.198019801980198</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="I123">
-        <v>0.7128712871287128</v>
+        <v>0.8686868686868686</v>
       </c>
       <c r="J123">
-        <v>0.0891089108910891</v>
+        <v>0.0202020202020202</v>
       </c>
       <c r="K123">
-        <v>33</v>
+        <v>97</v>
       </c>
       <c r="L123">
         <v>1</v>
       </c>
       <c r="M123">
-        <v>1200000</v>
+        <v>1025000</v>
+      </c>
+      <c r="N123">
+        <v>25665.93554013964</v>
       </c>
       <c r="P123">
         <v>0.05</v>
@@ -6696,7 +6672,7 @@
     </row>
     <row r="124">
       <c r="A124">
-        <v>2000</v>
+        <v>1998</v>
       </c>
       <c r="B124" t="inlineStr">
         <is>
@@ -6704,37 +6680,40 @@
         </is>
       </c>
       <c r="C124">
-        <v>25100</v>
+        <v>92100</v>
       </c>
       <c r="D124">
-        <v>25100</v>
+        <v>91819.1456043956</v>
       </c>
       <c r="E124">
-        <v>25354</v>
+        <v>119301</v>
       </c>
       <c r="F124">
-        <v>254</v>
+        <v>27201</v>
       </c>
       <c r="G124">
-        <v>0</v>
+        <v>0.00304945054945055</v>
       </c>
       <c r="H124">
-        <v>0.92</v>
+        <v>0.08815018315018315</v>
       </c>
       <c r="I124">
-        <v>0.08</v>
+        <v>0.8834829059829059</v>
       </c>
       <c r="J124">
-        <v>0</v>
+        <v>0.02531746031746032</v>
       </c>
       <c r="K124">
-        <v>247</v>
+        <v>364</v>
       </c>
       <c r="L124">
         <v>0</v>
       </c>
       <c r="M124">
-        <v>1900000</v>
+        <v>860000</v>
+      </c>
+      <c r="N124">
+        <v>8584.788943186799</v>
       </c>
       <c r="P124">
         <v>0.05</v>
@@ -6745,7 +6724,7 @@
     </row>
     <row r="125">
       <c r="A125">
-        <v>2001</v>
+        <v>1999</v>
       </c>
       <c r="B125" t="inlineStr">
         <is>
@@ -6753,37 +6732,37 @@
         </is>
       </c>
       <c r="C125">
-        <v>19900</v>
+        <v>13400</v>
       </c>
       <c r="D125">
-        <v>19900</v>
+        <v>13400</v>
       </c>
       <c r="E125">
-        <v>21940</v>
+        <v>14709</v>
       </c>
       <c r="F125">
-        <v>2040</v>
+        <v>1309</v>
       </c>
       <c r="G125">
         <v>0</v>
       </c>
       <c r="H125">
-        <v>0.2841842445114077</v>
+        <v>0.198019801980198</v>
       </c>
       <c r="I125">
-        <v>0.6794102453723634</v>
+        <v>0.7128712871287128</v>
       </c>
       <c r="J125">
-        <v>0.03640551011622901</v>
+        <v>0.0891089108910891</v>
       </c>
       <c r="K125">
-        <v>230</v>
+        <v>33</v>
       </c>
       <c r="L125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M125">
-        <v>2100000</v>
+        <v>1200000</v>
       </c>
       <c r="P125">
         <v>0.05</v>
@@ -6794,7 +6773,7 @@
     </row>
     <row r="126">
       <c r="A126">
-        <v>2002</v>
+        <v>2000</v>
       </c>
       <c r="B126" t="inlineStr">
         <is>
@@ -6802,37 +6781,37 @@
         </is>
       </c>
       <c r="C126">
-        <v>17700</v>
+        <v>25100</v>
       </c>
       <c r="D126">
-        <v>17700</v>
+        <v>25100</v>
       </c>
       <c r="E126">
-        <v>21612</v>
+        <v>25354</v>
       </c>
       <c r="F126">
-        <v>3912</v>
+        <v>254</v>
       </c>
       <c r="G126">
         <v>0</v>
       </c>
       <c r="H126">
-        <v>0.3026315789</v>
+        <v>0.92</v>
       </c>
       <c r="I126">
-        <v>0.6118421052999999</v>
+        <v>0.08</v>
       </c>
       <c r="J126">
-        <v>0.0855263158</v>
+        <v>0</v>
       </c>
       <c r="K126">
-        <v>152</v>
+        <v>247</v>
       </c>
       <c r="L126">
         <v>0</v>
       </c>
       <c r="M126">
-        <v>2300000</v>
+        <v>1900000</v>
       </c>
       <c r="P126">
         <v>0.05</v>
@@ -6843,7 +6822,7 @@
     </row>
     <row r="127">
       <c r="A127">
-        <v>2003</v>
+        <v>2001</v>
       </c>
       <c r="B127" t="inlineStr">
         <is>
@@ -6851,40 +6830,37 @@
         </is>
       </c>
       <c r="C127">
-        <v>3300</v>
+        <v>19900</v>
       </c>
       <c r="D127">
-        <v>3300</v>
+        <v>19900</v>
       </c>
       <c r="E127">
-        <v>3537</v>
+        <v>21940</v>
       </c>
       <c r="F127">
-        <v>237</v>
+        <v>2040</v>
       </c>
       <c r="G127">
         <v>0</v>
       </c>
       <c r="H127">
-        <v>0.42202</v>
+        <v>0.28</v>
       </c>
       <c r="I127">
-        <v>0.5779799999999999</v>
+        <v>0.66</v>
       </c>
       <c r="J127">
-        <v>0</v>
+        <v>0.06</v>
       </c>
       <c r="K127">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="L127">
         <v>0</v>
       </c>
       <c r="M127">
-        <v>783000</v>
-      </c>
-      <c r="N127">
-        <v>4457.478632583055</v>
+        <v>2100000</v>
       </c>
       <c r="P127">
         <v>0.05</v>
@@ -6895,7 +6871,7 @@
     </row>
     <row r="128">
       <c r="A128">
-        <v>2007</v>
+        <v>2001</v>
       </c>
       <c r="B128" t="inlineStr">
         <is>
@@ -6903,40 +6879,37 @@
         </is>
       </c>
       <c r="C128">
-        <v>12500</v>
+        <v>19900</v>
       </c>
       <c r="D128">
-        <v>12500</v>
+        <v>19900</v>
       </c>
       <c r="E128">
-        <v>12781</v>
+        <v>21940</v>
       </c>
       <c r="F128">
-        <v>281</v>
+        <v>2040</v>
       </c>
       <c r="G128">
         <v>0</v>
       </c>
       <c r="H128">
-        <v>0.04221824310090583</v>
+        <v>0.2871287128712871</v>
       </c>
       <c r="I128">
-        <v>0.946616810617232</v>
+        <v>0.693069306930693</v>
       </c>
       <c r="J128">
-        <v>0.01116494628186223</v>
+        <v>0.0198019801980198</v>
       </c>
       <c r="K128">
-        <v>94</v>
+        <v>135</v>
       </c>
       <c r="L128">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M128">
-        <v>0</v>
-      </c>
-      <c r="N128">
-        <v>14304.31984967649</v>
+        <v>2100000</v>
       </c>
       <c r="P128">
         <v>0.05</v>
@@ -6947,7 +6920,7 @@
     </row>
     <row r="129">
       <c r="A129">
-        <v>2008</v>
+        <v>2002</v>
       </c>
       <c r="B129" t="inlineStr">
         <is>
@@ -6955,40 +6928,37 @@
         </is>
       </c>
       <c r="C129">
-        <v>13100</v>
+        <v>17700</v>
       </c>
       <c r="D129">
-        <v>12314</v>
+        <v>17700</v>
       </c>
       <c r="E129">
-        <v>13100</v>
+        <v>21612</v>
       </c>
       <c r="F129">
-        <v>0</v>
+        <v>3912</v>
       </c>
       <c r="G129">
-        <v>0.06</v>
+        <v>0</v>
       </c>
       <c r="H129">
-        <v>0.66</v>
+        <v>0.3026315789</v>
       </c>
       <c r="I129">
-        <v>0.28</v>
+        <v>0.6118421052999999</v>
       </c>
       <c r="J129">
-        <v>0</v>
+        <v>0.0855263158</v>
       </c>
       <c r="K129">
-        <v>52</v>
+        <v>152</v>
       </c>
       <c r="L129">
         <v>0</v>
       </c>
       <c r="M129">
-        <v>0</v>
-      </c>
-      <c r="N129">
-        <v>17385.5835483871</v>
+        <v>2300000</v>
       </c>
       <c r="P129">
         <v>0.05</v>
@@ -6999,7 +6969,7 @@
     </row>
     <row r="130">
       <c r="A130">
-        <v>2009</v>
+        <v>2003</v>
       </c>
       <c r="B130" t="inlineStr">
         <is>
@@ -7007,46 +6977,43 @@
         </is>
       </c>
       <c r="C130">
-        <v>30000</v>
+        <v>3300</v>
       </c>
       <c r="D130">
-        <v>29362.37623762376</v>
+        <v>3300</v>
       </c>
       <c r="E130">
-        <v>36055.16288364011</v>
+        <v>3537</v>
       </c>
       <c r="F130">
-        <v>6055.162883640109</v>
+        <v>237</v>
       </c>
       <c r="G130">
-        <v>0.02125412541254126</v>
+        <v>0</v>
       </c>
       <c r="H130">
-        <v>0.5317491749174917</v>
+        <v>0.42202</v>
       </c>
       <c r="I130">
-        <v>0.4400660066006601</v>
+        <v>0.5779799999999999</v>
       </c>
       <c r="J130">
-        <v>0.00693069306930693</v>
+        <v>0</v>
       </c>
       <c r="K130">
-        <v>303</v>
+        <v>109</v>
       </c>
       <c r="L130">
         <v>0</v>
       </c>
       <c r="M130">
-        <v>0</v>
+        <v>783000</v>
       </c>
       <c r="N130">
-        <v>34386.77385321101</v>
-      </c>
-      <c r="O130">
-        <v>0.1679416316376597</v>
+        <v>4457.478632583055</v>
       </c>
       <c r="P130">
-        <v>0.399812753899036</v>
+        <v>0.05</v>
       </c>
       <c r="Q130">
         <v>0.05</v>
@@ -7054,7 +7021,7 @@
     </row>
     <row r="131">
       <c r="A131">
-        <v>2010</v>
+        <v>2004</v>
       </c>
       <c r="B131" t="inlineStr">
         <is>
@@ -7062,46 +7029,28 @@
         </is>
       </c>
       <c r="C131">
-        <v>30000</v>
-      </c>
-      <c r="D131">
-        <v>29696.9696969697</v>
+        <v>2600</v>
       </c>
       <c r="E131">
-        <v>56370.16995668155</v>
+        <v>2610</v>
       </c>
       <c r="F131">
-        <v>26370.16995668155</v>
-      </c>
-      <c r="G131">
-        <v>0.0101010101010101</v>
-      </c>
-      <c r="H131">
-        <v>0.888888888888889</v>
-      </c>
-      <c r="I131">
-        <v>0.101010101010101</v>
-      </c>
-      <c r="J131">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K131">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="L131">
         <v>0</v>
       </c>
       <c r="M131">
-        <v>0</v>
+        <v>755300</v>
       </c>
       <c r="N131">
-        <v>8643.726146788991</v>
-      </c>
-      <c r="O131">
-        <v>0.4678036269350629</v>
+        <v>24512.65154753984</v>
       </c>
       <c r="P131">
-        <v>0.399812753899036</v>
+        <v>0.05</v>
       </c>
       <c r="Q131">
         <v>0.05</v>
@@ -7109,7 +7058,7 @@
     </row>
     <row r="132">
       <c r="A132">
-        <v>2011</v>
+        <v>2005</v>
       </c>
       <c r="B132" t="inlineStr">
         <is>
@@ -7117,40 +7066,25 @@
         </is>
       </c>
       <c r="C132">
-        <v>20423</v>
-      </c>
-      <c r="D132">
-        <v>20057.36241935484</v>
+        <v>1300</v>
       </c>
       <c r="E132">
-        <v>27388</v>
+        <v>1601</v>
       </c>
       <c r="F132">
-        <v>6965</v>
-      </c>
-      <c r="G132">
-        <v>0.01790322580645161</v>
-      </c>
-      <c r="H132">
-        <v>0.1266129032258065</v>
-      </c>
-      <c r="I132">
-        <v>0.8554838709677419</v>
-      </c>
-      <c r="J132">
-        <v>0</v>
+        <v>301</v>
       </c>
       <c r="K132">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="L132">
         <v>0</v>
       </c>
       <c r="M132">
-        <v>0</v>
+        <v>97750</v>
       </c>
       <c r="N132">
-        <v>43839.87877920145</v>
+        <v>25652.25967617237</v>
       </c>
       <c r="P132">
         <v>0.05</v>
@@ -7161,7 +7095,7 @@
     </row>
     <row r="133">
       <c r="A133">
-        <v>2012</v>
+        <v>2006</v>
       </c>
       <c r="B133" t="inlineStr">
         <is>
@@ -7169,40 +7103,25 @@
         </is>
       </c>
       <c r="C133">
-        <v>17133</v>
-      </c>
-      <c r="D133">
-        <v>17133</v>
+        <v>3600</v>
       </c>
       <c r="E133">
-        <v>23075</v>
+        <v>3897</v>
       </c>
       <c r="F133">
-        <v>5942</v>
-      </c>
-      <c r="G133">
-        <v>0</v>
-      </c>
-      <c r="H133">
-        <v>0.62</v>
-      </c>
-      <c r="I133">
-        <v>0.38</v>
-      </c>
-      <c r="J133">
-        <v>0</v>
+        <v>297</v>
       </c>
       <c r="K133">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="L133">
         <v>0</v>
       </c>
       <c r="M133">
-        <v>0</v>
+        <v>1558240</v>
       </c>
       <c r="N133">
-        <v>10937.88288746522</v>
+        <v>74303.13095103549</v>
       </c>
       <c r="P133">
         <v>0.05</v>
@@ -7213,7 +7132,7 @@
     </row>
     <row r="134">
       <c r="A134">
-        <v>2013</v>
+        <v>2007</v>
       </c>
       <c r="B134" t="inlineStr">
         <is>
@@ -7224,37 +7143,37 @@
         <v>12500</v>
       </c>
       <c r="D134">
-        <v>12125</v>
+        <v>12500</v>
       </c>
       <c r="E134">
-        <v>13625</v>
+        <v>12781</v>
       </c>
       <c r="F134">
-        <v>1125</v>
+        <v>281</v>
       </c>
       <c r="G134">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="H134">
-        <v>0.67</v>
+        <v>0.04221824310090583</v>
       </c>
       <c r="I134">
-        <v>0.19</v>
+        <v>0.946616810617232</v>
       </c>
       <c r="J134">
-        <v>0.11</v>
+        <v>0.01116494628186223</v>
       </c>
       <c r="K134">
-        <v>36</v>
+        <v>94</v>
       </c>
       <c r="L134">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M134">
         <v>0</v>
       </c>
       <c r="N134">
-        <v>26414.05275956284</v>
+        <v>14304.31984967649</v>
       </c>
       <c r="P134">
         <v>0.05</v>
@@ -7265,7 +7184,7 @@
     </row>
     <row r="135">
       <c r="A135">
-        <v>2014</v>
+        <v>2008</v>
       </c>
       <c r="B135" t="inlineStr">
         <is>
@@ -7273,31 +7192,31 @@
         </is>
       </c>
       <c r="C135">
-        <v>11837</v>
+        <v>13100</v>
       </c>
       <c r="D135">
-        <v>11837</v>
+        <v>12314</v>
       </c>
       <c r="E135">
-        <v>33493</v>
+        <v>13100</v>
       </c>
       <c r="F135">
-        <v>21656</v>
+        <v>0</v>
       </c>
       <c r="G135">
-        <v>0</v>
+        <v>0.06</v>
       </c>
       <c r="H135">
-        <v>0.2458715596330275</v>
+        <v>0.66</v>
       </c>
       <c r="I135">
-        <v>0.7541284403669724</v>
+        <v>0.28</v>
       </c>
       <c r="J135">
         <v>0</v>
       </c>
       <c r="K135">
-        <v>109</v>
+        <v>52</v>
       </c>
       <c r="L135">
         <v>0</v>
@@ -7306,7 +7225,7 @@
         <v>0</v>
       </c>
       <c r="N135">
-        <v>17167.38557377049</v>
+        <v>17385.5835483871</v>
       </c>
       <c r="P135">
         <v>0.05</v>
@@ -7317,7 +7236,7 @@
     </row>
     <row r="136">
       <c r="A136">
-        <v>2015</v>
+        <v>2009</v>
       </c>
       <c r="B136" t="inlineStr">
         <is>
@@ -7325,31 +7244,31 @@
         </is>
       </c>
       <c r="C136">
-        <v>6400</v>
+        <v>30000</v>
       </c>
       <c r="D136">
-        <v>6400</v>
+        <v>29362.37623762376</v>
       </c>
       <c r="E136">
-        <v>11592</v>
+        <v>36055.16288364011</v>
       </c>
       <c r="F136">
-        <v>5192</v>
+        <v>6055.162883640109</v>
       </c>
       <c r="G136">
-        <v>0</v>
+        <v>0.02125412541254126</v>
       </c>
       <c r="H136">
-        <v>1</v>
+        <v>0.5317491749174917</v>
       </c>
       <c r="I136">
-        <v>0</v>
+        <v>0.4400660066006601</v>
       </c>
       <c r="J136">
-        <v>0</v>
+        <v>0.00693069306930693</v>
       </c>
       <c r="K136">
-        <v>10</v>
+        <v>303</v>
       </c>
       <c r="L136">
         <v>0</v>
@@ -7358,10 +7277,13 @@
         <v>0</v>
       </c>
       <c r="N136">
-        <v>1239.474074074074</v>
+        <v>34386.77385321101</v>
+      </c>
+      <c r="O136">
+        <v>0.1679416316376597</v>
       </c>
       <c r="P136">
-        <v>0.05</v>
+        <v>0.399812753899036</v>
       </c>
       <c r="Q136">
         <v>0.05</v>
@@ -7369,7 +7291,7 @@
     </row>
     <row r="137">
       <c r="A137">
-        <v>2016</v>
+        <v>2010</v>
       </c>
       <c r="B137" t="inlineStr">
         <is>
@@ -7377,31 +7299,31 @@
         </is>
       </c>
       <c r="C137">
-        <v>10700</v>
+        <v>30000</v>
       </c>
       <c r="D137">
-        <v>10700</v>
+        <v>29696.9696969697</v>
       </c>
       <c r="E137">
-        <v>33811</v>
+        <v>56370.16995668155</v>
       </c>
       <c r="F137">
-        <v>23111</v>
+        <v>26370.16995668155</v>
       </c>
       <c r="G137">
-        <v>0</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="H137">
-        <v>0.06965637740244612</v>
+        <v>0.888888888888889</v>
       </c>
       <c r="I137">
-        <v>0.9303436225975539</v>
+        <v>0.101010101010101</v>
       </c>
       <c r="J137">
         <v>0</v>
       </c>
       <c r="K137">
-        <v>119</v>
+        <v>67</v>
       </c>
       <c r="L137">
         <v>0</v>
@@ -7410,10 +7332,13 @@
         <v>0</v>
       </c>
       <c r="N137">
-        <v>6640.959620596205</v>
+        <v>8643.726146788991</v>
+      </c>
+      <c r="O137">
+        <v>0.4678036269350629</v>
       </c>
       <c r="P137">
-        <v>0.05</v>
+        <v>0.399812753899036</v>
       </c>
       <c r="Q137">
         <v>0.05</v>
@@ -7421,7 +7346,7 @@
     </row>
     <row r="138">
       <c r="A138">
-        <v>2017</v>
+        <v>2011</v>
       </c>
       <c r="B138" t="inlineStr">
         <is>
@@ -7429,31 +7354,31 @@
         </is>
       </c>
       <c r="C138">
-        <v>22704</v>
+        <v>20423</v>
       </c>
       <c r="D138">
-        <v>22704</v>
+        <v>20057.36241935484</v>
       </c>
       <c r="E138">
-        <v>25921</v>
+        <v>27388</v>
       </c>
       <c r="F138">
-        <v>3217</v>
+        <v>6965</v>
       </c>
       <c r="G138">
-        <v>0</v>
+        <v>0.01790322580645161</v>
       </c>
       <c r="H138">
-        <v>0.6383333333333332</v>
+        <v>0.1266129032258065</v>
       </c>
       <c r="I138">
-        <v>0.3311111111111111</v>
+        <v>0.8554838709677419</v>
       </c>
       <c r="J138">
-        <v>0.03055555555555556</v>
+        <v>0</v>
       </c>
       <c r="K138">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="L138">
         <v>0</v>
@@ -7462,7 +7387,7 @@
         <v>0</v>
       </c>
       <c r="N138">
-        <v>32845.64926303271</v>
+        <v>43839.87877920145</v>
       </c>
       <c r="P138">
         <v>0.05</v>
@@ -7473,7 +7398,7 @@
     </row>
     <row r="139">
       <c r="A139">
-        <v>2018</v>
+        <v>2012</v>
       </c>
       <c r="B139" t="inlineStr">
         <is>
@@ -7481,37 +7406,40 @@
         </is>
       </c>
       <c r="C139">
-        <v>12203</v>
+        <v>17133</v>
       </c>
       <c r="D139">
-        <v>12203</v>
+        <v>17133</v>
       </c>
       <c r="E139">
-        <v>12829</v>
+        <v>23075</v>
       </c>
       <c r="F139">
-        <v>626</v>
+        <v>5942</v>
       </c>
       <c r="G139">
         <v>0</v>
       </c>
       <c r="H139">
-        <v>0.2308196721311475</v>
+        <v>0.62</v>
       </c>
       <c r="I139">
-        <v>0.7691803278688525</v>
+        <v>0.38</v>
       </c>
       <c r="J139">
         <v>0</v>
       </c>
       <c r="K139">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="L139">
         <v>0</v>
       </c>
       <c r="M139">
         <v>0</v>
+      </c>
+      <c r="N139">
+        <v>10937.88288746522</v>
       </c>
       <c r="P139">
         <v>0.05</v>
@@ -7522,7 +7450,7 @@
     </row>
     <row r="140">
       <c r="A140">
-        <v>2019</v>
+        <v>2013</v>
       </c>
       <c r="B140" t="inlineStr">
         <is>
@@ -7530,37 +7458,40 @@
         </is>
       </c>
       <c r="C140">
-        <v>13549</v>
+        <v>12500</v>
       </c>
       <c r="D140">
-        <v>13549</v>
+        <v>12125</v>
       </c>
       <c r="E140">
-        <v>13703</v>
+        <v>13625</v>
       </c>
       <c r="F140">
-        <v>154</v>
+        <v>1125</v>
       </c>
       <c r="G140">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="H140">
-        <v>0</v>
+        <v>0.67</v>
       </c>
       <c r="I140">
-        <v>1</v>
+        <v>0.19</v>
       </c>
       <c r="J140">
-        <v>0</v>
+        <v>0.11</v>
       </c>
       <c r="K140">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="L140">
         <v>0</v>
       </c>
       <c r="M140">
         <v>0</v>
+      </c>
+      <c r="N140">
+        <v>26414.05275956284</v>
       </c>
       <c r="P140">
         <v>0.05</v>
@@ -7571,7 +7502,7 @@
     </row>
     <row r="141">
       <c r="A141">
-        <v>2020</v>
+        <v>2014</v>
       </c>
       <c r="B141" t="inlineStr">
         <is>
@@ -7579,37 +7510,40 @@
         </is>
       </c>
       <c r="C141">
-        <v>4589</v>
+        <v>11837</v>
       </c>
       <c r="D141">
-        <v>4588.999999999999</v>
+        <v>11837</v>
       </c>
       <c r="E141">
-        <v>5032</v>
+        <v>33493</v>
       </c>
       <c r="F141">
-        <v>443</v>
+        <v>21656</v>
       </c>
       <c r="G141">
         <v>0</v>
       </c>
       <c r="H141">
-        <v>0.7</v>
+        <v>0.2458715596330275</v>
       </c>
       <c r="I141">
-        <v>0.2</v>
+        <v>0.7541284403669724</v>
       </c>
       <c r="J141">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="K141">
-        <v>10</v>
+        <v>109</v>
       </c>
       <c r="L141">
         <v>0</v>
       </c>
       <c r="M141">
         <v>0</v>
+      </c>
+      <c r="N141">
+        <v>17167.38557377049</v>
       </c>
       <c r="P141">
         <v>0.05</v>
@@ -7620,7 +7554,7 @@
     </row>
     <row r="142">
       <c r="A142">
-        <v>2021</v>
+        <v>2015</v>
       </c>
       <c r="B142" t="inlineStr">
         <is>
@@ -7628,37 +7562,40 @@
         </is>
       </c>
       <c r="C142">
-        <v>14520</v>
+        <v>6400</v>
       </c>
       <c r="D142">
-        <v>14520</v>
+        <v>6400</v>
       </c>
       <c r="E142">
-        <v>18879</v>
+        <v>11592</v>
       </c>
       <c r="F142">
-        <v>4359</v>
+        <v>5192</v>
       </c>
       <c r="G142">
         <v>0</v>
       </c>
       <c r="H142">
-        <v>0.8395061728395061</v>
+        <v>1</v>
       </c>
       <c r="I142">
-        <v>0.1481481481481481</v>
+        <v>0</v>
       </c>
       <c r="J142">
-        <v>0.01234567901234568</v>
+        <v>0</v>
       </c>
       <c r="K142">
-        <v>162</v>
+        <v>10</v>
       </c>
       <c r="L142">
         <v>0</v>
       </c>
       <c r="M142">
         <v>0</v>
+      </c>
+      <c r="N142">
+        <v>1239.474074074074</v>
       </c>
       <c r="P142">
         <v>0.05</v>
@@ -7669,7 +7606,7 @@
     </row>
     <row r="143">
       <c r="A143">
-        <v>2022</v>
+        <v>2016</v>
       </c>
       <c r="B143" t="inlineStr">
         <is>
@@ -7677,37 +7614,40 @@
         </is>
       </c>
       <c r="C143">
-        <v>18646</v>
+        <v>10700</v>
       </c>
       <c r="D143">
-        <v>18646</v>
+        <v>10700</v>
       </c>
       <c r="E143">
-        <v>26377</v>
+        <v>33811</v>
       </c>
       <c r="F143">
-        <v>7731</v>
+        <v>23111</v>
       </c>
       <c r="G143">
         <v>0</v>
       </c>
       <c r="H143">
-        <v>0.3536585365853658</v>
+        <v>0.06965637740244612</v>
       </c>
       <c r="I143">
-        <v>0.6341463414634146</v>
+        <v>0.9303436225975539</v>
       </c>
       <c r="J143">
-        <v>0.01219512195121951</v>
+        <v>0</v>
       </c>
       <c r="K143">
-        <v>82</v>
+        <v>119</v>
       </c>
       <c r="L143">
         <v>0</v>
       </c>
       <c r="M143">
         <v>0</v>
+      </c>
+      <c r="N143">
+        <v>6640.959620596205</v>
       </c>
       <c r="P143">
         <v>0.05</v>
@@ -7718,50 +7658,1923 @@
     </row>
     <row r="144">
       <c r="A144">
+        <v>2017</v>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C144">
+        <v>22704</v>
+      </c>
+      <c r="D144">
+        <v>22704</v>
+      </c>
+      <c r="E144">
+        <v>25921</v>
+      </c>
+      <c r="F144">
+        <v>3217</v>
+      </c>
+      <c r="G144">
+        <v>0</v>
+      </c>
+      <c r="H144">
+        <v>0.6383333333333332</v>
+      </c>
+      <c r="I144">
+        <v>0.3311111111111111</v>
+      </c>
+      <c r="J144">
+        <v>0.03055555555555556</v>
+      </c>
+      <c r="K144">
+        <v>72</v>
+      </c>
+      <c r="L144">
+        <v>0</v>
+      </c>
+      <c r="M144">
+        <v>0</v>
+      </c>
+      <c r="N144">
+        <v>32845.64926303271</v>
+      </c>
+      <c r="P144">
+        <v>0.05</v>
+      </c>
+      <c r="Q144">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145">
+        <v>2018</v>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C145">
+        <v>12203</v>
+      </c>
+      <c r="D145">
+        <v>12203</v>
+      </c>
+      <c r="E145">
+        <v>12829</v>
+      </c>
+      <c r="F145">
+        <v>626</v>
+      </c>
+      <c r="G145">
+        <v>0</v>
+      </c>
+      <c r="H145">
+        <v>0.2308196721311475</v>
+      </c>
+      <c r="I145">
+        <v>0.7691803278688525</v>
+      </c>
+      <c r="J145">
+        <v>0</v>
+      </c>
+      <c r="K145">
+        <v>61</v>
+      </c>
+      <c r="L145">
+        <v>0</v>
+      </c>
+      <c r="M145">
+        <v>0</v>
+      </c>
+      <c r="P145">
+        <v>0.05</v>
+      </c>
+      <c r="Q145">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146">
+        <v>2019</v>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C146">
+        <v>13549</v>
+      </c>
+      <c r="D146">
+        <v>13549</v>
+      </c>
+      <c r="E146">
+        <v>13703</v>
+      </c>
+      <c r="F146">
+        <v>154</v>
+      </c>
+      <c r="G146">
+        <v>0</v>
+      </c>
+      <c r="H146">
+        <v>0</v>
+      </c>
+      <c r="I146">
+        <v>1</v>
+      </c>
+      <c r="J146">
+        <v>0</v>
+      </c>
+      <c r="K146">
+        <v>21</v>
+      </c>
+      <c r="L146">
+        <v>0</v>
+      </c>
+      <c r="M146">
+        <v>0</v>
+      </c>
+      <c r="P146">
+        <v>0.05</v>
+      </c>
+      <c r="Q146">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147">
+        <v>2020</v>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C147">
+        <v>4589</v>
+      </c>
+      <c r="D147">
+        <v>4588.999999999999</v>
+      </c>
+      <c r="E147">
+        <v>5032</v>
+      </c>
+      <c r="F147">
+        <v>443</v>
+      </c>
+      <c r="G147">
+        <v>0</v>
+      </c>
+      <c r="H147">
+        <v>0.7</v>
+      </c>
+      <c r="I147">
+        <v>0.2</v>
+      </c>
+      <c r="J147">
+        <v>0.1</v>
+      </c>
+      <c r="K147">
+        <v>10</v>
+      </c>
+      <c r="L147">
+        <v>0</v>
+      </c>
+      <c r="M147">
+        <v>0</v>
+      </c>
+      <c r="P147">
+        <v>0.05</v>
+      </c>
+      <c r="Q147">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148">
+        <v>2021</v>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C148">
+        <v>14520</v>
+      </c>
+      <c r="D148">
+        <v>14520</v>
+      </c>
+      <c r="E148">
+        <v>18879</v>
+      </c>
+      <c r="F148">
+        <v>4359</v>
+      </c>
+      <c r="G148">
+        <v>0</v>
+      </c>
+      <c r="H148">
+        <v>0.8395061728395061</v>
+      </c>
+      <c r="I148">
+        <v>0.1481481481481481</v>
+      </c>
+      <c r="J148">
+        <v>0.01234567901234568</v>
+      </c>
+      <c r="K148">
+        <v>162</v>
+      </c>
+      <c r="L148">
+        <v>0</v>
+      </c>
+      <c r="M148">
+        <v>0</v>
+      </c>
+      <c r="P148">
+        <v>0.05</v>
+      </c>
+      <c r="Q148">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149">
+        <v>2022</v>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C149">
+        <v>18646</v>
+      </c>
+      <c r="D149">
+        <v>18646</v>
+      </c>
+      <c r="E149">
+        <v>26377</v>
+      </c>
+      <c r="F149">
+        <v>7731</v>
+      </c>
+      <c r="G149">
+        <v>0</v>
+      </c>
+      <c r="H149">
+        <v>0.3536585365853658</v>
+      </c>
+      <c r="I149">
+        <v>0.6341463414634146</v>
+      </c>
+      <c r="J149">
+        <v>0.01219512195121951</v>
+      </c>
+      <c r="K149">
+        <v>82</v>
+      </c>
+      <c r="L149">
+        <v>0</v>
+      </c>
+      <c r="M149">
+        <v>0</v>
+      </c>
+      <c r="P149">
+        <v>0.05</v>
+      </c>
+      <c r="Q149">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150">
         <v>2023</v>
       </c>
-      <c r="B144" t="inlineStr">
-        <is>
-          <t>HUC</t>
-        </is>
-      </c>
-      <c r="C144">
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C150">
         <v>13113</v>
       </c>
-      <c r="D144">
+      <c r="D150">
         <v>13113</v>
       </c>
-      <c r="E144">
+      <c r="E150">
         <v>21309</v>
       </c>
-      <c r="F144">
+      <c r="F150">
         <v>8196</v>
       </c>
-      <c r="G144">
-        <v>0</v>
-      </c>
-      <c r="H144">
+      <c r="G150">
+        <v>0</v>
+      </c>
+      <c r="H150">
         <v>0.1962025316455696</v>
       </c>
-      <c r="I144">
+      <c r="I150">
         <v>0.7911392405063291</v>
       </c>
-      <c r="J144">
+      <c r="J150">
         <v>0.01265822784810127</v>
       </c>
-      <c r="K144">
+      <c r="K150">
         <v>158</v>
       </c>
-      <c r="L144">
-        <v>0</v>
-      </c>
-      <c r="M144">
-        <v>0</v>
-      </c>
-      <c r="P144">
-        <v>0.05</v>
-      </c>
-      <c r="Q144">
+      <c r="L150">
+        <v>0</v>
+      </c>
+      <c r="M150">
+        <v>0</v>
+      </c>
+      <c r="P150">
+        <v>0.05</v>
+      </c>
+      <c r="Q150">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151">
+        <v>1915</v>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="K151">
+        <v>0</v>
+      </c>
+      <c r="M151">
+        <v>7400000</v>
+      </c>
+      <c r="P151">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="Q151">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152">
+        <v>1916</v>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="K152">
+        <v>0</v>
+      </c>
+      <c r="M152">
+        <v>4078000</v>
+      </c>
+      <c r="P152">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="Q152">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153">
+        <v>1917</v>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="K153">
+        <v>0</v>
+      </c>
+      <c r="M153">
+        <v>6995075</v>
+      </c>
+      <c r="P153">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="Q153">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154">
+        <v>1918</v>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C154">
+        <v>7000</v>
+      </c>
+      <c r="K154">
+        <v>0</v>
+      </c>
+      <c r="L154">
+        <v>0</v>
+      </c>
+      <c r="M154">
+        <v>1793477</v>
+      </c>
+      <c r="P154">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="Q154">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155">
+        <v>1919</v>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C155">
+        <v>8000</v>
+      </c>
+      <c r="K155">
+        <v>0</v>
+      </c>
+      <c r="L155">
+        <v>0</v>
+      </c>
+      <c r="M155">
+        <v>2234000</v>
+      </c>
+      <c r="P155">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="Q155">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156">
+        <v>1920</v>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C156">
+        <v>38000</v>
+      </c>
+      <c r="K156">
+        <v>0</v>
+      </c>
+      <c r="L156">
+        <v>0</v>
+      </c>
+      <c r="M156">
+        <v>7972841</v>
+      </c>
+      <c r="P156">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="Q156">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157">
+        <v>1921</v>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C157">
+        <v>1000</v>
+      </c>
+      <c r="K157">
+        <v>0</v>
+      </c>
+      <c r="L157">
+        <v>0</v>
+      </c>
+      <c r="M157">
+        <v>9103410</v>
+      </c>
+      <c r="P157">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="Q157">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158">
+        <v>1922</v>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C158">
+        <v>70000</v>
+      </c>
+      <c r="K158">
+        <v>0</v>
+      </c>
+      <c r="L158">
+        <v>0</v>
+      </c>
+      <c r="M158">
+        <v>4800925</v>
+      </c>
+      <c r="P158">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="Q158">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159">
+        <v>1923</v>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C159">
+        <v>90000</v>
+      </c>
+      <c r="K159">
+        <v>0</v>
+      </c>
+      <c r="L159">
+        <v>0</v>
+      </c>
+      <c r="M159">
+        <v>3274607</v>
+      </c>
+      <c r="P159">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="Q159">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160">
+        <v>1924</v>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C160">
+        <v>120000</v>
+      </c>
+      <c r="K160">
+        <v>0</v>
+      </c>
+      <c r="L160">
+        <v>0</v>
+      </c>
+      <c r="M160">
+        <v>3486821</v>
+      </c>
+      <c r="P160">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="Q160">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161">
+        <v>1925</v>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C161">
+        <v>80000</v>
+      </c>
+      <c r="K161">
+        <v>0</v>
+      </c>
+      <c r="L161">
+        <v>0</v>
+      </c>
+      <c r="M161">
+        <v>3251391</v>
+      </c>
+      <c r="P161">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="Q161">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162">
+        <v>1926</v>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C162">
+        <v>65000</v>
+      </c>
+      <c r="E162">
+        <v>100412</v>
+      </c>
+      <c r="F162">
+        <v>35412</v>
+      </c>
+      <c r="K162">
+        <v>0</v>
+      </c>
+      <c r="L162">
+        <v>0</v>
+      </c>
+      <c r="M162">
+        <v>3220359</v>
+      </c>
+      <c r="P162">
+        <v>0.05</v>
+      </c>
+      <c r="Q162">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163">
+        <v>1927</v>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C163">
+        <v>70000</v>
+      </c>
+      <c r="E163">
+        <v>95669</v>
+      </c>
+      <c r="F163">
+        <v>25669</v>
+      </c>
+      <c r="K163">
+        <v>0</v>
+      </c>
+      <c r="L163">
+        <v>0</v>
+      </c>
+      <c r="M163">
+        <v>3245014</v>
+      </c>
+      <c r="P163">
+        <v>0.05</v>
+      </c>
+      <c r="Q163">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164">
+        <v>1928</v>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C164">
+        <v>70000</v>
+      </c>
+      <c r="E164">
+        <v>85000</v>
+      </c>
+      <c r="F164">
+        <v>15000</v>
+      </c>
+      <c r="K164">
+        <v>0</v>
+      </c>
+      <c r="L164">
+        <v>0</v>
+      </c>
+      <c r="M164">
+        <v>3007880</v>
+      </c>
+      <c r="P164">
+        <v>0.05</v>
+      </c>
+      <c r="Q164">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165">
+        <v>1929</v>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C165">
+        <v>135000</v>
+      </c>
+      <c r="K165">
+        <v>0</v>
+      </c>
+      <c r="L165">
+        <v>0</v>
+      </c>
+      <c r="M165">
+        <v>3278881</v>
+      </c>
+      <c r="P165">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="Q165">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166">
+        <v>1930</v>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C166">
+        <v>40000</v>
+      </c>
+      <c r="E166">
+        <v>50600</v>
+      </c>
+      <c r="F166">
+        <v>10600</v>
+      </c>
+      <c r="K166">
+        <v>0</v>
+      </c>
+      <c r="L166">
+        <v>0</v>
+      </c>
+      <c r="M166">
+        <v>3135246</v>
+      </c>
+      <c r="P166">
+        <v>0.05</v>
+      </c>
+      <c r="Q166">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167">
+        <v>1931</v>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C167">
+        <v>50000</v>
+      </c>
+      <c r="E167">
+        <v>70260</v>
+      </c>
+      <c r="F167">
+        <v>20260</v>
+      </c>
+      <c r="K167">
+        <v>0</v>
+      </c>
+      <c r="L167">
+        <v>0</v>
+      </c>
+      <c r="M167">
+        <v>4158974</v>
+      </c>
+      <c r="P167">
+        <v>0.05</v>
+      </c>
+      <c r="Q167">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168">
+        <v>1932</v>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C168">
+        <v>35000</v>
+      </c>
+      <c r="E168">
+        <v>63000</v>
+      </c>
+      <c r="F168">
+        <v>28000</v>
+      </c>
+      <c r="K168">
+        <v>0</v>
+      </c>
+      <c r="L168">
+        <v>0</v>
+      </c>
+      <c r="M168">
+        <v>2859264</v>
+      </c>
+      <c r="P168">
+        <v>0.05</v>
+      </c>
+      <c r="Q168">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169">
+        <v>1933</v>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C169">
+        <v>7500</v>
+      </c>
+      <c r="E169">
+        <v>28000</v>
+      </c>
+      <c r="F169">
+        <v>20500</v>
+      </c>
+      <c r="K169">
+        <v>0</v>
+      </c>
+      <c r="L169">
+        <v>0</v>
+      </c>
+      <c r="M169">
+        <v>1995414</v>
+      </c>
+      <c r="P169">
+        <v>0.05</v>
+      </c>
+      <c r="Q169">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170">
+        <v>1934</v>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C170">
+        <v>15000</v>
+      </c>
+      <c r="E170">
+        <v>21500</v>
+      </c>
+      <c r="F170">
+        <v>6500</v>
+      </c>
+      <c r="K170">
+        <v>0</v>
+      </c>
+      <c r="L170">
+        <v>0</v>
+      </c>
+      <c r="M170">
+        <v>2910449</v>
+      </c>
+      <c r="P170">
+        <v>0.05</v>
+      </c>
+      <c r="Q170">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171">
+        <v>1935</v>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C171">
+        <v>45000</v>
+      </c>
+      <c r="K171">
+        <v>0</v>
+      </c>
+      <c r="L171">
+        <v>0</v>
+      </c>
+      <c r="M171">
+        <v>4897121</v>
+      </c>
+      <c r="P171">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="Q171">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172">
+        <v>1936</v>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C172">
+        <v>2000</v>
+      </c>
+      <c r="K172">
+        <v>0</v>
+      </c>
+      <c r="L172">
+        <v>0</v>
+      </c>
+      <c r="M172">
+        <v>5090972</v>
+      </c>
+      <c r="P172">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="Q172">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173">
+        <v>1937</v>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C173">
+        <v>38000</v>
+      </c>
+      <c r="K173">
+        <v>0</v>
+      </c>
+      <c r="L173">
+        <v>0</v>
+      </c>
+      <c r="M173">
+        <v>0</v>
+      </c>
+      <c r="P173">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="Q173">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174">
+        <v>1938</v>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C174">
+        <v>10000</v>
+      </c>
+      <c r="K174">
+        <v>0</v>
+      </c>
+      <c r="L174">
+        <v>0</v>
+      </c>
+      <c r="M174">
+        <v>0</v>
+      </c>
+      <c r="P174">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="Q174">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175">
+        <v>1939</v>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C175">
+        <v>14000</v>
+      </c>
+      <c r="K175">
+        <v>0</v>
+      </c>
+      <c r="L175">
+        <v>0</v>
+      </c>
+      <c r="M175">
+        <v>0</v>
+      </c>
+      <c r="P175">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="Q175">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176">
+        <v>1940</v>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C176">
+        <v>60000</v>
+      </c>
+      <c r="K176">
+        <v>0</v>
+      </c>
+      <c r="L176">
+        <v>0</v>
+      </c>
+      <c r="M176">
+        <v>0</v>
+      </c>
+      <c r="P176">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="Q176">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177">
+        <v>1941</v>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C177">
+        <v>2000</v>
+      </c>
+      <c r="K177">
+        <v>0</v>
+      </c>
+      <c r="L177">
+        <v>0</v>
+      </c>
+      <c r="M177">
+        <v>0</v>
+      </c>
+      <c r="P177">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="Q177">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178">
+        <v>1942</v>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C178">
+        <v>7000</v>
+      </c>
+      <c r="K178">
+        <v>0</v>
+      </c>
+      <c r="L178">
+        <v>0</v>
+      </c>
+      <c r="M178">
+        <v>0</v>
+      </c>
+      <c r="P178">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="Q178">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179">
+        <v>1943</v>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C179">
+        <v>5000</v>
+      </c>
+      <c r="K179">
+        <v>0</v>
+      </c>
+      <c r="L179">
+        <v>0</v>
+      </c>
+      <c r="M179">
+        <v>0</v>
+      </c>
+      <c r="P179">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="Q179">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180">
+        <v>1944</v>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C180">
+        <v>5000</v>
+      </c>
+      <c r="K180">
+        <v>0</v>
+      </c>
+      <c r="L180">
+        <v>0</v>
+      </c>
+      <c r="M180">
+        <v>0</v>
+      </c>
+      <c r="P180">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="Q180">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181">
+        <v>1945</v>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C181">
+        <v>14000</v>
+      </c>
+      <c r="K181">
+        <v>0</v>
+      </c>
+      <c r="L181">
+        <v>0</v>
+      </c>
+      <c r="M181">
+        <v>0</v>
+      </c>
+      <c r="P181">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="Q181">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182">
+        <v>1946</v>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C182">
+        <v>14000</v>
+      </c>
+      <c r="K182">
+        <v>0</v>
+      </c>
+      <c r="L182">
+        <v>0</v>
+      </c>
+      <c r="M182">
+        <v>0</v>
+      </c>
+      <c r="P182">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="Q182">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183">
+        <v>1947</v>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C183">
+        <v>7000</v>
+      </c>
+      <c r="K183">
+        <v>0</v>
+      </c>
+      <c r="L183">
+        <v>0</v>
+      </c>
+      <c r="M183">
+        <v>0</v>
+      </c>
+      <c r="P183">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="Q183">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184">
+        <v>1948</v>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C184">
+        <v>7000</v>
+      </c>
+      <c r="K184">
+        <v>0</v>
+      </c>
+      <c r="L184">
+        <v>0</v>
+      </c>
+      <c r="M184">
+        <v>0</v>
+      </c>
+      <c r="P184">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="Q184">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185">
+        <v>1949</v>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C185">
+        <v>30000</v>
+      </c>
+      <c r="K185">
+        <v>0</v>
+      </c>
+      <c r="L185">
+        <v>0</v>
+      </c>
+      <c r="M185">
+        <v>0</v>
+      </c>
+      <c r="P185">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="Q185">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186">
+        <v>1950</v>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C186">
+        <v>14000</v>
+      </c>
+      <c r="K186">
+        <v>0</v>
+      </c>
+      <c r="L186">
+        <v>0</v>
+      </c>
+      <c r="M186">
+        <v>0</v>
+      </c>
+      <c r="P186">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="Q186">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187">
+        <v>1951</v>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C187">
+        <v>14000</v>
+      </c>
+      <c r="K187">
+        <v>0</v>
+      </c>
+      <c r="L187">
+        <v>0</v>
+      </c>
+      <c r="M187">
+        <v>0</v>
+      </c>
+      <c r="P187">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="Q187">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188">
+        <v>1952</v>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C188">
+        <v>14000</v>
+      </c>
+      <c r="K188">
+        <v>0</v>
+      </c>
+      <c r="L188">
+        <v>0</v>
+      </c>
+      <c r="M188">
+        <v>0</v>
+      </c>
+      <c r="P188">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="Q188">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189">
+        <v>1953</v>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C189">
+        <v>14000</v>
+      </c>
+      <c r="K189">
+        <v>0</v>
+      </c>
+      <c r="L189">
+        <v>0</v>
+      </c>
+      <c r="M189">
+        <v>0</v>
+      </c>
+      <c r="P189">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="Q189">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190">
+        <v>1954</v>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C190">
+        <v>30000</v>
+      </c>
+      <c r="K190">
+        <v>0</v>
+      </c>
+      <c r="L190">
+        <v>0</v>
+      </c>
+      <c r="M190">
+        <v>0</v>
+      </c>
+      <c r="P190">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="Q190">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191">
+        <v>1955</v>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C191">
+        <v>14000</v>
+      </c>
+      <c r="K191">
+        <v>0</v>
+      </c>
+      <c r="L191">
+        <v>0</v>
+      </c>
+      <c r="M191">
+        <v>0</v>
+      </c>
+      <c r="P191">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="Q191">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192">
+        <v>1956</v>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C192">
+        <v>7000</v>
+      </c>
+      <c r="K192">
+        <v>0</v>
+      </c>
+      <c r="L192">
+        <v>0</v>
+      </c>
+      <c r="M192">
+        <v>0</v>
+      </c>
+      <c r="P192">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="Q192">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193">
+        <v>1957</v>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C193">
+        <v>7000</v>
+      </c>
+      <c r="K193">
+        <v>0</v>
+      </c>
+      <c r="L193">
+        <v>0</v>
+      </c>
+      <c r="M193">
+        <v>0</v>
+      </c>
+      <c r="P193">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="Q193">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194">
+        <v>1958</v>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C194">
+        <v>14000</v>
+      </c>
+      <c r="K194">
+        <v>0</v>
+      </c>
+      <c r="L194">
+        <v>0</v>
+      </c>
+      <c r="M194">
+        <v>0</v>
+      </c>
+      <c r="P194">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="Q194">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195">
+        <v>1959</v>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C195">
+        <v>14000</v>
+      </c>
+      <c r="K195">
+        <v>0</v>
+      </c>
+      <c r="L195">
+        <v>0</v>
+      </c>
+      <c r="M195">
+        <v>0</v>
+      </c>
+      <c r="P195">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="Q195">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196">
+        <v>1960</v>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C196">
+        <v>10000</v>
+      </c>
+      <c r="K196">
+        <v>0</v>
+      </c>
+      <c r="L196">
+        <v>0</v>
+      </c>
+      <c r="M196">
+        <v>0</v>
+      </c>
+      <c r="P196">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="Q196">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197">
+        <v>1961</v>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C197">
+        <v>14000</v>
+      </c>
+      <c r="K197">
+        <v>0</v>
+      </c>
+      <c r="L197">
+        <v>0</v>
+      </c>
+      <c r="M197">
+        <v>0</v>
+      </c>
+      <c r="P197">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="Q197">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198">
+        <v>1962</v>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C198">
+        <v>30000</v>
+      </c>
+      <c r="K198">
+        <v>0</v>
+      </c>
+      <c r="L198">
+        <v>0</v>
+      </c>
+      <c r="M198">
+        <v>0</v>
+      </c>
+      <c r="P198">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="Q198">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199">
+        <v>1963</v>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C199">
+        <v>18000</v>
+      </c>
+      <c r="K199">
+        <v>0</v>
+      </c>
+      <c r="L199">
+        <v>0</v>
+      </c>
+      <c r="M199">
+        <v>0</v>
+      </c>
+      <c r="P199">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="Q199">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200">
+        <v>1964</v>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C200">
+        <v>30000</v>
+      </c>
+      <c r="K200">
+        <v>0</v>
+      </c>
+      <c r="L200">
+        <v>0</v>
+      </c>
+      <c r="M200">
+        <v>0</v>
+      </c>
+      <c r="P200">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="Q200">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201">
+        <v>1965</v>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C201">
+        <v>18000</v>
+      </c>
+      <c r="K201">
+        <v>0</v>
+      </c>
+      <c r="L201">
+        <v>0</v>
+      </c>
+      <c r="M201">
+        <v>0</v>
+      </c>
+      <c r="P201">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="Q201">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202">
+        <v>1966</v>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C202">
+        <v>80000</v>
+      </c>
+      <c r="K202">
+        <v>0</v>
+      </c>
+      <c r="L202">
+        <v>0</v>
+      </c>
+      <c r="M202">
+        <v>0</v>
+      </c>
+      <c r="P202">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="Q202">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203">
+        <v>1967</v>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C203">
+        <v>80000</v>
+      </c>
+      <c r="K203">
+        <v>0</v>
+      </c>
+      <c r="L203">
+        <v>0</v>
+      </c>
+      <c r="M203">
+        <v>0</v>
+      </c>
+      <c r="P203">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="Q203">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204">
+        <v>1968</v>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C204">
+        <v>30000</v>
+      </c>
+      <c r="K204">
+        <v>0</v>
+      </c>
+      <c r="L204">
+        <v>0</v>
+      </c>
+      <c r="M204">
+        <v>0</v>
+      </c>
+      <c r="N204">
+        <v>23898.67</v>
+      </c>
+      <c r="P204">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="Q204">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205">
+        <v>1969</v>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>HUC</t>
+        </is>
+      </c>
+      <c r="C205">
+        <v>18000</v>
+      </c>
+      <c r="K205">
+        <v>0</v>
+      </c>
+      <c r="L205">
+        <v>0</v>
+      </c>
+      <c r="M205">
+        <v>0</v>
+      </c>
+      <c r="N205">
+        <v>42623.78396039605</v>
+      </c>
+      <c r="P205">
+        <v>0.399812753899036</v>
+      </c>
+      <c r="Q205">
         <v>0.05</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add updated CV estimates
</commit_message>
<xml_diff>
--- a/3. outputs/Stock-recruit data/Barkley_Sockeye_stock-recruit_infilled.xlsx
+++ b/3. outputs/Stock-recruit data/Barkley_Sockeye_stock-recruit_infilled.xlsx
@@ -717,10 +717,10 @@
         <v>633742.5637903768</v>
       </c>
       <c r="P2">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
       <c r="Q2">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="3">
@@ -766,10 +766,10 @@
         <v>526832.3053483891</v>
       </c>
       <c r="P3">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q3">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="4">
@@ -815,10 +815,10 @@
         <v>913809.5845034227</v>
       </c>
       <c r="P4">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q4">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="5">
@@ -864,10 +864,10 @@
         <v>480598.2568144404</v>
       </c>
       <c r="P5">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q5">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="6">
@@ -913,10 +913,10 @@
         <v>224122.9386567897</v>
       </c>
       <c r="P6">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q6">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="7">
@@ -962,10 +962,10 @@
         <v>137076.4333190075</v>
       </c>
       <c r="P7">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q7">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="8">
@@ -1011,10 +1011,10 @@
         <v>503092.30271186</v>
       </c>
       <c r="P8">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q8">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="9">
@@ -1060,10 +1060,10 @@
         <v>206726.5366225715</v>
       </c>
       <c r="P9">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q9">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="10">
@@ -1109,10 +1109,10 @@
         <v>292061.9392067303</v>
       </c>
       <c r="P10">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="Q10">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="11">
@@ -1158,10 +1158,10 @@
         <v>274311.7730009329</v>
       </c>
       <c r="P11">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q11">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="12">
@@ -1207,10 +1207,10 @@
         <v>1258256.636990258</v>
       </c>
       <c r="P12">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q12">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="13">
@@ -1256,10 +1256,10 @@
         <v>599789.3466079192</v>
       </c>
       <c r="P13">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q13">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="14">
@@ -1305,10 +1305,10 @@
         <v>400875.0350328542</v>
       </c>
       <c r="P14">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q14">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="15">
@@ -1354,10 +1354,10 @@
         <v>138601.997986058</v>
       </c>
       <c r="P15">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q15">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="16">
@@ -1403,10 +1403,10 @@
         <v>74102.68990164486</v>
       </c>
       <c r="P16">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q16">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="17">
@@ -1452,10 +1452,10 @@
         <v>290004.5944304451</v>
       </c>
       <c r="P17">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q17">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="18">
@@ -1501,10 +1501,10 @@
         <v>421979.6878094974</v>
       </c>
       <c r="P18">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q18">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="19">
@@ -1550,10 +1550,10 @@
         <v>240203.9760283087</v>
       </c>
       <c r="P19">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q19">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="20">
@@ -1599,10 +1599,10 @@
         <v>241682.5691475399</v>
       </c>
       <c r="P20">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q20">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="21">
@@ -1648,10 +1648,10 @@
         <v>261943.5622247388</v>
       </c>
       <c r="P21">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q21">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="22">
@@ -1697,10 +1697,10 @@
         <v>717175.1613370343</v>
       </c>
       <c r="P22">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="Q22">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="23">
@@ -1746,10 +1746,10 @@
         <v>518419.7394188421</v>
       </c>
       <c r="P23">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="Q23">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="24">
@@ -1795,10 +1795,10 @@
         <v>569643.4153128543</v>
       </c>
       <c r="P24">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="Q24">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="25">
@@ -1844,10 +1844,10 @@
         <v>213509.8577738418</v>
       </c>
       <c r="P25">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="Q25">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="26">
@@ -1893,10 +1893,10 @@
         <v>329840.2664919504</v>
       </c>
       <c r="P26">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="Q26">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="27">
@@ -1942,10 +1942,10 @@
         <v>97065.40537030963</v>
       </c>
       <c r="P27">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="Q27">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="28">
@@ -1991,10 +1991,10 @@
         <v>17687.78978304791</v>
       </c>
       <c r="P28">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="Q28">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="29">
@@ -2040,10 +2040,10 @@
         <v>189217.8905235089</v>
       </c>
       <c r="P29">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="Q29">
-        <v>0.05</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="30">
@@ -2089,10 +2089,10 @@
         <v>454549.7827114371</v>
       </c>
       <c r="P30">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="Q30">
-        <v>0.05</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="31">
@@ -2138,10 +2138,10 @@
         <v>966912.7522210542</v>
       </c>
       <c r="P31">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="Q31">
-        <v>0.05</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="32">
@@ -2187,10 +2187,10 @@
         <v>645290.4618712433</v>
       </c>
       <c r="P32">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="Q32">
-        <v>0.05</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="33">
@@ -2236,10 +2236,10 @@
         <v>100032.3097210799</v>
       </c>
       <c r="P33">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q33">
-        <v>0.05</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="34">
@@ -2285,10 +2285,10 @@
         <v>147482.6115069279</v>
       </c>
       <c r="P34">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q34">
-        <v>0.05</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="35">
@@ -2334,7 +2334,7 @@
         <v>530209.3761206279</v>
       </c>
       <c r="P35">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q35">
         <v>0.05</v>
@@ -2383,7 +2383,7 @@
         <v>1383229.190991441</v>
       </c>
       <c r="P36">
-        <v>0.05</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="Q36">
         <v>0.05</v>
@@ -2432,7 +2432,7 @@
         <v>189975.3795417092</v>
       </c>
       <c r="P37">
-        <v>0.05</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="Q37">
         <v>0.05</v>
@@ -2481,7 +2481,7 @@
         <v>31701.9128248074</v>
       </c>
       <c r="P38">
-        <v>0.05</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="Q38">
         <v>0.05</v>
@@ -2530,7 +2530,7 @@
         <v>99890.87941789668</v>
       </c>
       <c r="P39">
-        <v>0.05</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="Q39">
         <v>0.05</v>
@@ -2579,7 +2579,7 @@
         <v>140758.2659394757</v>
       </c>
       <c r="P40">
-        <v>0.05</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="Q40">
         <v>0.05</v>
@@ -2628,7 +2628,7 @@
         <v>291403.081691474</v>
       </c>
       <c r="P41">
-        <v>0.05</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="Q41">
         <v>0.05</v>
@@ -3054,10 +3054,10 @@
         <v>15100.33608247423</v>
       </c>
       <c r="P50">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
       <c r="Q50">
-        <v>0.05</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51">
@@ -3106,10 +3106,10 @@
         <v>30906.24950495049</v>
       </c>
       <c r="P51">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
       <c r="Q51">
-        <v>0.05</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52">
@@ -3158,10 +3158,10 @@
         <v>23668.15049504951</v>
       </c>
       <c r="P52">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
       <c r="Q52">
-        <v>0.05</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53">
@@ -3210,10 +3210,10 @@
         <v>153237.7705882353</v>
       </c>
       <c r="P53">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
       <c r="Q53">
-        <v>0.05</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54">
@@ -3262,10 +3262,10 @@
         <v>127138.0294117647</v>
       </c>
       <c r="P54">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
       <c r="Q54">
-        <v>0.05</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55">
@@ -3314,10 +3314,10 @@
         <v>120962.5</v>
       </c>
       <c r="P55">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
       <c r="Q55">
-        <v>0.05</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56">
@@ -3366,10 +3366,10 @@
         <v>44237.05555555555</v>
       </c>
       <c r="P56">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q56">
-        <v>0.05</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57">
@@ -3418,10 +3418,10 @@
         <v>55570.94949494949</v>
       </c>
       <c r="P57">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q57">
-        <v>0.05</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58">
@@ -3470,10 +3470,10 @@
         <v>43470.02494949495</v>
       </c>
       <c r="P58">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q58">
-        <v>0.05</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59">
@@ -3522,10 +3522,10 @@
         <v>6318.54</v>
       </c>
       <c r="P59">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q59">
-        <v>0.05</v>
+        <v>0.2225214537678117</v>
       </c>
     </row>
     <row r="60">
@@ -3574,10 +3574,10 @@
         <v>9106.809999999999</v>
       </c>
       <c r="P60">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q60">
-        <v>0.05</v>
+        <v>0.1906696104737557</v>
       </c>
     </row>
     <row r="61">
@@ -3626,10 +3626,10 @@
         <v>60399.48</v>
       </c>
       <c r="P61">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q61">
-        <v>0.05</v>
+        <v>0.2820913854008965</v>
       </c>
     </row>
     <row r="62">
@@ -3678,10 +3678,10 @@
         <v>28890.6</v>
       </c>
       <c r="P62">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q62">
-        <v>0.05</v>
+        <v>0.2244482713685047</v>
       </c>
     </row>
     <row r="63">
@@ -3730,10 +3730,10 @@
         <v>49682.78747474747</v>
       </c>
       <c r="P63">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="Q63">
-        <v>0.05</v>
+        <v>0.2175887370668531</v>
       </c>
     </row>
     <row r="64">
@@ -3782,10 +3782,10 @@
         <v>20800.80252525253</v>
       </c>
       <c r="P64">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q64">
-        <v>0.05</v>
+        <v>0.2112446659500309</v>
       </c>
     </row>
     <row r="65">
@@ -3834,10 +3834,10 @@
         <v>54856.33</v>
       </c>
       <c r="P65">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q65">
-        <v>0.05</v>
+        <v>0.2502121517117331</v>
       </c>
     </row>
     <row r="66">
@@ -3886,10 +3886,10 @@
         <v>200973.82</v>
       </c>
       <c r="P66">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q66">
-        <v>0.05</v>
+        <v>0.2125816213529137</v>
       </c>
     </row>
     <row r="67">
@@ -3938,10 +3938,10 @@
         <v>45367.62</v>
       </c>
       <c r="P67">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q67">
-        <v>0.05</v>
+        <v>0.2177525887416372</v>
       </c>
     </row>
     <row r="68">
@@ -3990,10 +3990,10 @@
         <v>39447.62</v>
       </c>
       <c r="P68">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q68">
-        <v>0.05</v>
+        <v>0.2176218842885509</v>
       </c>
     </row>
     <row r="69">
@@ -4042,10 +4042,10 @@
         <v>14078.56927536232</v>
       </c>
       <c r="P69">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q69">
-        <v>0.05</v>
+        <v>0.2265346576411295</v>
       </c>
     </row>
     <row r="70">
@@ -4094,10 +4094,10 @@
         <v>109194.2223913043</v>
       </c>
       <c r="P70">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q70">
-        <v>0.05</v>
+        <v>0.2251548753188609</v>
       </c>
     </row>
     <row r="71">
@@ -4146,10 +4146,10 @@
         <v>113334.7638036304</v>
       </c>
       <c r="P71">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q71">
-        <v>0.05</v>
+        <v>0.2372746046452101</v>
       </c>
     </row>
     <row r="72">
@@ -4198,10 +4198,10 @@
         <v>21002.02876237624</v>
       </c>
       <c r="P72">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q72">
-        <v>0.05</v>
+        <v>0.2254977327673607</v>
       </c>
     </row>
     <row r="73">
@@ -4250,10 +4250,10 @@
         <v>6103.532659276798</v>
       </c>
       <c r="P73">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q73">
-        <v>0.05</v>
+        <v>0.2513686483152132</v>
       </c>
     </row>
     <row r="74">
@@ -4302,10 +4302,10 @@
         <v>40080.33552053925</v>
       </c>
       <c r="P74">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q74">
-        <v>0.05</v>
+        <v>0.2218800600265647</v>
       </c>
     </row>
     <row r="75">
@@ -4354,10 +4354,10 @@
         <v>19458.13390432388</v>
       </c>
       <c r="P75">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="Q75">
-        <v>0.05</v>
+        <v>0.1699117016239102</v>
       </c>
     </row>
     <row r="76">
@@ -4403,10 +4403,10 @@
         <v>860000</v>
       </c>
       <c r="P76">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="Q76">
-        <v>0.05</v>
+        <v>0.2320076990004557</v>
       </c>
     </row>
     <row r="77">
@@ -4452,10 +4452,10 @@
         <v>1200000</v>
       </c>
       <c r="P77">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="Q77">
-        <v>0.05</v>
+        <v>0.2348204737172755</v>
       </c>
     </row>
     <row r="78">
@@ -4501,10 +4501,10 @@
         <v>1900000</v>
       </c>
       <c r="P78">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="Q78">
-        <v>0.05</v>
+        <v>0.2114928124585719</v>
       </c>
     </row>
     <row r="79">
@@ -4550,10 +4550,10 @@
         <v>2100000</v>
       </c>
       <c r="P79">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="Q79">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="80">
@@ -4599,10 +4599,10 @@
         <v>2300000</v>
       </c>
       <c r="P80">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="Q80">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="81">
@@ -4651,10 +4651,10 @@
         <v>4464.647292102407</v>
       </c>
       <c r="P81">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="Q81">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="82">
@@ -4688,10 +4688,10 @@
         <v>24967.82729054477</v>
       </c>
       <c r="P82">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="Q82">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="83">
@@ -4725,10 +4725,10 @@
         <v>26458.95040901615</v>
       </c>
       <c r="P83">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="Q83">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="84">
@@ -4762,10 +4762,10 @@
         <v>76583.93285522016</v>
       </c>
       <c r="P84">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="Q84">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="85">
@@ -4814,10 +4814,10 @@
         <v>14329.98823621049</v>
       </c>
       <c r="P85">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="Q85">
-        <v>0.05</v>
+        <v>0.2200120092496774</v>
       </c>
     </row>
     <row r="86">
@@ -4866,10 +4866,10 @@
         <v>17385.5835483871</v>
       </c>
       <c r="P86">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q86">
-        <v>0.05</v>
+        <v>0.1729160862063066</v>
       </c>
     </row>
     <row r="87">
@@ -4924,7 +4924,7 @@
         <v>0.4448298647202095</v>
       </c>
       <c r="Q87">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="88">
@@ -4979,7 +4979,7 @@
         <v>0.4448298647202095</v>
       </c>
       <c r="Q88">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="89">
@@ -5028,10 +5028,10 @@
         <v>43839.87877920145</v>
       </c>
       <c r="P89">
-        <v>0.05</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="Q89">
-        <v>0.05</v>
+        <v>0.1249198497755794</v>
       </c>
     </row>
     <row r="90">
@@ -5080,10 +5080,10 @@
         <v>10937.88288746522</v>
       </c>
       <c r="P90">
-        <v>0.05</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="Q90">
-        <v>0.05</v>
+        <v>0.2051416732323674</v>
       </c>
     </row>
     <row r="91">
@@ -5132,10 +5132,10 @@
         <v>26414.05275956284</v>
       </c>
       <c r="P91">
-        <v>0.05</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="Q91">
-        <v>0.05</v>
+        <v>0.2863020443818129</v>
       </c>
     </row>
     <row r="92">
@@ -5184,10 +5184,10 @@
         <v>17167.38557377049</v>
       </c>
       <c r="P92">
-        <v>0.05</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="Q92">
-        <v>0.05</v>
+        <v>0.2243132431324313</v>
       </c>
     </row>
     <row r="93">
@@ -5236,10 +5236,10 @@
         <v>1239.474074074074</v>
       </c>
       <c r="P93">
-        <v>0.05</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="Q93">
-        <v>0.05</v>
+        <v>0.2159138945793906</v>
       </c>
     </row>
     <row r="94">
@@ -5288,10 +5288,10 @@
         <v>6640.959620596205</v>
       </c>
       <c r="P94">
-        <v>0.05</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="Q94">
-        <v>0.05</v>
+        <v>0.2225927690434598</v>
       </c>
     </row>
     <row r="95">
@@ -5343,7 +5343,7 @@
         <v>0.05</v>
       </c>
       <c r="Q95">
-        <v>0.05</v>
+        <v>0.2236050467284289</v>
       </c>
     </row>
     <row r="96">
@@ -5395,7 +5395,7 @@
         <v>0.05</v>
       </c>
       <c r="Q96">
-        <v>0.05</v>
+        <v>0.2145425374577343</v>
       </c>
     </row>
     <row r="97">
@@ -5444,7 +5444,7 @@
         <v>0.05</v>
       </c>
       <c r="Q97">
-        <v>0.05</v>
+        <v>0.2160584258445378</v>
       </c>
     </row>
     <row r="98">
@@ -5493,7 +5493,7 @@
         <v>0.05</v>
       </c>
       <c r="Q98">
-        <v>0.05</v>
+        <v>0.220378020986849</v>
       </c>
     </row>
     <row r="99">
@@ -5542,7 +5542,7 @@
         <v>0.05</v>
       </c>
       <c r="Q99">
-        <v>0.05</v>
+        <v>0.1387277073538455</v>
       </c>
     </row>
     <row r="100">
@@ -5591,7 +5591,7 @@
         <v>0.05</v>
       </c>
       <c r="Q100">
-        <v>0.05</v>
+        <v>0.1658471624667076</v>
       </c>
     </row>
     <row r="101">
@@ -5640,7 +5640,7 @@
         <v>0.05</v>
       </c>
       <c r="Q101">
-        <v>0.05</v>
+        <v>0.1660090684178094</v>
       </c>
     </row>
     <row r="102">
@@ -5689,7 +5689,7 @@
         <v>0.05</v>
       </c>
       <c r="Q102">
-        <v>0.05</v>
+        <v>0.156</v>
       </c>
     </row>
     <row r="103">
@@ -5735,10 +5735,10 @@
         <v>495061.8834075385</v>
       </c>
       <c r="P103">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
       <c r="Q103">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="104">
@@ -5784,10 +5784,10 @@
         <v>552803.0040534479</v>
       </c>
       <c r="P104">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q104">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="105">
@@ -5833,10 +5833,10 @@
         <v>570766.8540090187</v>
       </c>
       <c r="P105">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q105">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="106">
@@ -5882,10 +5882,10 @@
         <v>391376.4267260354</v>
       </c>
       <c r="P106">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q106">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="107">
@@ -5931,10 +5931,10 @@
         <v>288014.3071424381</v>
       </c>
       <c r="P107">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q107">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="108">
@@ -5980,10 +5980,10 @@
         <v>203184.164250254</v>
       </c>
       <c r="P108">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q108">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="109">
@@ -6029,10 +6029,10 @@
         <v>371601.962535504</v>
       </c>
       <c r="P109">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q109">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="110">
@@ -6078,10 +6078,10 @@
         <v>340157.6785086803</v>
       </c>
       <c r="P110">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q110">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="111">
@@ -6127,10 +6127,10 @@
         <v>172160.3662147925</v>
       </c>
       <c r="P111">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="Q111">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="112">
@@ -6176,10 +6176,10 @@
         <v>265697.028795797</v>
       </c>
       <c r="P112">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q112">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="113">
@@ -6225,10 +6225,10 @@
         <v>652446.9029476116</v>
       </c>
       <c r="P113">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q113">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="114">
@@ -6274,10 +6274,10 @@
         <v>625355.4802804298</v>
       </c>
       <c r="P114">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q114">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="115">
@@ -6323,10 +6323,10 @@
         <v>407468.2247957478</v>
       </c>
       <c r="P115">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q115">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="116">
@@ -6372,10 +6372,10 @@
         <v>181984.1898199186</v>
       </c>
       <c r="P116">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q116">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="117">
@@ -6421,10 +6421,10 @@
         <v>59697.7030353223</v>
       </c>
       <c r="P117">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q117">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="118">
@@ -6470,10 +6470,10 @@
         <v>320116.8393461921</v>
       </c>
       <c r="P118">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q118">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="119">
@@ -6519,10 +6519,10 @@
         <v>263927.9811106482</v>
       </c>
       <c r="P119">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q119">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="120">
@@ -6568,10 +6568,10 @@
         <v>189096.9567127897</v>
       </c>
       <c r="P120">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q120">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="121">
@@ -6617,10 +6617,10 @@
         <v>386548.9231194458</v>
       </c>
       <c r="P121">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q121">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="122">
@@ -6666,10 +6666,10 @@
         <v>145416.8103652774</v>
       </c>
       <c r="P122">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q122">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="123">
@@ -6715,10 +6715,10 @@
         <v>326804.0013846449</v>
       </c>
       <c r="P123">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="Q123">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="124">
@@ -6764,10 +6764,10 @@
         <v>732603.6241928141</v>
       </c>
       <c r="P124">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="Q124">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="125">
@@ -6813,10 +6813,10 @@
         <v>353959.4130974241</v>
       </c>
       <c r="P125">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="Q125">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="126">
@@ -6862,10 +6862,10 @@
         <v>219482.3284506314</v>
       </c>
       <c r="P126">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="Q126">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="127">
@@ -6911,10 +6911,10 @@
         <v>150478.2895093822</v>
       </c>
       <c r="P127">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="Q127">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="128">
@@ -6960,10 +6960,10 @@
         <v>131772.1820819404</v>
       </c>
       <c r="P128">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="Q128">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="129">
@@ -7009,10 +7009,10 @@
         <v>21882.51302978364</v>
       </c>
       <c r="P129">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="Q129">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="130">
@@ -7058,10 +7058,10 @@
         <v>114009.339885825</v>
       </c>
       <c r="P130">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="Q130">
-        <v>0.05</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="131">
@@ -7107,10 +7107,10 @@
         <v>333891.8889857767</v>
       </c>
       <c r="P131">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="Q131">
-        <v>0.05</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="132">
@@ -7156,10 +7156,10 @@
         <v>885638.3882038471</v>
       </c>
       <c r="P132">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="Q132">
-        <v>0.05</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="133">
@@ -7205,10 +7205,10 @@
         <v>811357.3188160737</v>
       </c>
       <c r="P133">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="Q133">
-        <v>0.05</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="134">
@@ -7254,10 +7254,10 @@
         <v>271240.703074521</v>
       </c>
       <c r="P134">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q134">
-        <v>0.05</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="135">
@@ -7303,10 +7303,10 @@
         <v>304274.706182281</v>
       </c>
       <c r="P135">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q135">
-        <v>0.05</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="136">
@@ -7352,7 +7352,7 @@
         <v>1046784.042950014</v>
       </c>
       <c r="P136">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="Q136">
         <v>0.05</v>
@@ -7401,7 +7401,7 @@
         <v>1456288.889933172</v>
       </c>
       <c r="P137">
-        <v>0.05</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="Q137">
         <v>0.05</v>
@@ -7450,7 +7450,7 @@
         <v>265560.8989697707</v>
       </c>
       <c r="P138">
-        <v>0.05</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="Q138">
         <v>0.05</v>
@@ -7499,7 +7499,7 @@
         <v>74647.11735710694</v>
       </c>
       <c r="P139">
-        <v>0.05</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="Q139">
         <v>0.05</v>
@@ -7548,7 +7548,7 @@
         <v>421399.4024497316</v>
       </c>
       <c r="P140">
-        <v>0.05</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="Q140">
         <v>0.05</v>
@@ -7597,7 +7597,7 @@
         <v>103582.4907797132</v>
       </c>
       <c r="P141">
-        <v>0.05</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="Q141">
         <v>0.05</v>
@@ -7646,7 +7646,7 @@
         <v>293354.5109088812</v>
       </c>
       <c r="P142">
-        <v>0.05</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="Q142">
         <v>0.05</v>

</xml_diff>

<commit_message>
update cleaned SR time series with new Hucuktlis CVs
</commit_message>
<xml_diff>
--- a/3. outputs/Stock-recruit data/Barkley_Sockeye_stock-recruit_infilled.xlsx
+++ b/3. outputs/Stock-recruit data/Barkley_Sockeye_stock-recruit_infilled.xlsx
@@ -558,7 +558,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Coefficient of variation on harvest data. Historical (prior to 2011) Hucuktlis Sockeye harvest rate predictions were derived from a linear model. CV for these data is calculated as RMSE of the model residuals divided by the mean of the observed Hucuktlis Sockeye harvest rates that informed the model fit (i.e. the dependent variable). Harvest data for Somass and Hucuktlis post-2011 are assumed to be precise.</t>
+          <t>Coefficient of variation on harvest data. Historical (prior to 2011) Hucuktlis Sockeye harvest rate predictions were derived from a linear model. Harvest data for Somass and Hucuktlis post-2011 are assumed to be precise.</t>
         </is>
       </c>
     </row>
@@ -3525,7 +3525,7 @@
         <v>0.2</v>
       </c>
       <c r="Q59">
-        <v>0.2225214537678117</v>
+        <v>0.2496267659213876</v>
       </c>
     </row>
     <row r="60">
@@ -3577,7 +3577,7 @@
         <v>0.2</v>
       </c>
       <c r="Q60">
-        <v>0.1906696104737557</v>
+        <v>0.2111714885758418</v>
       </c>
     </row>
     <row r="61">
@@ -3629,7 +3629,7 @@
         <v>0.2</v>
       </c>
       <c r="Q61">
-        <v>0.2820913854008965</v>
+        <v>0.2922206205809506</v>
       </c>
     </row>
     <row r="62">
@@ -3681,7 +3681,7 @@
         <v>0.2</v>
       </c>
       <c r="Q62">
-        <v>0.2244482713685047</v>
+        <v>0.2565178192417154</v>
       </c>
     </row>
     <row r="63">
@@ -3733,7 +3733,7 @@
         <v>0.3</v>
       </c>
       <c r="Q63">
-        <v>0.2175887370668531</v>
+        <v>0.2451098642822979</v>
       </c>
     </row>
     <row r="64">
@@ -3785,7 +3785,7 @@
         <v>0.2</v>
       </c>
       <c r="Q64">
-        <v>0.2112446659500309</v>
+        <v>0.2419729833867256</v>
       </c>
     </row>
     <row r="65">
@@ -3837,7 +3837,7 @@
         <v>0.2</v>
       </c>
       <c r="Q65">
-        <v>0.2502121517117331</v>
+        <v>0.2765457477820611</v>
       </c>
     </row>
     <row r="66">
@@ -3889,7 +3889,7 @@
         <v>0.2</v>
       </c>
       <c r="Q66">
-        <v>0.2125816213529137</v>
+        <v>0.231004202683785</v>
       </c>
     </row>
     <row r="67">
@@ -3941,7 +3941,7 @@
         <v>0.2</v>
       </c>
       <c r="Q67">
-        <v>0.2177525887416372</v>
+        <v>0.2464772207893425</v>
       </c>
     </row>
     <row r="68">
@@ -3993,7 +3993,7 @@
         <v>0.2</v>
       </c>
       <c r="Q68">
-        <v>0.2176218842885509</v>
+        <v>0.2480305876316884</v>
       </c>
     </row>
     <row r="69">
@@ -4045,7 +4045,7 @@
         <v>0.2</v>
       </c>
       <c r="Q69">
-        <v>0.2265346576411295</v>
+        <v>0.2553852420154066</v>
       </c>
     </row>
     <row r="70">
@@ -4097,7 +4097,7 @@
         <v>0.2</v>
       </c>
       <c r="Q70">
-        <v>0.2251548753188609</v>
+        <v>0.2550631891375683</v>
       </c>
     </row>
     <row r="71">
@@ -4149,7 +4149,7 @@
         <v>0.2</v>
       </c>
       <c r="Q71">
-        <v>0.2372746046452101</v>
+        <v>0.2553581160154582</v>
       </c>
     </row>
     <row r="72">
@@ -4201,7 +4201,7 @@
         <v>0.2</v>
       </c>
       <c r="Q72">
-        <v>0.2254977327673607</v>
+        <v>0.2553220566127163</v>
       </c>
     </row>
     <row r="73">
@@ -4253,7 +4253,7 @@
         <v>0.2</v>
       </c>
       <c r="Q73">
-        <v>0.2513686483152132</v>
+        <v>0.2821999907530116</v>
       </c>
     </row>
     <row r="74">
@@ -4305,7 +4305,7 @@
         <v>0.2</v>
       </c>
       <c r="Q74">
-        <v>0.2218800600265647</v>
+        <v>0.2525725048464748</v>
       </c>
     </row>
     <row r="75">
@@ -4357,7 +4357,7 @@
         <v>0.15</v>
       </c>
       <c r="Q75">
-        <v>0.1699117016239102</v>
+        <v>0.178692682150781</v>
       </c>
     </row>
     <row r="76">
@@ -4406,7 +4406,7 @@
         <v>0.15</v>
       </c>
       <c r="Q76">
-        <v>0.2320076990004557</v>
+        <v>0.2562130945777705</v>
       </c>
     </row>
     <row r="77">
@@ -4455,7 +4455,7 @@
         <v>0.15</v>
       </c>
       <c r="Q77">
-        <v>0.2348204737172755</v>
+        <v>0.2620673654633024</v>
       </c>
     </row>
     <row r="78">
@@ -4504,7 +4504,7 @@
         <v>0.15</v>
       </c>
       <c r="Q78">
-        <v>0.2114928124585719</v>
+        <v>0.2450461298290044</v>
       </c>
     </row>
     <row r="79">
@@ -4817,7 +4817,7 @@
         <v>0.15</v>
       </c>
       <c r="Q85">
-        <v>0.2200120092496774</v>
+        <v>0.2487218717321054</v>
       </c>
     </row>
     <row r="86">
@@ -4869,7 +4869,7 @@
         <v>0.2</v>
       </c>
       <c r="Q86">
-        <v>0.1729160862063066</v>
+        <v>0.1827938490156061</v>
       </c>
     </row>
     <row r="87">
@@ -5031,7 +5031,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="Q89">
-        <v>0.1249198497755794</v>
+        <v>0.1276418702964884</v>
       </c>
     </row>
     <row r="90">
@@ -5083,7 +5083,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="Q90">
-        <v>0.2051416732323674</v>
+        <v>0.2288747452863037</v>
       </c>
     </row>
     <row r="91">
@@ -5135,7 +5135,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="Q91">
-        <v>0.2863020443818129</v>
+        <v>0.2903052391163663</v>
       </c>
     </row>
     <row r="92">
@@ -5187,7 +5187,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="Q92">
-        <v>0.2243132431324313</v>
+        <v>0.2556215086392382</v>
       </c>
     </row>
     <row r="93">
@@ -5239,7 +5239,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="Q93">
-        <v>0.2159138945793906</v>
+        <v>0.241441424039182</v>
       </c>
     </row>
     <row r="94">
@@ -5291,7 +5291,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="Q94">
-        <v>0.2225927690434598</v>
+        <v>0.2497769802817572</v>
       </c>
     </row>
     <row r="95">
@@ -5343,7 +5343,7 @@
         <v>0.05</v>
       </c>
       <c r="Q95">
-        <v>0.2236050467284289</v>
+        <v>0.2440455592874953</v>
       </c>
     </row>
     <row r="96">
@@ -5395,7 +5395,7 @@
         <v>0.05</v>
       </c>
       <c r="Q96">
-        <v>0.2145425374577343</v>
+        <v>0.2425905410682488</v>
       </c>
     </row>
     <row r="97">
@@ -5444,7 +5444,7 @@
         <v>0.05</v>
       </c>
       <c r="Q97">
-        <v>0.2160584258445378</v>
+        <v>0.2388851566095718</v>
       </c>
     </row>
     <row r="98">
@@ -5493,7 +5493,7 @@
         <v>0.05</v>
       </c>
       <c r="Q98">
-        <v>0.220378020986849</v>
+        <v>0.2506997776881581</v>
       </c>
     </row>
     <row r="99">
@@ -5542,7 +5542,7 @@
         <v>0.05</v>
       </c>
       <c r="Q99">
-        <v>0.1387277073538455</v>
+        <v>0.1397559218405289</v>
       </c>
     </row>
     <row r="100">
@@ -5591,7 +5591,7 @@
         <v>0.05</v>
       </c>
       <c r="Q100">
-        <v>0.1658471624667076</v>
+        <v>0.1759984840093463</v>
       </c>
     </row>
     <row r="101">
@@ -5640,7 +5640,7 @@
         <v>0.05</v>
       </c>
       <c r="Q101">
-        <v>0.1660090684178094</v>
+        <v>0.1761708452318516</v>
       </c>
     </row>
     <row r="102">
@@ -5689,7 +5689,7 @@
         <v>0.05</v>
       </c>
       <c r="Q102">
-        <v>0.156</v>
+        <v>0.1677283430730512</v>
       </c>
     </row>
     <row r="103">

</xml_diff>

<commit_message>
fix issue where Somass age comp columns were not proportions
</commit_message>
<xml_diff>
--- a/3. outputs/Stock-recruit data/Barkley_Sockeye_stock-recruit_infilled.xlsx
+++ b/3. outputs/Stock-recruit data/Barkley_Sockeye_stock-recruit_infilled.xlsx
@@ -510,7 +510,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Binary variable describing whether (1) or not (0) the CU nursary lake was fertilized in each year. Note that fertilization affects abundances of pre-smolts in year + 1 (e.g. fertilizing a lake in 2010 is expected to bolster the abundances of pre-smolts counted during the winter 2011 ATS.</t>
+          <t>Binary variable describing whether (1) or not (0) the CU nursary lake was fertilized in each year. Note that fertilization affects abundances of pre-smolts in year + 1 (e.g. fertilizing a lake in 2010 is expected to affect the fry arising from brood year 2009).</t>
         </is>
       </c>
     </row>
@@ -690,22 +690,22 @@
         <v>209810.3603603604</v>
       </c>
       <c r="E2">
-        <v>1007462.356674952</v>
+        <v>1006504.356674952</v>
       </c>
       <c r="F2">
-        <v>795262.356674952</v>
+        <v>794304.356674952</v>
       </c>
       <c r="G2">
-        <v>18705.34149585965</v>
+        <v>0.01858446152946012</v>
       </c>
       <c r="H2">
-        <v>486058.0518288189</v>
+        <v>0.4829169874977403</v>
       </c>
       <c r="I2">
-        <v>461591.3305823656</v>
+        <v>0.4586083781169716</v>
       </c>
       <c r="J2">
-        <v>40149.63276790781</v>
+        <v>0.03989017285582801</v>
       </c>
       <c r="K2">
         <v>958</v>
@@ -739,22 +739,22 @@
         <v>84373.10195227766</v>
       </c>
       <c r="E3">
-        <v>260889.0318997159</v>
+        <v>259931.0318997159</v>
       </c>
       <c r="F3">
-        <v>146489.0318997159</v>
+        <v>145531.0318997159</v>
       </c>
       <c r="G3">
-        <v>32646.20304870381</v>
+        <v>0.1255956351579409</v>
       </c>
       <c r="H3">
-        <v>66531.65371027162</v>
+        <v>0.2559588719516192</v>
       </c>
       <c r="I3">
-        <v>148026.284518126</v>
+        <v>0.5694829256678983</v>
       </c>
       <c r="J3">
-        <v>12726.89062261444</v>
+        <v>0.0489625672225416</v>
       </c>
       <c r="K3">
         <v>958</v>
@@ -788,22 +788,22 @@
         <v>247475.4572803851</v>
       </c>
       <c r="E4">
-        <v>805916.2816986635</v>
+        <v>804958.2816986635</v>
       </c>
       <c r="F4">
-        <v>541921.2816986635</v>
+        <v>540963.2816986635</v>
       </c>
       <c r="G4">
-        <v>28765.03103738358</v>
+        <v>0.03573480973036536</v>
       </c>
       <c r="H4">
-        <v>460967.9540852145</v>
+        <v>0.5726606764172383</v>
       </c>
       <c r="I4">
-        <v>284466.5373341861</v>
+        <v>0.3533928947645467</v>
       </c>
       <c r="J4">
-        <v>30758.75924187931</v>
+        <v>0.03821161908784965</v>
       </c>
       <c r="K4">
         <v>958</v>
@@ -837,22 +837,22 @@
         <v>246041.4109470026</v>
       </c>
       <c r="E5">
-        <v>679980.2559109447</v>
+        <v>678372.2559109447</v>
       </c>
       <c r="F5">
-        <v>423464.2559109447</v>
+        <v>421856.2559109447</v>
       </c>
       <c r="G5">
-        <v>18324.95803644111</v>
+        <v>0.02701313014612257</v>
       </c>
       <c r="H5">
-        <v>307911.7049030835</v>
+        <v>0.4538978447601866</v>
       </c>
       <c r="I5">
-        <v>331983.2586127611</v>
+        <v>0.4893821286469935</v>
       </c>
       <c r="J5">
-        <v>20152.33435865898</v>
+        <v>0.02970689644669745</v>
       </c>
       <c r="K5">
         <v>1608</v>
@@ -886,22 +886,22 @@
         <v>195123.9818456883</v>
       </c>
       <c r="E6">
-        <v>772582.3886574621</v>
+        <v>771077.3886574621</v>
       </c>
       <c r="F6">
-        <v>559044.3886574621</v>
+        <v>557539.3886574621</v>
       </c>
       <c r="G6">
-        <v>29773.8416143193</v>
+        <v>0.03861329881058906</v>
       </c>
       <c r="H6">
-        <v>373355.283741389</v>
+        <v>0.4841994970069673</v>
       </c>
       <c r="I6">
-        <v>339549.6683934664</v>
+        <v>0.440357444516254</v>
       </c>
       <c r="J6">
-        <v>28398.59490828737</v>
+        <v>0.03682975966618957</v>
       </c>
       <c r="K6">
         <v>1505</v>
@@ -935,22 +935,22 @@
         <v>155579.2602739726</v>
       </c>
       <c r="E7">
-        <v>365248.6637001739</v>
+        <v>364505.6637001739</v>
       </c>
       <c r="F7">
-        <v>185828.6637001739</v>
+        <v>185085.6637001739</v>
       </c>
       <c r="G7">
-        <v>26259.98075017477</v>
+        <v>0.07204272351656806</v>
       </c>
       <c r="H7">
-        <v>114027.5218211575</v>
+        <v>0.3128278465240844</v>
       </c>
       <c r="I7">
-        <v>209620.1935893639</v>
+        <v>0.5750807585853813</v>
       </c>
       <c r="J7">
-        <v>14597.96753947772</v>
+        <v>0.04004867137396623</v>
       </c>
       <c r="K7">
         <v>743</v>
@@ -984,22 +984,22 @@
         <v>339203.6871165644</v>
       </c>
       <c r="E8">
-        <v>857321.3034811231</v>
+        <v>856130.3034811231</v>
       </c>
       <c r="F8">
-        <v>509219.3034811231</v>
+        <v>508028.3034811231</v>
       </c>
       <c r="G8">
-        <v>19787.97083530527</v>
+        <v>0.02311326997169139</v>
       </c>
       <c r="H8">
-        <v>437729.5714753096</v>
+        <v>0.5112884915946222</v>
       </c>
       <c r="I8">
-        <v>366170.6327473255</v>
+        <v>0.4277043240479096</v>
       </c>
       <c r="J8">
-        <v>32442.12842318277</v>
+        <v>0.03789391438577678</v>
       </c>
       <c r="K8">
         <v>1191</v>
@@ -1033,22 +1033,22 @@
         <v>131000.4258534074</v>
       </c>
       <c r="E9">
-        <v>652990.7686808587</v>
+        <v>652144.7686808587</v>
       </c>
       <c r="F9">
-        <v>519680.7686808587</v>
+        <v>518834.7686808587</v>
       </c>
       <c r="G9">
-        <v>6232.489817349981</v>
+        <v>0.009556911466079683</v>
       </c>
       <c r="H9">
-        <v>222606.8040319289</v>
+        <v>0.3413456869127572</v>
       </c>
       <c r="I9">
-        <v>406445.1656659931</v>
+        <v>0.6232437722196863</v>
       </c>
       <c r="J9">
-        <v>16860.30916558677</v>
+        <v>0.02585362940147685</v>
       </c>
       <c r="K9">
         <v>846</v>
@@ -1082,22 +1082,22 @@
         <v>112339.1474501013</v>
       </c>
       <c r="E10">
-        <v>438234.9184047349</v>
+        <v>437873.9184047349</v>
       </c>
       <c r="F10">
-        <v>317960.9184047349</v>
+        <v>317599.9184047349</v>
       </c>
       <c r="G10">
-        <v>14150.31463943479</v>
+        <v>0.03231595681923077</v>
       </c>
       <c r="H10">
-        <v>143300.5374649186</v>
+        <v>0.3272643823751641</v>
       </c>
       <c r="I10">
-        <v>237048.1996884363</v>
+        <v>0.5413617704202429</v>
       </c>
       <c r="J10">
-        <v>43374.86661194525</v>
+        <v>0.09905789038536218</v>
       </c>
       <c r="K10">
         <v>361</v>
@@ -1131,22 +1131,22 @@
         <v>119819.7732215988</v>
       </c>
       <c r="E11">
-        <v>148341.7415129345</v>
+        <v>148122.7415129345</v>
       </c>
       <c r="F11">
-        <v>10534.7415129345</v>
+        <v>10315.7415129345</v>
       </c>
       <c r="G11">
-        <v>15809.11707899555</v>
+        <v>0.1067298438951392</v>
       </c>
       <c r="H11">
-        <v>66695.12401498479</v>
+        <v>0.4502693059401739</v>
       </c>
       <c r="I11">
-        <v>64463.2181601842</v>
+        <v>0.4352013573456248</v>
       </c>
       <c r="J11">
-        <v>1155.282258769916</v>
+        <v>0.007799492819062046</v>
       </c>
       <c r="K11">
         <v>219</v>
@@ -1180,22 +1180,22 @@
         <v>277561.6340898228</v>
       </c>
       <c r="E12">
-        <v>374690.4021386584</v>
+        <v>373732.4021386584</v>
       </c>
       <c r="F12">
-        <v>83975.40213865851</v>
+        <v>83017.40213865851</v>
       </c>
       <c r="G12">
-        <v>14798.31893753283</v>
+        <v>0.03959602874369587</v>
       </c>
       <c r="H12">
-        <v>299234.5749361129</v>
+        <v>0.8006653242367083</v>
       </c>
       <c r="I12">
-        <v>49572.81505067585</v>
+        <v>0.1326425398680948</v>
       </c>
       <c r="J12">
-        <v>10126.69321433694</v>
+        <v>0.02709610715150097</v>
       </c>
       <c r="K12">
         <v>958</v>
@@ -1229,22 +1229,22 @@
         <v>195326.5652956242</v>
       </c>
       <c r="E13">
-        <v>354669.0244309763</v>
+        <v>353509.0244309763</v>
       </c>
       <c r="F13">
-        <v>147993.0244309762</v>
+        <v>146833.0244309762</v>
       </c>
       <c r="G13">
-        <v>14134.82998717707</v>
+        <v>0.03998435403432518</v>
       </c>
       <c r="H13">
-        <v>151986.2792132869</v>
+        <v>0.4299360658696922</v>
       </c>
       <c r="I13">
-        <v>180729.7356166003</v>
+        <v>0.511245040794958</v>
       </c>
       <c r="J13">
-        <v>6658.17961391207</v>
+        <v>0.01883453930102455</v>
       </c>
       <c r="K13">
         <v>1160</v>
@@ -1278,22 +1278,22 @@
         <v>171651.5860436582</v>
       </c>
       <c r="E14">
-        <v>257174.0008752627</v>
+        <v>256187.0008752627</v>
       </c>
       <c r="F14">
-        <v>15911.00087526266</v>
+        <v>14924.00087526266</v>
       </c>
       <c r="G14">
-        <v>56852.22813051834</v>
+        <v>0.221916912006787</v>
       </c>
       <c r="H14">
-        <v>155297.0959718838</v>
+        <v>0.6061864787881953</v>
       </c>
       <c r="I14">
-        <v>36718.8016927092</v>
+        <v>0.1433281219080572</v>
       </c>
       <c r="J14">
-        <v>7318.875080151364</v>
+        <v>0.02856848729696055</v>
       </c>
       <c r="K14">
         <v>987</v>
@@ -1327,22 +1327,22 @@
         <v>163320.2965164308</v>
       </c>
       <c r="E15">
-        <v>199344.2037468761</v>
+        <v>198444.2037468761</v>
       </c>
       <c r="F15">
-        <v>20253.20374687613</v>
+        <v>19353.20374687613</v>
       </c>
       <c r="G15">
-        <v>14598.48927455422</v>
+        <v>0.07356470483348157</v>
       </c>
       <c r="H15">
-        <v>70168.70924139084</v>
+        <v>0.3535941484634842</v>
       </c>
       <c r="I15">
-        <v>110453.8684518885</v>
+        <v>0.5565991163580519</v>
       </c>
       <c r="J15">
-        <v>3223.136779042612</v>
+        <v>0.0162420303449823</v>
       </c>
       <c r="K15">
         <v>900</v>
@@ -1376,22 +1376,22 @@
         <v>402976.0582740782</v>
       </c>
       <c r="E16">
-        <v>1242632.475737115</v>
+        <v>1240904.475737115</v>
       </c>
       <c r="F16">
-        <v>809242.4757371148</v>
+        <v>807514.4757371148</v>
       </c>
       <c r="G16">
-        <v>37276.97619244541</v>
+        <v>0.03004016579946845</v>
       </c>
       <c r="H16">
-        <v>1047636.943546943</v>
+        <v>0.844252691509257</v>
       </c>
       <c r="I16">
-        <v>143814.4112019459</v>
+        <v>0.1158948283400445</v>
       </c>
       <c r="J16">
-        <v>12176.14479578094</v>
+        <v>0.009812314351230087</v>
       </c>
       <c r="K16">
         <v>1728</v>
@@ -1425,22 +1425,22 @@
         <v>149897.5377081351</v>
       </c>
       <c r="E17">
-        <v>367805.8334567148</v>
+        <v>366707.8334567148</v>
       </c>
       <c r="F17">
-        <v>179652.8334567147</v>
+        <v>178554.8334567147</v>
       </c>
       <c r="G17">
-        <v>37401.19694582894</v>
+        <v>0.1019918134643384</v>
       </c>
       <c r="H17">
-        <v>151068.7246797518</v>
+        <v>0.411959360823372</v>
       </c>
       <c r="I17">
-        <v>174761.4874040562</v>
+        <v>0.4765687325430003</v>
       </c>
       <c r="J17">
-        <v>3476.424427077865</v>
+        <v>0.009480093169289262</v>
       </c>
       <c r="K17">
         <v>1098</v>
@@ -1474,22 +1474,22 @@
         <v>227693.7005819493</v>
       </c>
       <c r="E18">
-        <v>675548.2165285624</v>
+        <v>674184.2165285624</v>
       </c>
       <c r="F18">
-        <v>433787.2165285624</v>
+        <v>432423.2165285624</v>
       </c>
       <c r="G18">
-        <v>19488.07852822151</v>
+        <v>0.02890616251529509</v>
       </c>
       <c r="H18">
-        <v>248302.7102725914</v>
+        <v>0.3683009838929859</v>
       </c>
       <c r="I18">
-        <v>385133.710963045</v>
+        <v>0.571258865931532</v>
       </c>
       <c r="J18">
-        <v>21259.71676470451</v>
+        <v>0.03153398766018698</v>
       </c>
       <c r="K18">
         <v>1364</v>
@@ -1523,22 +1523,22 @@
         <v>113120.7705627706</v>
       </c>
       <c r="E19">
-        <v>211736.9594842033</v>
+        <v>210845.9594842033</v>
       </c>
       <c r="F19">
-        <v>98243.95948420328</v>
+        <v>97352.95948420328</v>
       </c>
       <c r="G19">
-        <v>151.2696697384544</v>
+        <v>0.0007174416342077811</v>
       </c>
       <c r="H19">
-        <v>75108.38939107943</v>
+        <v>0.3562239920310475</v>
       </c>
       <c r="I19">
-        <v>109276.3656507083</v>
+        <v>0.5182758347280321</v>
       </c>
       <c r="J19">
-        <v>26309.93477267714</v>
+        <v>0.1247827316067126</v>
       </c>
       <c r="K19">
         <v>891</v>
@@ -1572,22 +1572,22 @@
         <v>40940.28608630573</v>
       </c>
       <c r="E20">
-        <v>82436.29743190458</v>
+        <v>81936.29743190458</v>
       </c>
       <c r="F20">
-        <v>18425.29743190457</v>
+        <v>17925.29743190457</v>
       </c>
       <c r="G20">
-        <v>19328.30272710248</v>
+        <v>0.235894265824811</v>
       </c>
       <c r="H20">
-        <v>14018.39353934088</v>
+        <v>0.1710889310197505</v>
       </c>
       <c r="I20">
-        <v>42694.83900173569</v>
+        <v>0.5210735698329353</v>
       </c>
       <c r="J20">
-        <v>5894.762163725529</v>
+        <v>0.07194323332250317</v>
       </c>
       <c r="K20">
         <v>500</v>
@@ -1621,22 +1621,22 @@
         <v>157087.470514674</v>
       </c>
       <c r="E21">
-        <v>214255.0437581833</v>
+        <v>213255.0437581833</v>
       </c>
       <c r="F21">
-        <v>27873.04375818334</v>
+        <v>26873.04375818334</v>
       </c>
       <c r="G21">
-        <v>26688.82978344283</v>
+        <v>0.1251498173881699</v>
       </c>
       <c r="H21">
-        <v>144183.8241595631</v>
+        <v>0.6761097961324549</v>
       </c>
       <c r="I21">
-        <v>41071.69875015606</v>
+        <v>0.1925942665943628</v>
       </c>
       <c r="J21">
-        <v>1310.691065021357</v>
+        <v>0.006146119885012387</v>
       </c>
       <c r="K21">
         <v>1000</v>
@@ -1670,22 +1670,22 @@
         <v>174088.073308042</v>
       </c>
       <c r="E22">
-        <v>277147.6404868294</v>
+        <v>275396.6404868294</v>
       </c>
       <c r="F22">
-        <v>99031.64048682951</v>
+        <v>97280.64048682951</v>
       </c>
       <c r="G22">
-        <v>300.0084067585789</v>
+        <v>0.001089368433210522</v>
       </c>
       <c r="H22">
-        <v>151203.604010767</v>
+        <v>0.5490393918512532</v>
       </c>
       <c r="I22">
-        <v>105031.7001268944</v>
+        <v>0.3813833746890511</v>
       </c>
       <c r="J22">
-        <v>18861.32794240946</v>
+        <v>0.06848786502648525</v>
       </c>
       <c r="K22">
         <v>1751</v>
@@ -1719,22 +1719,22 @@
         <v>184541.7668836023</v>
       </c>
       <c r="E23">
-        <v>407738.2741320956</v>
+        <v>406622.2741320956</v>
       </c>
       <c r="F23">
-        <v>133725.2741320956</v>
+        <v>132609.2741320956</v>
       </c>
       <c r="G23">
-        <v>88465.63853884122</v>
+        <v>0.2175622049423249</v>
       </c>
       <c r="H23">
-        <v>81200.41049539356</v>
+        <v>0.1996949396555062</v>
       </c>
       <c r="I23">
-        <v>215495.4576809758</v>
+        <v>0.5299647151424119</v>
       </c>
       <c r="J23">
-        <v>21460.76741688508</v>
+        <v>0.05277814025975695</v>
       </c>
       <c r="K23">
         <v>1116</v>
@@ -1768,22 +1768,22 @@
         <v>203969.2210342309</v>
       </c>
       <c r="E24">
-        <v>272968.1399680462</v>
+        <v>269747.1399680462</v>
       </c>
       <c r="F24">
-        <v>61856.86069137149</v>
+        <v>58635.86069137149</v>
       </c>
       <c r="G24">
-        <v>5428.090897890179</v>
+        <v>0.02012288582015432</v>
       </c>
       <c r="H24">
-        <v>90604.35825719417</v>
+        <v>0.3358862609921537</v>
       </c>
       <c r="I24">
-        <v>145122.89447865</v>
+        <v>0.5379960450955702</v>
       </c>
       <c r="J24">
-        <v>28591.79633431178</v>
+        <v>0.1059948080921218</v>
       </c>
       <c r="K24">
         <v>3221</v>
@@ -1817,22 +1817,22 @@
         <v>52042.75861096355</v>
       </c>
       <c r="E25">
-        <v>109363.0646568037</v>
+        <v>108772.0646568037</v>
       </c>
       <c r="F25">
-        <v>37704.06465680369</v>
+        <v>37113.06465680369</v>
       </c>
       <c r="G25">
-        <v>7824.685204646306</v>
+        <v>0.07193653287114349</v>
       </c>
       <c r="H25">
-        <v>27654.66272501663</v>
+        <v>0.2542441647335856</v>
       </c>
       <c r="I25">
-        <v>59712.0540796343</v>
+        <v>0.5489649779843477</v>
       </c>
       <c r="J25">
-        <v>13580.66264750648</v>
+        <v>0.1248543244109231</v>
       </c>
       <c r="K25">
         <v>591</v>
@@ -1866,22 +1866,22 @@
         <v>307105.9177138301</v>
       </c>
       <c r="E26">
-        <v>524677.8445647745</v>
+        <v>522690.8445647745</v>
       </c>
       <c r="F26">
-        <v>115850.9823215375</v>
+        <v>113863.9823215374</v>
       </c>
       <c r="G26">
-        <v>67123.414912671</v>
+        <v>0.1284189604823903</v>
       </c>
       <c r="H26">
-        <v>300090.6411863717</v>
+        <v>0.5741264541112178</v>
       </c>
       <c r="I26">
-        <v>152576.2701938616</v>
+        <v>0.291905381126211</v>
       </c>
       <c r="J26">
-        <v>2900.518271870184</v>
+        <v>0.005549204280180838</v>
       </c>
       <c r="K26">
         <v>1987</v>
@@ -1915,22 +1915,22 @@
         <v>259481.6302496267</v>
       </c>
       <c r="E27">
-        <v>672514.1779337378</v>
+        <v>669447.1779337378</v>
       </c>
       <c r="F27">
-        <v>387658.3972696845</v>
+        <v>384591.3972696845</v>
       </c>
       <c r="G27">
-        <v>16541.03772615557</v>
+        <v>0.02470850318199835</v>
       </c>
       <c r="H27">
-        <v>208982.045041776</v>
+        <v>0.3121710747766587</v>
       </c>
       <c r="I27">
-        <v>367639.5567578359</v>
+        <v>0.5491688797502483</v>
       </c>
       <c r="J27">
-        <v>76284.53840797034</v>
+        <v>0.1139515422910947</v>
       </c>
       <c r="K27">
         <v>3067</v>
@@ -1964,22 +1964,22 @@
         <v>223545.6124846652</v>
       </c>
       <c r="E28">
-        <v>529850.2970109106</v>
+        <v>527584.2970109106</v>
       </c>
       <c r="F28">
-        <v>278882.6663030458</v>
+        <v>276616.6663030458</v>
       </c>
       <c r="G28">
-        <v>15172.50331542371</v>
+        <v>0.02875844372432097</v>
       </c>
       <c r="H28">
-        <v>266253.3786066</v>
+        <v>0.5046650935501475</v>
       </c>
       <c r="I28">
-        <v>204538.1369007065</v>
+        <v>0.3876880681618858</v>
       </c>
       <c r="J28">
-        <v>41620.27818818036</v>
+        <v>0.0788883945636457</v>
       </c>
       <c r="K28">
         <v>2266</v>
@@ -2013,22 +2013,22 @@
         <v>213021.3820306078</v>
       </c>
       <c r="E29">
-        <v>428778.6849503428</v>
+        <v>427024.6849503428</v>
       </c>
       <c r="F29">
-        <v>204140.6849503427</v>
+        <v>202386.6849503427</v>
       </c>
       <c r="G29">
-        <v>9652.922779422113</v>
+        <v>0.02260506972927015</v>
       </c>
       <c r="H29">
-        <v>133209.3351178704</v>
+        <v>0.3119476222630101</v>
       </c>
       <c r="I29">
-        <v>246386.2844893615</v>
+        <v>0.5769837041575544</v>
       </c>
       <c r="J29">
-        <v>37776.14256368874</v>
+        <v>0.08846360385016525</v>
       </c>
       <c r="K29">
         <v>1754</v>
@@ -2062,22 +2062,22 @@
         <v>172961.8926665951</v>
       </c>
       <c r="E30">
-        <v>259674.0568902378</v>
+        <v>257985.0568902378</v>
       </c>
       <c r="F30">
-        <v>64995.91610701918</v>
+        <v>63306.91610701918</v>
       </c>
       <c r="G30">
-        <v>7812.055373346592</v>
+        <v>0.03028103824118118</v>
       </c>
       <c r="H30">
-        <v>148418.637606868</v>
+        <v>0.5752993580167478</v>
       </c>
       <c r="I30">
-        <v>61291.64941928598</v>
+        <v>0.2375782929371878</v>
       </c>
       <c r="J30">
-        <v>40462.71449073727</v>
+        <v>0.1568413108048832</v>
       </c>
       <c r="K30">
         <v>1689</v>
@@ -2111,22 +2111,22 @@
         <v>135492.6206186963</v>
       </c>
       <c r="E31">
-        <v>198813.4971440957</v>
+        <v>197534.4971440957</v>
       </c>
       <c r="F31">
-        <v>62566.7674585098</v>
+        <v>61287.7674585098</v>
       </c>
       <c r="G31">
-        <v>754.1090668896481</v>
+        <v>0.003817606938496152</v>
       </c>
       <c r="H31">
-        <v>37991.48465182235</v>
+        <v>0.192328353786775</v>
       </c>
       <c r="I31">
-        <v>154952.5335041221</v>
+        <v>0.7844327737402172</v>
       </c>
       <c r="J31">
-        <v>3836.369921261688</v>
+        <v>0.0194212655345115</v>
       </c>
       <c r="K31">
         <v>1279</v>
@@ -2160,22 +2160,22 @@
         <v>67716.87403025852</v>
       </c>
       <c r="E32">
-        <v>83311.30415284277</v>
+        <v>82625.30415284277</v>
       </c>
       <c r="F32">
-        <v>5689.304152842727</v>
+        <v>5003.304152842727</v>
       </c>
       <c r="G32">
-        <v>9774.078474597234</v>
+        <v>0.118294009018313</v>
       </c>
       <c r="H32">
-        <v>5853.267761186174</v>
+        <v>0.07084110395961295</v>
       </c>
       <c r="I32">
-        <v>50181.78531552112</v>
+        <v>0.6073416107817691</v>
       </c>
       <c r="J32">
-        <v>16816.17260153824</v>
+        <v>0.2035232762403051</v>
       </c>
       <c r="K32">
         <v>686</v>
@@ -2209,22 +2209,22 @@
         <v>59588.56228382845</v>
       </c>
       <c r="E33">
-        <v>74417.00675675675</v>
+        <v>74024.00675675675</v>
       </c>
       <c r="F33">
-        <v>393</v>
+        <v>0</v>
       </c>
       <c r="G33">
-        <v>12847.05456948411</v>
+        <v>0.1735525423758754</v>
       </c>
       <c r="H33">
-        <v>50491.47673421607</v>
+        <v>0.6820959705698088</v>
       </c>
       <c r="I33">
-        <v>9605.395423436996</v>
+        <v>0.1297605445082211</v>
       </c>
       <c r="J33">
-        <v>1080.080029619561</v>
+        <v>0.01459094254609466</v>
       </c>
       <c r="K33">
         <v>393</v>
@@ -2258,22 +2258,22 @@
         <v>203858.404320321</v>
       </c>
       <c r="E34">
-        <v>310164.4722622803</v>
+        <v>308881.4722622803</v>
       </c>
       <c r="F34">
-        <v>87923.184597357</v>
+        <v>86640.184597357</v>
       </c>
       <c r="G34">
-        <v>5509.096779057447</v>
+        <v>0.01783563364519162</v>
       </c>
       <c r="H34">
-        <v>189450.077455843</v>
+        <v>0.6133423156406589</v>
       </c>
       <c r="I34">
-        <v>112447.2804958448</v>
+        <v>0.3640466994419224</v>
       </c>
       <c r="J34">
-        <v>1475.017531535087</v>
+        <v>0.004775351272227188</v>
       </c>
       <c r="K34">
         <v>1283</v>
@@ -2307,22 +2307,22 @@
         <v>255339.0849044172</v>
       </c>
       <c r="E35">
-        <v>842775.0420667162</v>
+        <v>840564.0420667162</v>
       </c>
       <c r="F35">
-        <v>498776.0420667162</v>
+        <v>496565.0420667162</v>
       </c>
       <c r="G35">
-        <v>92046.30782282758</v>
+        <v>0.109505407341136</v>
       </c>
       <c r="H35">
-        <v>516021.3483160416</v>
+        <v>0.613898908936536</v>
       </c>
       <c r="I35">
-        <v>215991.3311089962</v>
+        <v>0.2569599938845026</v>
       </c>
       <c r="J35">
-        <v>16505.05481885077</v>
+        <v>0.01963568983782529</v>
       </c>
       <c r="K35">
         <v>2211</v>
@@ -2356,22 +2356,22 @@
         <v>431213.3766384768</v>
       </c>
       <c r="E36">
-        <v>768896.7875944228</v>
+        <v>767164.7875944228</v>
       </c>
       <c r="F36">
-        <v>323076.7875944229</v>
+        <v>321344.7875944229</v>
       </c>
       <c r="G36">
-        <v>12404.58606629006</v>
+        <v>0.01616938924580568</v>
       </c>
       <c r="H36">
-        <v>286605.1387812592</v>
+        <v>0.3735900596793017</v>
       </c>
       <c r="I36">
-        <v>431893.7431697596</v>
+        <v>0.5629738879492068</v>
       </c>
       <c r="J36">
-        <v>36261.31957711383</v>
+        <v>0.04726666312568573</v>
       </c>
       <c r="K36">
         <v>1732</v>
@@ -2405,22 +2405,22 @@
         <v>147440.4759431045</v>
       </c>
       <c r="E37">
-        <v>332233.9165734798</v>
+        <v>330860.9165734798</v>
       </c>
       <c r="F37">
-        <v>182889.9165734799</v>
+        <v>181516.9165734799</v>
       </c>
       <c r="G37">
-        <v>1941.389973665683</v>
+        <v>0.005867692061581186</v>
       </c>
       <c r="H37">
-        <v>62124.2425117114</v>
+        <v>0.1877654307286984</v>
       </c>
       <c r="I37">
-        <v>253306.7201319073</v>
+        <v>0.7655987982964171</v>
       </c>
       <c r="J37">
-        <v>13488.56395619551</v>
+        <v>0.04076807891330338</v>
       </c>
       <c r="K37">
         <v>1373</v>
@@ -2454,22 +2454,22 @@
         <v>66687.6663805545</v>
       </c>
       <c r="E38">
-        <v>212040.6391093959</v>
+        <v>211312.6391093959</v>
       </c>
       <c r="F38">
-        <v>27308.13910939579</v>
+        <v>26580.13910939579</v>
       </c>
       <c r="G38">
-        <v>98776.14282278641</v>
+        <v>0.4674407704105684</v>
       </c>
       <c r="H38">
-        <v>74520.03998514252</v>
+        <v>0.3526530182918389</v>
       </c>
       <c r="I38">
-        <v>24684.16116621768</v>
+        <v>0.1168134630765686</v>
       </c>
       <c r="J38">
-        <v>13332.29513524926</v>
+        <v>0.0630927482210242</v>
       </c>
       <c r="K38">
         <v>728</v>
@@ -2503,22 +2503,22 @@
         <v>66297.57875207638</v>
       </c>
       <c r="E39">
-        <v>355838.0138946447</v>
+        <v>354451.0138946447</v>
       </c>
       <c r="F39">
-        <v>193152.2559201121</v>
+        <v>191765.2559201121</v>
       </c>
       <c r="G39">
-        <v>96478.89907182282</v>
+        <v>0.2721924759411176</v>
       </c>
       <c r="H39">
-        <v>190099.9332978414</v>
+        <v>0.5363221597508134</v>
       </c>
       <c r="I39">
-        <v>67052.86154811966</v>
+        <v>0.1891738460876575</v>
       </c>
       <c r="J39">
-        <v>819.3199768607567</v>
+        <v>0.002311518220411375</v>
       </c>
       <c r="K39">
         <v>1387</v>
@@ -2552,22 +2552,22 @@
         <v>417774.4300000001</v>
       </c>
       <c r="E40">
-        <v>1006802.07</v>
+        <v>1003862.07</v>
       </c>
       <c r="F40">
-        <v>579263</v>
+        <v>576323</v>
       </c>
       <c r="G40">
-        <v>8568.24</v>
+        <v>0.008535276165977662</v>
       </c>
       <c r="H40">
-        <v>762049.3300000001</v>
+        <v>0.7591175648264109</v>
       </c>
       <c r="I40">
-        <v>229276.18</v>
+        <v>0.2283941059751366</v>
       </c>
       <c r="J40">
-        <v>3968.32</v>
+        <v>0.00395305303247487</v>
       </c>
       <c r="K40">
         <v>2940</v>
@@ -2601,22 +2601,22 @@
         <v>220952.45</v>
       </c>
       <c r="E41">
-        <v>573153.26</v>
+        <v>570963.26</v>
       </c>
       <c r="F41">
-        <v>348791</v>
+        <v>346601</v>
       </c>
       <c r="G41">
-        <v>4352.810000000004</v>
+        <v>0.007623625380028838</v>
       </c>
       <c r="H41">
-        <v>44237.67</v>
+        <v>0.07747901327311323</v>
       </c>
       <c r="I41">
-        <v>510315.66</v>
+        <v>0.8937802057526434</v>
       </c>
       <c r="J41">
-        <v>12057.12</v>
+        <v>0.02111715559421459</v>
       </c>
       <c r="K41">
         <v>2190</v>
@@ -2650,22 +2650,22 @@
         <v>125845.7399999999</v>
       </c>
       <c r="E42">
-        <v>175878.908424623</v>
+        <v>174769.908424623</v>
       </c>
       <c r="F42">
-        <v>37061.90842462308</v>
+        <v>35952.90842462308</v>
       </c>
       <c r="G42">
-        <v>12787.35334474858</v>
+        <v>0.07316679089675025</v>
       </c>
       <c r="H42">
-        <v>12067.36316792424</v>
+        <v>0.0690471447670799</v>
       </c>
       <c r="I42">
-        <v>135529.8899923326</v>
+        <v>0.775476117221779</v>
       </c>
       <c r="J42">
-        <v>14385.30191961763</v>
+        <v>0.08230994711439073</v>
       </c>
       <c r="K42">
         <v>1109</v>
@@ -2699,22 +2699,22 @@
         <v>36417.81</v>
       </c>
       <c r="E43">
-        <v>54346.03414467358</v>
+        <v>53891.03414467358</v>
       </c>
       <c r="F43">
-        <v>15726.24414467358</v>
+        <v>15271.24414467358</v>
       </c>
       <c r="G43">
-        <v>542.1235225398954</v>
+        <v>0.01005962366735316</v>
       </c>
       <c r="H43">
-        <v>38851.85308866152</v>
+        <v>0.7209335227147708</v>
       </c>
       <c r="I43">
-        <v>12857.47798409555</v>
+        <v>0.238582877247798</v>
       </c>
       <c r="J43">
-        <v>1639.579549376614</v>
+        <v>0.03042397637007796</v>
       </c>
       <c r="K43">
         <v>455</v>
@@ -2748,22 +2748,22 @@
         <v>35982.08</v>
       </c>
       <c r="E44">
-        <v>64382.07220666183</v>
+        <v>63683.07220666183</v>
       </c>
       <c r="F44">
-        <v>15562.06220666182</v>
+        <v>14863.06220666182</v>
       </c>
       <c r="G44">
-        <v>5426.668127924149</v>
+        <v>0.08521366730414226</v>
       </c>
       <c r="H44">
-        <v>21469.62678818674</v>
+        <v>0.3371323971072618</v>
       </c>
       <c r="I44">
-        <v>34362.51561776333</v>
+        <v>0.5395863363226484</v>
       </c>
       <c r="J44">
-        <v>2424.261672787607</v>
+        <v>0.03806759926594758</v>
       </c>
       <c r="K44">
         <v>699</v>
@@ -2794,22 +2794,22 @@
         <v>109174.19</v>
       </c>
       <c r="E45">
-        <v>174998.009536926</v>
+        <v>174138.009536926</v>
       </c>
       <c r="F45">
-        <v>35021.94953692597</v>
+        <v>34161.94953692597</v>
       </c>
       <c r="G45">
-        <v>26810.92297790385</v>
+        <v>0.1539636467029824</v>
       </c>
       <c r="H45">
-        <v>68627.41356354978</v>
+        <v>0.3940978408220367</v>
       </c>
       <c r="I45">
-        <v>64810.5156287491</v>
+        <v>0.3721790308795623</v>
       </c>
       <c r="J45">
-        <v>13889.15736672325</v>
+        <v>0.07975948159541843</v>
       </c>
       <c r="K45">
         <v>860</v>
@@ -2840,22 +2840,22 @@
         <v>220319</v>
       </c>
       <c r="E46">
-        <v>341096</v>
+        <v>338856</v>
       </c>
       <c r="F46">
-        <v>115916</v>
+        <v>113676</v>
       </c>
       <c r="G46">
-        <v>4595</v>
+        <v>0.01356033241258824</v>
       </c>
       <c r="H46">
-        <v>118011</v>
+        <v>0.3482629789645159</v>
       </c>
       <c r="I46">
-        <v>162314</v>
+        <v>0.4790058313856033</v>
       </c>
       <c r="J46">
-        <v>53936</v>
+        <v>0.1591708572372925</v>
       </c>
       <c r="K46">
         <v>2240</v>
@@ -2886,22 +2886,22 @@
         <v>194787</v>
       </c>
       <c r="E47">
-        <v>346528</v>
+        <v>345775</v>
       </c>
       <c r="F47">
-        <v>110765</v>
+        <v>110012</v>
       </c>
       <c r="G47">
-        <v>46770</v>
+        <v>0.1352613693876075</v>
       </c>
       <c r="H47">
-        <v>67516</v>
+        <v>0.1952599233605669</v>
       </c>
       <c r="I47">
-        <v>176454</v>
+        <v>0.5103145108813535</v>
       </c>
       <c r="J47">
-        <v>55035</v>
+        <v>0.1591641963704721</v>
       </c>
       <c r="K47">
         <v>753</v>
@@ -2932,22 +2932,22 @@
         <v>120978.5770748142</v>
       </c>
       <c r="E48">
-        <v>352767.4059457993</v>
+        <v>350859.4059457993</v>
       </c>
       <c r="F48">
-        <v>143502.4059457992</v>
+        <v>141594.4059457992</v>
       </c>
       <c r="G48">
-        <v>90778.66436880779</v>
+        <v>0.2587323093821554</v>
       </c>
       <c r="H48">
-        <v>178315.0063342566</v>
+        <v>0.5082235314557955</v>
       </c>
       <c r="I48">
-        <v>62561.38303440162</v>
+        <v>0.1783089806749148</v>
       </c>
       <c r="J48">
-        <v>19204.35220833324</v>
+        <v>0.05473517848713433</v>
       </c>
       <c r="K48">
         <v>1908</v>
@@ -2978,22 +2978,22 @@
         <v>323972.2317319542</v>
       </c>
       <c r="E49">
-        <v>588384.0913601876</v>
+        <v>585337.0913601876</v>
       </c>
       <c r="F49">
-        <v>214725.0913601878</v>
+        <v>211678.0913601878</v>
       </c>
       <c r="G49">
-        <v>45867.95982992055</v>
+        <v>0.07836161505387271</v>
       </c>
       <c r="H49">
-        <v>433837.5008725198</v>
+        <v>0.7411754820873936</v>
       </c>
       <c r="I49">
-        <v>99592.05859163673</v>
+        <v>0.1701447935927106</v>
       </c>
       <c r="J49">
-        <v>6039.572066110554</v>
+        <v>0.01031810926602309</v>
       </c>
       <c r="K49">
         <v>3047</v>
@@ -5708,22 +5708,22 @@
         <v>76661.99460916442</v>
       </c>
       <c r="E103">
-        <v>384034.5382626585</v>
+        <v>383249.5382626585</v>
       </c>
       <c r="F103">
-        <v>303234.5382626585</v>
+        <v>302449.5382626585</v>
       </c>
       <c r="G103">
-        <v>11033.29629881419</v>
+        <v>0.02878880519681817</v>
       </c>
       <c r="H103">
-        <v>191522.0048231675</v>
+        <v>0.4997318605819395</v>
       </c>
       <c r="I103">
-        <v>166817.0300150177</v>
+        <v>0.4352700091205077</v>
       </c>
       <c r="J103">
-        <v>13877.20712565901</v>
+        <v>0.03620932510073455</v>
       </c>
       <c r="K103">
         <v>785</v>
@@ -5757,22 +5757,22 @@
         <v>34090.90909090909</v>
       </c>
       <c r="E104">
-        <v>85989.66517691736</v>
+        <v>85204.66517691736</v>
       </c>
       <c r="F104">
-        <v>48489.66517691736</v>
+        <v>47704.66517691736</v>
       </c>
       <c r="G104">
-        <v>4414.571922433571</v>
+        <v>0.0518113874782236</v>
       </c>
       <c r="H104">
-        <v>34459.25033435792</v>
+        <v>0.4044291502443838</v>
       </c>
       <c r="I104">
-        <v>42776.20161119862</v>
+        <v>0.5020406044948234</v>
       </c>
       <c r="J104">
-        <v>3554.641308927255</v>
+        <v>0.04171885778256935</v>
       </c>
       <c r="K104">
         <v>785</v>
@@ -5806,22 +5806,22 @@
         <v>42180.84255319149</v>
       </c>
       <c r="E105">
-        <v>233879.7207437111</v>
+        <v>233094.7207437111</v>
       </c>
       <c r="F105">
-        <v>157433.7207437111</v>
+        <v>156648.7207437111</v>
       </c>
       <c r="G105">
-        <v>38335.37548545442</v>
+        <v>0.1644626500469068</v>
       </c>
       <c r="H105">
-        <v>101848.1505819713</v>
+        <v>0.4369388987318761</v>
       </c>
       <c r="I105">
-        <v>86164.10744620691</v>
+        <v>0.3696527624962592</v>
       </c>
       <c r="J105">
-        <v>6747.087230078458</v>
+        <v>0.02894568872495793</v>
       </c>
       <c r="K105">
         <v>785</v>
@@ -5855,22 +5855,22 @@
         <v>124942.5340393344</v>
       </c>
       <c r="E106">
-        <v>365787.9973691748</v>
+        <v>364922.9973691748</v>
       </c>
       <c r="F106">
-        <v>227797.9973691748</v>
+        <v>226932.9973691748</v>
       </c>
       <c r="G106">
-        <v>17508.40581932702</v>
+        <v>0.04797835692885812</v>
       </c>
       <c r="H106">
-        <v>204515.5294969791</v>
+        <v>0.5604347519103617</v>
       </c>
       <c r="I106">
-        <v>132805.0078029786</v>
+        <v>0.3639261125234763</v>
       </c>
       <c r="J106">
-        <v>10094.05424989015</v>
+        <v>0.02766077863730382</v>
       </c>
       <c r="K106">
         <v>865</v>
@@ -5904,22 +5904,22 @@
         <v>118709.6861063465</v>
       </c>
       <c r="E107">
-        <v>503811.9293237749</v>
+        <v>502829.9293237749</v>
       </c>
       <c r="F107">
-        <v>364560.9293237749</v>
+        <v>363578.9293237749</v>
       </c>
       <c r="G107">
-        <v>26815.3848723824</v>
+        <v>0.05332893550796541</v>
       </c>
       <c r="H107">
-        <v>244967.1568461904</v>
+        <v>0.4871769609570211</v>
       </c>
       <c r="I107">
-        <v>214432.7621132417</v>
+        <v>0.4264518669396213</v>
       </c>
       <c r="J107">
-        <v>16614.62549196053</v>
+        <v>0.03304223659539225</v>
       </c>
       <c r="K107">
         <v>982</v>
@@ -5953,22 +5953,22 @@
         <v>213477.4162679426</v>
       </c>
       <c r="E108">
-        <v>506284.3639629543</v>
+        <v>505253.3639629543</v>
       </c>
       <c r="F108">
-        <v>257584.3639629543</v>
+        <v>256553.3639629543</v>
       </c>
       <c r="G108">
-        <v>41539.35441502423</v>
+        <v>0.08221489925215013</v>
       </c>
       <c r="H108">
-        <v>237787.4878362689</v>
+        <v>0.470630192288445</v>
       </c>
       <c r="I108">
-        <v>213873.6750614429</v>
+        <v>0.4232998537286816</v>
       </c>
       <c r="J108">
-        <v>12052.84665021836</v>
+        <v>0.02385505473072335</v>
       </c>
       <c r="K108">
         <v>1031</v>
@@ -6002,22 +6002,22 @@
         <v>239763.0621572212</v>
       </c>
       <c r="E109">
-        <v>633961.2506709985</v>
+        <v>633080.2506709985</v>
       </c>
       <c r="F109">
-        <v>376551.2506709985</v>
+        <v>375670.2506709985</v>
       </c>
       <c r="G109">
-        <v>24820.59376949406</v>
+        <v>0.03920607812862089</v>
       </c>
       <c r="H109">
-        <v>323220.5335714319</v>
+        <v>0.5105522297194584</v>
       </c>
       <c r="I109">
-        <v>266326.4776494942</v>
+        <v>0.420683597959684</v>
       </c>
       <c r="J109">
-        <v>18712.64568057827</v>
+        <v>0.02955809419223682</v>
       </c>
       <c r="K109">
         <v>881</v>
@@ -6051,22 +6051,22 @@
         <v>76373.17581599805</v>
       </c>
       <c r="E110">
-        <v>510710.2313191415</v>
+        <v>510049.2313191415</v>
       </c>
       <c r="F110">
-        <v>421610.2313191415</v>
+        <v>420949.2313191415</v>
       </c>
       <c r="G110">
-        <v>19031.47032065513</v>
+        <v>0.03731300657278514</v>
       </c>
       <c r="H110">
-        <v>268435.3013864441</v>
+        <v>0.5262929241010506</v>
       </c>
       <c r="I110">
-        <v>200708.8059167398</v>
+        <v>0.3935086920877151</v>
       </c>
       <c r="J110">
-        <v>21873.65369530245</v>
+        <v>0.04288537723844926</v>
       </c>
       <c r="K110">
         <v>661</v>
@@ -6100,22 +6100,22 @@
         <v>113688.1031567638</v>
       </c>
       <c r="E111">
-        <v>287156.9808822382</v>
+        <v>286919.9808822382</v>
       </c>
       <c r="F111">
-        <v>140205.9808822382</v>
+        <v>139968.9808822382</v>
       </c>
       <c r="G111">
-        <v>39662.13671849497</v>
+        <v>0.1382341396947662</v>
       </c>
       <c r="H111">
-        <v>145886.7713032815</v>
+        <v>0.508458040651963</v>
       </c>
       <c r="I111">
-        <v>96072.91275463889</v>
+        <v>0.3348421830338491</v>
       </c>
       <c r="J111">
-        <v>5298.160105822823</v>
+        <v>0.01846563661942167</v>
       </c>
       <c r="K111">
         <v>237</v>
@@ -6149,22 +6149,22 @@
         <v>173915.3582739309</v>
       </c>
       <c r="E112">
-        <v>239896.2584870655</v>
+        <v>239543.2584870655</v>
       </c>
       <c r="F112">
-        <v>46955.25848706553</v>
+        <v>46602.25848706553</v>
       </c>
       <c r="G112">
-        <v>16808.28570980255</v>
+        <v>0.07016805989850113</v>
       </c>
       <c r="H112">
-        <v>100314.5674725189</v>
+        <v>0.4187743295557431</v>
       </c>
       <c r="I112">
-        <v>120372.7864892857</v>
+        <v>0.50250959784696</v>
       </c>
       <c r="J112">
-        <v>2047.618815458349</v>
+        <v>0.008548012698795749</v>
       </c>
       <c r="K112">
         <v>353</v>
@@ -6198,22 +6198,22 @@
         <v>105457.4196508409</v>
       </c>
       <c r="E113">
-        <v>323985.5978613414</v>
+        <v>323200.5978613414</v>
       </c>
       <c r="F113">
-        <v>172150.5978613414</v>
+        <v>171365.5978613414</v>
       </c>
       <c r="G113">
-        <v>81108.20405088988</v>
+        <v>0.2509531374248469</v>
       </c>
       <c r="H113">
-        <v>182314.2684988095</v>
+        <v>0.5640901338215516</v>
       </c>
       <c r="I113">
-        <v>57054.84628242621</v>
+        <v>0.1765307572447738</v>
       </c>
       <c r="J113">
-        <v>2723.279029215764</v>
+        <v>0.008425971508827771</v>
       </c>
       <c r="K113">
         <v>785</v>
@@ -6247,22 +6247,22 @@
         <v>210518.4807253591</v>
       </c>
       <c r="E114">
-        <v>415044.5671690237</v>
+        <v>413687.5671690237</v>
       </c>
       <c r="F114">
-        <v>179627.5671690237</v>
+        <v>178270.5671690237</v>
       </c>
       <c r="G114">
-        <v>25465.27117531038</v>
+        <v>0.06155677181592897</v>
       </c>
       <c r="H114">
-        <v>221391.5983525023</v>
+        <v>0.535166188018521</v>
       </c>
       <c r="I114">
-        <v>160678.0838643972</v>
+        <v>0.388404430338482</v>
       </c>
       <c r="J114">
-        <v>6152.61377681388</v>
+        <v>0.01487260982706801</v>
       </c>
       <c r="K114">
         <v>1357</v>
@@ -6296,22 +6296,22 @@
         <v>133348.8706677649</v>
       </c>
       <c r="E115">
-        <v>182089.4704997374</v>
+        <v>181390.4704997374</v>
       </c>
       <c r="F115">
-        <v>14102.47049973736</v>
+        <v>13403.47049973736</v>
       </c>
       <c r="G115">
-        <v>34004.06958208667</v>
+        <v>0.1874633738387921</v>
       </c>
       <c r="H115">
-        <v>99420.66709643959</v>
+        <v>0.548103033321056</v>
       </c>
       <c r="I115">
-        <v>36164.40935871643</v>
+        <v>0.1993732595713665</v>
       </c>
       <c r="J115">
-        <v>11801.32446249472</v>
+        <v>0.06506033326878548</v>
       </c>
       <c r="K115">
         <v>699</v>
@@ -6345,22 +6345,22 @@
         <v>93631.45405437797</v>
       </c>
       <c r="E116">
-        <v>130615.7962531239</v>
+        <v>130025.7962531239</v>
       </c>
       <c r="F116">
-        <v>17825.79625312389</v>
+        <v>17235.79625312389</v>
       </c>
       <c r="G116">
-        <v>19540.43007724299</v>
+        <v>0.1502811798914366</v>
       </c>
       <c r="H116">
-        <v>67386.96767637755</v>
+        <v>0.5182584503862138</v>
       </c>
       <c r="I116">
-        <v>41604.93175293165</v>
+        <v>0.3199744431630971</v>
       </c>
       <c r="J116">
-        <v>1493.466746571709</v>
+        <v>0.01148592655925249</v>
       </c>
       <c r="K116">
         <v>590</v>
@@ -6394,22 +6394,22 @@
         <v>140122.8844337406</v>
       </c>
       <c r="E117">
-        <v>572869.5242628852</v>
+        <v>572072.5242628852</v>
       </c>
       <c r="F117">
-        <v>363394.5242628852</v>
+        <v>362597.5242628852</v>
       </c>
       <c r="G117">
-        <v>68735.78148019378</v>
+        <v>0.1201522159603099</v>
       </c>
       <c r="H117">
-        <v>343037.9205173994</v>
+        <v>0.5996406154261705</v>
       </c>
       <c r="I117">
-        <v>154629.3260751812</v>
+        <v>0.2702967185400503</v>
       </c>
       <c r="J117">
-        <v>5669.496190110898</v>
+        <v>0.009910450073469334</v>
       </c>
       <c r="K117">
         <v>797</v>
@@ -6443,22 +6443,22 @@
         <v>192641.2435207396</v>
       </c>
       <c r="E118">
-        <v>616120.3132087174</v>
+        <v>614281.3132087174</v>
       </c>
       <c r="F118">
-        <v>394182.3132087174</v>
+        <v>392343.3132087174</v>
       </c>
       <c r="G118">
-        <v>37610.70500416661</v>
+        <v>0.06122716774128441</v>
       </c>
       <c r="H118">
-        <v>314452.6101465253</v>
+        <v>0.5119032654663909</v>
       </c>
       <c r="I118">
-        <v>252541.3325958739</v>
+        <v>0.4111167427130682</v>
       </c>
       <c r="J118">
-        <v>9676.665462151648</v>
+        <v>0.0157528240792566</v>
       </c>
       <c r="K118">
         <v>1839</v>
@@ -6492,22 +6492,22 @@
         <v>187859.553457061</v>
       </c>
       <c r="E119">
-        <v>554615.7834714376</v>
+        <v>553495.7834714376</v>
       </c>
       <c r="F119">
-        <v>349326.7834714376</v>
+        <v>348206.7834714376</v>
       </c>
       <c r="G119">
-        <v>25779.53810670898</v>
+        <v>0.04657585274638193</v>
       </c>
       <c r="H119">
-        <v>253509.0026207823</v>
+        <v>0.4580143339680279</v>
       </c>
       <c r="I119">
-        <v>236880.022986851</v>
+        <v>0.4279707814595752</v>
       </c>
       <c r="J119">
-        <v>37327.21975709535</v>
+        <v>0.06743903182601493</v>
       </c>
       <c r="K119">
         <v>1120</v>
@@ -6541,22 +6541,22 @@
         <v>142161.6046520956</v>
       </c>
       <c r="E120">
-        <v>226745.0405157967</v>
+        <v>225790.0405157967</v>
       </c>
       <c r="F120">
-        <v>82975.04051579669</v>
+        <v>82020.04051579669</v>
       </c>
       <c r="G120">
-        <v>1902.437009285885</v>
+        <v>0.008425690543922759</v>
       </c>
       <c r="H120">
-        <v>109573.6160465505</v>
+        <v>0.4852898551071586</v>
       </c>
       <c r="I120">
-        <v>109026.9217931006</v>
+        <v>0.4828686045852089</v>
       </c>
       <c r="J120">
-        <v>5287.065666859837</v>
+        <v>0.02341584976370976</v>
       </c>
       <c r="K120">
         <v>955</v>
@@ -6590,22 +6590,22 @@
         <v>43254.28652665103</v>
       </c>
       <c r="E121">
-        <v>115623.7067697761</v>
+        <v>114921.7067697761</v>
       </c>
       <c r="F121">
-        <v>13223.70676977609</v>
+        <v>12521.70676977609</v>
       </c>
       <c r="G121">
-        <v>55368.17464043201</v>
+        <v>0.481790396233426</v>
       </c>
       <c r="H121">
-        <v>6793.195094746967</v>
+        <v>0.05911150543870575</v>
       </c>
       <c r="I121">
-        <v>45438.74165689872</v>
+        <v>0.395388677510043</v>
       </c>
       <c r="J121">
-        <v>7321.595377698375</v>
+        <v>0.0637094208178252</v>
       </c>
       <c r="K121">
         <v>702</v>
@@ -6639,22 +6639,22 @@
         <v>207716.095873672</v>
       </c>
       <c r="E122">
-        <v>290666.9562418167</v>
+        <v>289309.9562418167</v>
       </c>
       <c r="F122">
-        <v>35168.95624181666</v>
+        <v>33811.95624181666</v>
       </c>
       <c r="G122">
-        <v>41452.1561999403</v>
+        <v>0.1432793974269345</v>
       </c>
       <c r="H122">
-        <v>197510.2993637582</v>
+        <v>0.6826944427680578</v>
       </c>
       <c r="I122">
-        <v>49155.20666835771</v>
+        <v>0.1699049949987613</v>
       </c>
       <c r="J122">
-        <v>1192.294009760426</v>
+        <v>0.004121164806246279</v>
       </c>
       <c r="K122">
         <v>1357</v>
@@ -6688,22 +6688,22 @@
         <v>126348.693433955</v>
       </c>
       <c r="E123">
-        <v>178707.3595131705</v>
+        <v>177578.3595131705</v>
       </c>
       <c r="F123">
-        <v>46819.35951317049</v>
+        <v>45690.35951317049</v>
       </c>
       <c r="G123">
-        <v>6707.254170706236</v>
+        <v>0.03777067312196213</v>
       </c>
       <c r="H123">
-        <v>105691.3038208225</v>
+        <v>0.5951812152706798</v>
       </c>
       <c r="I123">
-        <v>63332.93725871002</v>
+        <v>0.3566478338483174</v>
       </c>
       <c r="J123">
-        <v>1846.86426293174</v>
+        <v>0.01040027775904059</v>
       </c>
       <c r="K123">
         <v>1129</v>
@@ -6737,22 +6737,22 @@
         <v>142359.7940300549</v>
       </c>
       <c r="E124">
-        <v>350292.4500167556</v>
+        <v>349334.4500167556</v>
       </c>
       <c r="F124">
-        <v>76278.45001675549</v>
+        <v>75320.45001675549</v>
       </c>
       <c r="G124">
-        <v>133733.2957117933</v>
+        <v>0.3828230960484398</v>
       </c>
       <c r="H124">
-        <v>97299.97213398576</v>
+        <v>0.2785295642308362</v>
       </c>
       <c r="I124">
-        <v>114395.7540876847</v>
+        <v>0.3274677149138821</v>
       </c>
       <c r="J124">
-        <v>3905.428083291782</v>
+        <v>0.01117962480684187</v>
       </c>
       <c r="K124">
         <v>958</v>
@@ -6786,22 +6786,22 @@
         <v>162775.9967020668</v>
       </c>
       <c r="E125">
-        <v>228241.1417344348</v>
+        <v>225547.1417344348</v>
       </c>
       <c r="F125">
-        <v>58605.20730862854</v>
+        <v>55911.20730862854</v>
       </c>
       <c r="G125">
-        <v>6878.240288200413</v>
+        <v>0.03049579895053175</v>
       </c>
       <c r="H125">
-        <v>139042.4855766293</v>
+        <v>0.6164675132099063</v>
       </c>
       <c r="I125">
-        <v>77237.64886740442</v>
+        <v>0.3424457001470055</v>
       </c>
       <c r="J125">
-        <v>2388.767002200685</v>
+        <v>0.01059098769255645</v>
       </c>
       <c r="K125">
         <v>2694</v>
@@ -6835,22 +6835,22 @@
         <v>108568.4424555644</v>
       </c>
       <c r="E126">
-        <v>195191.5247214137</v>
+        <v>194135.5247214137</v>
       </c>
       <c r="F126">
-        <v>68852.52472141365</v>
+        <v>67796.52472141365</v>
       </c>
       <c r="G126">
-        <v>15013.3128939171</v>
+        <v>0.07733418659702468</v>
       </c>
       <c r="H126">
-        <v>61587.69745567925</v>
+        <v>0.3172407396536939</v>
       </c>
       <c r="I126">
-        <v>109682.432831124</v>
+        <v>0.5649786817148452</v>
       </c>
       <c r="J126">
-        <v>7852.081540693271</v>
+        <v>0.04044639203443616</v>
       </c>
       <c r="K126">
         <v>1056</v>
@@ -6884,22 +6884,22 @@
         <v>158923.4835797619</v>
       </c>
       <c r="E127">
-        <v>491250.9382126621</v>
+        <v>489390.9382126621</v>
       </c>
       <c r="F127">
-        <v>119732.9382126621</v>
+        <v>117872.9382126621</v>
       </c>
       <c r="G127">
-        <v>215819.8286216896</v>
+        <v>0.440996781448181</v>
       </c>
       <c r="H127">
-        <v>193907.4002771812</v>
+        <v>0.3962218854835434</v>
       </c>
       <c r="I127">
-        <v>75573.00031389209</v>
+        <v>0.154422557536307</v>
       </c>
       <c r="J127">
-        <v>4090.708999899131</v>
+        <v>0.008358775531968548</v>
       </c>
       <c r="K127">
         <v>1860</v>
@@ -6933,22 +6933,22 @@
         <v>190971.2796305801</v>
       </c>
       <c r="E128">
-        <v>434120.3903106273</v>
+        <v>432141.3903106273</v>
       </c>
       <c r="F128">
-        <v>213931.3903106271</v>
+        <v>211952.3903106271</v>
       </c>
       <c r="G128">
-        <v>27890.10823587233</v>
+        <v>0.06453931250562381</v>
       </c>
       <c r="H128">
-        <v>290098.454043859</v>
+        <v>0.6713044863287302</v>
       </c>
       <c r="I128">
-        <v>112774.9557233904</v>
+        <v>0.2609677254991165</v>
       </c>
       <c r="J128">
-        <v>1377.872307505631</v>
+        <v>0.003188475666529429</v>
       </c>
       <c r="K128">
         <v>1979</v>
@@ -6982,22 +6982,22 @@
         <v>163806.536519134</v>
       </c>
       <c r="E129">
-        <v>445299.7055776317</v>
+        <v>443395.7055776317</v>
       </c>
       <c r="F129">
-        <v>256391.7055776318</v>
+        <v>254487.7055776318</v>
       </c>
       <c r="G129">
-        <v>25449.61937114237</v>
+        <v>0.0573970813226258</v>
       </c>
       <c r="H129">
-        <v>190835.1220844767</v>
+        <v>0.4303946106917457</v>
       </c>
       <c r="I129">
-        <v>222002.6316318564</v>
+        <v>0.5006873743683274</v>
       </c>
       <c r="J129">
-        <v>5108.3324901562</v>
+        <v>0.01152093361730092</v>
       </c>
       <c r="K129">
         <v>1904</v>
@@ -7031,22 +7031,22 @@
         <v>113797.5141178104</v>
       </c>
       <c r="E130">
-        <v>283641.4811496572</v>
+        <v>282481.4811496572</v>
       </c>
       <c r="F130">
-        <v>133198.4811496572</v>
+        <v>132038.4811496572</v>
       </c>
       <c r="G130">
-        <v>37431.69276791349</v>
+        <v>0.132510253824683</v>
       </c>
       <c r="H130">
-        <v>106174.6224932071</v>
+        <v>0.3758640108409666</v>
       </c>
       <c r="I130">
-        <v>134192.4559931275</v>
+        <v>0.4750486844198933</v>
       </c>
       <c r="J130">
-        <v>4682.709895409148</v>
+        <v>0.01657705091445719</v>
       </c>
       <c r="K130">
         <v>1160</v>
@@ -7080,22 +7080,22 @@
         <v>131949.3910043361</v>
       </c>
       <c r="E131">
-        <v>194139.4649786821</v>
+        <v>192876.4649786821</v>
       </c>
       <c r="F131">
-        <v>43000.46526580994</v>
+        <v>41737.46526580994</v>
       </c>
       <c r="G131">
-        <v>18473.45771713952</v>
+        <v>0.09577870332277878</v>
       </c>
       <c r="H131">
-        <v>87342.59678502149</v>
+        <v>0.4528421691815802</v>
       </c>
       <c r="I131">
-        <v>86018.68369257353</v>
+        <v>0.4459781223286151</v>
       </c>
       <c r="J131">
-        <v>1041.726783947557</v>
+        <v>0.005401005167025924</v>
       </c>
       <c r="K131">
         <v>1263</v>
@@ -7129,22 +7129,22 @@
         <v>61940.19361386459</v>
       </c>
       <c r="E132">
-        <v>93304.71794149016</v>
+        <v>92704.71794149016</v>
       </c>
       <c r="F132">
-        <v>29515.71794149018</v>
+        <v>28915.71794149018</v>
       </c>
       <c r="G132">
-        <v>1741.501072546535</v>
+        <v>0.01878546325598736</v>
       </c>
       <c r="H132">
-        <v>64290.47996073219</v>
+        <v>0.6934973902979632</v>
       </c>
       <c r="I132">
-        <v>24833.33401450295</v>
+        <v>0.2678756223623517</v>
       </c>
       <c r="J132">
-        <v>1839.402893708489</v>
+        <v>0.01984152408369781</v>
       </c>
       <c r="K132">
         <v>600</v>
@@ -7178,22 +7178,22 @@
         <v>52837.04901396133</v>
       </c>
       <c r="E133">
-        <v>78091.69584715727</v>
+        <v>77448.69584715727</v>
       </c>
       <c r="F133">
-        <v>5398.695847157273</v>
+        <v>4755.695847157273</v>
       </c>
       <c r="G133">
-        <v>19310.45198970257</v>
+        <v>0.2493321776238968</v>
       </c>
       <c r="H133">
-        <v>8948.393013992898</v>
+        <v>0.1155396216309735</v>
       </c>
       <c r="I133">
-        <v>48319.18490151758</v>
+        <v>0.6238863595182296</v>
       </c>
       <c r="J133">
-        <v>870.6659419442307</v>
+        <v>0.01124184122690025</v>
       </c>
       <c r="K133">
         <v>643</v>
@@ -7227,22 +7227,22 @@
         <v>65332.57981771554</v>
       </c>
       <c r="E134">
-        <v>117465</v>
+        <v>116844</v>
       </c>
       <c r="F134">
-        <v>621</v>
+        <v>0</v>
       </c>
       <c r="G134">
-        <v>49095.69595156021</v>
+        <v>0.4201815750193439</v>
       </c>
       <c r="H134">
-        <v>56274.68003399203</v>
+        <v>0.4816223343431587</v>
       </c>
       <c r="I134">
-        <v>10784.56451189669</v>
+        <v>0.09229883016583382</v>
       </c>
       <c r="J134">
-        <v>689.059502551051</v>
+        <v>0.005897260471663509</v>
       </c>
       <c r="K134">
         <v>621</v>
@@ -7276,22 +7276,22 @@
         <v>130289.2303333466</v>
       </c>
       <c r="E135">
-        <v>241711.4482929232</v>
+        <v>240712.4482929232</v>
       </c>
       <c r="F135">
-        <v>63880.44829292319</v>
+        <v>62881.44829292319</v>
       </c>
       <c r="G135">
-        <v>40270.76712627187</v>
+        <v>0.1672982324423302</v>
       </c>
       <c r="H135">
-        <v>161714.6272065068</v>
+        <v>0.6718166357965669</v>
       </c>
       <c r="I135">
-        <v>38318.99952879709</v>
+        <v>0.1591899372074296</v>
       </c>
       <c r="J135">
-        <v>408.0544313475194</v>
+        <v>0.001695194553673259</v>
       </c>
       <c r="K135">
         <v>999</v>
@@ -7325,22 +7325,22 @@
         <v>296956.4619695917</v>
       </c>
       <c r="E136">
-        <v>900357.6407605257</v>
+        <v>897995.6407605257</v>
       </c>
       <c r="F136">
-        <v>443921.6407605257</v>
+        <v>441559.6407605257</v>
       </c>
       <c r="G136">
-        <v>170510.0024657501</v>
+        <v>0.1898784300571245</v>
       </c>
       <c r="H136">
-        <v>629410.3854276737</v>
+        <v>0.7009058361292453</v>
       </c>
       <c r="I136">
-        <v>97970.04453376858</v>
+        <v>0.1090985747445236</v>
       </c>
       <c r="J136">
-        <v>105.2083333333333</v>
+        <v>0.0001171590691066505</v>
       </c>
       <c r="K136">
         <v>2362</v>
@@ -7374,22 +7374,22 @@
         <v>381979.5120743748</v>
       </c>
       <c r="E137">
-        <v>703403.5778045077</v>
+        <v>701818.5778045077</v>
       </c>
       <c r="F137">
-        <v>264189.5778045078</v>
+        <v>262604.5778045078</v>
       </c>
       <c r="G137">
-        <v>52371.23864402645</v>
+        <v>0.07462218912451547</v>
       </c>
       <c r="H137">
-        <v>417666.2777237308</v>
+        <v>0.5951200081227718</v>
       </c>
       <c r="I137">
-        <v>206669.5401428094</v>
+        <v>0.2944771578850644</v>
       </c>
       <c r="J137">
-        <v>25111.52129394113</v>
+        <v>0.03578064486764836</v>
       </c>
       <c r="K137">
         <v>1585</v>
@@ -7423,22 +7423,22 @@
         <v>192226.153255183</v>
       </c>
       <c r="E138">
-        <v>429287.6422917357</v>
+        <v>427514.6422917357</v>
       </c>
       <c r="F138">
-        <v>199906.6422917358</v>
+        <v>198133.6422917358</v>
       </c>
       <c r="G138">
-        <v>34858.12196674335</v>
+        <v>0.08153667387830939</v>
       </c>
       <c r="H138">
-        <v>165708.2577949162</v>
+        <v>0.3876083796957694</v>
       </c>
       <c r="I138">
-        <v>217660.5670229841</v>
+        <v>0.5091300869981726</v>
       </c>
       <c r="J138">
-        <v>9287.695507092154</v>
+        <v>0.02172485942774853</v>
       </c>
       <c r="K138">
         <v>1773</v>
@@ -7472,22 +7472,22 @@
         <v>119848.9748692562</v>
       </c>
       <c r="E139">
-        <v>531249.8763129682</v>
+        <v>529426.8763129682</v>
       </c>
       <c r="F139">
-        <v>63524.78985417978</v>
+        <v>61701.78985417978</v>
       </c>
       <c r="G139">
-        <v>352591.9989859592</v>
+        <v>0.6659880991336868</v>
       </c>
       <c r="H139">
-        <v>119288.2822915654</v>
+        <v>0.2253158795456554</v>
       </c>
       <c r="I139">
-        <v>52026.12343183497</v>
+        <v>0.09826876148440936</v>
       </c>
       <c r="J139">
-        <v>5520.471603608726</v>
+        <v>0.01042725983624852</v>
       </c>
       <c r="K139">
         <v>1823</v>
@@ -7521,22 +7521,22 @@
         <v>159750.6359031179</v>
       </c>
       <c r="E140">
-        <v>831752.1765858305</v>
+        <v>828511.1765858305</v>
       </c>
       <c r="F140">
-        <v>466323.0861011941</v>
+        <v>463082.0861011941</v>
       </c>
       <c r="G140">
-        <v>225654.13749406</v>
+        <v>0.2723610059479785</v>
       </c>
       <c r="H140">
-        <v>453970.1539640548</v>
+        <v>0.5479348580845913</v>
       </c>
       <c r="I140">
-        <v>147751.8019239723</v>
+        <v>0.1783341083373614</v>
       </c>
       <c r="J140">
-        <v>1135.08320374338</v>
+        <v>0.001370027630068778</v>
       </c>
       <c r="K140">
         <v>3241</v>
@@ -7570,22 +7570,22 @@
         <v>312265.2799999999</v>
       </c>
       <c r="E141">
-        <v>1061431.57</v>
+        <v>1058331.57</v>
       </c>
       <c r="F141">
-        <v>731184</v>
+        <v>728084</v>
       </c>
       <c r="G141">
-        <v>16689.38999999998</v>
+        <v>0.01576952863647447</v>
       </c>
       <c r="H141">
-        <v>808520.0699999999</v>
+        <v>0.7639572445145901</v>
       </c>
       <c r="I141">
-        <v>230745.61</v>
+        <v>0.2180277112965647</v>
       </c>
       <c r="J141">
-        <v>2376.5</v>
+        <v>0.002245515552370795</v>
       </c>
       <c r="K141">
         <v>3100</v>
@@ -7619,22 +7619,22 @@
         <v>211925.58</v>
       </c>
       <c r="E142">
-        <v>527584.75</v>
+        <v>525568.75</v>
       </c>
       <c r="F142">
-        <v>294432</v>
+        <v>292416</v>
       </c>
       <c r="G142">
-        <v>19663.32000000002</v>
+        <v>0.03741341166117661</v>
       </c>
       <c r="H142">
-        <v>83324.34000000003</v>
+        <v>0.1585412755229454</v>
       </c>
       <c r="I142">
-        <v>413104.81</v>
+        <v>0.7860147887407689</v>
       </c>
       <c r="J142">
-        <v>9476.279999999999</v>
+        <v>0.01803052407510911</v>
       </c>
       <c r="K142">
         <v>2016</v>
@@ -7668,22 +7668,22 @@
         <v>142683.8700000001</v>
       </c>
       <c r="E143">
-        <v>356840.2950084583</v>
+        <v>354590.2950084583</v>
       </c>
       <c r="F143">
-        <v>60368.61500845803</v>
+        <v>58118.61500845803</v>
       </c>
       <c r="G143">
-        <v>150529.1818094378</v>
+        <v>0.4245157973256068</v>
       </c>
       <c r="H143">
-        <v>34645.95369153097</v>
+        <v>0.09770699925869245</v>
       </c>
       <c r="I143">
-        <v>160405.287068377</v>
+        <v>0.4523679562762732</v>
       </c>
       <c r="J143">
-        <v>9009.872439112462</v>
+        <v>0.02540924713942761</v>
       </c>
       <c r="K143">
         <v>2250</v>
@@ -7717,22 +7717,22 @@
         <v>146311.7000000002</v>
       </c>
       <c r="E144">
-        <v>225966.6918328513</v>
+        <v>224073.6918328513</v>
       </c>
       <c r="F144">
-        <v>68154.37183285112</v>
+        <v>66261.37183285112</v>
       </c>
       <c r="G144">
-        <v>8504.795816288408</v>
+        <v>0.03795535186090742</v>
       </c>
       <c r="H144">
-        <v>192156.7951862505</v>
+        <v>0.8575607141314504</v>
       </c>
       <c r="I144">
-        <v>18270.21892891872</v>
+        <v>0.08153665331915659</v>
       </c>
       <c r="J144">
-        <v>5141.881901393666</v>
+        <v>0.02294728068848562</v>
       </c>
       <c r="K144">
         <v>1893</v>
@@ -7766,22 +7766,22 @@
         <v>91244.78999999999</v>
       </c>
       <c r="E145">
-        <v>170993.38566547</v>
+        <v>169136.38566547</v>
       </c>
       <c r="F145">
-        <v>41637.37566547004</v>
+        <v>39780.37566547004</v>
       </c>
       <c r="G145">
-        <v>37307.70892494247</v>
+        <v>0.2205776644579145</v>
       </c>
       <c r="H145">
-        <v>52955.34955098764</v>
+        <v>0.3130925929546969</v>
       </c>
       <c r="I145">
-        <v>76805.7024528827</v>
+        <v>0.4541051421353799</v>
       </c>
       <c r="J145">
-        <v>2067.62473665723</v>
+        <v>0.01222460045200874</v>
       </c>
       <c r="K145">
         <v>1857</v>
@@ -7812,22 +7812,22 @@
         <v>131529.48</v>
       </c>
       <c r="E146">
-        <v>209984.2366804202</v>
+        <v>208952.2366804202</v>
       </c>
       <c r="F146">
-        <v>40539.14668042018</v>
+        <v>39507.14668042018</v>
       </c>
       <c r="G146">
-        <v>40333.36628288364</v>
+        <v>0.1930267266991312</v>
       </c>
       <c r="H146">
-        <v>138725.8019839387</v>
+        <v>0.6639115435558196</v>
       </c>
       <c r="I146">
-        <v>27985.34541243719</v>
+        <v>0.1339317820045118</v>
       </c>
       <c r="J146">
-        <v>1907.723001160657</v>
+        <v>0.009129947740537488</v>
       </c>
       <c r="K146">
         <v>1032</v>
@@ -7858,22 +7858,22 @@
         <v>105441</v>
       </c>
       <c r="E147">
-        <v>253130</v>
+        <v>251468</v>
       </c>
       <c r="F147">
-        <v>70790</v>
+        <v>69128</v>
       </c>
       <c r="G147">
-        <v>75731</v>
+        <v>0.3011556142332225</v>
       </c>
       <c r="H147">
-        <v>49856</v>
+        <v>0.1982598183466684</v>
       </c>
       <c r="I147">
-        <v>111744</v>
+        <v>0.4443666788617239</v>
       </c>
       <c r="J147">
-        <v>14137</v>
+        <v>0.05621788855838517</v>
       </c>
       <c r="K147">
         <v>1662</v>
@@ -7904,22 +7904,22 @@
         <v>368156</v>
       </c>
       <c r="E148">
-        <v>650875</v>
+        <v>649187</v>
       </c>
       <c r="F148">
-        <v>235634</v>
+        <v>233946</v>
       </c>
       <c r="G148">
-        <v>58148</v>
+        <v>0.08957049355578593</v>
       </c>
       <c r="H148">
-        <v>549648</v>
+        <v>0.8466712981005473</v>
       </c>
       <c r="I148">
-        <v>35814</v>
+        <v>0.0551674633041019</v>
       </c>
       <c r="J148">
-        <v>5577</v>
+        <v>0.008590745039564871</v>
       </c>
       <c r="K148">
         <v>1688</v>
@@ -7950,22 +7950,22 @@
         <v>122621.6560924115</v>
       </c>
       <c r="E149">
-        <v>336292.2566479851</v>
+        <v>333723.2566479851</v>
       </c>
       <c r="F149">
-        <v>181274.2566479851</v>
+        <v>178705.2566479851</v>
       </c>
       <c r="G149">
-        <v>34453.35591884049</v>
+        <v>0.1032393015245631</v>
       </c>
       <c r="H149">
-        <v>167989.5012402972</v>
+        <v>0.5033796653180044</v>
       </c>
       <c r="I149">
-        <v>124533.034608577</v>
+        <v>0.3731625894443905</v>
       </c>
       <c r="J149">
-        <v>6747.364880270348</v>
+        <v>0.02021844371304198</v>
       </c>
       <c r="K149">
         <v>2569</v>
@@ -7996,22 +7996,22 @@
         <v>77872.43072344859</v>
       </c>
       <c r="E150">
-        <v>195333.6957705026</v>
+        <v>193762.6957705026</v>
       </c>
       <c r="F150">
-        <v>75338.6957705026</v>
+        <v>73767.6957705026</v>
       </c>
       <c r="G150">
-        <v>43561.93892789539</v>
+        <v>0.2248210820698492</v>
       </c>
       <c r="H150">
-        <v>115288.4466578857</v>
+        <v>0.5949981558598678</v>
       </c>
       <c r="I150">
-        <v>34456.6959116603</v>
+        <v>0.1778293586112761</v>
       </c>
       <c r="J150">
-        <v>455.6142730612697</v>
+        <v>0.002351403459006942</v>
       </c>
       <c r="K150">
         <v>1571</v>

</xml_diff>